<commit_message>
r145 push (by wuwu/kaitokiwa)
</commit_message>
<xml_diff>
--- a/docs/China Set Trains.xlsx
+++ b/docs/China Set Trains.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GRF\China-Set\China-Set-Trains\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C58CBE-8928-4BA0-9FFC-E71EF4C03163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9675C8E5-4570-4586-AA7E-37387B4A3357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="13770" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="13770" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Loco" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="351">
   <si>
     <t>name</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1201,6 +1201,185 @@
   </si>
   <si>
     <t>jsq5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RZ225Z</t>
+  </si>
+  <si>
+    <t>rz225z</t>
+  </si>
+  <si>
+    <t>CC_PASSENGERS</t>
+  </si>
+  <si>
+    <t>RZ125Z</t>
+  </si>
+  <si>
+    <t>rz125z</t>
+  </si>
+  <si>
+    <t>RZT25Z</t>
+  </si>
+  <si>
+    <t>rzt25z</t>
+  </si>
+  <si>
+    <t>CA25Z</t>
+  </si>
+  <si>
+    <t>ca25z</t>
+  </si>
+  <si>
+    <t>KD25Z</t>
+  </si>
+  <si>
+    <t>kd25z</t>
+  </si>
+  <si>
+    <t>RZXL25Z</t>
+  </si>
+  <si>
+    <t>rzxl25z</t>
+  </si>
+  <si>
+    <t>CC_MAIL</t>
+  </si>
+  <si>
+    <t>SRZ225Z</t>
+  </si>
+  <si>
+    <t>srz225z</t>
+  </si>
+  <si>
+    <t>SRZ125Z</t>
+  </si>
+  <si>
+    <t>srz125z</t>
+  </si>
+  <si>
+    <t>SCA25Z</t>
+  </si>
+  <si>
+    <t>sca25z</t>
+  </si>
+  <si>
+    <t>SRZXL25Z</t>
+  </si>
+  <si>
+    <t>srzxl25z</t>
+  </si>
+  <si>
+    <t>Xizi Livery by wuwu
+Guangzhou Livery by Haiyan
+Beijing Livery by DF43110</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DF4BK</t>
+  </si>
+  <si>
+    <t>df4bk</t>
+  </si>
+  <si>
+    <t>DF4B (Dongfeng 4 Diesel Locomotive, Passenger Version)</t>
+  </si>
+  <si>
+    <t>Diesel</t>
+  </si>
+  <si>
+    <t>model: Mikhail; alternative livery: DF43110</t>
+  </si>
+  <si>
+    <t>DF4BH</t>
+  </si>
+  <si>
+    <t>df4bh</t>
+  </si>
+  <si>
+    <t>DF4B (Dongfeng 4 Diesel Locomotive, Freight Version)</t>
+  </si>
+  <si>
+    <t>DF7G</t>
+  </si>
+  <si>
+    <t>df7g</t>
+  </si>
+  <si>
+    <t>DF7G (Dongfeng 7G Diesel Locomotive)</t>
+  </si>
+  <si>
+    <t>model: EMB190</t>
+  </si>
+  <si>
+    <t>DF7G-5000</t>
+  </si>
+  <si>
+    <t>df7g5000</t>
+  </si>
+  <si>
+    <t>DF7G-8000</t>
+  </si>
+  <si>
+    <t>df7g8000</t>
+  </si>
+  <si>
+    <t>DFH7</t>
+  </si>
+  <si>
+    <t>dfh7</t>
+  </si>
+  <si>
+    <t>mikhail</t>
+  </si>
+  <si>
+    <t>DFH7B</t>
+  </si>
+  <si>
+    <t>dfh7b</t>
+  </si>
+  <si>
+    <t>HXN5B</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>hxn5b</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>inf</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>wuwu</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>EMB190</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SYW25</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SRW25</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>syw25</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>srw25</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>wuwu</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>wuwu</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1254,10 +1433,16 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1539,18 +1724,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF37"/>
+  <dimension ref="A1:AF45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K31" sqref="K31"/>
+    <sheetView topLeftCell="X1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AE28" sqref="AE28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="28" width="8.6640625" style="1"/>
-    <col min="29" max="30" width="8.6640625" style="2"/>
+    <col min="26" max="28" width="8.58203125" style="1"/>
+    <col min="29" max="30" width="8.58203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.3">
@@ -1708,7 +1893,7 @@
         <v>165625</v>
       </c>
       <c r="T2">
-        <f t="shared" ref="T2:T24" si="0">MEDIAN(0, 255, ROUND(SQRT(K2)/100+SQRT(L2)+P2+40/J2-2,0))</f>
+        <f t="shared" ref="T2:T32" si="0">MEDIAN(0, 255, ROUND(SQRT(K2)/100+SQRT(L2)+P2+40/J2-2,0))</f>
         <v>39</v>
       </c>
       <c r="U2">
@@ -1756,19 +1941,19 @@
         <v>1934</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O29" si="1">M3-N3</f>
+        <f t="shared" ref="O3:O37" si="1">M3-N3</f>
         <v>0</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:Q29" si="2">O3*P3*9.8</f>
+        <f t="shared" ref="Q3:Q45" si="2">O3*P3*9.8</f>
         <v>0</v>
       </c>
       <c r="R3">
-        <f t="shared" ref="R3:R29" si="3">MEDIAN(255, ROUND((M3/10+SQRT(K3)/20+SQRT(L3)+P3+20-J3), 0), 0)</f>
+        <f t="shared" ref="R3:R37" si="3">MEDIAN(255, ROUND((M3/10+SQRT(K3)/20+SQRT(L3)+P3+20-J3), 0), 0)</f>
         <v>20</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="S3:S29" si="4">R3*50000/16</f>
+        <f t="shared" ref="S3:S37" si="4">R3*50000/16</f>
         <v>62500</v>
       </c>
       <c r="T3" t="e">
@@ -1776,15 +1961,15 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U3" t="e">
-        <f t="shared" ref="U3:U29" si="5">IF(E3="Steam", T3*350/16*12, IF(E3="Diesel", T3*325/16*12,  T3*300/16*12))</f>
+        <f t="shared" ref="U3:U37" si="5">IF(E3="Steam", T3*350/16*12, IF(E3="Diesel", T3*325/16*12,  T3*300/16*12))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="V3">
-        <f t="shared" ref="V3:V29" si="6">W3+X3+Y3</f>
+        <f t="shared" ref="V3:V37" si="6">W3+X3+Y3</f>
         <v>0</v>
       </c>
       <c r="AC3" s="2" t="e">
-        <f t="shared" ref="AC3:AC29" si="7">AVERAGE(Z3:AB3)</f>
+        <f t="shared" ref="AC3:AC37" si="7">AVERAGE(Z3:AB3)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2855,68 +3040,104 @@
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>319</v>
       </c>
       <c r="B21" t="s">
-        <v>72</v>
+        <v>320</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>321</v>
       </c>
       <c r="E21" t="s">
-        <v>52</v>
+        <v>322</v>
       </c>
       <c r="F21">
-        <v>1958</v>
+        <v>1969</v>
+      </c>
+      <c r="G21">
+        <v>30</v>
+      </c>
+      <c r="H21">
+        <v>60</v>
+      </c>
+      <c r="I21">
+        <v>40</v>
+      </c>
+      <c r="J21">
+        <v>14</v>
+      </c>
+      <c r="K21">
+        <v>120</v>
+      </c>
+      <c r="L21">
+        <v>2610</v>
+      </c>
+      <c r="M21">
+        <v>138</v>
       </c>
       <c r="O21">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>138</v>
+      </c>
+      <c r="P21">
+        <v>0.24199999999999999</v>
       </c>
       <c r="Q21">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>327.28080000000006</v>
       </c>
       <c r="R21">
-        <f t="shared" si="3"/>
-        <v>20</v>
+        <f t="shared" ref="R21:R45" si="32">MEDIAN(255, ROUND((M21/10+SQRT(K21)/20+SQRT(L21)+P21+20-J21), 0), 0)</f>
+        <v>72</v>
       </c>
       <c r="S21">
-        <f t="shared" si="4"/>
-        <v>62500</v>
-      </c>
-      <c r="T21" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="S21:S45" si="33">R21*50000/16</f>
+        <v>225000</v>
+      </c>
+      <c r="T21">
+        <f t="shared" ref="T21:T45" si="34">MEDIAN(0, 255, ROUND(SQRT(K21)/100+SQRT(L21)+P21+40/J21-2,0))</f>
+        <v>52</v>
+      </c>
+      <c r="U21">
+        <f t="shared" ref="U21:U45" si="35">IF(E21="Steam", T21*350/16*12, IF(E21="Diesel", T21*325/16*12,  T21*300/16*12))</f>
+        <v>12675</v>
+      </c>
+      <c r="V21">
+        <v>10</v>
+      </c>
+      <c r="W21">
+        <v>1</v>
+      </c>
+      <c r="X21">
+        <v>8</v>
+      </c>
+      <c r="Y21">
+        <v>1</v>
+      </c>
+      <c r="AC21" s="2" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="U21" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="V21">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AC21" s="2" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+      <c r="AD21" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>324</v>
       </c>
       <c r="B22" t="s">
-        <v>73</v>
+        <v>325</v>
       </c>
       <c r="D22" t="s">
-        <v>32</v>
+        <v>326</v>
       </c>
       <c r="E22" t="s">
-        <v>52</v>
+        <v>322</v>
       </c>
       <c r="F22">
-        <v>1978</v>
+        <v>1969</v>
       </c>
       <c r="G22">
         <v>30</v>
@@ -2925,80 +3146,101 @@
         <v>60</v>
       </c>
       <c r="I22">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="J22">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="K22">
         <v>100</v>
       </c>
       <c r="L22">
-        <v>5914</v>
+        <v>2610</v>
       </c>
       <c r="M22">
         <v>138</v>
       </c>
       <c r="O22">
-        <f t="shared" si="1"/>
         <v>138</v>
       </c>
       <c r="P22">
-        <v>0.34699999999999998</v>
+        <v>0.30499999999999999</v>
       </c>
       <c r="Q22">
         <f t="shared" si="2"/>
-        <v>469.28280000000001</v>
+        <v>412.48199999999997</v>
       </c>
       <c r="R22">
-        <f t="shared" si="3"/>
-        <v>102</v>
+        <f t="shared" si="32"/>
+        <v>72</v>
       </c>
       <c r="S22">
-        <f t="shared" si="4"/>
-        <v>318750</v>
+        <f t="shared" si="33"/>
+        <v>225000</v>
       </c>
       <c r="T22">
-        <f t="shared" si="0"/>
-        <v>79</v>
+        <f t="shared" si="34"/>
+        <v>52</v>
       </c>
       <c r="U22">
-        <f t="shared" si="5"/>
-        <v>17775</v>
+        <f t="shared" si="35"/>
+        <v>12675</v>
       </c>
       <c r="V22">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AC22" s="2" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <v>10</v>
+      </c>
+      <c r="W22">
+        <v>1</v>
+      </c>
+      <c r="X22">
+        <v>8</v>
+      </c>
+      <c r="Y22">
+        <v>1</v>
+      </c>
+      <c r="Z22" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA22" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB22" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC22" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD22" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>327</v>
       </c>
       <c r="B23" t="s">
-        <v>74</v>
+        <v>328</v>
       </c>
       <c r="D23" t="s">
-        <v>33</v>
+        <v>329</v>
       </c>
       <c r="E23" t="s">
-        <v>52</v>
+        <v>322</v>
       </c>
       <c r="F23">
-        <v>1985</v>
+        <v>2002</v>
       </c>
       <c r="G23">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="H23">
         <v>60</v>
       </c>
       <c r="I23">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="J23">
         <v>20</v>
@@ -3007,484 +3249,470 @@
         <v>100</v>
       </c>
       <c r="L23">
-        <v>8702</v>
+        <v>2189</v>
       </c>
       <c r="M23">
-        <v>184</v>
+        <v>138</v>
       </c>
       <c r="O23">
-        <f t="shared" si="1"/>
-        <v>184</v>
+        <v>138</v>
       </c>
       <c r="P23">
-        <v>0.34799999999999998</v>
+        <v>0.32700000000000001</v>
       </c>
       <c r="Q23">
         <f t="shared" si="2"/>
-        <v>627.5136</v>
+        <v>442.23480000000006</v>
       </c>
       <c r="R23">
-        <f t="shared" si="3"/>
-        <v>113</v>
+        <f t="shared" si="32"/>
+        <v>61</v>
       </c>
       <c r="S23">
-        <f t="shared" si="4"/>
-        <v>353125</v>
+        <f t="shared" si="33"/>
+        <v>190625</v>
       </c>
       <c r="T23">
-        <f t="shared" si="0"/>
-        <v>94</v>
+        <f t="shared" si="34"/>
+        <v>47</v>
       </c>
       <c r="U23">
-        <f t="shared" si="5"/>
-        <v>21150</v>
+        <f t="shared" si="35"/>
+        <v>11456.25</v>
       </c>
       <c r="V23">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AC23" s="2" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <f t="shared" ref="V23:V27" si="36">W23+X23+Y23</f>
+        <v>9</v>
+      </c>
+      <c r="W23">
+        <v>2</v>
+      </c>
+      <c r="X23">
+        <v>5</v>
+      </c>
+      <c r="Y23">
+        <v>2</v>
+      </c>
+      <c r="AD23" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="AE23" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>331</v>
       </c>
       <c r="B24" t="s">
-        <v>75</v>
+        <v>332</v>
       </c>
       <c r="D24" t="s">
-        <v>39</v>
+        <v>331</v>
       </c>
       <c r="E24" t="s">
-        <v>52</v>
+        <v>322</v>
       </c>
       <c r="F24">
-        <v>1994</v>
+        <v>2003</v>
       </c>
       <c r="G24">
-        <v>30</v>
-      </c>
-      <c r="H24">
-        <v>50</v>
-      </c>
-      <c r="I24">
-        <v>30</v>
+        <v>40</v>
+      </c>
+      <c r="H24" t="s">
+        <v>261</v>
       </c>
       <c r="J24">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="K24">
-        <v>170</v>
+        <v>100</v>
       </c>
       <c r="L24">
-        <v>4894</v>
+        <v>2039</v>
       </c>
       <c r="M24">
-        <v>88</v>
+        <v>138</v>
       </c>
       <c r="O24">
-        <f t="shared" si="1"/>
-        <v>88</v>
+        <v>138</v>
       </c>
       <c r="P24">
-        <v>0.24299999999999999</v>
+        <v>0.32200000000000001</v>
       </c>
       <c r="Q24">
         <f t="shared" si="2"/>
-        <v>209.56320000000002</v>
+        <v>435.47280000000001</v>
       </c>
       <c r="R24">
-        <f t="shared" si="3"/>
-        <v>90</v>
+        <f t="shared" si="32"/>
+        <v>64</v>
       </c>
       <c r="S24">
-        <f t="shared" si="4"/>
-        <v>281250</v>
+        <f t="shared" si="33"/>
+        <v>200000</v>
       </c>
       <c r="T24">
-        <f t="shared" si="0"/>
-        <v>72</v>
+        <f t="shared" si="34"/>
+        <v>46</v>
       </c>
       <c r="U24">
-        <f t="shared" si="5"/>
-        <v>16200</v>
+        <f t="shared" si="35"/>
+        <v>11212.5</v>
       </c>
       <c r="V24">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AC24" s="2" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="AD24" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>333</v>
+      </c>
+      <c r="B25" t="s">
+        <v>334</v>
+      </c>
+      <c r="D25" t="s">
+        <v>333</v>
+      </c>
+      <c r="E25" t="s">
+        <v>322</v>
+      </c>
+      <c r="F25">
+        <v>2006</v>
+      </c>
+      <c r="G25">
         <v>40</v>
       </c>
-      <c r="B25" t="s">
-        <v>76</v>
-      </c>
-      <c r="C25">
-        <v>6144</v>
-      </c>
-      <c r="D25" t="s">
-        <v>40</v>
-      </c>
-      <c r="E25" t="s">
-        <v>52</v>
-      </c>
-      <c r="F25">
-        <v>2010</v>
-      </c>
-      <c r="G25">
-        <v>30</v>
-      </c>
       <c r="H25" t="s">
-        <v>91</v>
+        <v>261</v>
       </c>
       <c r="J25">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="K25">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="L25">
-        <v>9655</v>
+        <v>2175</v>
       </c>
       <c r="M25">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="O25">
-        <f t="shared" si="1"/>
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="P25">
-        <v>0.38450000000000001</v>
+        <v>0.32100000000000001</v>
       </c>
       <c r="Q25">
         <f t="shared" si="2"/>
-        <v>519.99779999999998</v>
+        <v>440.41200000000003</v>
       </c>
       <c r="R25">
-        <f t="shared" si="3"/>
-        <v>127</v>
+        <f t="shared" si="32"/>
+        <v>65</v>
       </c>
       <c r="S25">
-        <f t="shared" si="4"/>
-        <v>396875</v>
+        <f t="shared" si="33"/>
+        <v>203125</v>
       </c>
       <c r="T25">
-        <f>MEDIAN(0, 255, ROUND(SQRT(K25)/100+SQRT(L25)+P25+40/J25-2,0))</f>
-        <v>103</v>
+        <f t="shared" si="34"/>
+        <v>48</v>
       </c>
       <c r="U25">
-        <f t="shared" si="5"/>
-        <v>23175</v>
+        <f t="shared" si="35"/>
+        <v>11700</v>
       </c>
       <c r="V25">
-        <f t="shared" si="6"/>
-        <v>10</v>
-      </c>
-      <c r="W25">
-        <v>1</v>
-      </c>
-      <c r="X25">
-        <v>8</v>
-      </c>
-      <c r="Y25">
-        <v>1</v>
-      </c>
-      <c r="Z25" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA25" s="1">
-        <v>1</v>
-      </c>
-      <c r="AB25" s="1">
-        <v>1</v>
-      </c>
-      <c r="AC25" s="2">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f t="shared" si="36"/>
+        <v>0</v>
       </c>
       <c r="AD25" s="2" t="s">
-        <v>92</v>
+        <v>262</v>
       </c>
       <c r="AE25" t="s">
-        <v>93</v>
+        <v>330</v>
       </c>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>335</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>336</v>
       </c>
       <c r="D26" t="s">
-        <v>41</v>
+        <v>335</v>
       </c>
       <c r="E26" t="s">
-        <v>52</v>
+        <v>322</v>
       </c>
       <c r="F26">
-        <v>2012</v>
+        <v>1988</v>
+      </c>
+      <c r="G26">
+        <v>30</v>
+      </c>
+      <c r="H26">
+        <v>60</v>
+      </c>
+      <c r="I26">
+        <v>30</v>
+      </c>
+      <c r="J26">
+        <v>24</v>
+      </c>
+      <c r="K26">
+        <v>80</v>
+      </c>
+      <c r="L26">
+        <v>1080</v>
+      </c>
+      <c r="M26">
+        <v>92</v>
       </c>
       <c r="O26">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>92</v>
+      </c>
+      <c r="P26">
+        <v>0.32900000000000001</v>
       </c>
       <c r="Q26">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>296.62640000000005</v>
       </c>
       <c r="R26">
-        <f t="shared" si="3"/>
-        <v>20</v>
+        <f t="shared" si="32"/>
+        <v>39</v>
       </c>
       <c r="S26">
-        <f t="shared" si="4"/>
-        <v>62500</v>
-      </c>
-      <c r="T26" t="e">
-        <f t="shared" ref="T26:T29" si="32">MEDIAN(0, 255, ROUND(SQRT(K26)/100+SQRT(L26)+P26+40/J26-2,0))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U26" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="33"/>
+        <v>121875</v>
+      </c>
+      <c r="T26">
+        <f t="shared" si="34"/>
+        <v>33</v>
+      </c>
+      <c r="U26">
+        <f t="shared" si="35"/>
+        <v>8043.75</v>
       </c>
       <c r="V26">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="AC26" s="2" t="e">
-        <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="AD26" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="AE26" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>139</v>
+        <v>338</v>
       </c>
       <c r="B27" t="s">
-        <v>140</v>
-      </c>
-      <c r="C27">
-        <v>6145</v>
+        <v>339</v>
       </c>
       <c r="D27" t="s">
-        <v>139</v>
+        <v>338</v>
       </c>
       <c r="E27" t="s">
-        <v>52</v>
+        <v>322</v>
       </c>
       <c r="F27">
-        <v>2012</v>
+        <v>1988</v>
       </c>
       <c r="G27">
         <v>30</v>
       </c>
-      <c r="H27" t="s">
-        <v>91</v>
+      <c r="H27">
+        <v>60</v>
+      </c>
+      <c r="I27">
+        <v>30</v>
       </c>
       <c r="J27">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="K27">
-        <v>170</v>
+        <v>80</v>
       </c>
       <c r="L27">
-        <v>9655</v>
+        <v>1080</v>
       </c>
       <c r="M27">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="O27">
-        <f t="shared" si="1"/>
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="P27">
-        <v>0.34</v>
+        <v>0.32900000000000001</v>
       </c>
       <c r="Q27">
         <f t="shared" si="2"/>
-        <v>419.83200000000005</v>
+        <v>296.62640000000005</v>
       </c>
       <c r="R27">
-        <f t="shared" si="3"/>
-        <v>126</v>
+        <f t="shared" si="32"/>
+        <v>39</v>
       </c>
       <c r="S27">
-        <f t="shared" si="4"/>
-        <v>393750</v>
+        <f t="shared" si="33"/>
+        <v>121875</v>
       </c>
       <c r="T27">
-        <f t="shared" si="32"/>
-        <v>103</v>
+        <f t="shared" si="34"/>
+        <v>33</v>
       </c>
       <c r="U27">
-        <f t="shared" si="5"/>
-        <v>23175</v>
+        <f t="shared" si="35"/>
+        <v>8043.75</v>
       </c>
       <c r="V27">
-        <f t="shared" si="6"/>
-        <v>10</v>
-      </c>
-      <c r="W27">
-        <v>1</v>
-      </c>
-      <c r="X27">
-        <v>8</v>
-      </c>
-      <c r="Y27">
-        <v>1</v>
-      </c>
-      <c r="Z27" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA27" s="1">
-        <v>1</v>
-      </c>
-      <c r="AB27" s="1">
-        <v>1</v>
-      </c>
-      <c r="AC27" s="2">
-        <f t="shared" si="7"/>
-        <v>1</v>
+        <f t="shared" si="36"/>
+        <v>0</v>
       </c>
       <c r="AD27" s="2" t="s">
-        <v>92</v>
+        <v>262</v>
       </c>
       <c r="AE27" t="s">
-        <v>93</v>
+        <v>337</v>
       </c>
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>194</v>
+        <v>340</v>
+      </c>
+      <c r="B28" t="s">
+        <v>341</v>
+      </c>
+      <c r="D28" t="s">
+        <v>340</v>
       </c>
       <c r="E28" t="s">
-        <v>52</v>
+        <v>322</v>
       </c>
       <c r="F28">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="G28">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="H28" t="s">
-        <v>91</v>
+        <v>342</v>
       </c>
       <c r="J28">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="K28">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="L28">
-        <v>13052</v>
+        <v>4800</v>
       </c>
       <c r="M28">
         <v>150</v>
       </c>
       <c r="O28">
-        <f t="shared" si="1"/>
         <v>150</v>
       </c>
       <c r="P28">
-        <v>0.38750000000000001</v>
+        <v>0.38100000000000001</v>
       </c>
       <c r="Q28">
         <f t="shared" si="2"/>
-        <v>569.625</v>
+        <v>560.07000000000005</v>
       </c>
       <c r="R28">
-        <f t="shared" si="3"/>
-        <v>144</v>
+        <f t="shared" si="32"/>
+        <v>91</v>
       </c>
       <c r="S28">
-        <f t="shared" si="4"/>
-        <v>450000</v>
+        <f t="shared" si="33"/>
+        <v>284375</v>
       </c>
       <c r="T28">
-        <f t="shared" si="32"/>
-        <v>119</v>
+        <f t="shared" si="34"/>
+        <v>71</v>
       </c>
       <c r="U28">
-        <f t="shared" si="5"/>
-        <v>26775</v>
+        <f t="shared" si="35"/>
+        <v>17306.25</v>
       </c>
       <c r="V28">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" ref="V28" si="37">W28+X28+Y28</f>
+        <v>11</v>
+      </c>
+      <c r="W28">
+        <v>2</v>
+      </c>
+      <c r="X28">
+        <v>7</v>
+      </c>
+      <c r="Y28">
+        <v>2</v>
       </c>
       <c r="AC28" s="2" t="e">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="AC28" si="38">AVERAGE(Z28:AB28)</f>
         <v>#DIV/0!</v>
+      </c>
+      <c r="AD28" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="AE28" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>197</v>
+        <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>198</v>
+        <v>72</v>
+      </c>
+      <c r="D29" t="s">
+        <v>31</v>
       </c>
       <c r="E29" t="s">
         <v>52</v>
       </c>
       <c r="F29">
-        <v>2006</v>
-      </c>
-      <c r="G29">
-        <v>30</v>
-      </c>
-      <c r="H29" t="s">
-        <v>91</v>
-      </c>
-      <c r="J29">
-        <v>8</v>
-      </c>
-      <c r="K29">
-        <v>120</v>
-      </c>
-      <c r="L29">
-        <v>13052</v>
-      </c>
-      <c r="M29">
-        <v>184</v>
+        <v>1958</v>
       </c>
       <c r="O29">
         <f t="shared" si="1"/>
-        <v>184</v>
-      </c>
-      <c r="P29">
-        <v>0.42099999999999999</v>
+        <v>0</v>
       </c>
       <c r="Q29">
         <f t="shared" si="2"/>
-        <v>759.1472</v>
+        <v>0</v>
       </c>
       <c r="R29">
-        <f t="shared" si="3"/>
-        <v>146</v>
+        <f t="shared" si="32"/>
+        <v>20</v>
       </c>
       <c r="S29">
-        <f t="shared" si="4"/>
-        <v>456250</v>
-      </c>
-      <c r="T29">
-        <f t="shared" si="32"/>
-        <v>118</v>
-      </c>
-      <c r="U29">
-        <f t="shared" si="5"/>
-        <v>26550</v>
+        <f t="shared" si="33"/>
+        <v>62500</v>
+      </c>
+      <c r="T29" t="e">
+        <f t="shared" si="34"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U29" t="e">
+        <f t="shared" si="35"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="V29">
         <f t="shared" si="6"/>
@@ -3497,188 +3725,171 @@
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>258</v>
+        <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>259</v>
+        <v>73</v>
       </c>
       <c r="D30" t="s">
-        <v>258</v>
+        <v>32</v>
       </c>
       <c r="E30" t="s">
-        <v>260</v>
+        <v>52</v>
       </c>
       <c r="F30">
-        <v>1993</v>
+        <v>1978</v>
       </c>
       <c r="G30">
         <v>30</v>
       </c>
-      <c r="H30" t="s">
-        <v>261</v>
+      <c r="H30">
+        <v>60</v>
+      </c>
+      <c r="I30">
+        <v>30</v>
       </c>
       <c r="J30">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K30">
         <v>100</v>
       </c>
       <c r="L30">
-        <v>8702</v>
+        <v>5914</v>
       </c>
       <c r="M30">
-        <v>184</v>
+        <v>138</v>
       </c>
       <c r="O30">
-        <v>184</v>
+        <f t="shared" si="1"/>
+        <v>138</v>
       </c>
       <c r="P30">
-        <v>0.34799999999999998</v>
+        <v>0.34699999999999998</v>
       </c>
       <c r="Q30">
-        <v>627.5136</v>
+        <f t="shared" si="2"/>
+        <v>469.28280000000001</v>
       </c>
       <c r="R30">
-        <v>125</v>
+        <f t="shared" si="32"/>
+        <v>102</v>
       </c>
       <c r="S30">
-        <v>390625</v>
+        <f t="shared" si="33"/>
+        <v>318750</v>
       </c>
       <c r="T30">
-        <v>97</v>
+        <f t="shared" si="34"/>
+        <v>79</v>
       </c>
       <c r="U30">
-        <v>21825</v>
+        <f t="shared" si="35"/>
+        <v>17775</v>
       </c>
       <c r="V30">
-        <v>8</v>
-      </c>
-      <c r="W30">
-        <v>2</v>
-      </c>
-      <c r="X30">
-        <v>4</v>
-      </c>
-      <c r="Y30">
-        <v>2</v>
-      </c>
-      <c r="Z30"/>
-      <c r="AA30"/>
-      <c r="AB30"/>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="AC30" s="2" t="e">
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
-      </c>
-      <c r="AD30" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="AE30" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>263</v>
+        <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>264</v>
+        <v>74</v>
       </c>
       <c r="D31" t="s">
-        <v>263</v>
+        <v>33</v>
       </c>
       <c r="E31" t="s">
-        <v>260</v>
+        <v>52</v>
       </c>
       <c r="F31">
-        <v>1990</v>
+        <v>1985</v>
       </c>
       <c r="G31">
         <v>30</v>
       </c>
       <c r="H31">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="I31">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="J31">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K31">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="L31">
-        <v>4351</v>
+        <v>8702</v>
       </c>
       <c r="M31">
-        <v>86</v>
+        <v>184</v>
       </c>
       <c r="O31">
-        <v>86</v>
+        <f t="shared" si="1"/>
+        <v>184</v>
       </c>
       <c r="P31">
-        <v>0.27900000000000003</v>
+        <v>0.34799999999999998</v>
       </c>
       <c r="Q31">
-        <v>235.14120000000005</v>
+        <f t="shared" si="2"/>
+        <v>627.5136</v>
       </c>
       <c r="R31">
-        <v>79</v>
+        <f t="shared" si="32"/>
+        <v>113</v>
       </c>
       <c r="S31">
-        <v>246875</v>
+        <f t="shared" si="33"/>
+        <v>353125</v>
       </c>
       <c r="T31">
-        <v>67</v>
+        <f t="shared" si="34"/>
+        <v>94</v>
       </c>
       <c r="U31">
-        <v>15075</v>
+        <f t="shared" si="35"/>
+        <v>21150</v>
       </c>
       <c r="V31">
-        <v>10</v>
-      </c>
-      <c r="W31">
-        <v>2</v>
-      </c>
-      <c r="X31">
-        <v>6</v>
-      </c>
-      <c r="Y31">
-        <v>2</v>
-      </c>
-      <c r="Z31"/>
-      <c r="AA31"/>
-      <c r="AB31"/>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="AC31" s="2" t="e">
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
-      </c>
-      <c r="AD31" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="AE31" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>265</v>
+        <v>39</v>
       </c>
       <c r="B32" t="s">
-        <v>266</v>
+        <v>75</v>
       </c>
       <c r="D32" t="s">
-        <v>265</v>
+        <v>39</v>
       </c>
       <c r="E32" t="s">
-        <v>260</v>
+        <v>52</v>
       </c>
       <c r="F32">
-        <v>1991</v>
+        <v>1994</v>
       </c>
       <c r="G32">
         <v>30</v>
       </c>
       <c r="H32">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="I32">
         <v>30</v>
@@ -3687,475 +3898,1125 @@
         <v>10</v>
       </c>
       <c r="K32">
-        <v>100</v>
+        <v>170</v>
       </c>
       <c r="L32">
-        <v>6526</v>
+        <v>4894</v>
       </c>
       <c r="M32">
-        <v>138</v>
+        <v>88</v>
       </c>
       <c r="O32">
-        <v>138</v>
+        <f t="shared" si="1"/>
+        <v>88</v>
       </c>
       <c r="P32">
-        <v>0.35899999999999999</v>
+        <v>0.24299999999999999</v>
       </c>
       <c r="Q32">
-        <v>485.51160000000004</v>
+        <f t="shared" si="2"/>
+        <v>209.56320000000002</v>
       </c>
       <c r="R32">
-        <v>105</v>
+        <f t="shared" si="32"/>
+        <v>90</v>
       </c>
       <c r="S32">
-        <v>328125</v>
+        <f t="shared" si="33"/>
+        <v>281250</v>
       </c>
       <c r="T32">
-        <v>83</v>
+        <f t="shared" si="34"/>
+        <v>72</v>
       </c>
       <c r="U32">
-        <v>18675</v>
+        <f t="shared" si="35"/>
+        <v>16200</v>
       </c>
       <c r="V32">
-        <v>10</v>
-      </c>
-      <c r="W32">
-        <v>2</v>
-      </c>
-      <c r="X32">
-        <v>6</v>
-      </c>
-      <c r="Y32">
-        <v>2</v>
-      </c>
-      <c r="Z32"/>
-      <c r="AA32"/>
-      <c r="AB32"/>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="AC32" s="2" t="e">
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
-      </c>
-      <c r="AD32" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="AE32" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="33" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>267</v>
+        <v>40</v>
       </c>
       <c r="B33" t="s">
-        <v>268</v>
+        <v>76</v>
+      </c>
+      <c r="C33">
+        <v>6144</v>
       </c>
       <c r="D33" t="s">
-        <v>267</v>
+        <v>40</v>
       </c>
       <c r="E33" t="s">
-        <v>260</v>
+        <v>52</v>
       </c>
       <c r="F33">
-        <v>1993</v>
+        <v>2010</v>
       </c>
       <c r="G33">
         <v>30</v>
       </c>
-      <c r="H33">
-        <v>60</v>
-      </c>
-      <c r="I33">
-        <v>30</v>
+      <c r="H33" t="s">
+        <v>91</v>
       </c>
       <c r="J33">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K33">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="L33">
-        <v>6526</v>
+        <v>9655</v>
       </c>
       <c r="M33">
         <v>138</v>
       </c>
       <c r="O33">
+        <f t="shared" si="1"/>
         <v>138</v>
       </c>
       <c r="P33">
-        <v>0.35899999999999999</v>
+        <v>0.38450000000000001</v>
       </c>
       <c r="Q33">
-        <v>485.51160000000004</v>
+        <f t="shared" si="2"/>
+        <v>519.99779999999998</v>
       </c>
       <c r="R33">
-        <v>107</v>
+        <f t="shared" si="32"/>
+        <v>127</v>
       </c>
       <c r="S33">
-        <v>334375</v>
+        <f t="shared" si="33"/>
+        <v>396875</v>
       </c>
       <c r="T33">
-        <v>84</v>
+        <f t="shared" si="34"/>
+        <v>103</v>
       </c>
       <c r="U33">
-        <v>18900</v>
+        <f t="shared" si="35"/>
+        <v>23175</v>
       </c>
       <c r="V33">
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="W33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X33">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="Y33">
-        <v>2</v>
-      </c>
-      <c r="Z33"/>
-      <c r="AA33"/>
-      <c r="AB33"/>
-      <c r="AC33" s="2" t="e">
-        <v>#DIV/0!</v>
+        <v>1</v>
+      </c>
+      <c r="Z33" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA33" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB33" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC33" s="2">
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="AD33" s="2" t="s">
-        <v>262</v>
+        <v>92</v>
       </c>
       <c r="AE33" t="s">
-        <v>262</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>269</v>
+        <v>41</v>
       </c>
       <c r="B34" t="s">
-        <v>270</v>
+        <v>77</v>
       </c>
       <c r="D34" t="s">
-        <v>269</v>
+        <v>41</v>
       </c>
       <c r="E34" t="s">
-        <v>260</v>
+        <v>52</v>
       </c>
       <c r="F34">
-        <v>1992</v>
-      </c>
-      <c r="G34">
-        <v>30</v>
-      </c>
-      <c r="H34">
-        <v>60</v>
-      </c>
-      <c r="I34">
-        <v>30</v>
-      </c>
-      <c r="J34">
-        <v>16</v>
-      </c>
-      <c r="K34">
-        <v>100</v>
-      </c>
-      <c r="L34">
-        <v>6526</v>
-      </c>
-      <c r="M34">
-        <v>138</v>
+        <v>2012</v>
       </c>
       <c r="O34">
-        <v>138</v>
-      </c>
-      <c r="P34">
-        <v>0.35899999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="Q34">
-        <v>485.51160000000004</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="R34">
-        <v>99</v>
+        <f t="shared" si="32"/>
+        <v>20</v>
       </c>
       <c r="S34">
-        <v>309375</v>
-      </c>
-      <c r="T34">
-        <v>82</v>
-      </c>
-      <c r="U34">
-        <v>18450</v>
+        <f t="shared" si="33"/>
+        <v>62500</v>
+      </c>
+      <c r="T34" t="e">
+        <f t="shared" si="34"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U34" t="e">
+        <f t="shared" si="35"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="V34">
-        <v>10</v>
-      </c>
-      <c r="W34">
-        <v>2</v>
-      </c>
-      <c r="X34">
-        <v>6</v>
-      </c>
-      <c r="Y34">
-        <v>2</v>
-      </c>
-      <c r="Z34"/>
-      <c r="AA34"/>
-      <c r="AB34"/>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="AC34" s="2" t="e">
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
-      </c>
-      <c r="AD34" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="AE34" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="35" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>272</v>
+        <v>139</v>
       </c>
       <c r="B35" t="s">
-        <v>273</v>
+        <v>140</v>
+      </c>
+      <c r="C35">
+        <v>6145</v>
       </c>
       <c r="D35" t="s">
-        <v>272</v>
+        <v>139</v>
       </c>
       <c r="E35" t="s">
-        <v>260</v>
+        <v>52</v>
       </c>
       <c r="F35">
-        <v>1997</v>
+        <v>2012</v>
       </c>
       <c r="G35">
         <v>30</v>
       </c>
-      <c r="H35">
-        <v>60</v>
-      </c>
-      <c r="I35">
-        <v>50</v>
+      <c r="H35" t="s">
+        <v>91</v>
       </c>
       <c r="J35">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="K35">
-        <v>100</v>
+        <v>170</v>
       </c>
       <c r="L35">
-        <v>6526</v>
+        <v>9655</v>
       </c>
       <c r="M35">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="O35">
-        <v>150</v>
+        <f t="shared" si="1"/>
+        <v>126</v>
       </c>
       <c r="P35">
-        <v>0.33</v>
+        <v>0.34</v>
       </c>
       <c r="Q35">
-        <v>485.1</v>
+        <f t="shared" si="2"/>
+        <v>419.83200000000005</v>
       </c>
       <c r="R35">
-        <v>101</v>
+        <f t="shared" si="32"/>
+        <v>126</v>
       </c>
       <c r="S35">
-        <v>315625</v>
+        <f t="shared" si="33"/>
+        <v>393750</v>
       </c>
       <c r="T35">
-        <v>82</v>
+        <f t="shared" si="34"/>
+        <v>103</v>
       </c>
       <c r="U35">
-        <v>18450</v>
+        <f t="shared" si="35"/>
+        <v>23175</v>
       </c>
       <c r="V35">
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="W35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X35">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="Y35">
-        <v>2</v>
-      </c>
-      <c r="Z35"/>
-      <c r="AA35"/>
-      <c r="AB35"/>
-      <c r="AC35" s="2" t="e">
-        <v>#DIV/0!</v>
+        <v>1</v>
+      </c>
+      <c r="Z35" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA35" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB35" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC35" s="2">
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="AD35" s="2" t="s">
-        <v>262</v>
+        <v>92</v>
       </c>
       <c r="AE35" t="s">
-        <v>271</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>274</v>
-      </c>
-      <c r="B36" t="s">
-        <v>275</v>
-      </c>
-      <c r="D36" t="s">
-        <v>274</v>
+        <v>194</v>
       </c>
       <c r="E36" t="s">
-        <v>260</v>
+        <v>52</v>
       </c>
       <c r="F36">
-        <v>1998</v>
+        <v>2009</v>
       </c>
       <c r="G36">
         <v>30</v>
       </c>
-      <c r="H36">
-        <v>60</v>
-      </c>
-      <c r="I36">
-        <v>30</v>
+      <c r="H36" t="s">
+        <v>91</v>
       </c>
       <c r="J36">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="K36">
         <v>120</v>
       </c>
       <c r="L36">
-        <v>6526</v>
+        <v>13052</v>
       </c>
       <c r="M36">
-        <v>132</v>
+        <v>150</v>
       </c>
       <c r="O36">
-        <v>132</v>
+        <f t="shared" si="1"/>
+        <v>150</v>
       </c>
       <c r="P36">
-        <v>0.24099999999999999</v>
+        <v>0.38750000000000001</v>
       </c>
       <c r="Q36">
-        <v>311.75760000000002</v>
+        <f t="shared" si="2"/>
+        <v>569.625</v>
       </c>
       <c r="R36">
-        <v>105</v>
+        <f t="shared" si="32"/>
+        <v>144</v>
       </c>
       <c r="S36">
-        <v>328125</v>
+        <f t="shared" si="33"/>
+        <v>450000</v>
       </c>
       <c r="T36">
-        <v>83</v>
+        <f t="shared" si="34"/>
+        <v>119</v>
       </c>
       <c r="U36">
-        <v>18675</v>
+        <f t="shared" si="35"/>
+        <v>26775</v>
       </c>
       <c r="V36">
-        <v>10</v>
-      </c>
-      <c r="W36">
-        <v>2</v>
-      </c>
-      <c r="X36">
-        <v>6</v>
-      </c>
-      <c r="Y36">
-        <v>2</v>
-      </c>
-      <c r="Z36"/>
-      <c r="AA36"/>
-      <c r="AB36"/>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="AC36" s="2" t="e">
+        <f t="shared" si="7"/>
         <v>#DIV/0!</v>
-      </c>
-      <c r="AD36" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="AE36" t="s">
-        <v>271</v>
-      </c>
-      <c r="AF36" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="37" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>277</v>
+        <v>197</v>
       </c>
       <c r="B37" t="s">
-        <v>278</v>
-      </c>
-      <c r="D37" t="s">
-        <v>277</v>
+        <v>198</v>
       </c>
       <c r="E37" t="s">
-        <v>260</v>
+        <v>52</v>
       </c>
       <c r="F37">
-        <v>2001</v>
+        <v>2006</v>
       </c>
       <c r="G37">
         <v>30</v>
       </c>
       <c r="H37" t="s">
+        <v>91</v>
+      </c>
+      <c r="J37">
+        <v>8</v>
+      </c>
+      <c r="K37">
+        <v>120</v>
+      </c>
+      <c r="L37">
+        <v>13052</v>
+      </c>
+      <c r="M37">
+        <v>184</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="1"/>
+        <v>184</v>
+      </c>
+      <c r="P37">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="2"/>
+        <v>759.1472</v>
+      </c>
+      <c r="R37">
+        <f t="shared" si="32"/>
+        <v>146</v>
+      </c>
+      <c r="S37">
+        <f t="shared" si="33"/>
+        <v>456250</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="34"/>
+        <v>118</v>
+      </c>
+      <c r="U37">
+        <f t="shared" si="35"/>
+        <v>26550</v>
+      </c>
+      <c r="V37">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AC37" s="2" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>258</v>
+      </c>
+      <c r="B38" t="s">
+        <v>259</v>
+      </c>
+      <c r="D38" t="s">
+        <v>258</v>
+      </c>
+      <c r="E38" t="s">
+        <v>260</v>
+      </c>
+      <c r="F38">
+        <v>1993</v>
+      </c>
+      <c r="G38">
+        <v>30</v>
+      </c>
+      <c r="H38" t="s">
         <v>261</v>
       </c>
-      <c r="J37">
+      <c r="J38">
+        <v>8</v>
+      </c>
+      <c r="K38">
+        <v>100</v>
+      </c>
+      <c r="L38">
+        <v>8702</v>
+      </c>
+      <c r="M38">
+        <v>184</v>
+      </c>
+      <c r="O38">
+        <v>184</v>
+      </c>
+      <c r="P38">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" si="2"/>
+        <v>627.5136</v>
+      </c>
+      <c r="R38">
+        <f t="shared" si="32"/>
+        <v>125</v>
+      </c>
+      <c r="S38">
+        <f t="shared" si="33"/>
+        <v>390625</v>
+      </c>
+      <c r="T38">
+        <f t="shared" si="34"/>
+        <v>97</v>
+      </c>
+      <c r="U38">
+        <f t="shared" si="35"/>
+        <v>21825</v>
+      </c>
+      <c r="V38">
+        <v>8</v>
+      </c>
+      <c r="W38">
+        <v>2</v>
+      </c>
+      <c r="X38">
+        <v>4</v>
+      </c>
+      <c r="Y38">
+        <v>2</v>
+      </c>
+      <c r="Z38"/>
+      <c r="AA38"/>
+      <c r="AB38"/>
+      <c r="AC38" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD38" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="AE38" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="39" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>263</v>
+      </c>
+      <c r="B39" t="s">
+        <v>264</v>
+      </c>
+      <c r="D39" t="s">
+        <v>263</v>
+      </c>
+      <c r="E39" t="s">
+        <v>260</v>
+      </c>
+      <c r="F39">
+        <v>1990</v>
+      </c>
+      <c r="G39">
+        <v>30</v>
+      </c>
+      <c r="H39">
+        <v>25</v>
+      </c>
+      <c r="I39">
+        <v>15</v>
+      </c>
+      <c r="J39">
+        <v>16</v>
+      </c>
+      <c r="K39">
+        <v>140</v>
+      </c>
+      <c r="L39">
+        <v>4351</v>
+      </c>
+      <c r="M39">
+        <v>86</v>
+      </c>
+      <c r="O39">
+        <v>86</v>
+      </c>
+      <c r="P39">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="Q39">
+        <f t="shared" si="2"/>
+        <v>235.14120000000005</v>
+      </c>
+      <c r="R39">
+        <f t="shared" si="32"/>
+        <v>79</v>
+      </c>
+      <c r="S39">
+        <f t="shared" si="33"/>
+        <v>246875</v>
+      </c>
+      <c r="T39">
+        <f t="shared" si="34"/>
+        <v>67</v>
+      </c>
+      <c r="U39">
+        <f t="shared" si="35"/>
+        <v>15075</v>
+      </c>
+      <c r="V39">
+        <v>10</v>
+      </c>
+      <c r="W39">
+        <v>2</v>
+      </c>
+      <c r="X39">
         <v>6</v>
       </c>
-      <c r="K37">
+      <c r="Y39">
+        <v>2</v>
+      </c>
+      <c r="Z39"/>
+      <c r="AA39"/>
+      <c r="AB39"/>
+      <c r="AC39" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD39" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="AE39" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="40" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>265</v>
+      </c>
+      <c r="B40" t="s">
+        <v>266</v>
+      </c>
+      <c r="D40" t="s">
+        <v>265</v>
+      </c>
+      <c r="E40" t="s">
+        <v>260</v>
+      </c>
+      <c r="F40">
+        <v>1991</v>
+      </c>
+      <c r="G40">
+        <v>30</v>
+      </c>
+      <c r="H40">
+        <v>60</v>
+      </c>
+      <c r="I40">
+        <v>30</v>
+      </c>
+      <c r="J40">
+        <v>10</v>
+      </c>
+      <c r="K40">
+        <v>100</v>
+      </c>
+      <c r="L40">
+        <v>6526</v>
+      </c>
+      <c r="M40">
+        <v>138</v>
+      </c>
+      <c r="O40">
+        <v>138</v>
+      </c>
+      <c r="P40">
+        <v>0.35899999999999999</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" si="2"/>
+        <v>485.51160000000004</v>
+      </c>
+      <c r="R40">
+        <f t="shared" si="32"/>
+        <v>105</v>
+      </c>
+      <c r="S40">
+        <f t="shared" si="33"/>
+        <v>328125</v>
+      </c>
+      <c r="T40">
+        <f t="shared" si="34"/>
+        <v>83</v>
+      </c>
+      <c r="U40">
+        <f t="shared" si="35"/>
+        <v>18675</v>
+      </c>
+      <c r="V40">
+        <v>10</v>
+      </c>
+      <c r="W40">
+        <v>2</v>
+      </c>
+      <c r="X40">
+        <v>6</v>
+      </c>
+      <c r="Y40">
+        <v>2</v>
+      </c>
+      <c r="Z40"/>
+      <c r="AA40"/>
+      <c r="AB40"/>
+      <c r="AC40" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD40" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="AE40" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="41" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>267</v>
+      </c>
+      <c r="B41" t="s">
+        <v>268</v>
+      </c>
+      <c r="D41" t="s">
+        <v>267</v>
+      </c>
+      <c r="E41" t="s">
+        <v>260</v>
+      </c>
+      <c r="F41">
+        <v>1993</v>
+      </c>
+      <c r="G41">
+        <v>30</v>
+      </c>
+      <c r="H41">
+        <v>60</v>
+      </c>
+      <c r="I41">
+        <v>30</v>
+      </c>
+      <c r="J41">
+        <v>8</v>
+      </c>
+      <c r="K41">
+        <v>100</v>
+      </c>
+      <c r="L41">
+        <v>6526</v>
+      </c>
+      <c r="M41">
+        <v>138</v>
+      </c>
+      <c r="O41">
+        <v>138</v>
+      </c>
+      <c r="P41">
+        <v>0.35899999999999999</v>
+      </c>
+      <c r="Q41">
+        <f t="shared" si="2"/>
+        <v>485.51160000000004</v>
+      </c>
+      <c r="R41">
+        <f t="shared" si="32"/>
+        <v>107</v>
+      </c>
+      <c r="S41">
+        <f t="shared" si="33"/>
+        <v>334375</v>
+      </c>
+      <c r="T41">
+        <f t="shared" si="34"/>
+        <v>84</v>
+      </c>
+      <c r="U41">
+        <f t="shared" si="35"/>
+        <v>18900</v>
+      </c>
+      <c r="V41">
+        <v>10</v>
+      </c>
+      <c r="W41">
+        <v>2</v>
+      </c>
+      <c r="X41">
+        <v>6</v>
+      </c>
+      <c r="Y41">
+        <v>2</v>
+      </c>
+      <c r="Z41"/>
+      <c r="AA41"/>
+      <c r="AB41"/>
+      <c r="AC41" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD41" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="AE41" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="42" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>269</v>
+      </c>
+      <c r="B42" t="s">
+        <v>270</v>
+      </c>
+      <c r="D42" t="s">
+        <v>269</v>
+      </c>
+      <c r="E42" t="s">
+        <v>260</v>
+      </c>
+      <c r="F42">
+        <v>1992</v>
+      </c>
+      <c r="G42">
+        <v>30</v>
+      </c>
+      <c r="H42">
+        <v>60</v>
+      </c>
+      <c r="I42">
+        <v>30</v>
+      </c>
+      <c r="J42">
+        <v>16</v>
+      </c>
+      <c r="K42">
+        <v>100</v>
+      </c>
+      <c r="L42">
+        <v>6526</v>
+      </c>
+      <c r="M42">
+        <v>138</v>
+      </c>
+      <c r="O42">
+        <v>138</v>
+      </c>
+      <c r="P42">
+        <v>0.35899999999999999</v>
+      </c>
+      <c r="Q42">
+        <f t="shared" si="2"/>
+        <v>485.51160000000004</v>
+      </c>
+      <c r="R42">
+        <f t="shared" si="32"/>
+        <v>99</v>
+      </c>
+      <c r="S42">
+        <f t="shared" si="33"/>
+        <v>309375</v>
+      </c>
+      <c r="T42">
+        <f t="shared" si="34"/>
+        <v>82</v>
+      </c>
+      <c r="U42">
+        <f t="shared" si="35"/>
+        <v>18450</v>
+      </c>
+      <c r="V42">
+        <v>10</v>
+      </c>
+      <c r="W42">
+        <v>2</v>
+      </c>
+      <c r="X42">
+        <v>6</v>
+      </c>
+      <c r="Y42">
+        <v>2</v>
+      </c>
+      <c r="Z42"/>
+      <c r="AA42"/>
+      <c r="AB42"/>
+      <c r="AC42" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD42" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="AE42" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="43" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>272</v>
+      </c>
+      <c r="B43" t="s">
+        <v>273</v>
+      </c>
+      <c r="D43" t="s">
+        <v>272</v>
+      </c>
+      <c r="E43" t="s">
+        <v>260</v>
+      </c>
+      <c r="F43">
+        <v>1997</v>
+      </c>
+      <c r="G43">
+        <v>30</v>
+      </c>
+      <c r="H43">
+        <v>60</v>
+      </c>
+      <c r="I43">
+        <v>50</v>
+      </c>
+      <c r="J43">
+        <v>16</v>
+      </c>
+      <c r="K43">
+        <v>100</v>
+      </c>
+      <c r="L43">
+        <v>6526</v>
+      </c>
+      <c r="M43">
+        <v>150</v>
+      </c>
+      <c r="O43">
+        <v>150</v>
+      </c>
+      <c r="P43">
+        <v>0.33</v>
+      </c>
+      <c r="Q43">
+        <f t="shared" si="2"/>
+        <v>485.1</v>
+      </c>
+      <c r="R43">
+        <f t="shared" si="32"/>
+        <v>101</v>
+      </c>
+      <c r="S43">
+        <f t="shared" si="33"/>
+        <v>315625</v>
+      </c>
+      <c r="T43">
+        <f t="shared" si="34"/>
+        <v>82</v>
+      </c>
+      <c r="U43">
+        <f t="shared" si="35"/>
+        <v>18450</v>
+      </c>
+      <c r="V43">
+        <v>10</v>
+      </c>
+      <c r="W43">
+        <v>2</v>
+      </c>
+      <c r="X43">
+        <v>6</v>
+      </c>
+      <c r="Y43">
+        <v>2</v>
+      </c>
+      <c r="Z43"/>
+      <c r="AA43"/>
+      <c r="AB43"/>
+      <c r="AC43" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD43" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="AE43" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="44" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>274</v>
+      </c>
+      <c r="B44" t="s">
+        <v>275</v>
+      </c>
+      <c r="D44" t="s">
+        <v>274</v>
+      </c>
+      <c r="E44" t="s">
+        <v>260</v>
+      </c>
+      <c r="F44">
+        <v>1998</v>
+      </c>
+      <c r="G44">
+        <v>30</v>
+      </c>
+      <c r="H44">
+        <v>60</v>
+      </c>
+      <c r="I44">
+        <v>30</v>
+      </c>
+      <c r="J44">
+        <v>10</v>
+      </c>
+      <c r="K44">
+        <v>120</v>
+      </c>
+      <c r="L44">
+        <v>6526</v>
+      </c>
+      <c r="M44">
+        <v>132</v>
+      </c>
+      <c r="O44">
+        <v>132</v>
+      </c>
+      <c r="P44">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="Q44">
+        <f t="shared" si="2"/>
+        <v>311.75760000000002</v>
+      </c>
+      <c r="R44">
+        <f t="shared" si="32"/>
+        <v>105</v>
+      </c>
+      <c r="S44">
+        <f t="shared" si="33"/>
+        <v>328125</v>
+      </c>
+      <c r="T44">
+        <f t="shared" si="34"/>
+        <v>83</v>
+      </c>
+      <c r="U44">
+        <f t="shared" si="35"/>
+        <v>18675</v>
+      </c>
+      <c r="V44">
+        <v>10</v>
+      </c>
+      <c r="W44">
+        <v>2</v>
+      </c>
+      <c r="X44">
+        <v>6</v>
+      </c>
+      <c r="Y44">
+        <v>2</v>
+      </c>
+      <c r="Z44"/>
+      <c r="AA44"/>
+      <c r="AB44"/>
+      <c r="AC44" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD44" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="AE44" t="s">
+        <v>271</v>
+      </c>
+      <c r="AF44" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="45" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>277</v>
+      </c>
+      <c r="B45" t="s">
+        <v>278</v>
+      </c>
+      <c r="D45" t="s">
+        <v>277</v>
+      </c>
+      <c r="E45" t="s">
+        <v>260</v>
+      </c>
+      <c r="F45">
+        <v>2001</v>
+      </c>
+      <c r="G45">
+        <v>30</v>
+      </c>
+      <c r="H45" t="s">
+        <v>261</v>
+      </c>
+      <c r="J45">
+        <v>6</v>
+      </c>
+      <c r="K45">
         <v>160</v>
       </c>
-      <c r="L37">
+      <c r="L45">
         <v>6526</v>
       </c>
-      <c r="M37">
+      <c r="M45">
         <v>126</v>
       </c>
-      <c r="O37">
+      <c r="O45">
         <v>126</v>
       </c>
-      <c r="P37">
+      <c r="P45">
         <v>0.19800000000000001</v>
       </c>
-      <c r="Q37">
+      <c r="Q45">
+        <f t="shared" si="2"/>
         <v>244.49040000000002</v>
       </c>
-      <c r="R37">
+      <c r="R45">
+        <f t="shared" si="32"/>
         <v>108</v>
       </c>
-      <c r="S37">
+      <c r="S45">
+        <f t="shared" si="33"/>
         <v>337500</v>
       </c>
-      <c r="T37">
+      <c r="T45">
+        <f t="shared" si="34"/>
         <v>86</v>
       </c>
-      <c r="U37">
+      <c r="U45">
+        <f t="shared" si="35"/>
         <v>19350</v>
       </c>
-      <c r="V37">
+      <c r="V45">
         <v>10</v>
       </c>
-      <c r="W37">
+      <c r="W45">
         <v>2</v>
       </c>
-      <c r="X37">
+      <c r="X45">
         <v>6</v>
       </c>
-      <c r="Y37">
+      <c r="Y45">
         <v>2</v>
       </c>
-      <c r="Z37"/>
-      <c r="AA37"/>
-      <c r="AB37"/>
-      <c r="AC37" s="2" t="e">
+      <c r="Z45"/>
+      <c r="AA45"/>
+      <c r="AB45"/>
+      <c r="AC45" s="2" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="AD37" s="2" t="s">
+      <c r="AD45" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="AE37" t="s">
+      <c r="AE45" t="s">
         <v>271</v>
       </c>
-      <c r="AF37" t="s">
+      <c r="AF45" t="s">
         <v>276</v>
       </c>
     </row>
@@ -4169,8 +5030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB4625FC-685F-4E56-AE60-F05D51350408}">
   <dimension ref="A1:AF111"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="U81" sqref="U81"/>
     </sheetView>
   </sheetViews>
@@ -9905,10 +10766,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392CFCAE-41E9-4295-93E2-AE0B308CC62A}">
-  <dimension ref="A1:Z47"/>
+  <dimension ref="A1:Z59"/>
   <sheetViews>
-    <sheetView topLeftCell="L25" workbookViewId="0">
-      <selection activeCell="S47" sqref="S47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Z48" sqref="Z48:Z57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -11628,7 +12490,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>208</v>
       </c>
@@ -11679,7 +12541,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>215</v>
       </c>
@@ -11730,7 +12592,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>216</v>
       </c>
@@ -11781,7 +12643,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>219</v>
       </c>
@@ -11832,7 +12694,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>221</v>
       </c>
@@ -11883,7 +12745,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>172</v>
       </c>
@@ -11934,7 +12796,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>178</v>
       </c>
@@ -11985,7 +12847,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>183</v>
       </c>
@@ -12036,7 +12898,7 @@
         <v>2475</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>185</v>
       </c>
@@ -12087,7 +12949,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>186</v>
       </c>
@@ -12138,7 +13000,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>187</v>
       </c>
@@ -12189,7 +13051,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>188</v>
       </c>
@@ -12240,7 +13102,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>279</v>
       </c>
@@ -12291,7 +13153,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>281</v>
       </c>
@@ -12342,7 +13204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>292</v>
       </c>
@@ -12393,7 +13255,706 @@
         <v>1125</v>
       </c>
     </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>296</v>
+      </c>
+      <c r="B48" t="s">
+        <v>297</v>
+      </c>
+      <c r="D48" t="s">
+        <v>296</v>
+      </c>
+      <c r="E48">
+        <v>1993</v>
+      </c>
+      <c r="F48">
+        <v>30</v>
+      </c>
+      <c r="G48">
+        <v>20</v>
+      </c>
+      <c r="H48">
+        <v>140</v>
+      </c>
+      <c r="I48" t="s">
+        <v>298</v>
+      </c>
+      <c r="M48">
+        <v>96</v>
+      </c>
+      <c r="N48">
+        <v>16</v>
+      </c>
+      <c r="O48">
+        <v>240</v>
+      </c>
+      <c r="P48">
+        <v>46.4</v>
+      </c>
+      <c r="Q48">
+        <f t="shared" ref="Q48:Q59" si="29">MEDIAN(0,255,ROUND(P48/20+SQRT(H48)/40+SQRT(M48)/2+(SQRT(O48)-SQRT(185)), 0))</f>
+        <v>9</v>
+      </c>
+      <c r="R48">
+        <f t="shared" ref="R48:R59" si="30">Q48*50000/16</f>
+        <v>28125</v>
+      </c>
+      <c r="S48">
+        <f t="shared" ref="S48:S59" si="31">MEDIAN(0,255,ROUND(SQRT(H48)/200+SQRT(M48)/2+(SQRT(O48)-SQRT(185)),0))</f>
+        <v>7</v>
+      </c>
+      <c r="T48">
+        <f t="shared" ref="T48:T59" si="32">S48*300/16*12</f>
+        <v>1575</v>
+      </c>
+      <c r="Y48" t="s">
+        <v>350</v>
+      </c>
+      <c r="Z48" s="3" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>299</v>
+      </c>
+      <c r="B49" t="s">
+        <v>300</v>
+      </c>
+      <c r="D49" t="s">
+        <v>299</v>
+      </c>
+      <c r="E49">
+        <v>1993</v>
+      </c>
+      <c r="F49">
+        <v>30</v>
+      </c>
+      <c r="G49">
+        <v>20</v>
+      </c>
+      <c r="H49">
+        <v>140</v>
+      </c>
+      <c r="I49" t="s">
+        <v>298</v>
+      </c>
+      <c r="M49">
+        <v>80</v>
+      </c>
+      <c r="N49">
+        <v>16</v>
+      </c>
+      <c r="O49">
+        <v>320</v>
+      </c>
+      <c r="P49">
+        <v>46.9</v>
+      </c>
+      <c r="Q49">
+        <f t="shared" si="29"/>
+        <v>11</v>
+      </c>
+      <c r="R49">
+        <f t="shared" si="30"/>
+        <v>34375</v>
+      </c>
+      <c r="S49">
+        <f t="shared" si="31"/>
+        <v>9</v>
+      </c>
+      <c r="T49">
+        <f t="shared" si="32"/>
+        <v>2025</v>
+      </c>
+      <c r="Y49" t="s">
+        <v>350</v>
+      </c>
+      <c r="Z49" s="4"/>
+    </row>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>301</v>
+      </c>
+      <c r="B50" t="s">
+        <v>302</v>
+      </c>
+      <c r="D50" t="s">
+        <v>301</v>
+      </c>
+      <c r="E50">
+        <v>1993</v>
+      </c>
+      <c r="F50">
+        <v>30</v>
+      </c>
+      <c r="G50">
+        <v>20</v>
+      </c>
+      <c r="H50">
+        <v>140</v>
+      </c>
+      <c r="I50" t="s">
+        <v>298</v>
+      </c>
+      <c r="M50">
+        <v>42</v>
+      </c>
+      <c r="N50">
+        <v>16</v>
+      </c>
+      <c r="O50">
+        <v>400</v>
+      </c>
+      <c r="P50">
+        <v>48</v>
+      </c>
+      <c r="Q50">
+        <f t="shared" si="29"/>
+        <v>12</v>
+      </c>
+      <c r="R50">
+        <f t="shared" si="30"/>
+        <v>37500</v>
+      </c>
+      <c r="S50">
+        <f t="shared" si="31"/>
+        <v>10</v>
+      </c>
+      <c r="T50">
+        <f t="shared" si="32"/>
+        <v>2250</v>
+      </c>
+      <c r="Y50" t="s">
+        <v>350</v>
+      </c>
+      <c r="Z50" s="4"/>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>303</v>
+      </c>
+      <c r="B51" t="s">
+        <v>304</v>
+      </c>
+      <c r="D51" t="s">
+        <v>303</v>
+      </c>
+      <c r="E51">
+        <v>1993</v>
+      </c>
+      <c r="F51">
+        <v>30</v>
+      </c>
+      <c r="G51">
+        <v>20</v>
+      </c>
+      <c r="H51">
+        <v>140</v>
+      </c>
+      <c r="I51" t="s">
+        <v>298</v>
+      </c>
+      <c r="M51">
+        <v>36</v>
+      </c>
+      <c r="N51">
+        <v>16</v>
+      </c>
+      <c r="O51">
+        <v>240</v>
+      </c>
+      <c r="P51">
+        <v>46.3</v>
+      </c>
+      <c r="Q51">
+        <f t="shared" si="29"/>
+        <v>8</v>
+      </c>
+      <c r="R51">
+        <f t="shared" si="30"/>
+        <v>25000</v>
+      </c>
+      <c r="S51">
+        <f t="shared" si="31"/>
+        <v>5</v>
+      </c>
+      <c r="T51">
+        <f t="shared" si="32"/>
+        <v>1125</v>
+      </c>
+      <c r="Y51" t="s">
+        <v>350</v>
+      </c>
+      <c r="Z51" s="4"/>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>305</v>
+      </c>
+      <c r="B52" t="s">
+        <v>306</v>
+      </c>
+      <c r="D52" t="s">
+        <v>305</v>
+      </c>
+      <c r="E52">
+        <v>1993</v>
+      </c>
+      <c r="F52">
+        <v>30</v>
+      </c>
+      <c r="G52">
+        <v>20</v>
+      </c>
+      <c r="H52">
+        <v>140</v>
+      </c>
+      <c r="I52" t="s">
+        <v>298</v>
+      </c>
+      <c r="M52">
+        <v>0</v>
+      </c>
+      <c r="N52">
+        <v>16</v>
+      </c>
+      <c r="O52">
+        <v>200</v>
+      </c>
+      <c r="P52">
+        <v>59</v>
+      </c>
+      <c r="Q52">
+        <f t="shared" si="29"/>
+        <v>4</v>
+      </c>
+      <c r="R52">
+        <f t="shared" si="30"/>
+        <v>12500</v>
+      </c>
+      <c r="S52">
+        <f t="shared" si="31"/>
+        <v>1</v>
+      </c>
+      <c r="T52">
+        <f t="shared" si="32"/>
+        <v>225</v>
+      </c>
+      <c r="Y52" t="s">
+        <v>350</v>
+      </c>
+      <c r="Z52" s="4"/>
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>307</v>
+      </c>
+      <c r="B53" t="s">
+        <v>308</v>
+      </c>
+      <c r="D53" t="s">
+        <v>307</v>
+      </c>
+      <c r="E53">
+        <v>1993</v>
+      </c>
+      <c r="F53">
+        <v>30</v>
+      </c>
+      <c r="G53">
+        <v>20</v>
+      </c>
+      <c r="H53">
+        <v>140</v>
+      </c>
+      <c r="I53" t="s">
+        <v>309</v>
+      </c>
+      <c r="M53">
+        <v>71</v>
+      </c>
+      <c r="N53">
+        <v>12</v>
+      </c>
+      <c r="O53">
+        <v>200</v>
+      </c>
+      <c r="P53">
+        <v>42</v>
+      </c>
+      <c r="Q53">
+        <f t="shared" si="29"/>
+        <v>7</v>
+      </c>
+      <c r="R53">
+        <f t="shared" si="30"/>
+        <v>21875</v>
+      </c>
+      <c r="S53">
+        <f t="shared" si="31"/>
+        <v>5</v>
+      </c>
+      <c r="T53">
+        <f t="shared" si="32"/>
+        <v>1125</v>
+      </c>
+      <c r="Y53" t="s">
+        <v>350</v>
+      </c>
+      <c r="Z53" s="4"/>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>310</v>
+      </c>
+      <c r="B54" t="s">
+        <v>311</v>
+      </c>
+      <c r="D54" t="s">
+        <v>310</v>
+      </c>
+      <c r="E54">
+        <v>1993</v>
+      </c>
+      <c r="F54">
+        <v>30</v>
+      </c>
+      <c r="G54">
+        <v>20</v>
+      </c>
+      <c r="H54">
+        <v>140</v>
+      </c>
+      <c r="I54" t="s">
+        <v>298</v>
+      </c>
+      <c r="M54">
+        <v>124</v>
+      </c>
+      <c r="N54">
+        <v>16</v>
+      </c>
+      <c r="O54">
+        <v>240</v>
+      </c>
+      <c r="P54">
+        <v>52.7</v>
+      </c>
+      <c r="Q54">
+        <f t="shared" si="29"/>
+        <v>10</v>
+      </c>
+      <c r="R54">
+        <f t="shared" si="30"/>
+        <v>31250</v>
+      </c>
+      <c r="S54">
+        <f t="shared" si="31"/>
+        <v>8</v>
+      </c>
+      <c r="T54">
+        <f t="shared" si="32"/>
+        <v>1800</v>
+      </c>
+      <c r="Y54" t="s">
+        <v>350</v>
+      </c>
+      <c r="Z54" s="4"/>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>312</v>
+      </c>
+      <c r="B55" t="s">
+        <v>313</v>
+      </c>
+      <c r="D55" t="s">
+        <v>312</v>
+      </c>
+      <c r="E55">
+        <v>1993</v>
+      </c>
+      <c r="F55">
+        <v>30</v>
+      </c>
+      <c r="G55">
+        <v>20</v>
+      </c>
+      <c r="H55">
+        <v>140</v>
+      </c>
+      <c r="I55" t="s">
+        <v>298</v>
+      </c>
+      <c r="M55">
+        <v>108</v>
+      </c>
+      <c r="N55">
+        <v>16</v>
+      </c>
+      <c r="O55">
+        <v>320</v>
+      </c>
+      <c r="P55">
+        <v>53</v>
+      </c>
+      <c r="Q55">
+        <f t="shared" si="29"/>
+        <v>12</v>
+      </c>
+      <c r="R55">
+        <f t="shared" si="30"/>
+        <v>37500</v>
+      </c>
+      <c r="S55">
+        <f t="shared" si="31"/>
+        <v>10</v>
+      </c>
+      <c r="T55">
+        <f t="shared" si="32"/>
+        <v>2250</v>
+      </c>
+      <c r="Y55" t="s">
+        <v>350</v>
+      </c>
+      <c r="Z55" s="4"/>
+    </row>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>314</v>
+      </c>
+      <c r="B56" t="s">
+        <v>315</v>
+      </c>
+      <c r="D56" t="s">
+        <v>314</v>
+      </c>
+      <c r="E56">
+        <v>1993</v>
+      </c>
+      <c r="F56">
+        <v>30</v>
+      </c>
+      <c r="G56">
+        <v>20</v>
+      </c>
+      <c r="H56">
+        <v>140</v>
+      </c>
+      <c r="I56" t="s">
+        <v>298</v>
+      </c>
+      <c r="M56">
+        <v>60</v>
+      </c>
+      <c r="N56">
+        <v>16</v>
+      </c>
+      <c r="O56">
+        <v>240</v>
+      </c>
+      <c r="P56">
+        <v>50.1</v>
+      </c>
+      <c r="Q56">
+        <f t="shared" si="29"/>
+        <v>9</v>
+      </c>
+      <c r="R56">
+        <f t="shared" si="30"/>
+        <v>28125</v>
+      </c>
+      <c r="S56">
+        <f t="shared" si="31"/>
+        <v>6</v>
+      </c>
+      <c r="T56">
+        <f t="shared" si="32"/>
+        <v>1350</v>
+      </c>
+      <c r="Y56" t="s">
+        <v>350</v>
+      </c>
+      <c r="Z56" s="4"/>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>316</v>
+      </c>
+      <c r="B57" t="s">
+        <v>317</v>
+      </c>
+      <c r="D57" t="s">
+        <v>316</v>
+      </c>
+      <c r="E57">
+        <v>1993</v>
+      </c>
+      <c r="F57">
+        <v>30</v>
+      </c>
+      <c r="G57">
+        <v>20</v>
+      </c>
+      <c r="H57">
+        <v>140</v>
+      </c>
+      <c r="I57" t="s">
+        <v>309</v>
+      </c>
+      <c r="M57">
+        <v>92</v>
+      </c>
+      <c r="N57">
+        <v>12</v>
+      </c>
+      <c r="O57">
+        <v>200</v>
+      </c>
+      <c r="P57">
+        <v>49.2</v>
+      </c>
+      <c r="Q57">
+        <f t="shared" si="29"/>
+        <v>8</v>
+      </c>
+      <c r="R57">
+        <f t="shared" si="30"/>
+        <v>25000</v>
+      </c>
+      <c r="S57">
+        <f t="shared" si="31"/>
+        <v>5</v>
+      </c>
+      <c r="T57">
+        <f t="shared" si="32"/>
+        <v>1125</v>
+      </c>
+      <c r="Y57" t="s">
+        <v>350</v>
+      </c>
+      <c r="Z57" s="4"/>
+    </row>
+    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>345</v>
+      </c>
+      <c r="B58" t="s">
+        <v>347</v>
+      </c>
+      <c r="E58">
+        <v>2014</v>
+      </c>
+      <c r="F58">
+        <v>30</v>
+      </c>
+      <c r="G58" t="s">
+        <v>91</v>
+      </c>
+      <c r="H58">
+        <v>140</v>
+      </c>
+      <c r="I58" t="s">
+        <v>90</v>
+      </c>
+      <c r="M58">
+        <v>80</v>
+      </c>
+      <c r="N58">
+        <v>16</v>
+      </c>
+      <c r="O58">
+        <v>360</v>
+      </c>
+      <c r="P58">
+        <v>53.6</v>
+      </c>
+      <c r="Q58">
+        <f t="shared" si="29"/>
+        <v>13</v>
+      </c>
+      <c r="R58">
+        <f t="shared" si="30"/>
+        <v>40625</v>
+      </c>
+      <c r="S58">
+        <f t="shared" si="31"/>
+        <v>10</v>
+      </c>
+      <c r="T58">
+        <f t="shared" si="32"/>
+        <v>2250</v>
+      </c>
+      <c r="Y58" t="s">
+        <v>350</v>
+      </c>
+      <c r="Z58" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="59" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>346</v>
+      </c>
+      <c r="B59" t="s">
+        <v>348</v>
+      </c>
+      <c r="E59">
+        <v>2014</v>
+      </c>
+      <c r="F59">
+        <v>30</v>
+      </c>
+      <c r="G59" t="s">
+        <v>91</v>
+      </c>
+      <c r="H59">
+        <v>140</v>
+      </c>
+      <c r="I59" t="s">
+        <v>90</v>
+      </c>
+      <c r="M59">
+        <v>50</v>
+      </c>
+      <c r="N59">
+        <v>16</v>
+      </c>
+      <c r="O59">
+        <v>480</v>
+      </c>
+      <c r="P59">
+        <v>56</v>
+      </c>
+      <c r="Q59">
+        <f t="shared" si="29"/>
+        <v>15</v>
+      </c>
+      <c r="R59">
+        <f t="shared" si="30"/>
+        <v>46875</v>
+      </c>
+      <c r="S59">
+        <f t="shared" si="31"/>
+        <v>12</v>
+      </c>
+      <c r="T59">
+        <f t="shared" si="32"/>
+        <v>2700</v>
+      </c>
+      <c r="Y59" t="s">
+        <v>350</v>
+      </c>
+      <c r="Z59" t="s">
+        <v>349</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="Z48:Z57"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12403,7 +13964,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8540264-B3C1-4C71-9FC9-001ABF042657}">
   <dimension ref="A1:AD12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
r146 push by wuwu (kaitokiwa)
</commit_message>
<xml_diff>
--- a/docs/China Set Trains.xlsx
+++ b/docs/China Set Trains.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GRF\China-Set\China-Set-Trains\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projcet china set\China-Set-Trains-0.1.6.146\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9675C8E5-4570-4586-AA7E-37387B4A3357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76D7D23-A0AE-4D05-82DD-9FB5C3C8FC07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="13770" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Loco" sheetId="1" r:id="rId1"/>
@@ -18,28 +18,17 @@
     <sheet name="Coaches" sheetId="3" r:id="rId3"/>
     <sheet name="Wagons" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="365">
   <si>
     <t>name</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1380,6 +1369,56 @@
   </si>
   <si>
     <t>wuwu</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DF4DF</t>
+  </si>
+  <si>
+    <t>DF4D with Locomotive Power Supply</t>
+  </si>
+  <si>
+    <t>DF4C</t>
+  </si>
+  <si>
+    <t>DF4C(Dongfeng 4C/Dongfeng4 4000series Diesel Locomotive)</t>
+  </si>
+  <si>
+    <t>DF8B</t>
+  </si>
+  <si>
+    <t>DF8B(Dongfeng 8B Diesel Locomotive)</t>
+  </si>
+  <si>
+    <t>original:EMB190 baorixile:DF43110</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DF43110</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DF4D-7000</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>df4d7000</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>df4df</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>df4c</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>df8b</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>alternative livery:DF4D3110</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1387,7 +1426,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1404,6 +1443,14 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
@@ -1433,7 +1480,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
@@ -1443,10 +1490,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
+    <cellStyle name="百分比" xfId="1" builtinId="5"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1724,21 +1781,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF45"/>
+  <dimension ref="A1:AF49"/>
   <sheetViews>
-    <sheetView topLeftCell="X1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AE28" sqref="AE28"/>
+      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="28" width="8.58203125" style="1"/>
-    <col min="29" max="30" width="8.58203125" style="2"/>
+    <col min="26" max="28" width="8.625" style="1"/>
+    <col min="29" max="30" width="8.625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1833,7 +1890,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -1893,7 +1950,7 @@
         <v>165625</v>
       </c>
       <c r="T2">
-        <f t="shared" ref="T2:T32" si="0">MEDIAN(0, 255, ROUND(SQRT(K2)/100+SQRT(L2)+P2+40/J2-2,0))</f>
+        <f t="shared" ref="T2:T20" si="0">MEDIAN(0, 255, ROUND(SQRT(K2)/100+SQRT(L2)+P2+40/J2-2,0))</f>
         <v>39</v>
       </c>
       <c r="U2">
@@ -1924,7 +1981,7 @@
         <v>0.44444444444444442</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -1949,11 +2006,11 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <f t="shared" ref="R3:R37" si="3">MEDIAN(255, ROUND((M3/10+SQRT(K3)/20+SQRT(L3)+P3+20-J3), 0), 0)</f>
+        <f t="shared" ref="R3:R20" si="3">MEDIAN(255, ROUND((M3/10+SQRT(K3)/20+SQRT(L3)+P3+20-J3), 0), 0)</f>
         <v>20</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="S3:S37" si="4">R3*50000/16</f>
+        <f t="shared" ref="S3:S20" si="4">R3*50000/16</f>
         <v>62500</v>
       </c>
       <c r="T3" t="e">
@@ -1961,7 +2018,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="U3" t="e">
-        <f t="shared" ref="U3:U37" si="5">IF(E3="Steam", T3*350/16*12, IF(E3="Diesel", T3*325/16*12,  T3*300/16*12))</f>
+        <f t="shared" ref="U3:U19" si="5">IF(E3="Steam", T3*350/16*12, IF(E3="Diesel", T3*325/16*12,  T3*300/16*12))</f>
         <v>#DIV/0!</v>
       </c>
       <c r="V3">
@@ -1973,7 +2030,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -2022,7 +2079,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -2071,7 +2128,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -2120,7 +2177,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -2166,7 +2223,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>106</v>
       </c>
@@ -2248,7 +2305,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>107</v>
       </c>
@@ -2345,7 +2402,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>200</v>
       </c>
@@ -2410,8 +2467,11 @@
         <f t="shared" ref="V10:V12" si="15">W10+X10+Y10</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AE10" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>201</v>
       </c>
@@ -2477,7 +2537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>202</v>
       </c>
@@ -2542,8 +2602,11 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AE12" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>234</v>
       </c>
@@ -2592,7 +2655,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -2661,7 +2724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -2710,7 +2773,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -2783,7 +2846,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -2829,7 +2892,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>235</v>
       </c>
@@ -2895,7 +2958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -2944,7 +3007,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>152</v>
       </c>
@@ -3038,7 +3101,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>319</v>
       </c>
@@ -3123,7 +3186,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>324</v>
       </c>
@@ -3217,7 +3280,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>327</v>
       </c>
@@ -3300,7 +3363,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>331</v>
       </c>
@@ -3371,7 +3434,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>333</v>
       </c>
@@ -3442,7 +3505,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>335</v>
       </c>
@@ -3516,7 +3579,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>338</v>
       </c>
@@ -3590,7 +3653,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>340</v>
       </c>
@@ -3674,7 +3737,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -3723,7 +3786,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -3796,7 +3859,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -3869,7 +3932,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -3942,7 +4005,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -4039,7 +4102,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -4088,7 +4151,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>139</v>
       </c>
@@ -4185,7 +4248,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>194</v>
       </c>
@@ -4249,7 +4312,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>197</v>
       </c>
@@ -4316,7 +4379,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>258</v>
       </c>
@@ -4401,7 +4464,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>263</v>
       </c>
@@ -4489,7 +4552,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>265</v>
       </c>
@@ -4577,7 +4640,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>267</v>
       </c>
@@ -4665,7 +4728,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>269</v>
       </c>
@@ -4753,7 +4816,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>272</v>
       </c>
@@ -4841,7 +4904,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>274</v>
       </c>
@@ -4932,7 +4995,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>277</v>
       </c>
@@ -5018,6 +5081,322 @@
       </c>
       <c r="AF45" t="s">
         <v>276</v>
+      </c>
+    </row>
+    <row r="46" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A46" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="C46" s="6"/>
+      <c r="D46" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="F46" s="7">
+        <v>1999</v>
+      </c>
+      <c r="G46" s="7">
+        <v>30</v>
+      </c>
+      <c r="H46" s="7">
+        <v>60</v>
+      </c>
+      <c r="I46" s="7">
+        <v>30</v>
+      </c>
+      <c r="J46" s="7">
+        <v>16</v>
+      </c>
+      <c r="K46" s="7">
+        <v>120</v>
+      </c>
+      <c r="L46" s="7">
+        <v>3300</v>
+      </c>
+      <c r="M46" s="7">
+        <v>138</v>
+      </c>
+      <c r="N46" s="6"/>
+      <c r="O46" s="7">
+        <v>138</v>
+      </c>
+      <c r="P46" s="7">
+        <v>0.27876367899999999</v>
+      </c>
+      <c r="Q46" s="7">
+        <v>377</v>
+      </c>
+      <c r="R46" s="7">
+        <v>76</v>
+      </c>
+      <c r="S46" s="7">
+        <v>237500</v>
+      </c>
+      <c r="T46" s="7">
+        <v>58</v>
+      </c>
+      <c r="U46" s="7">
+        <v>14137.5</v>
+      </c>
+      <c r="V46" s="7">
+        <v>10</v>
+      </c>
+      <c r="W46">
+        <v>2</v>
+      </c>
+      <c r="X46">
+        <v>6</v>
+      </c>
+      <c r="Y46">
+        <v>2</v>
+      </c>
+      <c r="AD46" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="AE46" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="47" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A47" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="C47" s="6"/>
+      <c r="D47" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="F47" s="7">
+        <v>1985</v>
+      </c>
+      <c r="G47" s="7">
+        <v>30</v>
+      </c>
+      <c r="H47" s="7">
+        <v>60</v>
+      </c>
+      <c r="I47" s="7">
+        <v>30</v>
+      </c>
+      <c r="J47" s="7">
+        <v>16</v>
+      </c>
+      <c r="K47" s="7">
+        <v>100</v>
+      </c>
+      <c r="L47" s="7">
+        <v>3600</v>
+      </c>
+      <c r="M47" s="7">
+        <v>138</v>
+      </c>
+      <c r="N47" s="6"/>
+      <c r="O47" s="7">
+        <v>138</v>
+      </c>
+      <c r="P47" s="7">
+        <v>0.32534753</v>
+      </c>
+      <c r="Q47" s="7">
+        <v>440</v>
+      </c>
+      <c r="R47" s="7">
+        <v>81</v>
+      </c>
+      <c r="S47" s="7">
+        <v>253125</v>
+      </c>
+      <c r="T47" s="7">
+        <v>61</v>
+      </c>
+      <c r="U47" s="7">
+        <v>14868.75</v>
+      </c>
+      <c r="V47" s="7">
+        <v>10</v>
+      </c>
+      <c r="W47">
+        <v>2</v>
+      </c>
+      <c r="X47">
+        <v>6</v>
+      </c>
+      <c r="Y47">
+        <v>2</v>
+      </c>
+      <c r="AD47" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="AE47" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="48" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A48" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="C48" s="6"/>
+      <c r="D48" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="F48" s="7">
+        <v>1997.6</v>
+      </c>
+      <c r="G48" s="7">
+        <v>30</v>
+      </c>
+      <c r="H48" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="I48" s="8"/>
+      <c r="J48" s="7">
+        <v>14</v>
+      </c>
+      <c r="K48" s="7">
+        <v>100</v>
+      </c>
+      <c r="L48" s="7">
+        <v>4214</v>
+      </c>
+      <c r="M48" s="7">
+        <v>143.5</v>
+      </c>
+      <c r="N48" s="6"/>
+      <c r="O48" s="7">
+        <v>143.5</v>
+      </c>
+      <c r="P48" s="7">
+        <v>0.34132119700000002</v>
+      </c>
+      <c r="Q48" s="7">
+        <v>480</v>
+      </c>
+      <c r="R48" s="7">
+        <v>86</v>
+      </c>
+      <c r="S48" s="7">
+        <v>268750</v>
+      </c>
+      <c r="T48" s="7">
+        <v>66</v>
+      </c>
+      <c r="U48" s="7">
+        <v>16087.5</v>
+      </c>
+      <c r="V48" s="7">
+        <v>10</v>
+      </c>
+      <c r="W48">
+        <v>2</v>
+      </c>
+      <c r="X48">
+        <v>6</v>
+      </c>
+      <c r="Y48">
+        <v>2</v>
+      </c>
+      <c r="AD48" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="AE48" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="49" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>359</v>
+      </c>
+      <c r="B49" t="s">
+        <v>360</v>
+      </c>
+      <c r="E49" t="s">
+        <v>51</v>
+      </c>
+      <c r="F49">
+        <v>1998</v>
+      </c>
+      <c r="G49">
+        <v>30</v>
+      </c>
+      <c r="H49">
+        <v>50</v>
+      </c>
+      <c r="I49">
+        <v>35</v>
+      </c>
+      <c r="J49">
+        <v>14</v>
+      </c>
+      <c r="K49">
+        <v>100</v>
+      </c>
+      <c r="L49">
+        <v>4000</v>
+      </c>
+      <c r="M49">
+        <v>138</v>
+      </c>
+      <c r="O49">
+        <f t="shared" ref="O49" si="39">M49-N49</f>
+        <v>138</v>
+      </c>
+      <c r="P49">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="Q49">
+        <f t="shared" ref="Q49" si="40">O49*P49*9.8</f>
+        <v>480.10199999999998</v>
+      </c>
+      <c r="R49">
+        <f t="shared" ref="R49" si="41">MEDIAN(255, ROUND((M49/10+SQRT(K49)/20+SQRT(L49)+P49+20-J49), 0), 0)</f>
+        <v>84</v>
+      </c>
+      <c r="S49">
+        <f t="shared" ref="S49" si="42">R49*50000/16</f>
+        <v>262500</v>
+      </c>
+      <c r="T49">
+        <f t="shared" ref="T49" si="43">MEDIAN(0, 255, ROUND(SQRT(K49)/100+SQRT(L49)+P49+40/J49-2,0))</f>
+        <v>65</v>
+      </c>
+      <c r="U49">
+        <f t="shared" ref="U49" si="44">IF(E49="Steam", T49*350/16*12, IF(E49="Diesel", T49*325/16*12,  T49*300/16*12))</f>
+        <v>15843.75</v>
+      </c>
+      <c r="V49">
+        <f t="shared" ref="V49" si="45">W49+X49+Y49</f>
+        <v>10</v>
+      </c>
+      <c r="W49">
+        <v>2</v>
+      </c>
+      <c r="X49">
+        <v>6</v>
+      </c>
+      <c r="Y49">
+        <v>2</v>
+      </c>
+      <c r="AD49" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="AE49" s="2" t="s">
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -5035,9 +5414,9 @@
       <selection pane="bottomLeft" activeCell="U81" sqref="U81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5135,7 +5514,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>133</v>
       </c>
@@ -5203,7 +5582,7 @@
         <v>1650</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="I3">
         <v>20</v>
       </c>
@@ -5253,7 +5632,7 @@
         <v>2325</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>130</v>
       </c>
@@ -5306,7 +5685,7 @@
         <v>131.25</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>131</v>
       </c>
@@ -5359,7 +5738,7 @@
         <v>206.25</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>132</v>
       </c>
@@ -5412,7 +5791,7 @@
         <v>281.25</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>134</v>
       </c>
@@ -5465,7 +5844,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>138</v>
       </c>
@@ -5518,7 +5897,7 @@
         <v>93.75</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>135</v>
       </c>
@@ -5571,7 +5950,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>136</v>
       </c>
@@ -5624,7 +6003,7 @@
         <v>281.25</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>137</v>
       </c>
@@ -5677,7 +6056,7 @@
         <v>318.75</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>150</v>
       </c>
@@ -5730,7 +6109,7 @@
         <v>937.5</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>130</v>
       </c>
@@ -5783,7 +6162,7 @@
         <v>862.5</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>131</v>
       </c>
@@ -5836,7 +6215,7 @@
         <v>937.5</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>132</v>
       </c>
@@ -5889,7 +6268,7 @@
         <v>1012.5</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>134</v>
       </c>
@@ -5942,7 +6321,7 @@
         <v>1031.25</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>138</v>
       </c>
@@ -5995,7 +6374,7 @@
         <v>843.75</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>151</v>
       </c>
@@ -6051,7 +6430,7 @@
         <v>131.25</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>131</v>
       </c>
@@ -6104,7 +6483,7 @@
         <v>206.25</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>132</v>
       </c>
@@ -6157,7 +6536,7 @@
         <v>281.25</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>134</v>
       </c>
@@ -6210,7 +6589,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>138</v>
       </c>
@@ -6263,7 +6642,7 @@
         <v>112.5</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>158</v>
       </c>
@@ -6316,7 +6695,7 @@
         <v>1406.25</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>130</v>
       </c>
@@ -6369,7 +6748,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>131</v>
       </c>
@@ -6422,7 +6801,7 @@
         <v>1406.25</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>132</v>
       </c>
@@ -6475,7 +6854,7 @@
         <v>1481.25</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>134</v>
       </c>
@@ -6528,7 +6907,7 @@
         <v>1518.75</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>138</v>
       </c>
@@ -6581,7 +6960,7 @@
         <v>1312.5</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>151</v>
       </c>
@@ -6637,7 +7016,7 @@
         <v>243.75</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>131</v>
       </c>
@@ -6690,7 +7069,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>132</v>
       </c>
@@ -6743,7 +7122,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>134</v>
       </c>
@@ -6796,7 +7175,7 @@
         <v>412.5</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>138</v>
       </c>
@@ -6849,7 +7228,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>247</v>
       </c>
@@ -6899,7 +7278,7 @@
         <v>843.75</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>248</v>
       </c>
@@ -6949,7 +7328,7 @@
         <v>881.25</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>249</v>
       </c>
@@ -6999,7 +7378,7 @@
         <v>937.5</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>250</v>
       </c>
@@ -7049,7 +7428,7 @@
         <v>1012.5</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>251</v>
       </c>
@@ -7099,7 +7478,7 @@
         <v>1031.25</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>252</v>
       </c>
@@ -7149,7 +7528,7 @@
         <v>843.75</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>248</v>
       </c>
@@ -7199,7 +7578,7 @@
         <v>131.25</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>249</v>
       </c>
@@ -7249,7 +7628,7 @@
         <v>206.25</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>250</v>
       </c>
@@ -7299,7 +7678,7 @@
         <v>281.25</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>251</v>
       </c>
@@ -7349,7 +7728,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>252</v>
       </c>
@@ -7399,7 +7778,7 @@
         <v>112.5</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>253</v>
       </c>
@@ -7449,7 +7828,7 @@
         <v>937.5</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>248</v>
       </c>
@@ -7499,7 +7878,7 @@
         <v>956.25</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>249</v>
       </c>
@@ -7549,7 +7928,7 @@
         <v>1012.5</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>250</v>
       </c>
@@ -7599,7 +7978,7 @@
         <v>1106.25</v>
       </c>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>251</v>
       </c>
@@ -7649,7 +8028,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>252</v>
       </c>
@@ -7699,7 +8078,7 @@
         <v>937.5</v>
       </c>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>248</v>
       </c>
@@ -7749,7 +8128,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>249</v>
       </c>
@@ -7799,7 +8178,7 @@
         <v>206.25</v>
       </c>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>250</v>
       </c>
@@ -7849,7 +8228,7 @@
         <v>281.25</v>
       </c>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>251</v>
       </c>
@@ -7899,7 +8278,7 @@
         <v>318.75</v>
       </c>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>252</v>
       </c>
@@ -7949,7 +8328,7 @@
         <v>131.25</v>
       </c>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>254</v>
       </c>
@@ -7999,7 +8378,7 @@
         <v>1668.75</v>
       </c>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>248</v>
       </c>
@@ -8049,7 +8428,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
         <v>249</v>
       </c>
@@ -8099,7 +8478,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>250</v>
       </c>
@@ -8149,7 +8528,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>251</v>
       </c>
@@ -8199,7 +8578,7 @@
         <v>318.75</v>
       </c>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>252</v>
       </c>
@@ -8249,7 +8628,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>255</v>
       </c>
@@ -8299,7 +8678,7 @@
         <v>1031.25</v>
       </c>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>248</v>
       </c>
@@ -8349,7 +8728,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>249</v>
       </c>
@@ -8399,7 +8778,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
         <v>250</v>
       </c>
@@ -8449,7 +8828,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
         <v>251</v>
       </c>
@@ -8499,7 +8878,7 @@
         <v>1143.75</v>
       </c>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>252</v>
       </c>
@@ -8549,7 +8928,7 @@
         <v>956.25</v>
       </c>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>248</v>
       </c>
@@ -8599,7 +8978,7 @@
         <v>187.5</v>
       </c>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
         <v>249</v>
       </c>
@@ -8649,7 +9028,7 @@
         <v>262.5</v>
       </c>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
         <v>250</v>
       </c>
@@ -8699,7 +9078,7 @@
         <v>337.5</v>
       </c>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
         <v>251</v>
       </c>
@@ -8749,7 +9128,7 @@
         <v>356.25</v>
       </c>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
         <v>252</v>
       </c>
@@ -8799,7 +9178,7 @@
         <v>168.75</v>
       </c>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>256</v>
       </c>
@@ -8849,7 +9228,7 @@
         <v>1106.25</v>
       </c>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
         <v>248</v>
       </c>
@@ -8899,7 +9278,7 @@
         <v>206.25</v>
       </c>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
         <v>249</v>
       </c>
@@ -8949,7 +9328,7 @@
         <v>281.25</v>
       </c>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
         <v>252</v>
       </c>
@@ -8999,7 +9378,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>257</v>
       </c>
@@ -9049,7 +9428,7 @@
         <v>1518.75</v>
       </c>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
         <v>249</v>
       </c>
@@ -9099,7 +9478,7 @@
         <v>112.5</v>
       </c>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>284</v>
       </c>
@@ -9149,7 +9528,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
         <v>285</v>
       </c>
@@ -9199,7 +9578,7 @@
         <v>1293.75</v>
       </c>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
         <v>286</v>
       </c>
@@ -9249,7 +9628,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
         <v>287</v>
       </c>
@@ -9299,7 +9678,7 @@
         <v>1443.75</v>
       </c>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>288</v>
       </c>
@@ -9349,7 +9728,7 @@
         <v>1462.5</v>
       </c>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
         <v>289</v>
       </c>
@@ -9399,7 +9778,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>151</v>
       </c>
@@ -9452,7 +9831,7 @@
         <v>243.75</v>
       </c>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
         <v>286</v>
       </c>
@@ -9502,7 +9881,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
         <v>287</v>
       </c>
@@ -9552,7 +9931,7 @@
         <v>393.75</v>
       </c>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
         <v>288</v>
       </c>
@@ -9602,7 +9981,7 @@
         <v>412.5</v>
       </c>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
         <v>289</v>
       </c>
@@ -9652,7 +10031,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>290</v>
       </c>
@@ -9702,7 +10081,7 @@
         <v>1181.25</v>
       </c>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
         <v>285</v>
       </c>
@@ -9752,7 +10131,7 @@
         <v>1181.25</v>
       </c>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
         <v>286</v>
       </c>
@@ -9802,7 +10181,7 @@
         <v>1256.25</v>
       </c>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
         <v>287</v>
       </c>
@@ -9852,7 +10231,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
         <v>288</v>
       </c>
@@ -9902,7 +10281,7 @@
         <v>1368.75</v>
       </c>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
         <v>289</v>
       </c>
@@ -9952,7 +10331,7 @@
         <v>1162.5</v>
       </c>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>151</v>
       </c>
@@ -10005,7 +10384,7 @@
         <v>168.75</v>
       </c>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
         <v>286</v>
       </c>
@@ -10055,7 +10434,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
         <v>287</v>
       </c>
@@ -10105,7 +10484,7 @@
         <v>318.75</v>
       </c>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
         <v>288</v>
       </c>
@@ -10155,7 +10534,7 @@
         <v>337.5</v>
       </c>
     </row>
-    <row r="100" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
         <v>289</v>
       </c>
@@ -10205,7 +10584,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="101" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>291</v>
       </c>
@@ -10255,7 +10634,7 @@
         <v>937.5</v>
       </c>
     </row>
-    <row r="102" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
         <v>285</v>
       </c>
@@ -10305,7 +10684,7 @@
         <v>862.5</v>
       </c>
     </row>
-    <row r="103" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
         <v>286</v>
       </c>
@@ -10355,7 +10734,7 @@
         <v>956.25</v>
       </c>
     </row>
-    <row r="104" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
         <v>287</v>
       </c>
@@ -10405,7 +10784,7 @@
         <v>1031.25</v>
       </c>
     </row>
-    <row r="105" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B105" t="s">
         <v>288</v>
       </c>
@@ -10455,7 +10834,7 @@
         <v>1031.25</v>
       </c>
     </row>
-    <row r="106" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
         <v>289</v>
       </c>
@@ -10505,7 +10884,7 @@
         <v>862.5</v>
       </c>
     </row>
-    <row r="107" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>151</v>
       </c>
@@ -10558,7 +10937,7 @@
         <v>168.75</v>
       </c>
     </row>
-    <row r="108" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B108" t="s">
         <v>286</v>
       </c>
@@ -10608,7 +10987,7 @@
         <v>243.75</v>
       </c>
     </row>
-    <row r="109" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
         <v>287</v>
       </c>
@@ -10658,7 +11037,7 @@
         <v>318.75</v>
       </c>
     </row>
-    <row r="110" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B110" t="s">
         <v>288</v>
       </c>
@@ -10708,7 +11087,7 @@
         <v>318.75</v>
       </c>
     </row>
-    <row r="111" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B111" t="s">
         <v>289</v>
       </c>
@@ -10768,14 +11147,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392CFCAE-41E9-4295-93E2-AE0B308CC62A}">
   <dimension ref="A1:Z59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z48" sqref="Z48:Z57"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10855,7 +11234,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -10909,7 +11288,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -10963,7 +11342,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>82</v>
       </c>
@@ -11017,7 +11396,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>83</v>
       </c>
@@ -11071,7 +11450,7 @@
         <v>2475</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>96</v>
       </c>
@@ -11125,7 +11504,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>97</v>
       </c>
@@ -11179,7 +11558,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>98</v>
       </c>
@@ -11233,7 +11612,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>99</v>
       </c>
@@ -11287,7 +11666,7 @@
         <v>2475</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>159</v>
       </c>
@@ -11341,7 +11720,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>110</v>
       </c>
@@ -11395,7 +11774,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>114</v>
       </c>
@@ -11449,7 +11828,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>166</v>
       </c>
@@ -11500,7 +11879,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>117</v>
       </c>
@@ -11554,7 +11933,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>118</v>
       </c>
@@ -11608,7 +11987,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>119</v>
       </c>
@@ -11662,7 +12041,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>120</v>
       </c>
@@ -11716,7 +12095,7 @@
         <v>2475</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>214</v>
       </c>
@@ -11767,7 +12146,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>213</v>
       </c>
@@ -11818,7 +12197,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>223</v>
       </c>
@@ -11869,7 +12248,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>224</v>
       </c>
@@ -11920,7 +12299,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>225</v>
       </c>
@@ -11971,7 +12350,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>226</v>
       </c>
@@ -12022,7 +12401,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>231</v>
       </c>
@@ -12073,7 +12452,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>141</v>
       </c>
@@ -12127,7 +12506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>154</v>
       </c>
@@ -12181,7 +12560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>156</v>
       </c>
@@ -12235,7 +12614,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>168</v>
       </c>
@@ -12286,7 +12665,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>169</v>
       </c>
@@ -12337,7 +12716,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>170</v>
       </c>
@@ -12388,7 +12767,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>171</v>
       </c>
@@ -12439,7 +12818,7 @@
         <v>2475</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>207</v>
       </c>
@@ -12490,7 +12869,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>208</v>
       </c>
@@ -12541,7 +12920,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>215</v>
       </c>
@@ -12592,7 +12971,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>216</v>
       </c>
@@ -12643,7 +13022,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>219</v>
       </c>
@@ -12694,7 +13073,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>221</v>
       </c>
@@ -12745,7 +13124,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>172</v>
       </c>
@@ -12796,7 +13175,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>178</v>
       </c>
@@ -12847,7 +13226,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>183</v>
       </c>
@@ -12898,7 +13277,7 @@
         <v>2475</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>185</v>
       </c>
@@ -12949,7 +13328,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>186</v>
       </c>
@@ -13000,7 +13379,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>187</v>
       </c>
@@ -13051,7 +13430,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>188</v>
       </c>
@@ -13102,7 +13481,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>279</v>
       </c>
@@ -13153,7 +13532,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>281</v>
       </c>
@@ -13204,7 +13583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>292</v>
       </c>
@@ -13255,7 +13634,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>296</v>
       </c>
@@ -13315,7 +13694,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>299</v>
       </c>
@@ -13373,7 +13752,7 @@
       </c>
       <c r="Z49" s="4"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>301</v>
       </c>
@@ -13431,7 +13810,7 @@
       </c>
       <c r="Z50" s="4"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>303</v>
       </c>
@@ -13489,7 +13868,7 @@
       </c>
       <c r="Z51" s="4"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>305</v>
       </c>
@@ -13547,7 +13926,7 @@
       </c>
       <c r="Z52" s="4"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>307</v>
       </c>
@@ -13605,7 +13984,7 @@
       </c>
       <c r="Z53" s="4"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>310</v>
       </c>
@@ -13663,7 +14042,7 @@
       </c>
       <c r="Z54" s="4"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>312</v>
       </c>
@@ -13721,7 +14100,7 @@
       </c>
       <c r="Z55" s="4"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>314</v>
       </c>
@@ -13779,7 +14158,7 @@
       </c>
       <c r="Z56" s="4"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>316</v>
       </c>
@@ -13837,7 +14216,7 @@
       </c>
       <c r="Z57" s="4"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>345</v>
       </c>
@@ -13894,7 +14273,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>346</v>
       </c>
@@ -13968,9 +14347,9 @@
       <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -14062,7 +14441,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>144</v>
       </c>
@@ -14108,7 +14487,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>148</v>
       </c>
@@ -14148,7 +14527,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>181</v>
       </c>
@@ -14191,7 +14570,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>192</v>
       </c>
@@ -14231,7 +14610,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>196</v>
       </c>
@@ -14274,7 +14653,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>205</v>
       </c>
@@ -14314,7 +14693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>237</v>
       </c>
@@ -14357,7 +14736,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>239</v>
       </c>
@@ -14397,7 +14776,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>240</v>
       </c>
@@ -14437,7 +14816,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>241</v>
       </c>
@@ -14477,7 +14856,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>294</v>
       </c>

</xml_diff>

<commit_message>
r146 push by wuwu
</commit_message>
<xml_diff>
--- a/docs/China Set Trains.xlsx
+++ b/docs/China Set Trains.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projcet china set\China-Set-Trains-0.1.6.146\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projcet china set\China-Set-Trains-Github\China-Set-Trains-main (4)\China-Set-Trains-main\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76D7D23-A0AE-4D05-82DD-9FB5C3C8FC07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D086BD-6865-4E25-9065-03931AF1244D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Loco" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="366">
   <si>
     <t>name</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1419,6 +1419,10 @@
   </si>
   <si>
     <t>alternative livery:DF4D3110</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DF4B3110</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1484,12 +1488,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1499,7 +1497,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="百分比" xfId="1" builtinId="5"/>
@@ -1783,7 +1787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
     </sheetView>
@@ -5084,66 +5088,66 @@
       </c>
     </row>
     <row r="46" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A46" s="5" t="s">
+      <c r="A46" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="3" t="s">
         <v>361</v>
       </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="5" t="s">
+      <c r="C46" s="4"/>
+      <c r="D46" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="E46" s="5" t="s">
+      <c r="E46" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="F46" s="7">
+      <c r="F46" s="5">
         <v>1999</v>
       </c>
-      <c r="G46" s="7">
+      <c r="G46" s="5">
         <v>30</v>
       </c>
-      <c r="H46" s="7">
+      <c r="H46" s="5">
         <v>60</v>
       </c>
-      <c r="I46" s="7">
+      <c r="I46" s="5">
         <v>30</v>
       </c>
-      <c r="J46" s="7">
+      <c r="J46" s="5">
         <v>16</v>
       </c>
-      <c r="K46" s="7">
+      <c r="K46" s="5">
         <v>120</v>
       </c>
-      <c r="L46" s="7">
+      <c r="L46" s="5">
         <v>3300</v>
       </c>
-      <c r="M46" s="7">
+      <c r="M46" s="5">
         <v>138</v>
       </c>
-      <c r="N46" s="6"/>
-      <c r="O46" s="7">
+      <c r="N46" s="4"/>
+      <c r="O46" s="5">
         <v>138</v>
       </c>
-      <c r="P46" s="7">
+      <c r="P46" s="5">
         <v>0.27876367899999999</v>
       </c>
-      <c r="Q46" s="7">
+      <c r="Q46" s="5">
         <v>377</v>
       </c>
-      <c r="R46" s="7">
+      <c r="R46" s="5">
         <v>76</v>
       </c>
-      <c r="S46" s="7">
+      <c r="S46" s="5">
         <v>237500</v>
       </c>
-      <c r="T46" s="7">
+      <c r="T46" s="5">
         <v>58</v>
       </c>
-      <c r="U46" s="7">
+      <c r="U46" s="5">
         <v>14137.5</v>
       </c>
-      <c r="V46" s="7">
+      <c r="V46" s="5">
         <v>10</v>
       </c>
       <c r="W46">
@@ -5163,66 +5167,66 @@
       </c>
     </row>
     <row r="47" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="C47" s="6"/>
-      <c r="D47" s="5" t="s">
+      <c r="C47" s="4"/>
+      <c r="D47" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="E47" s="5" t="s">
+      <c r="E47" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="F47" s="7">
+      <c r="F47" s="5">
         <v>1985</v>
       </c>
-      <c r="G47" s="7">
+      <c r="G47" s="5">
         <v>30</v>
       </c>
-      <c r="H47" s="7">
+      <c r="H47" s="5">
         <v>60</v>
       </c>
-      <c r="I47" s="7">
+      <c r="I47" s="5">
         <v>30</v>
       </c>
-      <c r="J47" s="7">
+      <c r="J47" s="5">
         <v>16</v>
       </c>
-      <c r="K47" s="7">
+      <c r="K47" s="5">
         <v>100</v>
       </c>
-      <c r="L47" s="7">
+      <c r="L47" s="5">
         <v>3600</v>
       </c>
-      <c r="M47" s="7">
+      <c r="M47" s="5">
         <v>138</v>
       </c>
-      <c r="N47" s="6"/>
-      <c r="O47" s="7">
+      <c r="N47" s="4"/>
+      <c r="O47" s="5">
         <v>138</v>
       </c>
-      <c r="P47" s="7">
+      <c r="P47" s="5">
         <v>0.32534753</v>
       </c>
-      <c r="Q47" s="7">
+      <c r="Q47" s="5">
         <v>440</v>
       </c>
-      <c r="R47" s="7">
+      <c r="R47" s="5">
         <v>81</v>
       </c>
-      <c r="S47" s="7">
+      <c r="S47" s="5">
         <v>253125</v>
       </c>
-      <c r="T47" s="7">
+      <c r="T47" s="5">
         <v>61</v>
       </c>
-      <c r="U47" s="7">
+      <c r="U47" s="5">
         <v>14868.75</v>
       </c>
-      <c r="V47" s="7">
+      <c r="V47" s="5">
         <v>10</v>
       </c>
       <c r="W47">
@@ -5242,64 +5246,64 @@
       </c>
     </row>
     <row r="48" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="C48" s="6"/>
-      <c r="D48" s="5" t="s">
+      <c r="C48" s="4"/>
+      <c r="D48" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="E48" s="5" t="s">
+      <c r="E48" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="F48" s="7">
+      <c r="F48" s="5">
         <v>1997.6</v>
       </c>
-      <c r="G48" s="7">
+      <c r="G48" s="5">
         <v>30</v>
       </c>
-      <c r="H48" s="8" t="s">
+      <c r="H48" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="I48" s="8"/>
-      <c r="J48" s="7">
+      <c r="I48" s="6"/>
+      <c r="J48" s="5">
         <v>14</v>
       </c>
-      <c r="K48" s="7">
+      <c r="K48" s="5">
         <v>100</v>
       </c>
-      <c r="L48" s="7">
+      <c r="L48" s="5">
         <v>4214</v>
       </c>
-      <c r="M48" s="7">
+      <c r="M48" s="5">
         <v>143.5</v>
       </c>
-      <c r="N48" s="6"/>
-      <c r="O48" s="7">
+      <c r="N48" s="4"/>
+      <c r="O48" s="5">
         <v>143.5</v>
       </c>
-      <c r="P48" s="7">
+      <c r="P48" s="5">
         <v>0.34132119700000002</v>
       </c>
-      <c r="Q48" s="7">
+      <c r="Q48" s="5">
         <v>480</v>
       </c>
-      <c r="R48" s="7">
+      <c r="R48" s="5">
         <v>86</v>
       </c>
-      <c r="S48" s="7">
+      <c r="S48" s="5">
         <v>268750</v>
       </c>
-      <c r="T48" s="7">
+      <c r="T48" s="5">
         <v>66</v>
       </c>
-      <c r="U48" s="7">
+      <c r="U48" s="5">
         <v>16087.5</v>
       </c>
-      <c r="V48" s="7">
+      <c r="V48" s="5">
         <v>10</v>
       </c>
       <c r="W48">
@@ -13690,7 +13694,7 @@
       <c r="Y48" t="s">
         <v>350</v>
       </c>
-      <c r="Z48" s="3" t="s">
+      <c r="Z48" s="7" t="s">
         <v>318</v>
       </c>
     </row>
@@ -13750,7 +13754,7 @@
       <c r="Y49" t="s">
         <v>350</v>
       </c>
-      <c r="Z49" s="4"/>
+      <c r="Z49" s="8"/>
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
@@ -13808,7 +13812,7 @@
       <c r="Y50" t="s">
         <v>350</v>
       </c>
-      <c r="Z50" s="4"/>
+      <c r="Z50" s="8"/>
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
@@ -13866,7 +13870,7 @@
       <c r="Y51" t="s">
         <v>350</v>
       </c>
-      <c r="Z51" s="4"/>
+      <c r="Z51" s="8"/>
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
@@ -13924,7 +13928,7 @@
       <c r="Y52" t="s">
         <v>350</v>
       </c>
-      <c r="Z52" s="4"/>
+      <c r="Z52" s="8"/>
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
@@ -13982,7 +13986,7 @@
       <c r="Y53" t="s">
         <v>350</v>
       </c>
-      <c r="Z53" s="4"/>
+      <c r="Z53" s="8"/>
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
@@ -14040,7 +14044,7 @@
       <c r="Y54" t="s">
         <v>350</v>
       </c>
-      <c r="Z54" s="4"/>
+      <c r="Z54" s="8"/>
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
@@ -14098,7 +14102,7 @@
       <c r="Y55" t="s">
         <v>350</v>
       </c>
-      <c r="Z55" s="4"/>
+      <c r="Z55" s="8"/>
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
@@ -14156,7 +14160,7 @@
       <c r="Y56" t="s">
         <v>350</v>
       </c>
-      <c r="Z56" s="4"/>
+      <c r="Z56" s="8"/>
     </row>
     <row r="57" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
@@ -14214,7 +14218,7 @@
       <c r="Y57" t="s">
         <v>350</v>
       </c>
-      <c r="Z57" s="4"/>
+      <c r="Z57" s="8"/>
     </row>
     <row r="58" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
@@ -14343,8 +14347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8540264-B3C1-4C71-9FC9-001ABF042657}">
   <dimension ref="A1:AD12"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -14526,6 +14530,9 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
+      <c r="AD3" t="s">
+        <v>365</v>
+      </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" t="s">

</xml_diff>

<commit_message>
r147 push by wuwu
</commit_message>
<xml_diff>
--- a/docs/China Set Trains.xlsx
+++ b/docs/China Set Trains.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projcet china set\China-Set-Trains-Github\China-Set-Trains-main (4)\China-Set-Trains-main\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projcet china set\China-Set-Trains-site\China-Set-Trains-230207\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D086BD-6865-4E25-9065-03931AF1244D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21AF65D-A774-49FA-95E1-33E37A01E42A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Loco" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="392">
   <si>
     <t>name</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1423,6 +1423,110 @@
   </si>
   <si>
     <t>DF4B3110</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>JSQ6</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>jsq6</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>B6</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>b6</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RW19K</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RW19T</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>rw19k</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>rw19t</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>haiyan</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UZ22</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>uz22</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CC_MAIL, GOOD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>yz22aircon</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>YZ22AIRCON</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RZ22AIRCON</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>rz22aircon</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>YW22AIRCON</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>yw22aircon</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RW22AIRCON</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>rw22aircon</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TZ</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>tz</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CA23AIRCON</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ca23aircon</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ca23</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CA23</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1788,8 +1892,8 @@
   <dimension ref="A1:AF49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5413,7 +5517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB4625FC-685F-4E56-AE60-F05D51350408}">
   <dimension ref="A1:AF111"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="U81" sqref="U81"/>
     </sheetView>
@@ -11149,11 +11253,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392CFCAE-41E9-4295-93E2-AE0B308CC62A}">
-  <dimension ref="A1:Z59"/>
+  <dimension ref="A1:Z69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B61" sqref="B61"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -13676,19 +13780,19 @@
         <v>46.4</v>
       </c>
       <c r="Q48">
-        <f t="shared" ref="Q48:Q59" si="29">MEDIAN(0,255,ROUND(P48/20+SQRT(H48)/40+SQRT(M48)/2+(SQRT(O48)-SQRT(185)), 0))</f>
+        <f t="shared" ref="Q48:Q62" si="29">MEDIAN(0,255,ROUND(P48/20+SQRT(H48)/40+SQRT(M48)/2+(SQRT(O48)-SQRT(185)), 0))</f>
         <v>9</v>
       </c>
       <c r="R48">
-        <f t="shared" ref="R48:R59" si="30">Q48*50000/16</f>
+        <f t="shared" ref="R48:R62" si="30">Q48*50000/16</f>
         <v>28125</v>
       </c>
       <c r="S48">
-        <f t="shared" ref="S48:S59" si="31">MEDIAN(0,255,ROUND(SQRT(H48)/200+SQRT(M48)/2+(SQRT(O48)-SQRT(185)),0))</f>
+        <f t="shared" ref="S48:S62" si="31">MEDIAN(0,255,ROUND(SQRT(H48)/200+SQRT(M48)/2+(SQRT(O48)-SQRT(185)),0))</f>
         <v>7</v>
       </c>
       <c r="T48">
-        <f t="shared" ref="T48:T59" si="32">S48*300/16*12</f>
+        <f t="shared" ref="T48:T62" si="32">S48*300/16*12</f>
         <v>1575</v>
       </c>
       <c r="Y48" t="s">
@@ -14332,6 +14436,576 @@
       </c>
       <c r="Z59" t="s">
         <v>349</v>
+      </c>
+    </row>
+    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>370</v>
+      </c>
+      <c r="B60" t="s">
+        <v>372</v>
+      </c>
+      <c r="E60">
+        <v>1997</v>
+      </c>
+      <c r="F60">
+        <v>30</v>
+      </c>
+      <c r="G60" t="s">
+        <v>91</v>
+      </c>
+      <c r="H60">
+        <v>160</v>
+      </c>
+      <c r="I60" t="s">
+        <v>90</v>
+      </c>
+      <c r="M60">
+        <v>16</v>
+      </c>
+      <c r="N60">
+        <v>16</v>
+      </c>
+      <c r="O60">
+        <v>640</v>
+      </c>
+      <c r="P60">
+        <v>50</v>
+      </c>
+      <c r="Q60">
+        <f t="shared" si="29"/>
+        <v>17</v>
+      </c>
+      <c r="R60">
+        <f t="shared" si="30"/>
+        <v>53125</v>
+      </c>
+      <c r="S60">
+        <f t="shared" si="31"/>
+        <v>14</v>
+      </c>
+      <c r="T60">
+        <f t="shared" si="32"/>
+        <v>3150</v>
+      </c>
+      <c r="Y60" t="s">
+        <v>343</v>
+      </c>
+      <c r="Z60" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>371</v>
+      </c>
+      <c r="B61" t="s">
+        <v>373</v>
+      </c>
+      <c r="E61">
+        <v>2007.5</v>
+      </c>
+      <c r="F61">
+        <v>30</v>
+      </c>
+      <c r="G61" t="s">
+        <v>91</v>
+      </c>
+      <c r="H61">
+        <v>160</v>
+      </c>
+      <c r="I61" t="s">
+        <v>90</v>
+      </c>
+      <c r="M61">
+        <v>16</v>
+      </c>
+      <c r="N61">
+        <v>16</v>
+      </c>
+      <c r="O61">
+        <v>640</v>
+      </c>
+      <c r="P61">
+        <v>54</v>
+      </c>
+      <c r="Q61">
+        <f t="shared" si="29"/>
+        <v>17</v>
+      </c>
+      <c r="R61">
+        <f t="shared" si="30"/>
+        <v>53125</v>
+      </c>
+      <c r="S61">
+        <f t="shared" si="31"/>
+        <v>14</v>
+      </c>
+      <c r="T61">
+        <f t="shared" si="32"/>
+        <v>3150</v>
+      </c>
+      <c r="Y61" t="s">
+        <v>343</v>
+      </c>
+      <c r="Z61" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="62" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>375</v>
+      </c>
+      <c r="B62" t="s">
+        <v>376</v>
+      </c>
+      <c r="E62">
+        <v>1959</v>
+      </c>
+      <c r="F62">
+        <v>30</v>
+      </c>
+      <c r="G62">
+        <v>35</v>
+      </c>
+      <c r="H62">
+        <v>120</v>
+      </c>
+      <c r="I62" t="s">
+        <v>377</v>
+      </c>
+      <c r="M62">
+        <v>68</v>
+      </c>
+      <c r="N62">
+        <v>12</v>
+      </c>
+      <c r="O62">
+        <v>200</v>
+      </c>
+      <c r="P62">
+        <v>43</v>
+      </c>
+      <c r="Q62">
+        <f t="shared" si="29"/>
+        <v>7</v>
+      </c>
+      <c r="R62">
+        <f t="shared" si="30"/>
+        <v>21875</v>
+      </c>
+      <c r="S62">
+        <f t="shared" si="31"/>
+        <v>5</v>
+      </c>
+      <c r="T62">
+        <f t="shared" si="32"/>
+        <v>1125</v>
+      </c>
+      <c r="Y62" t="s">
+        <v>343</v>
+      </c>
+      <c r="Z62" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="63" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>379</v>
+      </c>
+      <c r="B63" t="s">
+        <v>378</v>
+      </c>
+      <c r="E63">
+        <v>1985</v>
+      </c>
+      <c r="F63">
+        <v>30</v>
+      </c>
+      <c r="G63">
+        <v>35</v>
+      </c>
+      <c r="H63">
+        <v>100</v>
+      </c>
+      <c r="I63" t="s">
+        <v>90</v>
+      </c>
+      <c r="M63">
+        <v>118</v>
+      </c>
+      <c r="N63">
+        <v>16</v>
+      </c>
+      <c r="O63">
+        <v>200</v>
+      </c>
+      <c r="P63">
+        <v>42.5</v>
+      </c>
+      <c r="Q63">
+        <f t="shared" ref="Q63:Q69" si="33">MEDIAN(0,255,ROUND(P63/20+SQRT(H63)/40+SQRT(M63)/2+(SQRT(O63)-SQRT(185)), 0))</f>
+        <v>8</v>
+      </c>
+      <c r="R63">
+        <f t="shared" ref="R63:R69" si="34">Q63*50000/16</f>
+        <v>25000</v>
+      </c>
+      <c r="S63">
+        <f t="shared" ref="S63:S69" si="35">MEDIAN(0,255,ROUND(SQRT(H63)/200+SQRT(M63)/2+(SQRT(O63)-SQRT(185)),0))</f>
+        <v>6</v>
+      </c>
+      <c r="T63">
+        <f t="shared" ref="T63:T69" si="36">S63*300/16*12</f>
+        <v>1350</v>
+      </c>
+      <c r="Y63" t="s">
+        <v>343</v>
+      </c>
+      <c r="Z63" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="64" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>380</v>
+      </c>
+      <c r="B64" t="s">
+        <v>381</v>
+      </c>
+      <c r="E64">
+        <v>1985</v>
+      </c>
+      <c r="F64">
+        <v>30</v>
+      </c>
+      <c r="G64">
+        <v>35</v>
+      </c>
+      <c r="H64">
+        <v>100</v>
+      </c>
+      <c r="I64" t="s">
+        <v>90</v>
+      </c>
+      <c r="M64">
+        <v>64</v>
+      </c>
+      <c r="N64">
+        <v>16</v>
+      </c>
+      <c r="O64">
+        <v>240</v>
+      </c>
+      <c r="P64">
+        <v>46</v>
+      </c>
+      <c r="Q64">
+        <f t="shared" si="33"/>
+        <v>8</v>
+      </c>
+      <c r="R64">
+        <f t="shared" si="34"/>
+        <v>25000</v>
+      </c>
+      <c r="S64">
+        <f t="shared" si="35"/>
+        <v>6</v>
+      </c>
+      <c r="T64">
+        <f t="shared" si="36"/>
+        <v>1350</v>
+      </c>
+      <c r="Y64" t="s">
+        <v>343</v>
+      </c>
+      <c r="Z64" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="65" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>382</v>
+      </c>
+      <c r="B65" t="s">
+        <v>383</v>
+      </c>
+      <c r="E65">
+        <v>1985</v>
+      </c>
+      <c r="F65">
+        <v>30</v>
+      </c>
+      <c r="G65">
+        <v>35</v>
+      </c>
+      <c r="H65">
+        <v>100</v>
+      </c>
+      <c r="I65" t="s">
+        <v>90</v>
+      </c>
+      <c r="M65">
+        <v>60</v>
+      </c>
+      <c r="N65">
+        <v>16</v>
+      </c>
+      <c r="O65">
+        <v>360</v>
+      </c>
+      <c r="P65">
+        <v>45</v>
+      </c>
+      <c r="Q65">
+        <f t="shared" si="33"/>
+        <v>12</v>
+      </c>
+      <c r="R65">
+        <f t="shared" si="34"/>
+        <v>37500</v>
+      </c>
+      <c r="S65">
+        <f t="shared" si="35"/>
+        <v>9</v>
+      </c>
+      <c r="T65">
+        <f t="shared" si="36"/>
+        <v>2025</v>
+      </c>
+      <c r="Y65" t="s">
+        <v>343</v>
+      </c>
+      <c r="Z65" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>384</v>
+      </c>
+      <c r="B66" t="s">
+        <v>385</v>
+      </c>
+      <c r="E66">
+        <v>1985</v>
+      </c>
+      <c r="F66">
+        <v>30</v>
+      </c>
+      <c r="G66">
+        <v>35</v>
+      </c>
+      <c r="H66">
+        <v>100</v>
+      </c>
+      <c r="I66" t="s">
+        <v>90</v>
+      </c>
+      <c r="M66">
+        <v>32</v>
+      </c>
+      <c r="N66">
+        <v>16</v>
+      </c>
+      <c r="O66">
+        <v>480</v>
+      </c>
+      <c r="P66">
+        <v>47</v>
+      </c>
+      <c r="Q66">
+        <f t="shared" si="33"/>
+        <v>14</v>
+      </c>
+      <c r="R66">
+        <f t="shared" si="34"/>
+        <v>43750</v>
+      </c>
+      <c r="S66">
+        <f t="shared" si="35"/>
+        <v>11</v>
+      </c>
+      <c r="T66">
+        <f t="shared" si="36"/>
+        <v>2475</v>
+      </c>
+      <c r="Y66" t="s">
+        <v>343</v>
+      </c>
+      <c r="Z66" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="67" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>388</v>
+      </c>
+      <c r="B67" t="s">
+        <v>389</v>
+      </c>
+      <c r="E67">
+        <v>1985</v>
+      </c>
+      <c r="F67">
+        <v>30</v>
+      </c>
+      <c r="G67">
+        <v>35</v>
+      </c>
+      <c r="H67">
+        <v>100</v>
+      </c>
+      <c r="I67" t="s">
+        <v>90</v>
+      </c>
+      <c r="M67">
+        <v>48</v>
+      </c>
+      <c r="N67">
+        <v>8</v>
+      </c>
+      <c r="O67">
+        <v>200</v>
+      </c>
+      <c r="P67">
+        <v>45</v>
+      </c>
+      <c r="Q67">
+        <f t="shared" si="33"/>
+        <v>7</v>
+      </c>
+      <c r="R67">
+        <f t="shared" si="34"/>
+        <v>21875</v>
+      </c>
+      <c r="S67">
+        <f t="shared" si="35"/>
+        <v>4</v>
+      </c>
+      <c r="T67">
+        <f t="shared" si="36"/>
+        <v>900</v>
+      </c>
+      <c r="Y67" t="s">
+        <v>343</v>
+      </c>
+      <c r="Z67" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="68" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>391</v>
+      </c>
+      <c r="B68" t="s">
+        <v>390</v>
+      </c>
+      <c r="E68">
+        <v>1963</v>
+      </c>
+      <c r="F68">
+        <v>30</v>
+      </c>
+      <c r="G68">
+        <v>35</v>
+      </c>
+      <c r="H68">
+        <v>120</v>
+      </c>
+      <c r="I68" t="s">
+        <v>90</v>
+      </c>
+      <c r="M68">
+        <v>48</v>
+      </c>
+      <c r="N68">
+        <v>8</v>
+      </c>
+      <c r="O68">
+        <v>144</v>
+      </c>
+      <c r="P68">
+        <v>45</v>
+      </c>
+      <c r="Q68">
+        <f t="shared" si="33"/>
+        <v>4</v>
+      </c>
+      <c r="R68">
+        <f t="shared" si="34"/>
+        <v>12500</v>
+      </c>
+      <c r="S68">
+        <f t="shared" si="35"/>
+        <v>2</v>
+      </c>
+      <c r="T68">
+        <f t="shared" si="36"/>
+        <v>450</v>
+      </c>
+      <c r="Y68" t="s">
+        <v>343</v>
+      </c>
+      <c r="Z68" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="69" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>386</v>
+      </c>
+      <c r="B69" t="s">
+        <v>387</v>
+      </c>
+      <c r="E69">
+        <v>1985</v>
+      </c>
+      <c r="F69">
+        <v>30</v>
+      </c>
+      <c r="G69">
+        <v>35</v>
+      </c>
+      <c r="H69">
+        <v>120</v>
+      </c>
+      <c r="I69" t="s">
+        <v>90</v>
+      </c>
+      <c r="M69">
+        <v>0</v>
+      </c>
+      <c r="N69">
+        <v>16</v>
+      </c>
+      <c r="O69">
+        <v>185</v>
+      </c>
+      <c r="P69">
+        <v>60</v>
+      </c>
+      <c r="Q69">
+        <f t="shared" si="33"/>
+        <v>3</v>
+      </c>
+      <c r="R69">
+        <f t="shared" si="34"/>
+        <v>9375</v>
+      </c>
+      <c r="S69">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="T69">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="Y69" t="s">
+        <v>343</v>
+      </c>
+      <c r="Z69" t="s">
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -14345,10 +15019,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8540264-B3C1-4C71-9FC9-001ABF042657}">
-  <dimension ref="A1:AD12"/>
+  <dimension ref="A1:AD14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X14" sqref="X14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -14483,7 +15157,7 @@
         <v>22.5</v>
       </c>
       <c r="U2">
-        <f t="shared" ref="U2:U12" si="0">MEDIAN(0,255,ROUND(S2/20+SQRT(J2)/40+SQRT(P2)/2+(SQRT(R2)-SQRT(185)),0))</f>
+        <f t="shared" ref="U2:U14" si="0">MEDIAN(0,255,ROUND(S2/20+SQRT(J2)/40+SQRT(P2)/2+(SQRT(R2)-SQRT(185)),0))</f>
         <v>5</v>
       </c>
       <c r="W2">
@@ -14901,6 +15575,89 @@
       <c r="W12">
         <f>MEDIAN(0,255,ROUND(SQRT(J12)/200+SQRT(P12)/2+(SQRT(R12)-SQRT(185)),0))</f>
         <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>366</v>
+      </c>
+      <c r="B13" t="s">
+        <v>367</v>
+      </c>
+      <c r="F13">
+        <v>2008</v>
+      </c>
+      <c r="G13">
+        <v>30</v>
+      </c>
+      <c r="H13" t="s">
+        <v>91</v>
+      </c>
+      <c r="J13">
+        <v>120</v>
+      </c>
+      <c r="P13">
+        <v>22</v>
+      </c>
+      <c r="Q13">
+        <v>6</v>
+      </c>
+      <c r="R13">
+        <v>400</v>
+      </c>
+      <c r="S13">
+        <v>37</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="W13">
+        <f>MEDIAN(0,255,ROUND(SQRT(J13)/200+SQRT(P13)/2+(SQRT(R13)-SQRT(185)),0))</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>368</v>
+      </c>
+      <c r="B14" t="s">
+        <v>369</v>
+      </c>
+      <c r="F14">
+        <v>1980</v>
+      </c>
+      <c r="G14">
+        <v>30</v>
+      </c>
+      <c r="H14">
+        <v>60</v>
+      </c>
+      <c r="I14">
+        <v>30</v>
+      </c>
+      <c r="J14">
+        <v>100</v>
+      </c>
+      <c r="P14">
+        <v>45</v>
+      </c>
+      <c r="Q14">
+        <v>12</v>
+      </c>
+      <c r="R14">
+        <v>800</v>
+      </c>
+      <c r="S14">
+        <v>34</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="W14">
+        <f>MEDIAN(0,255,ROUND(SQRT(J14)/200+SQRT(P14)/2+(SQRT(R14)-SQRT(185)),0))</f>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
r149 push by wuwu
</commit_message>
<xml_diff>
--- a/docs/China Set Trains.xlsx
+++ b/docs/China Set Trains.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GRF\China-Set\China-Set-Trains\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projcet china set\China-Set-Trains-site\China-Set-Trains-230215\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB4C339-F8E3-4739-A59D-84B13F55F428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12442D9-BF5A-46C8-924E-3BE0CC015F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="13770" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Loco" sheetId="1" r:id="rId1"/>
@@ -18,28 +18,17 @@
     <sheet name="Wagons" sheetId="4" r:id="rId3"/>
     <sheet name="Coaches" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="399">
   <si>
     <t>name</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1538,6 +1527,34 @@
   </si>
   <si>
     <t>CA23</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>B22</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>b22</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SS3B</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ss3b</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sunjuzhensun</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>L70</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>l70</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1621,8 +1638,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
+    <cellStyle name="百分比" xfId="1" builtinId="5"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1900,21 +1917,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF49"/>
+  <dimension ref="A1:AF50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J49" sqref="J49"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S51" sqref="S51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="28" width="8.58203125" style="1"/>
-    <col min="29" max="30" width="8.58203125" style="2"/>
+    <col min="26" max="28" width="8.625" style="1"/>
+    <col min="29" max="30" width="8.625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2009,7 +2026,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -2100,7 +2117,7 @@
         <v>0.44444444444444442</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -2149,7 +2166,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -2198,7 +2215,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -2247,7 +2264,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -2296,7 +2313,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -2342,7 +2359,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>106</v>
       </c>
@@ -2424,7 +2441,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>107</v>
       </c>
@@ -2521,7 +2538,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>200</v>
       </c>
@@ -2590,7 +2607,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>201</v>
       </c>
@@ -2656,7 +2673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>202</v>
       </c>
@@ -2725,7 +2742,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>234</v>
       </c>
@@ -2774,7 +2791,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -2843,7 +2860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -2892,7 +2909,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -2965,7 +2982,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -3011,7 +3028,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>235</v>
       </c>
@@ -3077,7 +3094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -3126,7 +3143,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>152</v>
       </c>
@@ -3220,7 +3237,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>319</v>
       </c>
@@ -3305,7 +3322,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>324</v>
       </c>
@@ -3399,7 +3416,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>327</v>
       </c>
@@ -3482,7 +3499,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>331</v>
       </c>
@@ -3553,7 +3570,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>333</v>
       </c>
@@ -3624,7 +3641,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>335</v>
       </c>
@@ -3698,7 +3715,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>338</v>
       </c>
@@ -3772,7 +3789,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>340</v>
       </c>
@@ -3856,7 +3873,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -3905,7 +3922,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -3978,7 +3995,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -4051,7 +4068,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -4124,7 +4141,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -4221,7 +4238,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -4270,7 +4287,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>139</v>
       </c>
@@ -4367,7 +4384,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>194</v>
       </c>
@@ -4431,7 +4448,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>197</v>
       </c>
@@ -4498,7 +4515,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>258</v>
       </c>
@@ -4583,7 +4600,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>263</v>
       </c>
@@ -4671,7 +4688,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>265</v>
       </c>
@@ -4759,7 +4776,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>267</v>
       </c>
@@ -4847,7 +4864,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>269</v>
       </c>
@@ -4935,7 +4952,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>272</v>
       </c>
@@ -5023,7 +5040,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>274</v>
       </c>
@@ -5114,7 +5131,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>277</v>
       </c>
@@ -5202,7 +5219,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>351</v>
       </c>
@@ -5281,7 +5298,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>353</v>
       </c>
@@ -5360,7 +5377,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>355</v>
       </c>
@@ -5437,7 +5454,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>359</v>
       </c>
@@ -5483,19 +5500,19 @@
         <v>480.10199999999998</v>
       </c>
       <c r="R49">
-        <f t="shared" ref="R49" si="41">MEDIAN(255, ROUND((M49/10+SQRT(K49)/20+SQRT(L49)+P49+20-J49), 0), 0)</f>
+        <f t="shared" ref="R49:R50" si="41">MEDIAN(255, ROUND((M49/10+SQRT(K49)/20+SQRT(L49)+P49+20-J49), 0), 0)</f>
         <v>84</v>
       </c>
       <c r="S49">
-        <f t="shared" ref="S49" si="42">R49*50000/16</f>
+        <f t="shared" ref="S49:S50" si="42">R49*50000/16</f>
         <v>262500</v>
       </c>
       <c r="T49">
-        <f t="shared" ref="T49" si="43">MEDIAN(0, 255, ROUND(SQRT(K49)/100+SQRT(L49)+P49+40/J49-2,0))</f>
+        <f t="shared" ref="T49:T50" si="43">MEDIAN(0, 255, ROUND(SQRT(K49)/100+SQRT(L49)+P49+40/J49-2,0))</f>
         <v>65</v>
       </c>
       <c r="U49">
-        <f t="shared" ref="U49" si="44">IF(E49="Steam", T49*350/16*12, IF(E49="Diesel", T49*325/16*12,  T49*300/16*12))</f>
+        <f t="shared" ref="U49:U50" si="44">IF(E49="Steam", T49*350/16*12, IF(E49="Diesel", T49*325/16*12,  T49*300/16*12))</f>
         <v>15843.75</v>
       </c>
       <c r="V49">
@@ -5516,6 +5533,85 @@
       </c>
       <c r="AE49" s="2" t="s">
         <v>262</v>
+      </c>
+    </row>
+    <row r="50" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="E50" t="s">
+        <v>260</v>
+      </c>
+      <c r="F50" s="5">
+        <v>2002</v>
+      </c>
+      <c r="G50" s="5">
+        <v>30</v>
+      </c>
+      <c r="H50">
+        <v>60</v>
+      </c>
+      <c r="I50">
+        <v>30</v>
+      </c>
+      <c r="J50" s="5">
+        <v>10</v>
+      </c>
+      <c r="K50" s="5">
+        <v>100</v>
+      </c>
+      <c r="L50" s="5">
+        <v>11828</v>
+      </c>
+      <c r="M50" s="5">
+        <v>276</v>
+      </c>
+      <c r="O50" s="5">
+        <v>276</v>
+      </c>
+      <c r="P50">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="Q50">
+        <f>2*Q30</f>
+        <v>938.56560000000002</v>
+      </c>
+      <c r="R50">
+        <f t="shared" si="41"/>
+        <v>147</v>
+      </c>
+      <c r="S50">
+        <f t="shared" si="42"/>
+        <v>459375</v>
+      </c>
+      <c r="T50">
+        <f t="shared" si="43"/>
+        <v>111</v>
+      </c>
+      <c r="U50">
+        <f t="shared" si="44"/>
+        <v>24975</v>
+      </c>
+      <c r="V50" s="5">
+        <v>10</v>
+      </c>
+      <c r="W50">
+        <v>2</v>
+      </c>
+      <c r="X50">
+        <v>6</v>
+      </c>
+      <c r="Y50">
+        <v>2</v>
+      </c>
+      <c r="AD50" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="AE50" t="s">
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -5533,9 +5629,9 @@
       <selection pane="bottomLeft" activeCell="U81" sqref="U81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5633,7 +5729,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>133</v>
       </c>
@@ -5701,7 +5797,7 @@
         <v>1650</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="I3">
         <v>20</v>
       </c>
@@ -5751,7 +5847,7 @@
         <v>2325</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>130</v>
       </c>
@@ -5804,7 +5900,7 @@
         <v>131.25</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>131</v>
       </c>
@@ -5857,7 +5953,7 @@
         <v>206.25</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>132</v>
       </c>
@@ -5910,7 +6006,7 @@
         <v>281.25</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>134</v>
       </c>
@@ -5963,7 +6059,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>138</v>
       </c>
@@ -6016,7 +6112,7 @@
         <v>93.75</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>135</v>
       </c>
@@ -6069,7 +6165,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>136</v>
       </c>
@@ -6122,7 +6218,7 @@
         <v>281.25</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>137</v>
       </c>
@@ -6175,7 +6271,7 @@
         <v>318.75</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>150</v>
       </c>
@@ -6228,7 +6324,7 @@
         <v>937.5</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>130</v>
       </c>
@@ -6281,7 +6377,7 @@
         <v>862.5</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>131</v>
       </c>
@@ -6334,7 +6430,7 @@
         <v>937.5</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>132</v>
       </c>
@@ -6387,7 +6483,7 @@
         <v>1012.5</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>134</v>
       </c>
@@ -6440,7 +6536,7 @@
         <v>1031.25</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>138</v>
       </c>
@@ -6493,7 +6589,7 @@
         <v>843.75</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>151</v>
       </c>
@@ -6549,7 +6645,7 @@
         <v>131.25</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>131</v>
       </c>
@@ -6602,7 +6698,7 @@
         <v>206.25</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>132</v>
       </c>
@@ -6655,7 +6751,7 @@
         <v>281.25</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>134</v>
       </c>
@@ -6708,7 +6804,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>138</v>
       </c>
@@ -6761,7 +6857,7 @@
         <v>112.5</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>158</v>
       </c>
@@ -6814,7 +6910,7 @@
         <v>1406.25</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>130</v>
       </c>
@@ -6867,7 +6963,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>131</v>
       </c>
@@ -6920,7 +7016,7 @@
         <v>1406.25</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>132</v>
       </c>
@@ -6973,7 +7069,7 @@
         <v>1481.25</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>134</v>
       </c>
@@ -7026,7 +7122,7 @@
         <v>1518.75</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>138</v>
       </c>
@@ -7079,7 +7175,7 @@
         <v>1312.5</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>151</v>
       </c>
@@ -7135,7 +7231,7 @@
         <v>243.75</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>131</v>
       </c>
@@ -7188,7 +7284,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>132</v>
       </c>
@@ -7241,7 +7337,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>134</v>
       </c>
@@ -7294,7 +7390,7 @@
         <v>412.5</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>138</v>
       </c>
@@ -7347,7 +7443,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>247</v>
       </c>
@@ -7397,7 +7493,7 @@
         <v>843.75</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>248</v>
       </c>
@@ -7447,7 +7543,7 @@
         <v>881.25</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>249</v>
       </c>
@@ -7497,7 +7593,7 @@
         <v>937.5</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>250</v>
       </c>
@@ -7547,7 +7643,7 @@
         <v>1012.5</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>251</v>
       </c>
@@ -7597,7 +7693,7 @@
         <v>1031.25</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>252</v>
       </c>
@@ -7647,7 +7743,7 @@
         <v>843.75</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>248</v>
       </c>
@@ -7697,7 +7793,7 @@
         <v>131.25</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>249</v>
       </c>
@@ -7747,7 +7843,7 @@
         <v>206.25</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>250</v>
       </c>
@@ -7797,7 +7893,7 @@
         <v>281.25</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>251</v>
       </c>
@@ -7847,7 +7943,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>252</v>
       </c>
@@ -7897,7 +7993,7 @@
         <v>112.5</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>253</v>
       </c>
@@ -7947,7 +8043,7 @@
         <v>937.5</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>248</v>
       </c>
@@ -7997,7 +8093,7 @@
         <v>956.25</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>249</v>
       </c>
@@ -8047,7 +8143,7 @@
         <v>1012.5</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>250</v>
       </c>
@@ -8097,7 +8193,7 @@
         <v>1106.25</v>
       </c>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>251</v>
       </c>
@@ -8147,7 +8243,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>252</v>
       </c>
@@ -8197,7 +8293,7 @@
         <v>937.5</v>
       </c>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>248</v>
       </c>
@@ -8247,7 +8343,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>249</v>
       </c>
@@ -8297,7 +8393,7 @@
         <v>206.25</v>
       </c>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>250</v>
       </c>
@@ -8347,7 +8443,7 @@
         <v>281.25</v>
       </c>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>251</v>
       </c>
@@ -8397,7 +8493,7 @@
         <v>318.75</v>
       </c>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>252</v>
       </c>
@@ -8447,7 +8543,7 @@
         <v>131.25</v>
       </c>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>254</v>
       </c>
@@ -8497,7 +8593,7 @@
         <v>1668.75</v>
       </c>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>248</v>
       </c>
@@ -8547,7 +8643,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
         <v>249</v>
       </c>
@@ -8597,7 +8693,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>250</v>
       </c>
@@ -8647,7 +8743,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>251</v>
       </c>
@@ -8697,7 +8793,7 @@
         <v>318.75</v>
       </c>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>252</v>
       </c>
@@ -8747,7 +8843,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>255</v>
       </c>
@@ -8797,7 +8893,7 @@
         <v>1031.25</v>
       </c>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>248</v>
       </c>
@@ -8847,7 +8943,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>249</v>
       </c>
@@ -8897,7 +8993,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
         <v>250</v>
       </c>
@@ -8947,7 +9043,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
         <v>251</v>
       </c>
@@ -8997,7 +9093,7 @@
         <v>1143.75</v>
       </c>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>252</v>
       </c>
@@ -9047,7 +9143,7 @@
         <v>956.25</v>
       </c>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>248</v>
       </c>
@@ -9097,7 +9193,7 @@
         <v>187.5</v>
       </c>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
         <v>249</v>
       </c>
@@ -9147,7 +9243,7 @@
         <v>262.5</v>
       </c>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
         <v>250</v>
       </c>
@@ -9197,7 +9293,7 @@
         <v>337.5</v>
       </c>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
         <v>251</v>
       </c>
@@ -9247,7 +9343,7 @@
         <v>356.25</v>
       </c>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
         <v>252</v>
       </c>
@@ -9297,7 +9393,7 @@
         <v>168.75</v>
       </c>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>256</v>
       </c>
@@ -9347,7 +9443,7 @@
         <v>1106.25</v>
       </c>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
         <v>248</v>
       </c>
@@ -9397,7 +9493,7 @@
         <v>206.25</v>
       </c>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
         <v>249</v>
       </c>
@@ -9447,7 +9543,7 @@
         <v>281.25</v>
       </c>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
         <v>252</v>
       </c>
@@ -9497,7 +9593,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>257</v>
       </c>
@@ -9547,7 +9643,7 @@
         <v>1518.75</v>
       </c>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
         <v>249</v>
       </c>
@@ -9597,7 +9693,7 @@
         <v>112.5</v>
       </c>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>284</v>
       </c>
@@ -9647,7 +9743,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
         <v>285</v>
       </c>
@@ -9697,7 +9793,7 @@
         <v>1293.75</v>
       </c>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
         <v>286</v>
       </c>
@@ -9747,7 +9843,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
         <v>287</v>
       </c>
@@ -9797,7 +9893,7 @@
         <v>1443.75</v>
       </c>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>288</v>
       </c>
@@ -9847,7 +9943,7 @@
         <v>1462.5</v>
       </c>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
         <v>289</v>
       </c>
@@ -9897,7 +9993,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>151</v>
       </c>
@@ -9950,7 +10046,7 @@
         <v>243.75</v>
       </c>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
         <v>286</v>
       </c>
@@ -10000,7 +10096,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
         <v>287</v>
       </c>
@@ -10050,7 +10146,7 @@
         <v>393.75</v>
       </c>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
         <v>288</v>
       </c>
@@ -10100,7 +10196,7 @@
         <v>412.5</v>
       </c>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
         <v>289</v>
       </c>
@@ -10150,7 +10246,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>290</v>
       </c>
@@ -10200,7 +10296,7 @@
         <v>1181.25</v>
       </c>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
         <v>285</v>
       </c>
@@ -10250,7 +10346,7 @@
         <v>1181.25</v>
       </c>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
         <v>286</v>
       </c>
@@ -10300,7 +10396,7 @@
         <v>1256.25</v>
       </c>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
         <v>287</v>
       </c>
@@ -10350,7 +10446,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
         <v>288</v>
       </c>
@@ -10400,7 +10496,7 @@
         <v>1368.75</v>
       </c>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
         <v>289</v>
       </c>
@@ -10450,7 +10546,7 @@
         <v>1162.5</v>
       </c>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>151</v>
       </c>
@@ -10503,7 +10599,7 @@
         <v>168.75</v>
       </c>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
         <v>286</v>
       </c>
@@ -10553,7 +10649,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
         <v>287</v>
       </c>
@@ -10603,7 +10699,7 @@
         <v>318.75</v>
       </c>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
         <v>288</v>
       </c>
@@ -10653,7 +10749,7 @@
         <v>337.5</v>
       </c>
     </row>
-    <row r="100" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
         <v>289</v>
       </c>
@@ -10703,7 +10799,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="101" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>291</v>
       </c>
@@ -10753,7 +10849,7 @@
         <v>937.5</v>
       </c>
     </row>
-    <row r="102" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
         <v>285</v>
       </c>
@@ -10803,7 +10899,7 @@
         <v>862.5</v>
       </c>
     </row>
-    <row r="103" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
         <v>286</v>
       </c>
@@ -10853,7 +10949,7 @@
         <v>956.25</v>
       </c>
     </row>
-    <row r="104" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
         <v>287</v>
       </c>
@@ -10903,7 +10999,7 @@
         <v>1031.25</v>
       </c>
     </row>
-    <row r="105" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B105" t="s">
         <v>288</v>
       </c>
@@ -10953,7 +11049,7 @@
         <v>1031.25</v>
       </c>
     </row>
-    <row r="106" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
         <v>289</v>
       </c>
@@ -11003,7 +11099,7 @@
         <v>862.5</v>
       </c>
     </row>
-    <row r="107" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>151</v>
       </c>
@@ -11056,7 +11152,7 @@
         <v>168.75</v>
       </c>
     </row>
-    <row r="108" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B108" t="s">
         <v>286</v>
       </c>
@@ -11106,7 +11202,7 @@
         <v>243.75</v>
       </c>
     </row>
-    <row r="109" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
         <v>287</v>
       </c>
@@ -11156,7 +11252,7 @@
         <v>318.75</v>
       </c>
     </row>
-    <row r="110" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B110" t="s">
         <v>288</v>
       </c>
@@ -11206,7 +11302,7 @@
         <v>318.75</v>
       </c>
     </row>
-    <row r="111" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B111" t="s">
         <v>289</v>
       </c>
@@ -11264,15 +11360,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8540264-B3C1-4C71-9FC9-001ABF042657}">
-  <dimension ref="A1:AD14"/>
+  <dimension ref="A1:AD16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X14" sqref="X14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11364,7 +11460,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>144</v>
       </c>
@@ -11402,7 +11498,7 @@
         <v>22.5</v>
       </c>
       <c r="U2">
-        <f t="shared" ref="U2:U14" si="0">MEDIAN(0,255,ROUND(S2/20+SQRT(J2)/40+SQRT(P2)/2+(SQRT(R2)-SQRT(185)),0))</f>
+        <f t="shared" ref="U2:U16" si="0">MEDIAN(0,255,ROUND(S2/20+SQRT(J2)/40+SQRT(P2)/2+(SQRT(R2)-SQRT(185)),0))</f>
         <v>5</v>
       </c>
       <c r="W2">
@@ -11410,7 +11506,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>148</v>
       </c>
@@ -11453,7 +11549,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>181</v>
       </c>
@@ -11496,7 +11592,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>192</v>
       </c>
@@ -11536,7 +11632,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>196</v>
       </c>
@@ -11579,7 +11675,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>205</v>
       </c>
@@ -11619,7 +11715,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>237</v>
       </c>
@@ -11662,7 +11758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>239</v>
       </c>
@@ -11702,7 +11798,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>240</v>
       </c>
@@ -11742,7 +11838,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>241</v>
       </c>
@@ -11782,7 +11878,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>294</v>
       </c>
@@ -11822,7 +11918,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>366</v>
       </c>
@@ -11862,7 +11958,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>368</v>
       </c>
@@ -11903,6 +11999,92 @@
       <c r="W14">
         <f>MEDIAN(0,255,ROUND(SQRT(J14)/200+SQRT(P14)/2+(SQRT(R14)-SQRT(185)),0))</f>
         <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>392</v>
+      </c>
+      <c r="B15" t="s">
+        <v>393</v>
+      </c>
+      <c r="F15">
+        <v>1986</v>
+      </c>
+      <c r="G15">
+        <v>30</v>
+      </c>
+      <c r="H15" t="s">
+        <v>91</v>
+      </c>
+      <c r="J15">
+        <v>120</v>
+      </c>
+      <c r="P15">
+        <v>184</v>
+      </c>
+      <c r="Q15">
+        <v>48</v>
+      </c>
+      <c r="R15">
+        <v>1600</v>
+      </c>
+      <c r="S15">
+        <v>184</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="W15">
+        <f>MEDIAN(0,255,ROUND(SQRT(J15)/200+SQRT(P15)/2+(SQRT(R15)-SQRT(185)),0))</f>
+        <v>33</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>397</v>
+      </c>
+      <c r="B16" t="s">
+        <v>398</v>
+      </c>
+      <c r="F16">
+        <v>2010</v>
+      </c>
+      <c r="G16">
+        <v>30</v>
+      </c>
+      <c r="H16" t="s">
+        <v>91</v>
+      </c>
+      <c r="J16">
+        <v>120</v>
+      </c>
+      <c r="P16">
+        <v>70</v>
+      </c>
+      <c r="Q16">
+        <v>24</v>
+      </c>
+      <c r="R16">
+        <v>185</v>
+      </c>
+      <c r="S16">
+        <v>23</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="W16">
+        <f>MEDIAN(0,255,ROUND(SQRT(J16)/200+SQRT(P16)/2+(SQRT(R16)-SQRT(185)),0))</f>
+        <v>4</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>396</v>
       </c>
     </row>
   </sheetData>
@@ -11915,14 +12097,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392CFCAE-41E9-4295-93E2-AE0B308CC62A}">
   <dimension ref="A1:Z69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="Z60" sqref="Z60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -12002,7 +12184,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -12056,7 +12238,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -12110,7 +12292,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>82</v>
       </c>
@@ -12164,7 +12346,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>83</v>
       </c>
@@ -12218,7 +12400,7 @@
         <v>2475</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>96</v>
       </c>
@@ -12272,7 +12454,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>97</v>
       </c>
@@ -12326,7 +12508,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>98</v>
       </c>
@@ -12380,7 +12562,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>99</v>
       </c>
@@ -12434,7 +12616,7 @@
         <v>2475</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>159</v>
       </c>
@@ -12488,7 +12670,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>110</v>
       </c>
@@ -12542,7 +12724,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>114</v>
       </c>
@@ -12596,7 +12778,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>166</v>
       </c>
@@ -12647,7 +12829,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>117</v>
       </c>
@@ -12701,7 +12883,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>118</v>
       </c>
@@ -12755,7 +12937,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>119</v>
       </c>
@@ -12809,7 +12991,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>120</v>
       </c>
@@ -12863,7 +13045,7 @@
         <v>2475</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>214</v>
       </c>
@@ -12914,7 +13096,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>213</v>
       </c>
@@ -12965,7 +13147,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>223</v>
       </c>
@@ -13016,7 +13198,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>224</v>
       </c>
@@ -13067,7 +13249,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>225</v>
       </c>
@@ -13118,7 +13300,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>226</v>
       </c>
@@ -13169,7 +13351,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>231</v>
       </c>
@@ -13220,7 +13402,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>141</v>
       </c>
@@ -13274,7 +13456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>154</v>
       </c>
@@ -13328,7 +13510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>156</v>
       </c>
@@ -13382,7 +13564,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>168</v>
       </c>
@@ -13433,7 +13615,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>169</v>
       </c>
@@ -13484,7 +13666,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>170</v>
       </c>
@@ -13535,7 +13717,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>171</v>
       </c>
@@ -13586,7 +13768,7 @@
         <v>2475</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>207</v>
       </c>
@@ -13637,7 +13819,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>208</v>
       </c>
@@ -13688,7 +13870,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>215</v>
       </c>
@@ -13739,7 +13921,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>216</v>
       </c>
@@ -13790,7 +13972,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>219</v>
       </c>
@@ -13841,7 +14023,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>221</v>
       </c>
@@ -13892,7 +14074,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>172</v>
       </c>
@@ -13943,7 +14125,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>178</v>
       </c>
@@ -13994,7 +14176,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>183</v>
       </c>
@@ -14045,7 +14227,7 @@
         <v>2475</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>185</v>
       </c>
@@ -14096,7 +14278,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>186</v>
       </c>
@@ -14147,7 +14329,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>187</v>
       </c>
@@ -14198,7 +14380,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>188</v>
       </c>
@@ -14249,7 +14431,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>279</v>
       </c>
@@ -14300,7 +14482,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>281</v>
       </c>
@@ -14351,7 +14533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>292</v>
       </c>
@@ -14402,7 +14584,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>296</v>
       </c>
@@ -14462,7 +14644,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>299</v>
       </c>
@@ -14520,7 +14702,7 @@
       </c>
       <c r="Z49" s="8"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>301</v>
       </c>
@@ -14578,7 +14760,7 @@
       </c>
       <c r="Z50" s="8"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>303</v>
       </c>
@@ -14636,7 +14818,7 @@
       </c>
       <c r="Z51" s="8"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>305</v>
       </c>
@@ -14694,7 +14876,7 @@
       </c>
       <c r="Z52" s="8"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>307</v>
       </c>
@@ -14752,7 +14934,7 @@
       </c>
       <c r="Z53" s="8"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>310</v>
       </c>
@@ -14810,7 +14992,7 @@
       </c>
       <c r="Z54" s="8"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>312</v>
       </c>
@@ -14868,7 +15050,7 @@
       </c>
       <c r="Z55" s="8"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>314</v>
       </c>
@@ -14926,7 +15108,7 @@
       </c>
       <c r="Z56" s="8"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>316</v>
       </c>
@@ -14984,7 +15166,7 @@
       </c>
       <c r="Z57" s="8"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>345</v>
       </c>
@@ -15041,7 +15223,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>346</v>
       </c>
@@ -15098,7 +15280,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>370</v>
       </c>
@@ -15155,7 +15337,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>371</v>
       </c>
@@ -15212,7 +15394,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>375</v>
       </c>
@@ -15269,7 +15451,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>379</v>
       </c>
@@ -15326,7 +15508,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>380</v>
       </c>
@@ -15383,7 +15565,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>382</v>
       </c>
@@ -15440,7 +15622,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>384</v>
       </c>
@@ -15497,7 +15679,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>388</v>
       </c>
@@ -15554,7 +15736,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>391</v>
       </c>
@@ -15611,7 +15793,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>386</v>
       </c>

</xml_diff>

<commit_message>
240301 push by wuwu
</commit_message>
<xml_diff>
--- a/docs/China Set Trains.xlsx
+++ b/docs/China Set Trains.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projcet china set\China-Set-Trains-site\China-Set-Trains-230215\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projcet china set\China-Set-Trains-site\China-Set-Trains-240301\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12442D9-BF5A-46C8-924E-3BE0CC015F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9337625A-F4C0-49E1-B98D-25A9B26A8FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Loco" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="401">
   <si>
     <t>name</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1555,6 +1555,14 @@
   </si>
   <si>
     <t>l70</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NX70A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>nx70a</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -11360,10 +11368,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8540264-B3C1-4C71-9FC9-001ABF042657}">
-  <dimension ref="A1:AD16"/>
+  <dimension ref="A1:AD17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -11498,7 +11506,7 @@
         <v>22.5</v>
       </c>
       <c r="U2">
-        <f t="shared" ref="U2:U16" si="0">MEDIAN(0,255,ROUND(S2/20+SQRT(J2)/40+SQRT(P2)/2+(SQRT(R2)-SQRT(185)),0))</f>
+        <f t="shared" ref="U2:U17" si="0">MEDIAN(0,255,ROUND(S2/20+SQRT(J2)/40+SQRT(P2)/2+(SQRT(R2)-SQRT(185)),0))</f>
         <v>5</v>
       </c>
       <c r="W2">
@@ -12085,6 +12093,46 @@
       </c>
       <c r="AD16" t="s">
         <v>396</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>399</v>
+      </c>
+      <c r="B17" t="s">
+        <v>400</v>
+      </c>
+      <c r="F17">
+        <v>2010</v>
+      </c>
+      <c r="G17">
+        <v>30</v>
+      </c>
+      <c r="H17" t="s">
+        <v>91</v>
+      </c>
+      <c r="J17">
+        <v>120</v>
+      </c>
+      <c r="P17">
+        <v>70</v>
+      </c>
+      <c r="Q17">
+        <v>20</v>
+      </c>
+      <c r="R17">
+        <v>185</v>
+      </c>
+      <c r="S17">
+        <v>23.8</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="W17">
+        <f>MEDIAN(0,255,ROUND(SQRT(J17)/200+SQRT(P17)/2+(SQRT(R17)-SQRT(185)),0))</f>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add crh380a and some fix
</commit_message>
<xml_diff>
--- a/docs/China Set Trains.xlsx
+++ b/docs/China Set Trains.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CNS\CNST\local\China-Set-Trains\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90DCD15-8A9B-449F-A7B2-9F7B0C5A44EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BDFBBC6-D0B3-4C06-A18F-82FB28C56F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-860" yWindow="2220" windowWidth="20910" windowHeight="13290" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="460" yWindow="2070" windowWidth="20910" windowHeight="13290" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Loco" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="422">
   <si>
     <t>name</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -5744,11 +5744,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB4625FC-685F-4E56-AE60-F05D51350408}">
-  <dimension ref="A1:AF167"/>
+  <dimension ref="A1:AF178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W160" sqref="W160"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W169" sqref="W169:W173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -13813,7 +13813,7 @@
         <v>350</v>
       </c>
       <c r="K157">
-        <f t="shared" ref="K157:K167" si="25">ROUND(L157/0.73549875,0)</f>
+        <f t="shared" ref="K157:K178" si="25">ROUND(L157/0.73549875,0)</f>
         <v>3314</v>
       </c>
       <c r="L157">
@@ -13835,23 +13835,23 @@
         <v>0.127</v>
       </c>
       <c r="V157">
-        <f t="shared" ref="V157:V167" si="26">T157*U157*9.8</f>
+        <f t="shared" ref="V157:V178" si="26">T157*U157*9.8</f>
         <v>67.208400000000012</v>
       </c>
       <c r="W157">
-        <f t="shared" ref="W157:W167" si="27">MAX(1, INT(T157/10+SQRT(J157)/20+SQRT(K157)+U157+SQRT(Q157)/2+SQRT(S157)-SQRT(185)+20-I157))</f>
+        <f t="shared" ref="W157:W178" si="27">MAX(1, INT(T157/10+SQRT(J157)/20+SQRT(K157)+U157+SQRT(Q157)/2+SQRT(S157)-SQRT(185)+20-I157))</f>
         <v>88</v>
       </c>
       <c r="X157">
-        <f t="shared" ref="X157:X167" si="28">W157*50000/16</f>
+        <f t="shared" ref="X157:X178" si="28">W157*50000/16</f>
         <v>275000</v>
       </c>
       <c r="Y157">
-        <f t="shared" ref="Y157:Y167" si="29">MAX(1, ROUND((SQRT(J157)/100+SQRT(K157)+U157+(40/I157-2)+SQRT(Q157)/2+SQRT(S157)-SQRT(185)), 0))</f>
+        <f t="shared" ref="Y157:Y178" si="29">MAX(1, ROUND((SQRT(J157)/100+SQRT(K157)+U157+(40/I157-2)+SQRT(Q157)/2+SQRT(S157)-SQRT(185)), 0))</f>
         <v>73</v>
       </c>
       <c r="Z157">
-        <f t="shared" ref="Z157:Z167" si="30">Y157*300/16</f>
+        <f t="shared" ref="Z157:Z178" si="30">Y157*300/16</f>
         <v>1368.75</v>
       </c>
     </row>
@@ -14386,6 +14386,559 @@
       <c r="Z167">
         <f t="shared" si="30"/>
         <v>225</v>
+      </c>
+    </row>
+    <row r="168" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A168" t="s">
+        <v>284</v>
+      </c>
+      <c r="I168">
+        <v>12</v>
+      </c>
+      <c r="J168">
+        <v>310</v>
+      </c>
+      <c r="K168">
+        <f t="shared" si="25"/>
+        <v>2067</v>
+      </c>
+      <c r="L168">
+        <v>1520</v>
+      </c>
+      <c r="Q168">
+        <v>36</v>
+      </c>
+      <c r="S168">
+        <v>400</v>
+      </c>
+      <c r="T168">
+        <v>51</v>
+      </c>
+      <c r="U168">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="V168">
+        <f t="shared" si="26"/>
+        <v>41.48340000000001</v>
+      </c>
+      <c r="W168">
+        <f t="shared" si="27"/>
+        <v>68</v>
+      </c>
+      <c r="X168">
+        <f t="shared" si="28"/>
+        <v>212500</v>
+      </c>
+      <c r="Y168">
+        <f t="shared" si="29"/>
+        <v>56</v>
+      </c>
+      <c r="Z168">
+        <f t="shared" si="30"/>
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="169" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="B169" t="s">
+        <v>130</v>
+      </c>
+      <c r="I169">
+        <v>12</v>
+      </c>
+      <c r="J169">
+        <v>310</v>
+      </c>
+      <c r="K169">
+        <f t="shared" si="25"/>
+        <v>2067</v>
+      </c>
+      <c r="L169">
+        <v>1520</v>
+      </c>
+      <c r="Q169">
+        <v>85</v>
+      </c>
+      <c r="S169">
+        <v>240</v>
+      </c>
+      <c r="T169">
+        <v>51</v>
+      </c>
+      <c r="U169">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="V169">
+        <f t="shared" si="26"/>
+        <v>41.48340000000001</v>
+      </c>
+      <c r="W169">
+        <f t="shared" si="27"/>
+        <v>66</v>
+      </c>
+      <c r="X169">
+        <f t="shared" si="28"/>
+        <v>206250</v>
+      </c>
+      <c r="Y169">
+        <f t="shared" si="29"/>
+        <v>54</v>
+      </c>
+      <c r="Z169">
+        <f t="shared" si="30"/>
+        <v>1012.5</v>
+      </c>
+    </row>
+    <row r="170" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="B170" t="s">
+        <v>131</v>
+      </c>
+      <c r="I170">
+        <v>12</v>
+      </c>
+      <c r="J170">
+        <v>310</v>
+      </c>
+      <c r="K170">
+        <f t="shared" si="25"/>
+        <v>2067</v>
+      </c>
+      <c r="L170">
+        <v>1520</v>
+      </c>
+      <c r="Q170">
+        <v>56</v>
+      </c>
+      <c r="S170">
+        <v>400</v>
+      </c>
+      <c r="T170">
+        <v>51</v>
+      </c>
+      <c r="U170">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="V170">
+        <f t="shared" si="26"/>
+        <v>41.48340000000001</v>
+      </c>
+      <c r="W170">
+        <f t="shared" si="27"/>
+        <v>69</v>
+      </c>
+      <c r="X170">
+        <f t="shared" si="28"/>
+        <v>215625</v>
+      </c>
+      <c r="Y170">
+        <f t="shared" si="29"/>
+        <v>57</v>
+      </c>
+      <c r="Z170">
+        <f t="shared" si="30"/>
+        <v>1068.75</v>
+      </c>
+    </row>
+    <row r="171" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="B171" t="s">
+        <v>132</v>
+      </c>
+      <c r="I171">
+        <v>12</v>
+      </c>
+      <c r="J171">
+        <v>310</v>
+      </c>
+      <c r="K171">
+        <f t="shared" si="25"/>
+        <v>2067</v>
+      </c>
+      <c r="L171">
+        <v>1520</v>
+      </c>
+      <c r="Q171">
+        <v>24</v>
+      </c>
+      <c r="S171">
+        <v>640</v>
+      </c>
+      <c r="T171">
+        <v>51</v>
+      </c>
+      <c r="U171">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="V171">
+        <f t="shared" si="26"/>
+        <v>41.48340000000001</v>
+      </c>
+      <c r="W171">
+        <f t="shared" si="27"/>
+        <v>73</v>
+      </c>
+      <c r="X171">
+        <f t="shared" si="28"/>
+        <v>228125</v>
+      </c>
+      <c r="Y171">
+        <f t="shared" si="29"/>
+        <v>61</v>
+      </c>
+      <c r="Z171">
+        <f t="shared" si="30"/>
+        <v>1143.75</v>
+      </c>
+    </row>
+    <row r="172" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="B172" t="s">
+        <v>134</v>
+      </c>
+      <c r="I172">
+        <v>12</v>
+      </c>
+      <c r="J172">
+        <v>310</v>
+      </c>
+      <c r="K172">
+        <f t="shared" si="25"/>
+        <v>2067</v>
+      </c>
+      <c r="L172">
+        <v>1520</v>
+      </c>
+      <c r="Q172">
+        <v>15</v>
+      </c>
+      <c r="S172">
+        <v>720</v>
+      </c>
+      <c r="T172">
+        <v>51</v>
+      </c>
+      <c r="U172">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="V172">
+        <f t="shared" si="26"/>
+        <v>41.48340000000001</v>
+      </c>
+      <c r="W172">
+        <f t="shared" si="27"/>
+        <v>74</v>
+      </c>
+      <c r="X172">
+        <f t="shared" si="28"/>
+        <v>231250</v>
+      </c>
+      <c r="Y172">
+        <f t="shared" si="29"/>
+        <v>62</v>
+      </c>
+      <c r="Z172">
+        <f t="shared" si="30"/>
+        <v>1162.5</v>
+      </c>
+    </row>
+    <row r="173" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="B173" t="s">
+        <v>138</v>
+      </c>
+      <c r="I173">
+        <v>12</v>
+      </c>
+      <c r="J173">
+        <v>310</v>
+      </c>
+      <c r="K173">
+        <f t="shared" si="25"/>
+        <v>2067</v>
+      </c>
+      <c r="L173">
+        <v>1520</v>
+      </c>
+      <c r="Q173">
+        <v>63</v>
+      </c>
+      <c r="S173">
+        <v>240</v>
+      </c>
+      <c r="T173">
+        <v>51</v>
+      </c>
+      <c r="U173">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="V173">
+        <f t="shared" si="26"/>
+        <v>41.48340000000001</v>
+      </c>
+      <c r="W173">
+        <f t="shared" si="27"/>
+        <v>65</v>
+      </c>
+      <c r="X173">
+        <f t="shared" si="28"/>
+        <v>203125</v>
+      </c>
+      <c r="Y173">
+        <f t="shared" si="29"/>
+        <v>53</v>
+      </c>
+      <c r="Z173">
+        <f t="shared" si="30"/>
+        <v>993.75</v>
+      </c>
+    </row>
+    <row r="174" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A174" t="s">
+        <v>151</v>
+      </c>
+      <c r="B174" t="s">
+        <v>130</v>
+      </c>
+      <c r="I174">
+        <v>12</v>
+      </c>
+      <c r="J174">
+        <v>310</v>
+      </c>
+      <c r="K174">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="L174">
+        <v>0</v>
+      </c>
+      <c r="Q174">
+        <v>85</v>
+      </c>
+      <c r="S174">
+        <v>240</v>
+      </c>
+      <c r="T174">
+        <v>51</v>
+      </c>
+      <c r="U174">
+        <v>0</v>
+      </c>
+      <c r="V174">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="W174">
+        <f t="shared" si="27"/>
+        <v>20</v>
+      </c>
+      <c r="X174">
+        <f t="shared" si="28"/>
+        <v>62500</v>
+      </c>
+      <c r="Y174">
+        <f t="shared" si="29"/>
+        <v>8</v>
+      </c>
+      <c r="Z174">
+        <f t="shared" si="30"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="175" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="B175" t="s">
+        <v>131</v>
+      </c>
+      <c r="I175">
+        <v>12</v>
+      </c>
+      <c r="J175">
+        <v>310</v>
+      </c>
+      <c r="K175">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="L175">
+        <v>0</v>
+      </c>
+      <c r="Q175">
+        <v>56</v>
+      </c>
+      <c r="S175">
+        <v>400</v>
+      </c>
+      <c r="T175">
+        <v>51</v>
+      </c>
+      <c r="U175">
+        <v>0</v>
+      </c>
+      <c r="V175">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="W175">
+        <f t="shared" si="27"/>
+        <v>24</v>
+      </c>
+      <c r="X175">
+        <f t="shared" si="28"/>
+        <v>75000</v>
+      </c>
+      <c r="Y175">
+        <f t="shared" si="29"/>
+        <v>12</v>
+      </c>
+      <c r="Z175">
+        <f t="shared" si="30"/>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="176" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="B176" t="s">
+        <v>132</v>
+      </c>
+      <c r="I176">
+        <v>12</v>
+      </c>
+      <c r="J176">
+        <v>310</v>
+      </c>
+      <c r="K176">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="L176">
+        <v>0</v>
+      </c>
+      <c r="Q176">
+        <v>24</v>
+      </c>
+      <c r="S176">
+        <v>640</v>
+      </c>
+      <c r="T176">
+        <v>51</v>
+      </c>
+      <c r="U176">
+        <v>0</v>
+      </c>
+      <c r="V176">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="W176">
+        <f t="shared" si="27"/>
+        <v>28</v>
+      </c>
+      <c r="X176">
+        <f t="shared" si="28"/>
+        <v>87500</v>
+      </c>
+      <c r="Y176">
+        <f t="shared" si="29"/>
+        <v>16</v>
+      </c>
+      <c r="Z176">
+        <f t="shared" si="30"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="177" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B177" t="s">
+        <v>134</v>
+      </c>
+      <c r="I177">
+        <v>12</v>
+      </c>
+      <c r="J177">
+        <v>310</v>
+      </c>
+      <c r="K177">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="L177">
+        <v>0</v>
+      </c>
+      <c r="Q177">
+        <v>15</v>
+      </c>
+      <c r="S177">
+        <v>720</v>
+      </c>
+      <c r="T177">
+        <v>51</v>
+      </c>
+      <c r="U177">
+        <v>0</v>
+      </c>
+      <c r="V177">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="W177">
+        <f t="shared" si="27"/>
+        <v>29</v>
+      </c>
+      <c r="X177">
+        <f t="shared" si="28"/>
+        <v>90625</v>
+      </c>
+      <c r="Y177">
+        <f t="shared" si="29"/>
+        <v>17</v>
+      </c>
+      <c r="Z177">
+        <f t="shared" si="30"/>
+        <v>318.75</v>
+      </c>
+    </row>
+    <row r="178" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="B178" t="s">
+        <v>138</v>
+      </c>
+      <c r="I178">
+        <v>12</v>
+      </c>
+      <c r="J178">
+        <v>310</v>
+      </c>
+      <c r="K178">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="L178">
+        <v>0</v>
+      </c>
+      <c r="Q178">
+        <v>63</v>
+      </c>
+      <c r="S178">
+        <v>240</v>
+      </c>
+      <c r="T178">
+        <v>51</v>
+      </c>
+      <c r="U178">
+        <v>0</v>
+      </c>
+      <c r="V178">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="W178">
+        <f t="shared" si="27"/>
+        <v>19</v>
+      </c>
+      <c r="X178">
+        <f t="shared" si="28"/>
+        <v>59375</v>
+      </c>
+      <c r="Y178">
+        <f t="shared" si="29"/>
+        <v>7</v>
+      </c>
+      <c r="Z178">
+        <f t="shared" si="30"/>
+        <v>131.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
turn crh380a to reconect
</commit_message>
<xml_diff>
--- a/docs/China Set Trains.xlsx
+++ b/docs/China Set Trains.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CNS\CNST\local\China-Set-Trains\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD17B37-7080-4521-B3EB-DA2C1E8242CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F06711-4C5B-4F5C-BF89-07AC9F6FC5AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4470" yWindow="260" windowWidth="20910" windowHeight="13290" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5754,9 +5754,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB4625FC-685F-4E56-AE60-F05D51350408}">
   <dimension ref="A1:AF187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A170" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W179" sqref="W179"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K168" sqref="K168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
r155 push by wuwu
</commit_message>
<xml_diff>
--- a/docs/China Set Trains.xlsx
+++ b/docs/China Set Trains.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\John Franklin\Documents\GitHub\China-Set-Trains\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projcet china set\China-Set-Trains-site\China-Set-Trains-240320\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86DD7796-9307-4087-AA9F-B41D7FF85565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E35E46BE-CA63-4772-8C46-068A59698F1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9518" yWindow="0" windowWidth="9765" windowHeight="11363" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Loco" sheetId="1" r:id="rId1"/>
@@ -18,26 +18,17 @@
     <sheet name="Wagons" sheetId="4" r:id="rId3"/>
     <sheet name="Coaches" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="437">
   <si>
     <t>name</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1708,6 +1699,14 @@
   </si>
   <si>
     <t>NZJ1-Jinlun</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>YZ31</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>yz31</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2077,14 +2076,14 @@
       <selection pane="bottomLeft" activeCell="AE54" sqref="AE54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.46484375" bestFit="1" customWidth="1"/>
-    <col min="26" max="28" width="8.59765625" style="1"/>
-    <col min="29" max="30" width="8.59765625" style="2"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="28" width="8.625" style="1"/>
+    <col min="29" max="30" width="8.625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2179,7 +2178,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -2270,7 +2269,7 @@
         <v>0.44444444444444442</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -2319,7 +2318,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -2368,7 +2367,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -2417,7 +2416,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -2466,7 +2465,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -2512,7 +2511,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>106</v>
       </c>
@@ -2594,7 +2593,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>107</v>
       </c>
@@ -2691,7 +2690,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>200</v>
       </c>
@@ -2760,7 +2759,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>201</v>
       </c>
@@ -2826,7 +2825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>202</v>
       </c>
@@ -2895,7 +2894,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>234</v>
       </c>
@@ -2944,7 +2943,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -3013,7 +3012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -3062,7 +3061,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -3135,7 +3134,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -3181,7 +3180,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>235</v>
       </c>
@@ -3247,7 +3246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -3296,7 +3295,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>152</v>
       </c>
@@ -3390,7 +3389,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>319</v>
       </c>
@@ -3475,7 +3474,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>324</v>
       </c>
@@ -3569,7 +3568,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>327</v>
       </c>
@@ -3652,7 +3651,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>331</v>
       </c>
@@ -3723,7 +3722,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>333</v>
       </c>
@@ -3794,7 +3793,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>335</v>
       </c>
@@ -3868,7 +3867,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>338</v>
       </c>
@@ -3942,7 +3941,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>340</v>
       </c>
@@ -4026,7 +4025,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -4075,7 +4074,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -4148,7 +4147,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -4221,7 +4220,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -4294,7 +4293,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -4391,7 +4390,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -4467,7 +4466,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>139</v>
       </c>
@@ -4564,7 +4563,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>194</v>
       </c>
@@ -4628,7 +4627,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>197</v>
       </c>
@@ -4695,7 +4694,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>258</v>
       </c>
@@ -4780,7 +4779,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>263</v>
       </c>
@@ -4868,7 +4867,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>265</v>
       </c>
@@ -4956,7 +4955,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>267</v>
       </c>
@@ -5044,7 +5043,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>269</v>
       </c>
@@ -5132,7 +5131,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>272</v>
       </c>
@@ -5220,7 +5219,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>274</v>
       </c>
@@ -5311,7 +5310,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>277</v>
       </c>
@@ -5399,7 +5398,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>351</v>
       </c>
@@ -5479,7 +5478,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>353</v>
       </c>
@@ -5559,7 +5558,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>355</v>
       </c>
@@ -5637,7 +5636,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>359</v>
       </c>
@@ -5718,7 +5717,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>394</v>
       </c>
@@ -5797,7 +5796,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>424</v>
       </c>
@@ -5873,7 +5872,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>425</v>
       </c>
@@ -5949,7 +5948,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="53" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:31" x14ac:dyDescent="0.2">
       <c r="R53" s="5"/>
     </row>
   </sheetData>
@@ -5962,17 +5961,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB4625FC-685F-4E56-AE60-F05D51350408}">
   <dimension ref="A1:AF190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A179" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AA189" sqref="AA189"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="32" max="32" width="20.33203125" customWidth="1"/>
+    <col min="32" max="32" width="20.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6070,7 +6069,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>133</v>
       </c>
@@ -6138,7 +6137,7 @@
         <v>1650</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="I3">
         <v>20</v>
       </c>
@@ -6188,7 +6187,7 @@
         <v>2325</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>130</v>
       </c>
@@ -6241,7 +6240,7 @@
         <v>131.25</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>131</v>
       </c>
@@ -6294,7 +6293,7 @@
         <v>206.25</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>132</v>
       </c>
@@ -6347,7 +6346,7 @@
         <v>281.25</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>134</v>
       </c>
@@ -6400,7 +6399,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>138</v>
       </c>
@@ -6453,7 +6452,7 @@
         <v>93.75</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>135</v>
       </c>
@@ -6506,7 +6505,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>136</v>
       </c>
@@ -6559,7 +6558,7 @@
         <v>281.25</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>137</v>
       </c>
@@ -6612,7 +6611,7 @@
         <v>318.75</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>150</v>
       </c>
@@ -6665,7 +6664,7 @@
         <v>937.5</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>130</v>
       </c>
@@ -6718,7 +6717,7 @@
         <v>862.5</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>131</v>
       </c>
@@ -6771,7 +6770,7 @@
         <v>937.5</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>132</v>
       </c>
@@ -6824,7 +6823,7 @@
         <v>1012.5</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>134</v>
       </c>
@@ -6877,7 +6876,7 @@
         <v>1031.25</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>138</v>
       </c>
@@ -6930,7 +6929,7 @@
         <v>843.75</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>151</v>
       </c>
@@ -6986,7 +6985,7 @@
         <v>131.25</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>131</v>
       </c>
@@ -7039,7 +7038,7 @@
         <v>206.25</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>132</v>
       </c>
@@ -7092,7 +7091,7 @@
         <v>281.25</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>134</v>
       </c>
@@ -7145,7 +7144,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>138</v>
       </c>
@@ -7198,7 +7197,7 @@
         <v>112.5</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>158</v>
       </c>
@@ -7251,7 +7250,7 @@
         <v>1406.25</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>130</v>
       </c>
@@ -7304,7 +7303,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>131</v>
       </c>
@@ -7357,7 +7356,7 @@
         <v>1406.25</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>132</v>
       </c>
@@ -7410,7 +7409,7 @@
         <v>1481.25</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>134</v>
       </c>
@@ -7463,7 +7462,7 @@
         <v>1518.75</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>138</v>
       </c>
@@ -7516,7 +7515,7 @@
         <v>1312.5</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>151</v>
       </c>
@@ -7572,7 +7571,7 @@
         <v>243.75</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>131</v>
       </c>
@@ -7625,7 +7624,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>132</v>
       </c>
@@ -7678,7 +7677,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>134</v>
       </c>
@@ -7731,7 +7730,7 @@
         <v>412.5</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>138</v>
       </c>
@@ -7784,7 +7783,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>247</v>
       </c>
@@ -7834,7 +7833,7 @@
         <v>843.75</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>248</v>
       </c>
@@ -7884,7 +7883,7 @@
         <v>881.25</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>249</v>
       </c>
@@ -7934,7 +7933,7 @@
         <v>937.5</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>250</v>
       </c>
@@ -7984,7 +7983,7 @@
         <v>1012.5</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>251</v>
       </c>
@@ -8034,7 +8033,7 @@
         <v>1031.25</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>252</v>
       </c>
@@ -8084,7 +8083,7 @@
         <v>843.75</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>248</v>
       </c>
@@ -8134,7 +8133,7 @@
         <v>131.25</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>249</v>
       </c>
@@ -8184,7 +8183,7 @@
         <v>206.25</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>250</v>
       </c>
@@ -8234,7 +8233,7 @@
         <v>281.25</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>251</v>
       </c>
@@ -8284,7 +8283,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>252</v>
       </c>
@@ -8334,7 +8333,7 @@
         <v>112.5</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>253</v>
       </c>
@@ -8384,7 +8383,7 @@
         <v>937.5</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>248</v>
       </c>
@@ -8434,7 +8433,7 @@
         <v>956.25</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>249</v>
       </c>
@@ -8484,7 +8483,7 @@
         <v>1012.5</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>250</v>
       </c>
@@ -8534,7 +8533,7 @@
         <v>1106.25</v>
       </c>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>251</v>
       </c>
@@ -8584,7 +8583,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>252</v>
       </c>
@@ -8634,7 +8633,7 @@
         <v>937.5</v>
       </c>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>248</v>
       </c>
@@ -8684,7 +8683,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>249</v>
       </c>
@@ -8734,7 +8733,7 @@
         <v>206.25</v>
       </c>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>250</v>
       </c>
@@ -8784,7 +8783,7 @@
         <v>281.25</v>
       </c>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>251</v>
       </c>
@@ -8834,7 +8833,7 @@
         <v>318.75</v>
       </c>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>252</v>
       </c>
@@ -8884,7 +8883,7 @@
         <v>131.25</v>
       </c>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>254</v>
       </c>
@@ -8934,7 +8933,7 @@
         <v>1668.75</v>
       </c>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>248</v>
       </c>
@@ -8984,7 +8983,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
         <v>249</v>
       </c>
@@ -9034,7 +9033,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>250</v>
       </c>
@@ -9084,7 +9083,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>251</v>
       </c>
@@ -9134,7 +9133,7 @@
         <v>318.75</v>
       </c>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>252</v>
       </c>
@@ -9184,7 +9183,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>255</v>
       </c>
@@ -9234,7 +9233,7 @@
         <v>1031.25</v>
       </c>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>248</v>
       </c>
@@ -9284,7 +9283,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>249</v>
       </c>
@@ -9334,7 +9333,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
         <v>250</v>
       </c>
@@ -9384,7 +9383,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
         <v>251</v>
       </c>
@@ -9434,7 +9433,7 @@
         <v>1143.75</v>
       </c>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>252</v>
       </c>
@@ -9484,7 +9483,7 @@
         <v>956.25</v>
       </c>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>248</v>
       </c>
@@ -9534,7 +9533,7 @@
         <v>187.5</v>
       </c>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
         <v>249</v>
       </c>
@@ -9584,7 +9583,7 @@
         <v>262.5</v>
       </c>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
         <v>250</v>
       </c>
@@ -9634,7 +9633,7 @@
         <v>337.5</v>
       </c>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
         <v>251</v>
       </c>
@@ -9684,7 +9683,7 @@
         <v>356.25</v>
       </c>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
         <v>252</v>
       </c>
@@ -9734,7 +9733,7 @@
         <v>168.75</v>
       </c>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>256</v>
       </c>
@@ -9784,7 +9783,7 @@
         <v>1106.25</v>
       </c>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
         <v>248</v>
       </c>
@@ -9834,7 +9833,7 @@
         <v>206.25</v>
       </c>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
         <v>249</v>
       </c>
@@ -9884,7 +9883,7 @@
         <v>281.25</v>
       </c>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
         <v>252</v>
       </c>
@@ -9934,7 +9933,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>257</v>
       </c>
@@ -9984,7 +9983,7 @@
         <v>1518.75</v>
       </c>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
         <v>249</v>
       </c>
@@ -10034,7 +10033,7 @@
         <v>112.5</v>
       </c>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>284</v>
       </c>
@@ -10084,7 +10083,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
         <v>285</v>
       </c>
@@ -10134,7 +10133,7 @@
         <v>1293.75</v>
       </c>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
         <v>286</v>
       </c>
@@ -10184,7 +10183,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
         <v>287</v>
       </c>
@@ -10234,7 +10233,7 @@
         <v>1443.75</v>
       </c>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>288</v>
       </c>
@@ -10284,7 +10283,7 @@
         <v>1462.5</v>
       </c>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
         <v>289</v>
       </c>
@@ -10334,7 +10333,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>151</v>
       </c>
@@ -10387,7 +10386,7 @@
         <v>243.75</v>
       </c>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
         <v>286</v>
       </c>
@@ -10437,7 +10436,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
         <v>287</v>
       </c>
@@ -10487,7 +10486,7 @@
         <v>393.75</v>
       </c>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
         <v>288</v>
       </c>
@@ -10537,7 +10536,7 @@
         <v>412.5</v>
       </c>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
         <v>289</v>
       </c>
@@ -10587,7 +10586,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>290</v>
       </c>
@@ -10637,7 +10636,7 @@
         <v>1181.25</v>
       </c>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
         <v>285</v>
       </c>
@@ -10687,7 +10686,7 @@
         <v>1181.25</v>
       </c>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
         <v>286</v>
       </c>
@@ -10737,7 +10736,7 @@
         <v>1256.25</v>
       </c>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
         <v>287</v>
       </c>
@@ -10787,7 +10786,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
         <v>288</v>
       </c>
@@ -10837,7 +10836,7 @@
         <v>1368.75</v>
       </c>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
         <v>289</v>
       </c>
@@ -10887,7 +10886,7 @@
         <v>1162.5</v>
       </c>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>151</v>
       </c>
@@ -10940,7 +10939,7 @@
         <v>168.75</v>
       </c>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
         <v>286</v>
       </c>
@@ -10990,7 +10989,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
         <v>287</v>
       </c>
@@ -11040,7 +11039,7 @@
         <v>318.75</v>
       </c>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
         <v>288</v>
       </c>
@@ -11090,7 +11089,7 @@
         <v>337.5</v>
       </c>
     </row>
-    <row r="100" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
         <v>289</v>
       </c>
@@ -11140,7 +11139,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="101" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>291</v>
       </c>
@@ -11190,7 +11189,7 @@
         <v>937.5</v>
       </c>
     </row>
-    <row r="102" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
         <v>285</v>
       </c>
@@ -11240,7 +11239,7 @@
         <v>862.5</v>
       </c>
     </row>
-    <row r="103" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
         <v>286</v>
       </c>
@@ -11290,7 +11289,7 @@
         <v>956.25</v>
       </c>
     </row>
-    <row r="104" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
         <v>287</v>
       </c>
@@ -11340,7 +11339,7 @@
         <v>1031.25</v>
       </c>
     </row>
-    <row r="105" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B105" t="s">
         <v>288</v>
       </c>
@@ -11390,7 +11389,7 @@
         <v>1031.25</v>
       </c>
     </row>
-    <row r="106" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
         <v>289</v>
       </c>
@@ -11440,7 +11439,7 @@
         <v>862.5</v>
       </c>
     </row>
-    <row r="107" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>151</v>
       </c>
@@ -11493,7 +11492,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="108" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B108" t="s">
         <v>286</v>
       </c>
@@ -11543,7 +11542,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="109" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
         <v>287</v>
       </c>
@@ -11593,7 +11592,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="110" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B110" t="s">
         <v>288</v>
       </c>
@@ -11643,7 +11642,7 @@
         <v>318.75</v>
       </c>
     </row>
-    <row r="111" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B111" t="s">
         <v>289</v>
       </c>
@@ -11693,7 +11692,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="112" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>401</v>
       </c>
@@ -11746,7 +11745,7 @@
         <v>881.25</v>
       </c>
     </row>
-    <row r="113" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
         <v>130</v>
       </c>
@@ -11796,7 +11795,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="114" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B114" t="s">
         <v>402</v>
       </c>
@@ -11849,7 +11848,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="115" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B115" t="s">
         <v>137</v>
       </c>
@@ -11902,7 +11901,7 @@
         <v>1087.5</v>
       </c>
     </row>
-    <row r="116" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B116" t="s">
         <v>138</v>
       </c>
@@ -11955,7 +11954,7 @@
         <v>881.25</v>
       </c>
     </row>
-    <row r="117" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>151</v>
       </c>
@@ -12008,7 +12007,7 @@
         <v>187.5</v>
       </c>
     </row>
-    <row r="118" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B118" t="s">
         <v>402</v>
       </c>
@@ -12058,7 +12057,7 @@
         <v>356.25</v>
       </c>
     </row>
-    <row r="119" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
         <v>137</v>
       </c>
@@ -12108,7 +12107,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="120" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B120" t="s">
         <v>138</v>
       </c>
@@ -12158,7 +12157,7 @@
         <v>168.75</v>
       </c>
     </row>
-    <row r="121" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>405</v>
       </c>
@@ -12211,7 +12210,7 @@
         <v>956.25</v>
       </c>
     </row>
-    <row r="122" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B122" t="s">
         <v>130</v>
       </c>
@@ -12264,7 +12263,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="123" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B123" t="s">
         <v>131</v>
       </c>
@@ -12314,7 +12313,7 @@
         <v>956.25</v>
       </c>
     </row>
-    <row r="124" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B124" t="s">
         <v>132</v>
       </c>
@@ -12367,7 +12366,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="125" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B125" t="s">
         <v>134</v>
       </c>
@@ -12420,7 +12419,7 @@
         <v>1068.75</v>
       </c>
     </row>
-    <row r="126" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B126" t="s">
         <v>138</v>
       </c>
@@ -12473,7 +12472,7 @@
         <v>881.25</v>
       </c>
     </row>
-    <row r="127" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>151</v>
       </c>
@@ -12526,7 +12525,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="128" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B128" t="s">
         <v>131</v>
       </c>
@@ -12576,7 +12575,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="129" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B129" t="s">
         <v>132</v>
       </c>
@@ -12626,7 +12625,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="130" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B130" t="s">
         <v>134</v>
       </c>
@@ -12676,7 +12675,7 @@
         <v>318.75</v>
       </c>
     </row>
-    <row r="131" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B131" t="s">
         <v>138</v>
       </c>
@@ -12726,7 +12725,7 @@
         <v>131.25</v>
       </c>
     </row>
-    <row r="132" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="132" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>406</v>
       </c>
@@ -12779,7 +12778,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="133" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B133" t="s">
         <v>130</v>
       </c>
@@ -12832,7 +12831,7 @@
         <v>1312.5</v>
       </c>
     </row>
-    <row r="134" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B134" t="s">
         <v>131</v>
       </c>
@@ -12882,7 +12881,7 @@
         <v>1387.5</v>
       </c>
     </row>
-    <row r="135" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B135" t="s">
         <v>132</v>
       </c>
@@ -12935,7 +12934,7 @@
         <v>1462.5</v>
       </c>
     </row>
-    <row r="136" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B136" t="s">
         <v>134</v>
       </c>
@@ -12988,7 +12987,7 @@
         <v>1481.25</v>
       </c>
     </row>
-    <row r="137" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B137" t="s">
         <v>138</v>
       </c>
@@ -13041,7 +13040,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="138" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>151</v>
       </c>
@@ -13094,7 +13093,7 @@
         <v>243.75</v>
       </c>
     </row>
-    <row r="139" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B139" t="s">
         <v>131</v>
       </c>
@@ -13144,7 +13143,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="140" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B140" t="s">
         <v>132</v>
       </c>
@@ -13194,7 +13193,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="141" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B141" t="s">
         <v>134</v>
       </c>
@@ -13244,7 +13243,7 @@
         <v>412.5</v>
       </c>
     </row>
-    <row r="142" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B142" t="s">
         <v>138</v>
       </c>
@@ -13294,7 +13293,7 @@
         <v>206.25</v>
       </c>
     </row>
-    <row r="143" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>413</v>
       </c>
@@ -13347,7 +13346,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="144" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B144" t="s">
         <v>130</v>
       </c>
@@ -13397,7 +13396,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="145" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B145" t="s">
         <v>131</v>
       </c>
@@ -13447,7 +13446,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="146" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>151</v>
       </c>
@@ -13500,7 +13499,7 @@
         <v>168.75</v>
       </c>
     </row>
-    <row r="147" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B147" t="s">
         <v>131</v>
       </c>
@@ -13550,7 +13549,7 @@
         <v>243.75</v>
       </c>
     </row>
-    <row r="148" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>412</v>
       </c>
@@ -13603,7 +13602,7 @@
         <v>881.25</v>
       </c>
     </row>
-    <row r="149" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B149" t="s">
         <v>130</v>
       </c>
@@ -13653,7 +13652,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="150" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>151</v>
       </c>
@@ -13706,7 +13705,7 @@
         <v>168.75</v>
       </c>
     </row>
-    <row r="151" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>414</v>
       </c>
@@ -13762,7 +13761,7 @@
         <v>993.75</v>
       </c>
     </row>
-    <row r="152" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B152" t="s">
         <v>130</v>
       </c>
@@ -13812,7 +13811,7 @@
         <v>1012.5</v>
       </c>
     </row>
-    <row r="153" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>151</v>
       </c>
@@ -13865,7 +13864,7 @@
         <v>206.25</v>
       </c>
     </row>
-    <row r="154" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="154" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>415</v>
       </c>
@@ -13918,7 +13917,7 @@
         <v>937.5</v>
       </c>
     </row>
-    <row r="155" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="155" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B155" t="s">
         <v>130</v>
       </c>
@@ -13968,7 +13967,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="156" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="156" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>151</v>
       </c>
@@ -14021,7 +14020,7 @@
         <v>206.25</v>
       </c>
     </row>
-    <row r="157" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="157" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>421</v>
       </c>
@@ -14080,7 +14079,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="158" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="158" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B158" t="s">
         <v>130</v>
       </c>
@@ -14139,7 +14138,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="159" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="159" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B159" t="s">
         <v>131</v>
       </c>
@@ -14198,7 +14197,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="160" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="160" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B160" t="s">
         <v>132</v>
       </c>
@@ -14257,7 +14256,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="161" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="161" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B161" t="s">
         <v>134</v>
       </c>
@@ -14316,7 +14315,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="162" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="162" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B162" t="s">
         <v>138</v>
       </c>
@@ -14375,7 +14374,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="163" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="163" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>151</v>
       </c>
@@ -14437,7 +14436,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="164" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="164" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B164" t="s">
         <v>131</v>
       </c>
@@ -14496,7 +14495,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="165" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="165" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B165" t="s">
         <v>132</v>
       </c>
@@ -14555,7 +14554,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="166" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="166" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B166" t="s">
         <v>134</v>
       </c>
@@ -14614,7 +14613,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="167" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="167" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B167" t="s">
         <v>138</v>
       </c>
@@ -14673,7 +14672,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="168" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="168" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>423</v>
       </c>
@@ -14729,7 +14728,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="169" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="169" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B169" t="s">
         <v>130</v>
       </c>
@@ -14785,7 +14784,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="170" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="170" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B170" t="s">
         <v>131</v>
       </c>
@@ -14841,7 +14840,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="171" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="171" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B171" t="s">
         <v>132</v>
       </c>
@@ -14897,7 +14896,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="172" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="172" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B172" t="s">
         <v>134</v>
       </c>
@@ -14953,7 +14952,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="173" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="173" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B173" t="s">
         <v>138</v>
       </c>
@@ -15009,7 +15008,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="174" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="174" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>151</v>
       </c>
@@ -15068,7 +15067,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="175" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="175" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B175" t="s">
         <v>131</v>
       </c>
@@ -15124,7 +15123,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="176" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="176" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B176" t="s">
         <v>132</v>
       </c>
@@ -15180,7 +15179,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="177" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="177" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B177" t="s">
         <v>134</v>
       </c>
@@ -15236,7 +15235,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="178" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="178" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B178" t="s">
         <v>138</v>
       </c>
@@ -15292,7 +15291,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="179" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="179" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>422</v>
       </c>
@@ -15351,7 +15350,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="180" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="180" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B180" t="s">
         <v>130</v>
       </c>
@@ -15407,7 +15406,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="181" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="181" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B181" t="s">
         <v>131</v>
       </c>
@@ -15463,7 +15462,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="182" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="182" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B182" t="s">
         <v>132</v>
       </c>
@@ -15519,7 +15518,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="183" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="183" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B183" t="s">
         <v>134</v>
       </c>
@@ -15575,7 +15574,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="184" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="184" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B184" t="s">
         <v>138</v>
       </c>
@@ -15631,7 +15630,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="185" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="185" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B185" t="s">
         <v>135</v>
       </c>
@@ -15690,7 +15689,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="186" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="186" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B186" t="s">
         <v>136</v>
       </c>
@@ -15749,7 +15748,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="187" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="187" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B187" t="s">
         <v>137</v>
       </c>
@@ -15808,7 +15807,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="188" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="188" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>434</v>
       </c>
@@ -15858,7 +15857,7 @@
         <v>993.75</v>
       </c>
     </row>
-    <row r="189" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="189" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B189" t="s">
         <v>130</v>
       </c>
@@ -15908,7 +15907,7 @@
         <v>131.25</v>
       </c>
     </row>
-    <row r="190" spans="1:32" x14ac:dyDescent="0.4">
+    <row r="190" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B190" t="s">
         <v>131</v>
       </c>
@@ -15969,12 +15968,12 @@
   <dimension ref="A1:AD17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -16066,7 +16065,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>144</v>
       </c>
@@ -16112,7 +16111,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>148</v>
       </c>
@@ -16155,7 +16154,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>181</v>
       </c>
@@ -16198,7 +16197,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>192</v>
       </c>
@@ -16238,7 +16237,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>196</v>
       </c>
@@ -16281,7 +16280,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>205</v>
       </c>
@@ -16321,7 +16320,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>237</v>
       </c>
@@ -16364,7 +16363,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>239</v>
       </c>
@@ -16404,7 +16403,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>240</v>
       </c>
@@ -16444,7 +16443,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>241</v>
       </c>
@@ -16484,7 +16483,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>294</v>
       </c>
@@ -16524,7 +16523,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>366</v>
       </c>
@@ -16564,7 +16563,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>368</v>
       </c>
@@ -16607,7 +16606,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>392</v>
       </c>
@@ -16650,7 +16649,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>397</v>
       </c>
@@ -16693,7 +16692,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>399</v>
       </c>
@@ -16741,16 +16740,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392CFCAE-41E9-4295-93E2-AE0B308CC62A}">
-  <dimension ref="A1:Z74"/>
+  <dimension ref="A1:Z75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A75" sqref="A75"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AE75" sqref="AE75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -16830,7 +16829,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -16884,7 +16883,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -16938,7 +16937,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>82</v>
       </c>
@@ -16992,7 +16991,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>83</v>
       </c>
@@ -17046,7 +17045,7 @@
         <v>2475</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>96</v>
       </c>
@@ -17100,7 +17099,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>97</v>
       </c>
@@ -17154,7 +17153,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>98</v>
       </c>
@@ -17208,7 +17207,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>99</v>
       </c>
@@ -17262,7 +17261,7 @@
         <v>2475</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>159</v>
       </c>
@@ -17316,7 +17315,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>110</v>
       </c>
@@ -17370,7 +17369,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>114</v>
       </c>
@@ -17424,7 +17423,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>166</v>
       </c>
@@ -17475,7 +17474,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>117</v>
       </c>
@@ -17529,7 +17528,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>118</v>
       </c>
@@ -17583,7 +17582,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>119</v>
       </c>
@@ -17637,7 +17636,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>120</v>
       </c>
@@ -17691,7 +17690,7 @@
         <v>2475</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>214</v>
       </c>
@@ -17742,7 +17741,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>213</v>
       </c>
@@ -17793,7 +17792,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>223</v>
       </c>
@@ -17844,7 +17843,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>224</v>
       </c>
@@ -17895,7 +17894,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>225</v>
       </c>
@@ -17946,7 +17945,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>226</v>
       </c>
@@ -17997,7 +17996,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>231</v>
       </c>
@@ -18048,7 +18047,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>141</v>
       </c>
@@ -18102,7 +18101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>154</v>
       </c>
@@ -18156,7 +18155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>156</v>
       </c>
@@ -18210,7 +18209,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>168</v>
       </c>
@@ -18261,7 +18260,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>169</v>
       </c>
@@ -18312,7 +18311,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>170</v>
       </c>
@@ -18363,7 +18362,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>171</v>
       </c>
@@ -18414,7 +18413,7 @@
         <v>2475</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>207</v>
       </c>
@@ -18465,7 +18464,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>208</v>
       </c>
@@ -18516,7 +18515,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>215</v>
       </c>
@@ -18567,7 +18566,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>216</v>
       </c>
@@ -18618,7 +18617,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>219</v>
       </c>
@@ -18669,7 +18668,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>221</v>
       </c>
@@ -18720,7 +18719,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>172</v>
       </c>
@@ -18771,7 +18770,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>178</v>
       </c>
@@ -18822,7 +18821,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>183</v>
       </c>
@@ -18873,7 +18872,7 @@
         <v>2475</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>185</v>
       </c>
@@ -18924,7 +18923,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>186</v>
       </c>
@@ -18975,7 +18974,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>187</v>
       </c>
@@ -19026,7 +19025,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>188</v>
       </c>
@@ -19077,7 +19076,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>279</v>
       </c>
@@ -19128,7 +19127,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>281</v>
       </c>
@@ -19179,7 +19178,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>292</v>
       </c>
@@ -19230,7 +19229,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>296</v>
       </c>
@@ -19290,7 +19289,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>299</v>
       </c>
@@ -19348,7 +19347,7 @@
       </c>
       <c r="Z49" s="8"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>301</v>
       </c>
@@ -19406,7 +19405,7 @@
       </c>
       <c r="Z50" s="8"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>303</v>
       </c>
@@ -19464,7 +19463,7 @@
       </c>
       <c r="Z51" s="8"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>305</v>
       </c>
@@ -19522,7 +19521,7 @@
       </c>
       <c r="Z52" s="8"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>307</v>
       </c>
@@ -19580,7 +19579,7 @@
       </c>
       <c r="Z53" s="8"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>310</v>
       </c>
@@ -19638,7 +19637,7 @@
       </c>
       <c r="Z54" s="8"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>312</v>
       </c>
@@ -19696,7 +19695,7 @@
       </c>
       <c r="Z55" s="8"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>314</v>
       </c>
@@ -19754,7 +19753,7 @@
       </c>
       <c r="Z56" s="8"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>316</v>
       </c>
@@ -19812,7 +19811,7 @@
       </c>
       <c r="Z57" s="8"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>345</v>
       </c>
@@ -19869,7 +19868,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>346</v>
       </c>
@@ -19926,7 +19925,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>370</v>
       </c>
@@ -19983,7 +19982,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>371</v>
       </c>
@@ -20040,7 +20039,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>375</v>
       </c>
@@ -20097,7 +20096,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>379</v>
       </c>
@@ -20154,7 +20153,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>380</v>
       </c>
@@ -20211,7 +20210,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>382</v>
       </c>
@@ -20268,7 +20267,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>384</v>
       </c>
@@ -20325,7 +20324,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>388</v>
       </c>
@@ -20382,7 +20381,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>391</v>
       </c>
@@ -20439,7 +20438,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>386</v>
       </c>
@@ -20496,7 +20495,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="70" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>432</v>
       </c>
@@ -20547,7 +20546,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="71" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>433</v>
       </c>
@@ -20598,7 +20597,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="72" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>428</v>
       </c>
@@ -20649,7 +20648,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="73" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>430</v>
       </c>
@@ -20684,23 +20683,23 @@
         <v>49.2</v>
       </c>
       <c r="Q73">
-        <f t="shared" ref="Q73:Q74" si="45">MEDIAN(0,255,ROUND(P73/20+SQRT(H73)/40+SQRT(M73)/2+(SQRT(O73)-SQRT(185)), 0))</f>
+        <f t="shared" ref="Q73:Q75" si="45">MEDIAN(0,255,ROUND(P73/20+SQRT(H73)/40+SQRT(M73)/2+(SQRT(O73)-SQRT(185)), 0))</f>
         <v>5</v>
       </c>
       <c r="R73">
-        <f t="shared" ref="R73:R74" si="46">Q73*50000/16</f>
+        <f t="shared" ref="R73:R75" si="46">Q73*50000/16</f>
         <v>15625</v>
       </c>
       <c r="S73">
-        <f t="shared" ref="S73:S74" si="47">MEDIAN(0,255,ROUND(SQRT(H73)/200+SQRT(M73)/2+(SQRT(O73)-SQRT(185)),0))</f>
+        <f t="shared" ref="S73:S75" si="47">MEDIAN(0,255,ROUND(SQRT(H73)/200+SQRT(M73)/2+(SQRT(O73)-SQRT(185)),0))</f>
         <v>2</v>
       </c>
       <c r="T73">
-        <f t="shared" ref="T73:T74" si="48">S73*300/16*12</f>
+        <f t="shared" ref="T73:T75" si="48">S73*300/16*12</f>
         <v>450</v>
       </c>
     </row>
-    <row r="74" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>431</v>
       </c>
@@ -20749,6 +20748,57 @@
       <c r="T74">
         <f t="shared" si="48"/>
         <v>675</v>
+      </c>
+    </row>
+    <row r="75" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>435</v>
+      </c>
+      <c r="B75" t="s">
+        <v>436</v>
+      </c>
+      <c r="E75">
+        <v>1964</v>
+      </c>
+      <c r="F75">
+        <v>30</v>
+      </c>
+      <c r="G75">
+        <v>20</v>
+      </c>
+      <c r="H75">
+        <v>100</v>
+      </c>
+      <c r="I75" t="s">
+        <v>90</v>
+      </c>
+      <c r="M75">
+        <v>300</v>
+      </c>
+      <c r="N75">
+        <v>64</v>
+      </c>
+      <c r="O75">
+        <v>108</v>
+      </c>
+      <c r="P75">
+        <v>41</v>
+      </c>
+      <c r="Q75">
+        <f t="shared" si="45"/>
+        <v>8</v>
+      </c>
+      <c r="R75">
+        <f t="shared" si="46"/>
+        <v>25000</v>
+      </c>
+      <c r="S75">
+        <f t="shared" si="47"/>
+        <v>6</v>
+      </c>
+      <c r="T75">
+        <f t="shared" si="48"/>
+        <v>1350</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
r156 push by wuwu
</commit_message>
<xml_diff>
--- a/docs/China Set Trains.xlsx
+++ b/docs/China Set Trains.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CNS\CNST\local\China-Set-Trains\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projcet china set\China-Set-Trains-site\China-Set-Trains-240406\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162A554F-19B7-44EB-B3D2-5494173CEA4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF8664FB-91F4-4F09-A236-B07C43D1C268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Loco" sheetId="1" r:id="rId1"/>
@@ -18,26 +18,17 @@
     <sheet name="Wagons" sheetId="4" r:id="rId3"/>
     <sheet name="Coaches" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="459">
   <si>
     <t>name</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1725,6 +1716,66 @@
   <si>
     <t>CR300BF</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DF11Z</t>
+  </si>
+  <si>
+    <t>df11z</t>
+  </si>
+  <si>
+    <t>10+10</t>
+  </si>
+  <si>
+    <t>DF43110</t>
+  </si>
+  <si>
+    <t>DF5</t>
+  </si>
+  <si>
+    <t>df5kz</t>
+  </si>
+  <si>
+    <t>HXD11000</t>
+  </si>
+  <si>
+    <t>hxd11000</t>
+  </si>
+  <si>
+    <t>HXD1F</t>
+  </si>
+  <si>
+    <t>hxd1f</t>
+  </si>
+  <si>
+    <t>HXD1F/FXD1B</t>
+  </si>
+  <si>
+    <t>8+8</t>
+  </si>
+  <si>
+    <t>DF4E</t>
+  </si>
+  <si>
+    <t>df4e</t>
+  </si>
+  <si>
+    <t>SS1</t>
+  </si>
+  <si>
+    <t>ss1</t>
+  </si>
+  <si>
+    <t>DF4BNB</t>
+  </si>
+  <si>
+    <t>df4bnb</t>
+  </si>
+  <si>
+    <t>DF4B (New Bodyshell)</t>
+  </si>
+  <si>
+    <t>model: Mikhail; alternative livery: wuwu, DF43110</t>
   </si>
 </sst>
 </file>
@@ -2086,21 +2137,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF53"/>
+  <dimension ref="A1:AF59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AE54" sqref="AE54"/>
+      <selection pane="bottomLeft" activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="28" width="8.58203125" style="1"/>
-    <col min="29" max="30" width="8.58203125" style="2"/>
+    <col min="26" max="28" width="8.625" style="1"/>
+    <col min="29" max="30" width="8.625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2195,7 +2246,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -2286,7 +2337,7 @@
         <v>0.44444444444444442</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -2335,7 +2386,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -2384,7 +2435,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -2433,7 +2484,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -2482,7 +2533,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -2528,7 +2579,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>106</v>
       </c>
@@ -2610,7 +2661,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>107</v>
       </c>
@@ -2707,7 +2758,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>200</v>
       </c>
@@ -2776,7 +2827,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>201</v>
       </c>
@@ -2842,7 +2893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>202</v>
       </c>
@@ -2911,7 +2962,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>234</v>
       </c>
@@ -2960,7 +3011,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -3029,7 +3080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -3078,7 +3129,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -3151,7 +3202,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -3197,7 +3248,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>235</v>
       </c>
@@ -3263,7 +3314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -3312,7 +3363,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>152</v>
       </c>
@@ -3406,7 +3457,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>319</v>
       </c>
@@ -3491,7 +3542,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>324</v>
       </c>
@@ -3585,7 +3636,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>327</v>
       </c>
@@ -3668,7 +3719,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>331</v>
       </c>
@@ -3739,7 +3790,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>333</v>
       </c>
@@ -3810,7 +3861,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>335</v>
       </c>
@@ -3884,7 +3935,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>338</v>
       </c>
@@ -3958,7 +4009,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>340</v>
       </c>
@@ -4042,7 +4093,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -4091,7 +4142,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -4164,7 +4215,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -4237,7 +4288,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -4310,7 +4361,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -4407,7 +4458,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -4483,7 +4534,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>139</v>
       </c>
@@ -4580,7 +4631,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>194</v>
       </c>
@@ -4644,7 +4695,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>197</v>
       </c>
@@ -4711,7 +4762,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>258</v>
       </c>
@@ -4796,7 +4847,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>263</v>
       </c>
@@ -4884,7 +4935,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>265</v>
       </c>
@@ -4972,7 +5023,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>267</v>
       </c>
@@ -5060,7 +5111,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>269</v>
       </c>
@@ -5148,7 +5199,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>272</v>
       </c>
@@ -5236,7 +5287,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>274</v>
       </c>
@@ -5327,7 +5378,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>277</v>
       </c>
@@ -5415,7 +5466,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>351</v>
       </c>
@@ -5495,7 +5546,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>353</v>
       </c>
@@ -5575,7 +5626,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>355</v>
       </c>
@@ -5653,7 +5704,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>359</v>
       </c>
@@ -5734,7 +5785,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>394</v>
       </c>
@@ -5813,7 +5864,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>424</v>
       </c>
@@ -5889,7 +5940,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>425</v>
       </c>
@@ -5965,8 +6016,484 @@
         <v>343</v>
       </c>
     </row>
-    <row r="53" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="R53" s="5"/>
+    <row r="53" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>439</v>
+      </c>
+      <c r="B53" t="s">
+        <v>440</v>
+      </c>
+      <c r="D53" t="s">
+        <v>439</v>
+      </c>
+      <c r="E53" t="s">
+        <v>322</v>
+      </c>
+      <c r="F53">
+        <v>2002</v>
+      </c>
+      <c r="G53">
+        <v>30</v>
+      </c>
+      <c r="H53" t="s">
+        <v>261</v>
+      </c>
+      <c r="J53">
+        <v>14</v>
+      </c>
+      <c r="K53">
+        <v>160</v>
+      </c>
+      <c r="L53">
+        <v>9816</v>
+      </c>
+      <c r="M53">
+        <v>291</v>
+      </c>
+      <c r="O53">
+        <v>291</v>
+      </c>
+      <c r="P53">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="Q53">
+        <v>490.50959999999998</v>
+      </c>
+      <c r="R53" s="5">
+        <v>135</v>
+      </c>
+      <c r="S53">
+        <v>421875</v>
+      </c>
+      <c r="T53">
+        <v>100</v>
+      </c>
+      <c r="U53">
+        <v>24375</v>
+      </c>
+      <c r="V53" t="s">
+        <v>441</v>
+      </c>
+      <c r="W53">
+        <v>2</v>
+      </c>
+      <c r="X53">
+        <v>6</v>
+      </c>
+      <c r="Y53">
+        <v>2</v>
+      </c>
+      <c r="AD53" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="AE53" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="54" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>443</v>
+      </c>
+      <c r="B54" t="s">
+        <v>444</v>
+      </c>
+      <c r="D54" t="s">
+        <v>443</v>
+      </c>
+      <c r="E54" t="s">
+        <v>322</v>
+      </c>
+      <c r="F54">
+        <v>1976</v>
+      </c>
+      <c r="G54">
+        <v>25</v>
+      </c>
+      <c r="H54">
+        <v>60</v>
+      </c>
+      <c r="I54">
+        <v>30</v>
+      </c>
+      <c r="J54">
+        <v>20</v>
+      </c>
+      <c r="K54">
+        <v>100</v>
+      </c>
+      <c r="L54">
+        <v>1264</v>
+      </c>
+      <c r="M54">
+        <v>120</v>
+      </c>
+      <c r="O54">
+        <v>120</v>
+      </c>
+      <c r="P54">
+        <v>0.32300000000000001</v>
+      </c>
+      <c r="Q54">
+        <v>379.84800000000001</v>
+      </c>
+      <c r="R54">
+        <v>48</v>
+      </c>
+      <c r="S54">
+        <v>150000</v>
+      </c>
+      <c r="T54">
+        <v>36</v>
+      </c>
+      <c r="U54">
+        <v>8775</v>
+      </c>
+      <c r="AD54" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="AE54" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="55" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>445</v>
+      </c>
+      <c r="B55" t="s">
+        <v>446</v>
+      </c>
+      <c r="F55">
+        <v>2012</v>
+      </c>
+      <c r="G55">
+        <v>30</v>
+      </c>
+      <c r="H55" t="s">
+        <v>261</v>
+      </c>
+      <c r="J55">
+        <v>8</v>
+      </c>
+      <c r="K55">
+        <v>120</v>
+      </c>
+      <c r="L55">
+        <v>13052</v>
+      </c>
+      <c r="M55">
+        <v>184</v>
+      </c>
+      <c r="O55">
+        <v>184</v>
+      </c>
+      <c r="P55">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="Q55">
+        <v>759.1472</v>
+      </c>
+      <c r="R55">
+        <v>146</v>
+      </c>
+      <c r="S55">
+        <v>456250</v>
+      </c>
+      <c r="T55">
+        <v>118</v>
+      </c>
+      <c r="U55">
+        <v>26550</v>
+      </c>
+      <c r="V55">
+        <v>0</v>
+      </c>
+      <c r="AC55" s="2" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AD55" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="56" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>447</v>
+      </c>
+      <c r="B56" t="s">
+        <v>448</v>
+      </c>
+      <c r="C56" t="s">
+        <v>449</v>
+      </c>
+      <c r="E56" t="s">
+        <v>260</v>
+      </c>
+      <c r="F56">
+        <v>2013</v>
+      </c>
+      <c r="G56">
+        <v>30</v>
+      </c>
+      <c r="H56" t="s">
+        <v>261</v>
+      </c>
+      <c r="J56">
+        <v>8</v>
+      </c>
+      <c r="K56">
+        <v>100</v>
+      </c>
+      <c r="L56">
+        <v>13052</v>
+      </c>
+      <c r="M56">
+        <v>240</v>
+      </c>
+      <c r="O56">
+        <v>240</v>
+      </c>
+      <c r="P56">
+        <v>0.38690476200000001</v>
+      </c>
+      <c r="Q56">
+        <v>910.00000020000004</v>
+      </c>
+      <c r="R56">
+        <v>151</v>
+      </c>
+      <c r="S56">
+        <v>471875</v>
+      </c>
+      <c r="T56">
+        <v>118</v>
+      </c>
+      <c r="U56">
+        <v>26550</v>
+      </c>
+      <c r="V56" t="s">
+        <v>450</v>
+      </c>
+      <c r="AD56" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="57" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>451</v>
+      </c>
+      <c r="B57" t="s">
+        <v>452</v>
+      </c>
+      <c r="E57" t="s">
+        <v>322</v>
+      </c>
+      <c r="F57">
+        <v>1994</v>
+      </c>
+      <c r="G57">
+        <v>30</v>
+      </c>
+      <c r="H57">
+        <v>60</v>
+      </c>
+      <c r="I57">
+        <v>10</v>
+      </c>
+      <c r="J57">
+        <v>14</v>
+      </c>
+      <c r="K57">
+        <v>100</v>
+      </c>
+      <c r="L57">
+        <v>5438</v>
+      </c>
+      <c r="M57">
+        <v>276</v>
+      </c>
+      <c r="O57">
+        <v>276</v>
+      </c>
+      <c r="P57">
+        <v>0.31425613699999999</v>
+      </c>
+      <c r="Q57">
+        <v>849.99999939999998</v>
+      </c>
+      <c r="R57">
+        <v>108</v>
+      </c>
+      <c r="S57">
+        <v>337500</v>
+      </c>
+      <c r="T57">
+        <v>75</v>
+      </c>
+      <c r="U57">
+        <v>18281.25</v>
+      </c>
+      <c r="V57" t="s">
+        <v>441</v>
+      </c>
+      <c r="AD57" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="AE57" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="58" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>453</v>
+      </c>
+      <c r="B58" t="s">
+        <v>454</v>
+      </c>
+      <c r="E58" t="s">
+        <v>260</v>
+      </c>
+      <c r="F58">
+        <v>1958</v>
+      </c>
+      <c r="G58">
+        <v>30</v>
+      </c>
+      <c r="H58">
+        <v>60</v>
+      </c>
+      <c r="I58">
+        <v>30</v>
+      </c>
+      <c r="J58">
+        <v>20</v>
+      </c>
+      <c r="K58">
+        <v>90</v>
+      </c>
+      <c r="L58">
+        <v>5302</v>
+      </c>
+      <c r="M58">
+        <v>138</v>
+      </c>
+      <c r="O58">
+        <v>5302</v>
+      </c>
+      <c r="P58">
+        <v>0.36010056200000001</v>
+      </c>
+      <c r="Q58">
+        <v>18710.68116</v>
+      </c>
+      <c r="R58">
+        <v>87</v>
+      </c>
+      <c r="S58">
+        <v>271875</v>
+      </c>
+      <c r="T58">
+        <v>73</v>
+      </c>
+      <c r="U58">
+        <v>16425</v>
+      </c>
+      <c r="V58">
+        <v>10</v>
+      </c>
+      <c r="AD58" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="AE58" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="59" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>455</v>
+      </c>
+      <c r="B59" t="s">
+        <v>456</v>
+      </c>
+      <c r="D59" t="s">
+        <v>457</v>
+      </c>
+      <c r="E59" t="s">
+        <v>322</v>
+      </c>
+      <c r="F59">
+        <v>1984</v>
+      </c>
+      <c r="G59">
+        <v>30</v>
+      </c>
+      <c r="H59">
+        <v>60</v>
+      </c>
+      <c r="I59">
+        <v>40</v>
+      </c>
+      <c r="J59">
+        <v>14</v>
+      </c>
+      <c r="K59">
+        <v>100</v>
+      </c>
+      <c r="L59">
+        <v>2610</v>
+      </c>
+      <c r="M59">
+        <v>138</v>
+      </c>
+      <c r="O59">
+        <v>138</v>
+      </c>
+      <c r="P59">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="Q59">
+        <v>412.48200000000003</v>
+      </c>
+      <c r="R59">
+        <v>72</v>
+      </c>
+      <c r="S59">
+        <v>225000</v>
+      </c>
+      <c r="T59">
+        <v>52</v>
+      </c>
+      <c r="U59">
+        <v>12675</v>
+      </c>
+      <c r="V59">
+        <v>10</v>
+      </c>
+      <c r="W59">
+        <v>1</v>
+      </c>
+      <c r="X59">
+        <v>8</v>
+      </c>
+      <c r="Y59">
+        <v>1</v>
+      </c>
+      <c r="Z59" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA59" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB59" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC59" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD59" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="AE59" t="s">
+        <v>458</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -5978,17 +6505,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB4625FC-685F-4E56-AE60-F05D51350408}">
   <dimension ref="A1:AF202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A171" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="W197" sqref="W197:W201"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="32" max="32" width="20.33203125" customWidth="1"/>
+    <col min="32" max="32" width="20.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6086,7 +6613,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>133</v>
       </c>
@@ -6154,7 +6681,7 @@
         <v>1650</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="I3">
         <v>20</v>
       </c>
@@ -6204,7 +6731,7 @@
         <v>2325</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>130</v>
       </c>
@@ -6257,7 +6784,7 @@
         <v>131.25</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>131</v>
       </c>
@@ -6310,7 +6837,7 @@
         <v>206.25</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>132</v>
       </c>
@@ -6363,7 +6890,7 @@
         <v>281.25</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>134</v>
       </c>
@@ -6416,7 +6943,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>138</v>
       </c>
@@ -6469,7 +6996,7 @@
         <v>93.75</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>135</v>
       </c>
@@ -6522,7 +7049,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>136</v>
       </c>
@@ -6575,7 +7102,7 @@
         <v>281.25</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>137</v>
       </c>
@@ -6628,7 +7155,7 @@
         <v>318.75</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>150</v>
       </c>
@@ -6681,7 +7208,7 @@
         <v>937.5</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>130</v>
       </c>
@@ -6734,7 +7261,7 @@
         <v>862.5</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>131</v>
       </c>
@@ -6787,7 +7314,7 @@
         <v>937.5</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>132</v>
       </c>
@@ -6840,7 +7367,7 @@
         <v>1012.5</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>134</v>
       </c>
@@ -6893,7 +7420,7 @@
         <v>1031.25</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>138</v>
       </c>
@@ -6946,7 +7473,7 @@
         <v>843.75</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>151</v>
       </c>
@@ -7002,7 +7529,7 @@
         <v>131.25</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>131</v>
       </c>
@@ -7055,7 +7582,7 @@
         <v>206.25</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>132</v>
       </c>
@@ -7108,7 +7635,7 @@
         <v>281.25</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>134</v>
       </c>
@@ -7161,7 +7688,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>138</v>
       </c>
@@ -7214,7 +7741,7 @@
         <v>112.5</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>158</v>
       </c>
@@ -7267,7 +7794,7 @@
         <v>1406.25</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>130</v>
       </c>
@@ -7320,7 +7847,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>131</v>
       </c>
@@ -7373,7 +7900,7 @@
         <v>1406.25</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>132</v>
       </c>
@@ -7426,7 +7953,7 @@
         <v>1481.25</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>134</v>
       </c>
@@ -7479,7 +8006,7 @@
         <v>1518.75</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>138</v>
       </c>
@@ -7532,7 +8059,7 @@
         <v>1312.5</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>151</v>
       </c>
@@ -7588,7 +8115,7 @@
         <v>243.75</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>131</v>
       </c>
@@ -7641,7 +8168,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>132</v>
       </c>
@@ -7694,7 +8221,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>134</v>
       </c>
@@ -7747,7 +8274,7 @@
         <v>412.5</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>138</v>
       </c>
@@ -7800,7 +8327,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>247</v>
       </c>
@@ -7850,7 +8377,7 @@
         <v>843.75</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>248</v>
       </c>
@@ -7900,7 +8427,7 @@
         <v>881.25</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>249</v>
       </c>
@@ -7950,7 +8477,7 @@
         <v>937.5</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>250</v>
       </c>
@@ -8000,7 +8527,7 @@
         <v>1012.5</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>251</v>
       </c>
@@ -8050,7 +8577,7 @@
         <v>1031.25</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>252</v>
       </c>
@@ -8100,7 +8627,7 @@
         <v>843.75</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>248</v>
       </c>
@@ -8150,7 +8677,7 @@
         <v>131.25</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>249</v>
       </c>
@@ -8200,7 +8727,7 @@
         <v>206.25</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>250</v>
       </c>
@@ -8250,7 +8777,7 @@
         <v>281.25</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>251</v>
       </c>
@@ -8300,7 +8827,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>252</v>
       </c>
@@ -8350,7 +8877,7 @@
         <v>112.5</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>253</v>
       </c>
@@ -8400,7 +8927,7 @@
         <v>937.5</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>248</v>
       </c>
@@ -8450,7 +8977,7 @@
         <v>956.25</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>249</v>
       </c>
@@ -8500,7 +9027,7 @@
         <v>1012.5</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>250</v>
       </c>
@@ -8550,7 +9077,7 @@
         <v>1106.25</v>
       </c>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>251</v>
       </c>
@@ -8600,7 +9127,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>252</v>
       </c>
@@ -8650,7 +9177,7 @@
         <v>937.5</v>
       </c>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>248</v>
       </c>
@@ -8700,7 +9227,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>249</v>
       </c>
@@ -8750,7 +9277,7 @@
         <v>206.25</v>
       </c>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>250</v>
       </c>
@@ -8800,7 +9327,7 @@
         <v>281.25</v>
       </c>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>251</v>
       </c>
@@ -8850,7 +9377,7 @@
         <v>318.75</v>
       </c>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>252</v>
       </c>
@@ -8900,7 +9427,7 @@
         <v>131.25</v>
       </c>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>254</v>
       </c>
@@ -8950,7 +9477,7 @@
         <v>1668.75</v>
       </c>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>248</v>
       </c>
@@ -9000,7 +9527,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
         <v>249</v>
       </c>
@@ -9050,7 +9577,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>250</v>
       </c>
@@ -9100,7 +9627,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>251</v>
       </c>
@@ -9150,7 +9677,7 @@
         <v>318.75</v>
       </c>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>252</v>
       </c>
@@ -9200,7 +9727,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>255</v>
       </c>
@@ -9250,7 +9777,7 @@
         <v>1031.25</v>
       </c>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>248</v>
       </c>
@@ -9300,7 +9827,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>249</v>
       </c>
@@ -9350,7 +9877,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
         <v>250</v>
       </c>
@@ -9400,7 +9927,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
         <v>251</v>
       </c>
@@ -9450,7 +9977,7 @@
         <v>1143.75</v>
       </c>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>252</v>
       </c>
@@ -9500,7 +10027,7 @@
         <v>956.25</v>
       </c>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>248</v>
       </c>
@@ -9550,7 +10077,7 @@
         <v>187.5</v>
       </c>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
         <v>249</v>
       </c>
@@ -9600,7 +10127,7 @@
         <v>262.5</v>
       </c>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
         <v>250</v>
       </c>
@@ -9650,7 +10177,7 @@
         <v>337.5</v>
       </c>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
         <v>251</v>
       </c>
@@ -9700,7 +10227,7 @@
         <v>356.25</v>
       </c>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
         <v>252</v>
       </c>
@@ -9750,7 +10277,7 @@
         <v>168.75</v>
       </c>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>256</v>
       </c>
@@ -9800,7 +10327,7 @@
         <v>1106.25</v>
       </c>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
         <v>248</v>
       </c>
@@ -9850,7 +10377,7 @@
         <v>206.25</v>
       </c>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
         <v>249</v>
       </c>
@@ -9900,7 +10427,7 @@
         <v>281.25</v>
       </c>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
         <v>252</v>
       </c>
@@ -9950,7 +10477,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>257</v>
       </c>
@@ -10000,7 +10527,7 @@
         <v>1518.75</v>
       </c>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
         <v>249</v>
       </c>
@@ -10050,7 +10577,7 @@
         <v>112.5</v>
       </c>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>284</v>
       </c>
@@ -10100,7 +10627,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
         <v>285</v>
       </c>
@@ -10150,7 +10677,7 @@
         <v>1293.75</v>
       </c>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
         <v>286</v>
       </c>
@@ -10200,7 +10727,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
         <v>287</v>
       </c>
@@ -10250,7 +10777,7 @@
         <v>1443.75</v>
       </c>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>288</v>
       </c>
@@ -10300,7 +10827,7 @@
         <v>1462.5</v>
       </c>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
         <v>289</v>
       </c>
@@ -10350,7 +10877,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>151</v>
       </c>
@@ -10403,7 +10930,7 @@
         <v>243.75</v>
       </c>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
         <v>286</v>
       </c>
@@ -10453,7 +10980,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
         <v>287</v>
       </c>
@@ -10503,7 +11030,7 @@
         <v>393.75</v>
       </c>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
         <v>288</v>
       </c>
@@ -10553,7 +11080,7 @@
         <v>412.5</v>
       </c>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
         <v>289</v>
       </c>
@@ -10603,7 +11130,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>290</v>
       </c>
@@ -10653,7 +11180,7 @@
         <v>1181.25</v>
       </c>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
         <v>285</v>
       </c>
@@ -10703,7 +11230,7 @@
         <v>1181.25</v>
       </c>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
         <v>286</v>
       </c>
@@ -10753,7 +11280,7 @@
         <v>1256.25</v>
       </c>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
         <v>287</v>
       </c>
@@ -10803,7 +11330,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
         <v>288</v>
       </c>
@@ -10853,7 +11380,7 @@
         <v>1368.75</v>
       </c>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
         <v>289</v>
       </c>
@@ -10903,7 +11430,7 @@
         <v>1162.5</v>
       </c>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>151</v>
       </c>
@@ -10956,7 +11483,7 @@
         <v>168.75</v>
       </c>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
         <v>286</v>
       </c>
@@ -11006,7 +11533,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
         <v>287</v>
       </c>
@@ -11056,7 +11583,7 @@
         <v>318.75</v>
       </c>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
         <v>288</v>
       </c>
@@ -11106,7 +11633,7 @@
         <v>337.5</v>
       </c>
     </row>
-    <row r="100" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
         <v>289</v>
       </c>
@@ -11156,7 +11683,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="101" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>291</v>
       </c>
@@ -11206,7 +11733,7 @@
         <v>937.5</v>
       </c>
     </row>
-    <row r="102" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
         <v>285</v>
       </c>
@@ -11256,7 +11783,7 @@
         <v>862.5</v>
       </c>
     </row>
-    <row r="103" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
         <v>286</v>
       </c>
@@ -11306,7 +11833,7 @@
         <v>956.25</v>
       </c>
     </row>
-    <row r="104" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
         <v>287</v>
       </c>
@@ -11356,7 +11883,7 @@
         <v>1031.25</v>
       </c>
     </row>
-    <row r="105" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B105" t="s">
         <v>288</v>
       </c>
@@ -11406,7 +11933,7 @@
         <v>1031.25</v>
       </c>
     </row>
-    <row r="106" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
         <v>289</v>
       </c>
@@ -11456,7 +11983,7 @@
         <v>862.5</v>
       </c>
     </row>
-    <row r="107" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>151</v>
       </c>
@@ -11509,7 +12036,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="108" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B108" t="s">
         <v>286</v>
       </c>
@@ -11559,7 +12086,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="109" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
         <v>287</v>
       </c>
@@ -11609,7 +12136,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="110" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B110" t="s">
         <v>288</v>
       </c>
@@ -11659,7 +12186,7 @@
         <v>318.75</v>
       </c>
     </row>
-    <row r="111" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B111" t="s">
         <v>289</v>
       </c>
@@ -11709,7 +12236,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="112" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>401</v>
       </c>
@@ -11762,7 +12289,7 @@
         <v>881.25</v>
       </c>
     </row>
-    <row r="113" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
         <v>130</v>
       </c>
@@ -11812,7 +12339,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="114" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B114" t="s">
         <v>402</v>
       </c>
@@ -11865,7 +12392,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="115" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B115" t="s">
         <v>137</v>
       </c>
@@ -11918,7 +12445,7 @@
         <v>1087.5</v>
       </c>
     </row>
-    <row r="116" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B116" t="s">
         <v>138</v>
       </c>
@@ -11971,7 +12498,7 @@
         <v>881.25</v>
       </c>
     </row>
-    <row r="117" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>151</v>
       </c>
@@ -12024,7 +12551,7 @@
         <v>187.5</v>
       </c>
     </row>
-    <row r="118" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B118" t="s">
         <v>402</v>
       </c>
@@ -12074,7 +12601,7 @@
         <v>356.25</v>
       </c>
     </row>
-    <row r="119" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
         <v>137</v>
       </c>
@@ -12124,7 +12651,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="120" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B120" t="s">
         <v>138</v>
       </c>
@@ -12174,7 +12701,7 @@
         <v>168.75</v>
       </c>
     </row>
-    <row r="121" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>405</v>
       </c>
@@ -12227,7 +12754,7 @@
         <v>956.25</v>
       </c>
     </row>
-    <row r="122" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B122" t="s">
         <v>130</v>
       </c>
@@ -12280,7 +12807,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="123" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B123" t="s">
         <v>131</v>
       </c>
@@ -12330,7 +12857,7 @@
         <v>956.25</v>
       </c>
     </row>
-    <row r="124" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B124" t="s">
         <v>132</v>
       </c>
@@ -12383,7 +12910,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="125" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B125" t="s">
         <v>134</v>
       </c>
@@ -12436,7 +12963,7 @@
         <v>1068.75</v>
       </c>
     </row>
-    <row r="126" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B126" t="s">
         <v>138</v>
       </c>
@@ -12489,7 +13016,7 @@
         <v>881.25</v>
       </c>
     </row>
-    <row r="127" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>151</v>
       </c>
@@ -12542,7 +13069,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="128" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B128" t="s">
         <v>131</v>
       </c>
@@ -12592,7 +13119,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="129" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B129" t="s">
         <v>132</v>
       </c>
@@ -12642,7 +13169,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="130" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B130" t="s">
         <v>134</v>
       </c>
@@ -12692,7 +13219,7 @@
         <v>318.75</v>
       </c>
     </row>
-    <row r="131" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B131" t="s">
         <v>138</v>
       </c>
@@ -12742,7 +13269,7 @@
         <v>131.25</v>
       </c>
     </row>
-    <row r="132" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>406</v>
       </c>
@@ -12795,7 +13322,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="133" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B133" t="s">
         <v>130</v>
       </c>
@@ -12848,7 +13375,7 @@
         <v>1312.5</v>
       </c>
     </row>
-    <row r="134" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B134" t="s">
         <v>131</v>
       </c>
@@ -12898,7 +13425,7 @@
         <v>1387.5</v>
       </c>
     </row>
-    <row r="135" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B135" t="s">
         <v>132</v>
       </c>
@@ -12951,7 +13478,7 @@
         <v>1462.5</v>
       </c>
     </row>
-    <row r="136" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B136" t="s">
         <v>134</v>
       </c>
@@ -13004,7 +13531,7 @@
         <v>1481.25</v>
       </c>
     </row>
-    <row r="137" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B137" t="s">
         <v>138</v>
       </c>
@@ -13057,7 +13584,7 @@
         <v>1275</v>
       </c>
     </row>
-    <row r="138" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>151</v>
       </c>
@@ -13110,7 +13637,7 @@
         <v>243.75</v>
       </c>
     </row>
-    <row r="139" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B139" t="s">
         <v>131</v>
       </c>
@@ -13160,7 +13687,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="140" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B140" t="s">
         <v>132</v>
       </c>
@@ -13210,7 +13737,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="141" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B141" t="s">
         <v>134</v>
       </c>
@@ -13260,7 +13787,7 @@
         <v>412.5</v>
       </c>
     </row>
-    <row r="142" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B142" t="s">
         <v>138</v>
       </c>
@@ -13310,7 +13837,7 @@
         <v>206.25</v>
       </c>
     </row>
-    <row r="143" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>413</v>
       </c>
@@ -13363,7 +13890,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="144" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B144" t="s">
         <v>130</v>
       </c>
@@ -13413,7 +13940,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="145" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B145" t="s">
         <v>131</v>
       </c>
@@ -13463,7 +13990,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="146" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>151</v>
       </c>
@@ -13516,7 +14043,7 @@
         <v>168.75</v>
       </c>
     </row>
-    <row r="147" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B147" t="s">
         <v>131</v>
       </c>
@@ -13566,7 +14093,7 @@
         <v>243.75</v>
       </c>
     </row>
-    <row r="148" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>412</v>
       </c>
@@ -13619,7 +14146,7 @@
         <v>881.25</v>
       </c>
     </row>
-    <row r="149" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B149" t="s">
         <v>130</v>
       </c>
@@ -13669,7 +14196,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="150" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>151</v>
       </c>
@@ -13722,7 +14249,7 @@
         <v>168.75</v>
       </c>
     </row>
-    <row r="151" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>414</v>
       </c>
@@ -13778,7 +14305,7 @@
         <v>993.75</v>
       </c>
     </row>
-    <row r="152" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B152" t="s">
         <v>130</v>
       </c>
@@ -13828,7 +14355,7 @@
         <v>1012.5</v>
       </c>
     </row>
-    <row r="153" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>151</v>
       </c>
@@ -13881,7 +14408,7 @@
         <v>206.25</v>
       </c>
     </row>
-    <row r="154" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>415</v>
       </c>
@@ -13934,7 +14461,7 @@
         <v>937.5</v>
       </c>
     </row>
-    <row r="155" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B155" t="s">
         <v>130</v>
       </c>
@@ -13984,7 +14511,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="156" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>151</v>
       </c>
@@ -14037,7 +14564,7 @@
         <v>206.25</v>
       </c>
     </row>
-    <row r="157" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>421</v>
       </c>
@@ -14096,7 +14623,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="158" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B158" t="s">
         <v>130</v>
       </c>
@@ -14155,7 +14682,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="159" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B159" t="s">
         <v>131</v>
       </c>
@@ -14214,7 +14741,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="160" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B160" t="s">
         <v>132</v>
       </c>
@@ -14273,7 +14800,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="161" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B161" t="s">
         <v>134</v>
       </c>
@@ -14332,7 +14859,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="162" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B162" t="s">
         <v>138</v>
       </c>
@@ -14391,7 +14918,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="163" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>151</v>
       </c>
@@ -14453,7 +14980,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="164" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B164" t="s">
         <v>131</v>
       </c>
@@ -14512,7 +15039,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="165" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B165" t="s">
         <v>132</v>
       </c>
@@ -14571,7 +15098,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="166" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B166" t="s">
         <v>134</v>
       </c>
@@ -14630,7 +15157,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="167" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B167" t="s">
         <v>138</v>
       </c>
@@ -14689,7 +15216,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="168" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>423</v>
       </c>
@@ -14745,7 +15272,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="169" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B169" t="s">
         <v>130</v>
       </c>
@@ -14801,7 +15328,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="170" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B170" t="s">
         <v>131</v>
       </c>
@@ -14857,7 +15384,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="171" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B171" t="s">
         <v>132</v>
       </c>
@@ -14913,7 +15440,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="172" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B172" t="s">
         <v>134</v>
       </c>
@@ -14969,7 +15496,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="173" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B173" t="s">
         <v>138</v>
       </c>
@@ -15025,7 +15552,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="174" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>151</v>
       </c>
@@ -15084,7 +15611,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="175" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B175" t="s">
         <v>131</v>
       </c>
@@ -15140,7 +15667,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="176" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B176" t="s">
         <v>132</v>
       </c>
@@ -15196,7 +15723,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="177" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B177" t="s">
         <v>134</v>
       </c>
@@ -15252,7 +15779,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="178" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B178" t="s">
         <v>138</v>
       </c>
@@ -15308,7 +15835,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="179" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>422</v>
       </c>
@@ -15367,7 +15894,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="180" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B180" t="s">
         <v>130</v>
       </c>
@@ -15423,7 +15950,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="181" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B181" t="s">
         <v>131</v>
       </c>
@@ -15479,7 +16006,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="182" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B182" t="s">
         <v>132</v>
       </c>
@@ -15535,7 +16062,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="183" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B183" t="s">
         <v>134</v>
       </c>
@@ -15591,7 +16118,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="184" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B184" t="s">
         <v>138</v>
       </c>
@@ -15647,7 +16174,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="185" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B185" t="s">
         <v>135</v>
       </c>
@@ -15706,7 +16233,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="186" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B186" t="s">
         <v>136</v>
       </c>
@@ -15765,7 +16292,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="187" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B187" t="s">
         <v>137</v>
       </c>
@@ -15824,7 +16351,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="188" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>434</v>
       </c>
@@ -15874,7 +16401,7 @@
         <v>993.75</v>
       </c>
     </row>
-    <row r="189" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B189" t="s">
         <v>130</v>
       </c>
@@ -15924,7 +16451,7 @@
         <v>131.25</v>
       </c>
     </row>
-    <row r="190" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B190" t="s">
         <v>131</v>
       </c>
@@ -15974,7 +16501,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="191" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>438</v>
       </c>
@@ -16027,7 +16554,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="192" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B192" t="s">
         <v>130</v>
       </c>
@@ -16080,7 +16607,7 @@
         <v>956.25</v>
       </c>
     </row>
-    <row r="193" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B193" t="s">
         <v>131</v>
       </c>
@@ -16133,7 +16660,7 @@
         <v>1031.25</v>
       </c>
     </row>
-    <row r="194" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B194" t="s">
         <v>132</v>
       </c>
@@ -16186,7 +16713,7 @@
         <v>1087.5</v>
       </c>
     </row>
-    <row r="195" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B195" t="s">
         <v>134</v>
       </c>
@@ -16239,7 +16766,7 @@
         <v>1106.25</v>
       </c>
     </row>
-    <row r="196" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B196" t="s">
         <v>138</v>
       </c>
@@ -16292,7 +16819,7 @@
         <v>937.5</v>
       </c>
     </row>
-    <row r="197" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>151</v>
       </c>
@@ -16348,7 +16875,7 @@
         <v>131.25</v>
       </c>
     </row>
-    <row r="198" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B198" t="s">
         <v>131</v>
       </c>
@@ -16359,7 +16886,7 @@
         <v>250</v>
       </c>
       <c r="K198">
-        <f t="shared" ref="K197:K201" si="36">ROUND(L198/0.73549875,0)</f>
+        <f t="shared" ref="K198:K201" si="36">ROUND(L198/0.73549875,0)</f>
         <v>0</v>
       </c>
       <c r="L198">
@@ -16401,7 +16928,7 @@
         <v>206.25</v>
       </c>
     </row>
-    <row r="199" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B199" t="s">
         <v>132</v>
       </c>
@@ -16454,7 +16981,7 @@
         <v>281.25</v>
       </c>
     </row>
-    <row r="200" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B200" t="s">
         <v>134</v>
       </c>
@@ -16507,7 +17034,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="201" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B201" t="s">
         <v>138</v>
       </c>
@@ -16560,7 +17087,7 @@
         <v>131.25</v>
       </c>
     </row>
-    <row r="202" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:26" x14ac:dyDescent="0.2">
       <c r="L202">
         <v>0</v>
       </c>
@@ -16580,9 +17107,9 @@
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -16674,7 +17201,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>144</v>
       </c>
@@ -16720,7 +17247,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>148</v>
       </c>
@@ -16763,7 +17290,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>181</v>
       </c>
@@ -16806,7 +17333,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>192</v>
       </c>
@@ -16846,7 +17373,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>196</v>
       </c>
@@ -16889,7 +17416,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>205</v>
       </c>
@@ -16929,7 +17456,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>237</v>
       </c>
@@ -16972,7 +17499,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>239</v>
       </c>
@@ -17012,7 +17539,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>240</v>
       </c>
@@ -17052,7 +17579,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>241</v>
       </c>
@@ -17092,7 +17619,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>294</v>
       </c>
@@ -17132,7 +17659,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>366</v>
       </c>
@@ -17172,7 +17699,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>368</v>
       </c>
@@ -17215,7 +17742,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>392</v>
       </c>
@@ -17258,7 +17785,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>397</v>
       </c>
@@ -17301,7 +17828,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>399</v>
       </c>
@@ -17341,7 +17868,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>437</v>
       </c>
@@ -17361,9 +17888,9 @@
       <selection pane="bottomLeft" activeCell="AE75" sqref="AE75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -17443,7 +17970,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -17497,7 +18024,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -17551,7 +18078,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>82</v>
       </c>
@@ -17605,7 +18132,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>83</v>
       </c>
@@ -17659,7 +18186,7 @@
         <v>2475</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>96</v>
       </c>
@@ -17713,7 +18240,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>97</v>
       </c>
@@ -17767,7 +18294,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>98</v>
       </c>
@@ -17821,7 +18348,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>99</v>
       </c>
@@ -17875,7 +18402,7 @@
         <v>2475</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>159</v>
       </c>
@@ -17929,7 +18456,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>110</v>
       </c>
@@ -17983,7 +18510,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>114</v>
       </c>
@@ -18037,7 +18564,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>166</v>
       </c>
@@ -18088,7 +18615,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>117</v>
       </c>
@@ -18142,7 +18669,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>118</v>
       </c>
@@ -18196,7 +18723,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>119</v>
       </c>
@@ -18250,7 +18777,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>120</v>
       </c>
@@ -18304,7 +18831,7 @@
         <v>2475</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>214</v>
       </c>
@@ -18355,7 +18882,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>213</v>
       </c>
@@ -18406,7 +18933,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>223</v>
       </c>
@@ -18457,7 +18984,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>224</v>
       </c>
@@ -18508,7 +19035,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>225</v>
       </c>
@@ -18559,7 +19086,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>226</v>
       </c>
@@ -18610,7 +19137,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>231</v>
       </c>
@@ -18661,7 +19188,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>141</v>
       </c>
@@ -18715,7 +19242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>154</v>
       </c>
@@ -18769,7 +19296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>156</v>
       </c>
@@ -18823,7 +19350,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>168</v>
       </c>
@@ -18874,7 +19401,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>169</v>
       </c>
@@ -18925,7 +19452,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>170</v>
       </c>
@@ -18976,7 +19503,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>171</v>
       </c>
@@ -19027,7 +19554,7 @@
         <v>2475</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>207</v>
       </c>
@@ -19078,7 +19605,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>208</v>
       </c>
@@ -19129,7 +19656,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>215</v>
       </c>
@@ -19180,7 +19707,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>216</v>
       </c>
@@ -19231,7 +19758,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>219</v>
       </c>
@@ -19282,7 +19809,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>221</v>
       </c>
@@ -19333,7 +19860,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>172</v>
       </c>
@@ -19384,7 +19911,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>178</v>
       </c>
@@ -19435,7 +19962,7 @@
         <v>1575</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>183</v>
       </c>
@@ -19486,7 +20013,7 @@
         <v>2475</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>185</v>
       </c>
@@ -19537,7 +20064,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>186</v>
       </c>
@@ -19588,7 +20115,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>187</v>
       </c>
@@ -19639,7 +20166,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>188</v>
       </c>
@@ -19690,7 +20217,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>279</v>
       </c>
@@ -19741,7 +20268,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>281</v>
       </c>
@@ -19792,7 +20319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>292</v>
       </c>
@@ -19843,7 +20370,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>296</v>
       </c>
@@ -19903,7 +20430,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>299</v>
       </c>
@@ -19961,7 +20488,7 @@
       </c>
       <c r="Z49" s="8"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>301</v>
       </c>
@@ -20019,7 +20546,7 @@
       </c>
       <c r="Z50" s="8"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>303</v>
       </c>
@@ -20077,7 +20604,7 @@
       </c>
       <c r="Z51" s="8"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>305</v>
       </c>
@@ -20135,7 +20662,7 @@
       </c>
       <c r="Z52" s="8"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>307</v>
       </c>
@@ -20193,7 +20720,7 @@
       </c>
       <c r="Z53" s="8"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>310</v>
       </c>
@@ -20251,7 +20778,7 @@
       </c>
       <c r="Z54" s="8"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>312</v>
       </c>
@@ -20309,7 +20836,7 @@
       </c>
       <c r="Z55" s="8"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>314</v>
       </c>
@@ -20367,7 +20894,7 @@
       </c>
       <c r="Z56" s="8"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>316</v>
       </c>
@@ -20425,7 +20952,7 @@
       </c>
       <c r="Z57" s="8"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>345</v>
       </c>
@@ -20482,7 +21009,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>346</v>
       </c>
@@ -20539,7 +21066,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>370</v>
       </c>
@@ -20596,7 +21123,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>371</v>
       </c>
@@ -20653,7 +21180,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>375</v>
       </c>
@@ -20710,7 +21237,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>379</v>
       </c>
@@ -20767,7 +21294,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>380</v>
       </c>
@@ -20824,7 +21351,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>382</v>
       </c>
@@ -20881,7 +21408,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>384</v>
       </c>
@@ -20938,7 +21465,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>388</v>
       </c>
@@ -20995,7 +21522,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>391</v>
       </c>
@@ -21052,7 +21579,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>386</v>
       </c>
@@ -21109,7 +21636,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="70" spans="1:26" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>432</v>
       </c>
@@ -21160,7 +21687,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="71" spans="1:26" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>433</v>
       </c>
@@ -21211,7 +21738,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="72" spans="1:26" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>428</v>
       </c>
@@ -21262,7 +21789,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="73" spans="1:26" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>430</v>
       </c>
@@ -21313,7 +21840,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="74" spans="1:26" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:26" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>431</v>
       </c>
@@ -21364,7 +21891,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>435</v>
       </c>

</xml_diff>

<commit_message>
240417 add NC3 (#48)
* add nc3
</commit_message>
<xml_diff>
--- a/docs/China Set Trains.xlsx
+++ b/docs/China Set Trains.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CNS\CNST\local\China-Set-Trains\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A855C7DA-9F59-43A0-8CAC-9F6AF81DB2D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5299978-2C04-4BFF-816B-C70286864F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1594" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1598" uniqueCount="512">
   <si>
     <t>name</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1974,6 +1974,10 @@
   </si>
   <si>
     <t>CR300AF</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NC3</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2356,8 +2360,8 @@
   <dimension ref="A1:AD67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC46" sqref="AC46:AC47"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -7112,11 +7116,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB4625FC-685F-4E56-AE60-F05D51350408}">
-  <dimension ref="A1:AG256"/>
+  <dimension ref="A1:AG258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A230" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X235" sqref="X235"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A239" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X257" sqref="X257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -21021,7 +21025,7 @@
         <v>1830</v>
       </c>
       <c r="L236">
-        <f t="shared" ref="L236:L245" si="93">ROUND(M236/0.73549875,0)</f>
+        <f t="shared" ref="L236:L240" si="93">ROUND(M236/0.73549875,0)</f>
         <v>1856</v>
       </c>
       <c r="M236">
@@ -21650,11 +21654,11 @@
         <v>250</v>
       </c>
       <c r="K246">
-        <f>ROUND(M246/0.745699872,0)</f>
+        <f t="shared" ref="K246:K258" si="95">ROUND(M246/0.745699872,0)</f>
         <v>1830</v>
       </c>
       <c r="L246">
-        <f>ROUND(M246/0.73549875,0)</f>
+        <f t="shared" ref="L246:L258" si="96">ROUND(M246/0.73549875,0)</f>
         <v>1856</v>
       </c>
       <c r="M246">
@@ -21676,23 +21680,23 @@
         <v>0.13500000000000001</v>
       </c>
       <c r="W246">
-        <f>U246*V246*9.8</f>
+        <f t="shared" ref="W246:W258" si="97">U246*V246*9.8</f>
         <v>71.442000000000007</v>
       </c>
       <c r="X246">
-        <f>MAX(1, INT(U246/10+SQRT(J246)/20+SQRT(L246)+V246+SQRT(R246)/2+SQRT(T246)-SQRT(185)+20-I246))</f>
+        <f t="shared" ref="X246:X258" si="98">MAX(1, INT(U246/10+SQRT(J246)/20+SQRT(L246)+V246+SQRT(R246)/2+SQRT(T246)-SQRT(185)+20-I246))</f>
         <v>73</v>
       </c>
       <c r="Y246">
-        <f>X246*50000/16</f>
+        <f t="shared" ref="Y246:Y258" si="99">X246*50000/16</f>
         <v>228125</v>
       </c>
       <c r="Z246">
-        <f>MAX(1, ROUND((SQRT(J246)/100+SQRT(L246)+V246+(40/I246-2)+SQRT(R246)/2+SQRT(T246)-SQRT(185)), 0))</f>
+        <f t="shared" ref="Z246:Z258" si="100">MAX(1, ROUND((SQRT(J246)/100+SQRT(L246)+V246+(40/I246-2)+SQRT(R246)/2+SQRT(T246)-SQRT(185)), 0))</f>
         <v>59</v>
       </c>
       <c r="AA246">
-        <f>Z246*300/16</f>
+        <f t="shared" ref="AA246:AA258" si="101">Z246*300/16</f>
         <v>1106.25</v>
       </c>
       <c r="AF246" t="s">
@@ -21713,11 +21717,11 @@
         <v>250</v>
       </c>
       <c r="K247">
-        <f>ROUND(M247/0.745699872,0)</f>
+        <f t="shared" si="95"/>
         <v>1830</v>
       </c>
       <c r="L247">
-        <f>ROUND(M247/0.73549875,0)</f>
+        <f t="shared" si="96"/>
         <v>1856</v>
       </c>
       <c r="M247">
@@ -21739,23 +21743,23 @@
         <v>0.13500000000000001</v>
       </c>
       <c r="W247">
-        <f>U247*V247*9.8</f>
+        <f t="shared" si="97"/>
         <v>71.442000000000007</v>
       </c>
       <c r="X247">
-        <f>MAX(1, INT(U247/10+SQRT(J247)/20+SQRT(L247)+V247+SQRT(R247)/2+SQRT(T247)-SQRT(185)+20-I247))</f>
+        <f t="shared" si="98"/>
         <v>71</v>
       </c>
       <c r="Y247">
-        <f>X247*50000/16</f>
+        <f t="shared" si="99"/>
         <v>221875</v>
       </c>
       <c r="Z247">
-        <f>MAX(1, ROUND((SQRT(J247)/100+SQRT(L247)+V247+(40/I247-2)+SQRT(R247)/2+SQRT(T247)-SQRT(185)), 0))</f>
+        <f t="shared" si="100"/>
         <v>56</v>
       </c>
       <c r="AA247">
-        <f>Z247*300/16</f>
+        <f t="shared" si="101"/>
         <v>1050</v>
       </c>
       <c r="AF247" t="s">
@@ -21776,11 +21780,11 @@
         <v>250</v>
       </c>
       <c r="K248">
-        <f>ROUND(M248/0.745699872,0)</f>
+        <f t="shared" si="95"/>
         <v>1830</v>
       </c>
       <c r="L248">
-        <f>ROUND(M248/0.73549875,0)</f>
+        <f t="shared" si="96"/>
         <v>1856</v>
       </c>
       <c r="M248">
@@ -21802,23 +21806,23 @@
         <v>0.13500000000000001</v>
       </c>
       <c r="W248">
-        <f>U248*V248*9.8</f>
+        <f t="shared" si="97"/>
         <v>71.442000000000007</v>
       </c>
       <c r="X248">
-        <f>MAX(1, INT(U248/10+SQRT(J248)/20+SQRT(L248)+V248+SQRT(R248)/2+SQRT(T248)-SQRT(185)+20-I248))</f>
+        <f t="shared" si="98"/>
         <v>74</v>
       </c>
       <c r="Y248">
-        <f>X248*50000/16</f>
+        <f t="shared" si="99"/>
         <v>231250</v>
       </c>
       <c r="Z248">
-        <f>MAX(1, ROUND((SQRT(J248)/100+SQRT(L248)+V248+(40/I248-2)+SQRT(R248)/2+SQRT(T248)-SQRT(185)), 0))</f>
+        <f t="shared" si="100"/>
         <v>60</v>
       </c>
       <c r="AA248">
-        <f>Z248*300/16</f>
+        <f t="shared" si="101"/>
         <v>1125</v>
       </c>
       <c r="AF248" t="s">
@@ -21839,11 +21843,11 @@
         <v>250</v>
       </c>
       <c r="K249">
-        <f>ROUND(M249/0.745699872,0)</f>
+        <f t="shared" si="95"/>
         <v>1830</v>
       </c>
       <c r="L249">
-        <f>ROUND(M249/0.73549875,0)</f>
+        <f t="shared" si="96"/>
         <v>1856</v>
       </c>
       <c r="M249">
@@ -21865,23 +21869,23 @@
         <v>0.13500000000000001</v>
       </c>
       <c r="W249">
-        <f>U249*V249*9.8</f>
+        <f t="shared" si="97"/>
         <v>71.442000000000007</v>
       </c>
       <c r="X249">
-        <f>MAX(1, INT(U249/10+SQRT(J249)/20+SQRT(L249)+V249+SQRT(R249)/2+SQRT(T249)-SQRT(185)+20-I249))</f>
+        <f t="shared" si="98"/>
         <v>79</v>
       </c>
       <c r="Y249">
-        <f>X249*50000/16</f>
+        <f t="shared" si="99"/>
         <v>246875</v>
       </c>
       <c r="Z249">
-        <f>MAX(1, ROUND((SQRT(J249)/100+SQRT(L249)+V249+(40/I249-2)+SQRT(R249)/2+SQRT(T249)-SQRT(185)), 0))</f>
+        <f t="shared" si="100"/>
         <v>64</v>
       </c>
       <c r="AA249">
-        <f>Z249*300/16</f>
+        <f t="shared" si="101"/>
         <v>1200</v>
       </c>
       <c r="AF249" t="s">
@@ -21902,11 +21906,11 @@
         <v>250</v>
       </c>
       <c r="K250">
-        <f>ROUND(M250/0.745699872,0)</f>
+        <f t="shared" si="95"/>
         <v>1830</v>
       </c>
       <c r="L250">
-        <f>ROUND(M250/0.73549875,0)</f>
+        <f t="shared" si="96"/>
         <v>1856</v>
       </c>
       <c r="M250">
@@ -21928,23 +21932,23 @@
         <v>0.13500000000000001</v>
       </c>
       <c r="W250">
-        <f>U250*V250*9.8</f>
+        <f t="shared" si="97"/>
         <v>71.442000000000007</v>
       </c>
       <c r="X250">
-        <f>MAX(1, INT(U250/10+SQRT(J250)/20+SQRT(L250)+V250+SQRT(R250)/2+SQRT(T250)-SQRT(185)+20-I250))</f>
+        <f t="shared" si="98"/>
         <v>80</v>
       </c>
       <c r="Y250">
-        <f>X250*50000/16</f>
+        <f t="shared" si="99"/>
         <v>250000</v>
       </c>
       <c r="Z250">
-        <f>MAX(1, ROUND((SQRT(J250)/100+SQRT(L250)+V250+(40/I250-2)+SQRT(R250)/2+SQRT(T250)-SQRT(185)), 0))</f>
+        <f t="shared" si="100"/>
         <v>65</v>
       </c>
       <c r="AA250">
-        <f>Z250*300/16</f>
+        <f t="shared" si="101"/>
         <v>1218.75</v>
       </c>
       <c r="AF250" t="s">
@@ -21965,11 +21969,11 @@
         <v>250</v>
       </c>
       <c r="K251">
-        <f>ROUND(M251/0.745699872,0)</f>
+        <f t="shared" si="95"/>
         <v>1830</v>
       </c>
       <c r="L251">
-        <f>ROUND(M251/0.73549875,0)</f>
+        <f t="shared" si="96"/>
         <v>1856</v>
       </c>
       <c r="M251">
@@ -21991,23 +21995,23 @@
         <v>0.13500000000000001</v>
       </c>
       <c r="W251">
-        <f>U251*V251*9.8</f>
+        <f t="shared" si="97"/>
         <v>71.442000000000007</v>
       </c>
       <c r="X251">
-        <f>MAX(1, INT(U251/10+SQRT(J251)/20+SQRT(L251)+V251+SQRT(R251)/2+SQRT(T251)-SQRT(185)+20-I251))</f>
+        <f t="shared" si="98"/>
         <v>70</v>
       </c>
       <c r="Y251">
-        <f>X251*50000/16</f>
+        <f t="shared" si="99"/>
         <v>218750</v>
       </c>
       <c r="Z251">
-        <f>MAX(1, ROUND((SQRT(J251)/100+SQRT(L251)+V251+(40/I251-2)+SQRT(R251)/2+SQRT(T251)-SQRT(185)), 0))</f>
+        <f t="shared" si="100"/>
         <v>55</v>
       </c>
       <c r="AA251">
-        <f>Z251*300/16</f>
+        <f t="shared" si="101"/>
         <v>1031.25</v>
       </c>
       <c r="AF251" t="s">
@@ -22031,11 +22035,11 @@
         <v>250</v>
       </c>
       <c r="K252">
-        <f>ROUND(M252/0.745699872,0)</f>
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
       <c r="L252">
-        <f>ROUND(M252/0.73549875,0)</f>
+        <f t="shared" si="96"/>
         <v>0</v>
       </c>
       <c r="M252">
@@ -22057,23 +22061,23 @@
         <v>0</v>
       </c>
       <c r="W252">
-        <f>U252*V252*9.8</f>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="X252">
-        <f>MAX(1, INT(U252/10+SQRT(J252)/20+SQRT(L252)+V252+SQRT(R252)/2+SQRT(T252)-SQRT(185)+20-I252))</f>
+        <f t="shared" si="98"/>
         <v>27</v>
       </c>
       <c r="Y252">
-        <f>X252*50000/16</f>
+        <f t="shared" si="99"/>
         <v>84375</v>
       </c>
       <c r="Z252">
-        <f>MAX(1, ROUND((SQRT(J252)/100+SQRT(L252)+V252+(40/I252-2)+SQRT(R252)/2+SQRT(T252)-SQRT(185)), 0))</f>
+        <f t="shared" si="100"/>
         <v>13</v>
       </c>
       <c r="AA252">
-        <f>Z252*300/16</f>
+        <f t="shared" si="101"/>
         <v>243.75</v>
       </c>
       <c r="AF252" t="s">
@@ -22094,11 +22098,11 @@
         <v>250</v>
       </c>
       <c r="K253">
-        <f>ROUND(M253/0.745699872,0)</f>
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
       <c r="L253">
-        <f>ROUND(M253/0.73549875,0)</f>
+        <f t="shared" si="96"/>
         <v>0</v>
       </c>
       <c r="M253">
@@ -22120,23 +22124,23 @@
         <v>0</v>
       </c>
       <c r="W253">
-        <f>U253*V253*9.8</f>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="X253">
-        <f>MAX(1, INT(U253/10+SQRT(J253)/20+SQRT(L253)+V253+SQRT(R253)/2+SQRT(T253)-SQRT(185)+20-I253))</f>
+        <f t="shared" si="98"/>
         <v>31</v>
       </c>
       <c r="Y253">
-        <f>X253*50000/16</f>
+        <f t="shared" si="99"/>
         <v>96875</v>
       </c>
       <c r="Z253">
-        <f>MAX(1, ROUND((SQRT(J253)/100+SQRT(L253)+V253+(40/I253-2)+SQRT(R253)/2+SQRT(T253)-SQRT(185)), 0))</f>
+        <f t="shared" si="100"/>
         <v>16</v>
       </c>
       <c r="AA253">
-        <f>Z253*300/16</f>
+        <f t="shared" si="101"/>
         <v>300</v>
       </c>
       <c r="AF253" t="s">
@@ -22157,11 +22161,11 @@
         <v>250</v>
       </c>
       <c r="K254">
-        <f>ROUND(M254/0.745699872,0)</f>
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
       <c r="L254">
-        <f>ROUND(M254/0.73549875,0)</f>
+        <f t="shared" si="96"/>
         <v>0</v>
       </c>
       <c r="M254">
@@ -22183,23 +22187,23 @@
         <v>0</v>
       </c>
       <c r="W254">
-        <f>U254*V254*9.8</f>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="X254">
-        <f>MAX(1, INT(U254/10+SQRT(J254)/20+SQRT(L254)+V254+SQRT(R254)/2+SQRT(T254)-SQRT(185)+20-I254))</f>
+        <f t="shared" si="98"/>
         <v>35</v>
       </c>
       <c r="Y254">
-        <f>X254*50000/16</f>
+        <f t="shared" si="99"/>
         <v>109375</v>
       </c>
       <c r="Z254">
-        <f>MAX(1, ROUND((SQRT(J254)/100+SQRT(L254)+V254+(40/I254-2)+SQRT(R254)/2+SQRT(T254)-SQRT(185)), 0))</f>
+        <f t="shared" si="100"/>
         <v>21</v>
       </c>
       <c r="AA254">
-        <f>Z254*300/16</f>
+        <f t="shared" si="101"/>
         <v>393.75</v>
       </c>
       <c r="AF254" t="s">
@@ -22220,11 +22224,11 @@
         <v>250</v>
       </c>
       <c r="K255">
-        <f>ROUND(M255/0.745699872,0)</f>
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
       <c r="L255">
-        <f>ROUND(M255/0.73549875,0)</f>
+        <f t="shared" si="96"/>
         <v>0</v>
       </c>
       <c r="M255">
@@ -22246,23 +22250,23 @@
         <v>0</v>
       </c>
       <c r="W255">
-        <f>U255*V255*9.8</f>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="X255">
-        <f>MAX(1, INT(U255/10+SQRT(J255)/20+SQRT(L255)+V255+SQRT(R255)/2+SQRT(T255)-SQRT(185)+20-I255))</f>
+        <f t="shared" si="98"/>
         <v>36</v>
       </c>
       <c r="Y255">
-        <f>X255*50000/16</f>
+        <f t="shared" si="99"/>
         <v>112500</v>
       </c>
       <c r="Z255">
-        <f>MAX(1, ROUND((SQRT(J255)/100+SQRT(L255)+V255+(40/I255-2)+SQRT(R255)/2+SQRT(T255)-SQRT(185)), 0))</f>
+        <f t="shared" si="100"/>
         <v>22</v>
       </c>
       <c r="AA255">
-        <f>Z255*300/16</f>
+        <f t="shared" si="101"/>
         <v>412.5</v>
       </c>
       <c r="AF255" t="s">
@@ -22283,11 +22287,11 @@
         <v>250</v>
       </c>
       <c r="K256">
-        <f>ROUND(M256/0.745699872,0)</f>
+        <f t="shared" si="95"/>
         <v>0</v>
       </c>
       <c r="L256">
-        <f>ROUND(M256/0.73549875,0)</f>
+        <f t="shared" si="96"/>
         <v>0</v>
       </c>
       <c r="M256">
@@ -22309,23 +22313,23 @@
         <v>0</v>
       </c>
       <c r="W256">
-        <f>U256*V256*9.8</f>
+        <f t="shared" si="97"/>
         <v>0</v>
       </c>
       <c r="X256">
-        <f>MAX(1, INT(U256/10+SQRT(J256)/20+SQRT(L256)+V256+SQRT(R256)/2+SQRT(T256)-SQRT(185)+20-I256))</f>
+        <f t="shared" si="98"/>
         <v>27</v>
       </c>
       <c r="Y256">
-        <f>X256*50000/16</f>
+        <f t="shared" si="99"/>
         <v>84375</v>
       </c>
       <c r="Z256">
-        <f>MAX(1, ROUND((SQRT(J256)/100+SQRT(L256)+V256+(40/I256-2)+SQRT(R256)/2+SQRT(T256)-SQRT(185)), 0))</f>
+        <f t="shared" si="100"/>
         <v>12</v>
       </c>
       <c r="AA256">
-        <f>Z256*300/16</f>
+        <f t="shared" si="101"/>
         <v>225</v>
       </c>
       <c r="AF256" t="s">
@@ -22333,6 +22337,120 @@
       </c>
       <c r="AG256" t="s">
         <v>422</v>
+      </c>
+    </row>
+    <row r="257" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A257" t="s">
+        <v>511</v>
+      </c>
+      <c r="I257">
+        <v>16</v>
+      </c>
+      <c r="J257">
+        <v>128</v>
+      </c>
+      <c r="K257">
+        <f t="shared" si="95"/>
+        <v>493</v>
+      </c>
+      <c r="L257">
+        <f t="shared" si="96"/>
+        <v>500</v>
+      </c>
+      <c r="M257">
+        <v>368</v>
+      </c>
+      <c r="N257" t="s">
+        <v>88</v>
+      </c>
+      <c r="R257">
+        <v>78</v>
+      </c>
+      <c r="T257">
+        <v>185</v>
+      </c>
+      <c r="U257">
+        <v>58</v>
+      </c>
+      <c r="V257">
+        <v>9.4E-2</v>
+      </c>
+      <c r="W257">
+        <f t="shared" si="97"/>
+        <v>53.429600000000001</v>
+      </c>
+      <c r="X257">
+        <f t="shared" si="98"/>
+        <v>37</v>
+      </c>
+      <c r="Y257">
+        <f t="shared" si="99"/>
+        <v>115625</v>
+      </c>
+      <c r="Z257">
+        <f t="shared" si="100"/>
+        <v>27</v>
+      </c>
+      <c r="AA257">
+        <f t="shared" si="101"/>
+        <v>506.25</v>
+      </c>
+    </row>
+    <row r="258" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="B258" t="s">
+        <v>128</v>
+      </c>
+      <c r="I258">
+        <v>16</v>
+      </c>
+      <c r="J258">
+        <v>128</v>
+      </c>
+      <c r="K258">
+        <f t="shared" si="95"/>
+        <v>493</v>
+      </c>
+      <c r="L258">
+        <f t="shared" si="96"/>
+        <v>500</v>
+      </c>
+      <c r="M258">
+        <v>368</v>
+      </c>
+      <c r="N258" t="s">
+        <v>88</v>
+      </c>
+      <c r="R258">
+        <v>118</v>
+      </c>
+      <c r="T258">
+        <v>185</v>
+      </c>
+      <c r="U258">
+        <v>45</v>
+      </c>
+      <c r="V258">
+        <v>0</v>
+      </c>
+      <c r="W258">
+        <f t="shared" si="97"/>
+        <v>0</v>
+      </c>
+      <c r="X258">
+        <f t="shared" si="98"/>
+        <v>36</v>
+      </c>
+      <c r="Y258">
+        <f t="shared" si="99"/>
+        <v>112500</v>
+      </c>
+      <c r="Z258">
+        <f t="shared" si="100"/>
+        <v>28</v>
+      </c>
+      <c r="AA258">
+        <f t="shared" si="101"/>
+        <v>525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
renewl 25t add p80
</commit_message>
<xml_diff>
--- a/docs/China Set Trains.xlsx
+++ b/docs/China Set Trains.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CNS\CNST\local\China-Set-Trains\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5299978-2C04-4BFF-816B-C70286864F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE99AB7-9D29-4075-96EC-3EA8D7719553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Loco" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1598" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1604" uniqueCount="511">
   <si>
     <t>name</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1411,10 +1411,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>alternative livery:DF4D3110</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>DF4B3110</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -1815,9 +1811,6 @@
   </si>
   <si>
     <t>P61</t>
-  </si>
-  <si>
-    <t>损局</t>
   </si>
   <si>
     <t>P63</t>
@@ -1978,6 +1971,10 @@
   </si>
   <si>
     <t>NC3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>P80</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2359,9 +2356,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R22" sqref="R22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A37" sqref="A37:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3026,7 +3023,7 @@
         <v>0</v>
       </c>
       <c r="AC10" t="s">
-        <v>360</v>
+        <v>420</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.3">
@@ -3090,6 +3087,9 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
+      <c r="AC11" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -3153,7 +3153,7 @@
         <v>0</v>
       </c>
       <c r="AC12" t="s">
-        <v>360</v>
+        <v>420</v>
       </c>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.3">
@@ -3265,6 +3265,9 @@
         <f t="shared" ref="T14" si="12">U14+V14+W14</f>
         <v>0</v>
       </c>
+      <c r="AC14" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -3379,6 +3382,9 @@
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="AC16" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -3616,7 +3622,7 @@
         <v>90</v>
       </c>
       <c r="AC20" t="s">
-        <v>91</v>
+        <v>340</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.3">
@@ -4482,6 +4488,9 @@
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
+      <c r="AC32" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="33" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
@@ -4642,10 +4651,10 @@
         <v>#DIV/0!</v>
       </c>
       <c r="AB34" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AC34" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="35" spans="1:30" x14ac:dyDescent="0.3">
@@ -5849,10 +5858,10 @@
     </row>
     <row r="50" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>390</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>391</v>
       </c>
       <c r="E50" t="s">
         <v>256</v>
@@ -5925,7 +5934,7 @@
     </row>
     <row r="51" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E51" t="s">
         <v>51</v>
@@ -5990,7 +5999,7 @@
         <v>2</v>
       </c>
       <c r="AB51" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AC51" t="s">
         <v>340</v>
@@ -5998,7 +6007,7 @@
     </row>
     <row r="52" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E52" t="s">
         <v>256</v>
@@ -6063,7 +6072,7 @@
         <v>2</v>
       </c>
       <c r="AB52" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AC52" t="s">
         <v>339</v>
@@ -6071,13 +6080,13 @@
     </row>
     <row r="53" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>432</v>
+      </c>
+      <c r="B53" t="s">
         <v>433</v>
       </c>
-      <c r="B53" t="s">
-        <v>434</v>
-      </c>
       <c r="D53" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E53" t="s">
         <v>318</v>
@@ -6123,7 +6132,7 @@
         <v>24375</v>
       </c>
       <c r="T53" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="U53">
         <v>2</v>
@@ -6138,18 +6147,18 @@
         <v>258</v>
       </c>
       <c r="AC53" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="54" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
+        <v>436</v>
+      </c>
+      <c r="B54" t="s">
         <v>437</v>
       </c>
-      <c r="B54" t="s">
-        <v>438</v>
-      </c>
       <c r="D54" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E54" t="s">
         <v>318</v>
@@ -6201,15 +6210,15 @@
         <v>258</v>
       </c>
       <c r="AC54" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="55" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
+        <v>438</v>
+      </c>
+      <c r="B55" t="s">
         <v>439</v>
-      </c>
-      <c r="B55" t="s">
-        <v>440</v>
       </c>
       <c r="F55">
         <v>2012</v>
@@ -6263,13 +6272,13 @@
     </row>
     <row r="56" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>440</v>
+      </c>
+      <c r="B56" t="s">
         <v>441</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
         <v>442</v>
-      </c>
-      <c r="C56" t="s">
-        <v>443</v>
       </c>
       <c r="E56" t="s">
         <v>256</v>
@@ -6315,7 +6324,7 @@
         <v>26550</v>
       </c>
       <c r="T56" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="AB56" s="2" t="s">
         <v>258</v>
@@ -6323,10 +6332,10 @@
     </row>
     <row r="57" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>444</v>
+      </c>
+      <c r="B57" t="s">
         <v>445</v>
-      </c>
-      <c r="B57" t="s">
-        <v>446</v>
       </c>
       <c r="E57" t="s">
         <v>318</v>
@@ -6375,7 +6384,7 @@
         <v>18281.25</v>
       </c>
       <c r="T57" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="AB57" s="2" t="s">
         <v>258</v>
@@ -6386,10 +6395,10 @@
     </row>
     <row r="58" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
+        <v>446</v>
+      </c>
+      <c r="B58" t="s">
         <v>447</v>
-      </c>
-      <c r="B58" t="s">
-        <v>448</v>
       </c>
       <c r="E58" t="s">
         <v>256</v>
@@ -6449,13 +6458,13 @@
     </row>
     <row r="59" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
+        <v>448</v>
+      </c>
+      <c r="B59" t="s">
         <v>449</v>
       </c>
-      <c r="B59" t="s">
+      <c r="D59" t="s">
         <v>450</v>
-      </c>
-      <c r="D59" t="s">
-        <v>451</v>
       </c>
       <c r="E59" t="s">
         <v>318</v>
@@ -6531,21 +6540,21 @@
         <v>258</v>
       </c>
       <c r="AC59" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="60" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="s">
+        <v>452</v>
+      </c>
+      <c r="B60" s="7" t="s">
         <v>453</v>
       </c>
-      <c r="B60" s="7" t="s">
-        <v>454</v>
-      </c>
       <c r="D60" s="7" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F60" s="8">
         <v>1960</v>
@@ -6590,18 +6599,18 @@
         <v>10237.5</v>
       </c>
       <c r="AB60" s="2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="61" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
+        <v>454</v>
+      </c>
+      <c r="B61" s="7" t="s">
         <v>455</v>
       </c>
-      <c r="B61" s="7" t="s">
-        <v>456</v>
-      </c>
       <c r="D61" s="7" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E61" s="7" t="s">
         <v>256</v>
@@ -6670,13 +6679,13 @@
     </row>
     <row r="62" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A62" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="B62" s="7" t="s">
         <v>457</v>
       </c>
-      <c r="B62" s="7" t="s">
-        <v>458</v>
-      </c>
       <c r="D62" s="7" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E62" s="7" t="s">
         <v>256</v>
@@ -6745,13 +6754,13 @@
     </row>
     <row r="63" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="s">
+        <v>458</v>
+      </c>
+      <c r="B63" s="7" t="s">
         <v>459</v>
       </c>
-      <c r="B63" s="7" t="s">
-        <v>460</v>
-      </c>
       <c r="D63" s="7" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E63" s="7" t="s">
         <v>256</v>
@@ -6820,13 +6829,13 @@
     </row>
     <row r="64" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A64" s="7" t="s">
+        <v>460</v>
+      </c>
+      <c r="B64" s="7" t="s">
         <v>461</v>
       </c>
-      <c r="B64" s="7" t="s">
-        <v>462</v>
-      </c>
       <c r="D64" s="7" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E64" s="7" t="s">
         <v>318</v>
@@ -6890,18 +6899,18 @@
         <v>339</v>
       </c>
       <c r="AC64" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="65" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A65" s="7" t="s">
+        <v>462</v>
+      </c>
+      <c r="B65" s="7" t="s">
         <v>463</v>
       </c>
-      <c r="B65" s="7" t="s">
-        <v>464</v>
-      </c>
       <c r="D65" s="7" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E65" s="7" t="s">
         <v>318</v>
@@ -6965,15 +6974,15 @@
         <v>339</v>
       </c>
       <c r="AC65" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="66" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
@@ -7036,12 +7045,12 @@
         <v>339</v>
       </c>
       <c r="AC66" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="67" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
@@ -7105,7 +7114,7 @@
         <v>339</v>
       </c>
       <c r="AC67" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
   </sheetData>
@@ -7118,7 +7127,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB4625FC-685F-4E56-AE60-F05D51350408}">
   <dimension ref="A1:AG258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A239" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="X257" sqref="X257"/>
     </sheetView>
@@ -7162,7 +7171,7 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="L1" t="s">
         <v>242</v>
@@ -7303,10 +7312,10 @@
         <v>1650</v>
       </c>
       <c r="AF2" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.3">
@@ -7366,10 +7375,10 @@
         <v>2325</v>
       </c>
       <c r="AF3" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.3">
@@ -7429,10 +7438,10 @@
         <v>131.25</v>
       </c>
       <c r="AF4" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.3">
@@ -7492,10 +7501,10 @@
         <v>206.25</v>
       </c>
       <c r="AF5" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
@@ -7555,10 +7564,10 @@
         <v>281.25</v>
       </c>
       <c r="AF6" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.3">
@@ -7618,10 +7627,10 @@
         <v>300</v>
       </c>
       <c r="AF7" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG7" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.3">
@@ -7681,10 +7690,10 @@
         <v>93.75</v>
       </c>
       <c r="AF8" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG8" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.3">
@@ -7744,10 +7753,10 @@
         <v>225</v>
       </c>
       <c r="AF9" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG9" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.3">
@@ -7807,10 +7816,10 @@
         <v>281.25</v>
       </c>
       <c r="AF10" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG10" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.3">
@@ -7870,10 +7879,10 @@
         <v>318.75</v>
       </c>
       <c r="AF11" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG11" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.3">
@@ -8560,10 +8569,10 @@
         <v>937.5</v>
       </c>
       <c r="AF23" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG23" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.3">
@@ -8620,10 +8629,10 @@
         <v>956.25</v>
       </c>
       <c r="AF24" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG24" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.3">
@@ -8680,10 +8689,10 @@
         <v>1012.5</v>
       </c>
       <c r="AF25" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG25" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.3">
@@ -8740,10 +8749,10 @@
         <v>1106.25</v>
       </c>
       <c r="AF26" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG26" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.3">
@@ -8800,10 +8809,10 @@
         <v>1125</v>
       </c>
       <c r="AF27" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG27" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.3">
@@ -8860,10 +8869,10 @@
         <v>937.5</v>
       </c>
       <c r="AF28" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG28" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.3">
@@ -8920,10 +8929,10 @@
         <v>150</v>
       </c>
       <c r="AF29" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG29" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.3">
@@ -8980,10 +8989,10 @@
         <v>206.25</v>
       </c>
       <c r="AF30" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG30" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.3">
@@ -9040,10 +9049,10 @@
         <v>281.25</v>
       </c>
       <c r="AF31" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG31" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.3">
@@ -9100,10 +9109,10 @@
         <v>318.75</v>
       </c>
       <c r="AF32" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG32" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="33" spans="1:33" x14ac:dyDescent="0.3">
@@ -9160,10 +9169,10 @@
         <v>131.25</v>
       </c>
       <c r="AF33" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG33" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="34" spans="1:33" x14ac:dyDescent="0.3">
@@ -9220,10 +9229,10 @@
         <v>1668.75</v>
       </c>
       <c r="AF34" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG34" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="35" spans="1:33" x14ac:dyDescent="0.3">
@@ -9280,10 +9289,10 @@
         <v>150</v>
       </c>
       <c r="AF35" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG35" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="36" spans="1:33" x14ac:dyDescent="0.3">
@@ -9340,10 +9349,10 @@
         <v>225</v>
       </c>
       <c r="AF36" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG36" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="37" spans="1:33" x14ac:dyDescent="0.3">
@@ -9400,10 +9409,10 @@
         <v>300</v>
       </c>
       <c r="AF37" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG37" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="38" spans="1:33" x14ac:dyDescent="0.3">
@@ -9460,10 +9469,10 @@
         <v>318.75</v>
       </c>
       <c r="AF38" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG38" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="39" spans="1:33" x14ac:dyDescent="0.3">
@@ -9520,10 +9529,10 @@
         <v>150</v>
       </c>
       <c r="AF39" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG39" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="40" spans="1:33" x14ac:dyDescent="0.3">
@@ -12237,7 +12246,7 @@
     </row>
     <row r="90" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G90">
         <v>2009</v>
@@ -12348,7 +12357,7 @@
     </row>
     <row r="92" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I92">
         <v>8</v>
@@ -12368,7 +12377,7 @@
         <v>1060</v>
       </c>
       <c r="Q92" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="R92">
         <v>40</v>
@@ -12425,7 +12434,7 @@
         <v>1060</v>
       </c>
       <c r="Q93" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="R93">
         <v>16</v>
@@ -12482,7 +12491,7 @@
         <v>1060</v>
       </c>
       <c r="Q94" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="R94">
         <v>58</v>
@@ -12576,7 +12585,7 @@
     </row>
     <row r="96" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I96">
         <v>8</v>
@@ -12738,7 +12747,7 @@
     </row>
     <row r="99" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G99">
         <v>2014</v>
@@ -12793,10 +12802,10 @@
         <v>956.25</v>
       </c>
       <c r="AF99" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG99" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="100" spans="1:33" x14ac:dyDescent="0.3">
@@ -12856,10 +12865,10 @@
         <v>900</v>
       </c>
       <c r="AF100" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG100" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="101" spans="1:33" x14ac:dyDescent="0.3">
@@ -12916,10 +12925,10 @@
         <v>956.25</v>
       </c>
       <c r="AF101" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG101" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="102" spans="1:33" x14ac:dyDescent="0.3">
@@ -12944,7 +12953,7 @@
         <v>1140</v>
       </c>
       <c r="Q102" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="R102">
         <v>32</v>
@@ -12979,10 +12988,10 @@
         <v>1031.25</v>
       </c>
       <c r="AF102" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG102" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="103" spans="1:33" x14ac:dyDescent="0.3">
@@ -13007,7 +13016,7 @@
         <v>1140</v>
       </c>
       <c r="Q103" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="R103">
         <v>24</v>
@@ -13042,10 +13051,10 @@
         <v>1068.75</v>
       </c>
       <c r="AF103" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG103" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="104" spans="1:33" x14ac:dyDescent="0.3">
@@ -13070,7 +13079,7 @@
         <v>1140</v>
       </c>
       <c r="Q104" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="R104">
         <v>63</v>
@@ -13105,10 +13114,10 @@
         <v>881.25</v>
       </c>
       <c r="AF104" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG104" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="105" spans="1:33" x14ac:dyDescent="0.3">
@@ -13168,10 +13177,10 @@
         <v>150</v>
       </c>
       <c r="AF105" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG105" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="106" spans="1:33" x14ac:dyDescent="0.3">
@@ -13228,10 +13237,10 @@
         <v>225</v>
       </c>
       <c r="AF106" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG106" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="107" spans="1:33" x14ac:dyDescent="0.3">
@@ -13288,10 +13297,10 @@
         <v>300</v>
       </c>
       <c r="AF107" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG107" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="108" spans="1:33" x14ac:dyDescent="0.3">
@@ -13348,10 +13357,10 @@
         <v>318.75</v>
       </c>
       <c r="AF108" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG108" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="109" spans="1:33" x14ac:dyDescent="0.3">
@@ -13408,15 +13417,15 @@
         <v>131.25</v>
       </c>
       <c r="AF109" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="AG109" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="110" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G110">
         <v>2012</v>
@@ -13493,7 +13502,7 @@
         <v>2400</v>
       </c>
       <c r="Q111" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="R111">
         <v>80</v>
@@ -13604,7 +13613,7 @@
         <v>2400</v>
       </c>
       <c r="Q113" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="R113">
         <v>24</v>
@@ -13661,7 +13670,7 @@
         <v>2400</v>
       </c>
       <c r="Q114" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="R114">
         <v>18</v>
@@ -13718,7 +13727,7 @@
         <v>2400</v>
       </c>
       <c r="Q115" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="R115">
         <v>38</v>
@@ -14028,10 +14037,10 @@
     </row>
     <row r="121" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D121" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="I121">
         <v>8</v>
@@ -14304,10 +14313,10 @@
     </row>
     <row r="126" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D126" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I126">
         <v>8</v>
@@ -14472,13 +14481,13 @@
     </row>
     <row r="129" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B129" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D129" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="I129">
         <v>6</v>
@@ -14643,10 +14652,10 @@
     </row>
     <row r="132" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D132" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="I132">
         <v>6</v>
@@ -14811,7 +14820,7 @@
     </row>
     <row r="135" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="I135">
         <v>12</v>
@@ -14863,10 +14872,10 @@
         <v>1050</v>
       </c>
       <c r="AF135" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG135" t="s">
         <v>421</v>
-      </c>
-      <c r="AG135" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="136" spans="1:33" x14ac:dyDescent="0.3">
@@ -14923,10 +14932,10 @@
         <v>1012.5</v>
       </c>
       <c r="AF136" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG136" t="s">
         <v>421</v>
-      </c>
-      <c r="AG136" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="137" spans="1:33" x14ac:dyDescent="0.3">
@@ -14983,10 +14992,10 @@
         <v>1068.75</v>
       </c>
       <c r="AF137" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG137" t="s">
         <v>421</v>
-      </c>
-      <c r="AG137" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="138" spans="1:33" x14ac:dyDescent="0.3">
@@ -15043,10 +15052,10 @@
         <v>1143.75</v>
       </c>
       <c r="AF138" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG138" t="s">
         <v>421</v>
-      </c>
-      <c r="AG138" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="139" spans="1:33" x14ac:dyDescent="0.3">
@@ -15103,10 +15112,10 @@
         <v>1162.5</v>
       </c>
       <c r="AF139" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG139" t="s">
         <v>421</v>
-      </c>
-      <c r="AG139" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="140" spans="1:33" x14ac:dyDescent="0.3">
@@ -15163,10 +15172,10 @@
         <v>993.75</v>
       </c>
       <c r="AF140" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG140" t="s">
         <v>421</v>
-      </c>
-      <c r="AG140" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="141" spans="1:33" x14ac:dyDescent="0.3">
@@ -15226,10 +15235,10 @@
         <v>150</v>
       </c>
       <c r="AF141" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG141" t="s">
         <v>421</v>
-      </c>
-      <c r="AG141" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="142" spans="1:33" x14ac:dyDescent="0.3">
@@ -15286,10 +15295,10 @@
         <v>225</v>
       </c>
       <c r="AF142" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG142" t="s">
         <v>421</v>
-      </c>
-      <c r="AG142" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="143" spans="1:33" x14ac:dyDescent="0.3">
@@ -15346,10 +15355,10 @@
         <v>300</v>
       </c>
       <c r="AF143" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG143" t="s">
         <v>421</v>
-      </c>
-      <c r="AG143" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="144" spans="1:33" x14ac:dyDescent="0.3">
@@ -15406,10 +15415,10 @@
         <v>318.75</v>
       </c>
       <c r="AF144" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG144" t="s">
         <v>421</v>
-      </c>
-      <c r="AG144" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="145" spans="1:33" x14ac:dyDescent="0.3">
@@ -15466,15 +15475,15 @@
         <v>131.25</v>
       </c>
       <c r="AF145" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG145" t="s">
         <v>421</v>
-      </c>
-      <c r="AG145" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="146" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G146">
         <v>30</v>
@@ -15529,10 +15538,10 @@
         <v>1706.25</v>
       </c>
       <c r="AF146" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG146" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="147" spans="1:33" x14ac:dyDescent="0.3">
@@ -15589,10 +15598,10 @@
         <v>187.5</v>
       </c>
       <c r="AF147" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG147" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="148" spans="1:33" x14ac:dyDescent="0.3">
@@ -15649,10 +15658,10 @@
         <v>262.5</v>
       </c>
       <c r="AF148" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG148" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="149" spans="1:33" x14ac:dyDescent="0.3">
@@ -15709,10 +15718,10 @@
         <v>318.75</v>
       </c>
       <c r="AF149" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG149" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="150" spans="1:33" x14ac:dyDescent="0.3">
@@ -15769,10 +15778,10 @@
         <v>337.5</v>
       </c>
       <c r="AF150" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG150" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="151" spans="1:33" x14ac:dyDescent="0.3">
@@ -15829,10 +15838,10 @@
         <v>168.75</v>
       </c>
       <c r="AF151" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG151" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="152" spans="1:33" x14ac:dyDescent="0.3">
@@ -15892,10 +15901,10 @@
         <v>281.25</v>
       </c>
       <c r="AF152" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG152" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="153" spans="1:33" x14ac:dyDescent="0.3">
@@ -15955,10 +15964,10 @@
         <v>337.5</v>
       </c>
       <c r="AF153" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG153" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="154" spans="1:33" x14ac:dyDescent="0.3">
@@ -16018,15 +16027,15 @@
         <v>375</v>
       </c>
       <c r="AF154" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG154" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="155" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="I155">
         <v>16</v>
@@ -16188,7 +16197,7 @@
     </row>
     <row r="158" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="I158">
         <v>5</v>
@@ -16240,10 +16249,10 @@
         <v>1368.75</v>
       </c>
       <c r="AF158" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG158" t="s">
         <v>421</v>
-      </c>
-      <c r="AG158" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="159" spans="1:33" x14ac:dyDescent="0.3">
@@ -16300,10 +16309,10 @@
         <v>1312.5</v>
       </c>
       <c r="AF159" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG159" t="s">
         <v>421</v>
-      </c>
-      <c r="AG159" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="160" spans="1:33" x14ac:dyDescent="0.3">
@@ -16360,10 +16369,10 @@
         <v>1387.5</v>
       </c>
       <c r="AF160" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG160" t="s">
         <v>421</v>
-      </c>
-      <c r="AG160" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="161" spans="1:33" x14ac:dyDescent="0.3">
@@ -16420,10 +16429,10 @@
         <v>1462.5</v>
       </c>
       <c r="AF161" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG161" t="s">
         <v>421</v>
-      </c>
-      <c r="AG161" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="162" spans="1:33" x14ac:dyDescent="0.3">
@@ -16480,10 +16489,10 @@
         <v>1481.25</v>
       </c>
       <c r="AF162" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG162" t="s">
         <v>421</v>
-      </c>
-      <c r="AG162" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="163" spans="1:33" x14ac:dyDescent="0.3">
@@ -16540,10 +16549,10 @@
         <v>1293.75</v>
       </c>
       <c r="AF163" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG163" t="s">
         <v>421</v>
-      </c>
-      <c r="AG163" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="164" spans="1:33" x14ac:dyDescent="0.3">
@@ -16603,10 +16612,10 @@
         <v>243.75</v>
       </c>
       <c r="AF164" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG164" t="s">
         <v>421</v>
-      </c>
-      <c r="AG164" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="165" spans="1:33" x14ac:dyDescent="0.3">
@@ -16663,10 +16672,10 @@
         <v>300</v>
       </c>
       <c r="AF165" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG165" t="s">
         <v>421</v>
-      </c>
-      <c r="AG165" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="166" spans="1:33" x14ac:dyDescent="0.3">
@@ -16723,10 +16732,10 @@
         <v>393.75</v>
       </c>
       <c r="AF166" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG166" t="s">
         <v>421</v>
-      </c>
-      <c r="AG166" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="167" spans="1:33" x14ac:dyDescent="0.3">
@@ -16783,10 +16792,10 @@
         <v>393.75</v>
       </c>
       <c r="AF167" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG167" t="s">
         <v>421</v>
-      </c>
-      <c r="AG167" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="168" spans="1:33" x14ac:dyDescent="0.3">
@@ -16843,15 +16852,15 @@
         <v>225</v>
       </c>
       <c r="AF168" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG168" t="s">
         <v>421</v>
-      </c>
-      <c r="AG168" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="169" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="I169">
         <v>20</v>
@@ -16903,15 +16912,15 @@
         <v>862.5</v>
       </c>
       <c r="AF169" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG169" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="170" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="I170">
         <v>20</v>
@@ -16963,10 +16972,10 @@
         <v>843.75</v>
       </c>
       <c r="AF170" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG170" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="171" spans="1:33" x14ac:dyDescent="0.3">
@@ -17023,10 +17032,10 @@
         <v>881.25</v>
       </c>
       <c r="AF171" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG171" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="172" spans="1:33" x14ac:dyDescent="0.3">
@@ -17083,10 +17092,10 @@
         <v>937.5</v>
       </c>
       <c r="AF172" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG172" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="173" spans="1:33" x14ac:dyDescent="0.3">
@@ -17143,10 +17152,10 @@
         <v>1012.5</v>
       </c>
       <c r="AF173" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG173" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="174" spans="1:33" x14ac:dyDescent="0.3">
@@ -17203,10 +17212,10 @@
         <v>1031.25</v>
       </c>
       <c r="AF174" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG174" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="175" spans="1:33" x14ac:dyDescent="0.3">
@@ -17263,15 +17272,15 @@
         <v>843.75</v>
       </c>
       <c r="AF175" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG175" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="176" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B176" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I176">
         <v>20</v>
@@ -17323,10 +17332,10 @@
         <v>1012.5</v>
       </c>
       <c r="AF176" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG176" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="177" spans="1:33" x14ac:dyDescent="0.3">
@@ -17383,15 +17392,15 @@
         <v>1068.75</v>
       </c>
       <c r="AF177" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG177" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="178" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B178" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="I178">
         <v>20</v>
@@ -17443,15 +17452,15 @@
         <v>862.5</v>
       </c>
       <c r="AF178" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG178" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="179" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B179" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="I179">
         <v>20</v>
@@ -17503,15 +17512,15 @@
         <v>825</v>
       </c>
       <c r="AF179" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG179" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="180" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B180" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="I180">
         <v>20</v>
@@ -17563,15 +17572,15 @@
         <v>825</v>
       </c>
       <c r="AF180" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG180" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="181" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B181" t="s">
         <v>244</v>
@@ -17626,10 +17635,10 @@
         <v>131.25</v>
       </c>
       <c r="AF181" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG181" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="182" spans="1:33" x14ac:dyDescent="0.3">
@@ -17686,10 +17695,10 @@
         <v>206.25</v>
       </c>
       <c r="AF182" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG182" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="183" spans="1:33" x14ac:dyDescent="0.3">
@@ -17746,10 +17755,10 @@
         <v>281.25</v>
       </c>
       <c r="AF183" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG183" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="184" spans="1:33" x14ac:dyDescent="0.3">
@@ -17806,10 +17815,10 @@
         <v>300</v>
       </c>
       <c r="AF184" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG184" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="185" spans="1:33" x14ac:dyDescent="0.3">
@@ -17866,15 +17875,15 @@
         <v>112.5</v>
       </c>
       <c r="AF185" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG185" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="186" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B186" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I186">
         <v>20</v>
@@ -17926,10 +17935,10 @@
         <v>281.25</v>
       </c>
       <c r="AF186" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG186" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="187" spans="1:33" x14ac:dyDescent="0.3">
@@ -17986,15 +17995,15 @@
         <v>318.75</v>
       </c>
       <c r="AF187" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG187" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="188" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B188" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="I188">
         <v>20</v>
@@ -18046,15 +18055,15 @@
         <v>131.25</v>
       </c>
       <c r="AF188" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG188" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="189" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B189" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="I189">
         <v>20</v>
@@ -18106,15 +18115,15 @@
         <v>93.75</v>
       </c>
       <c r="AF189" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG189" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="190" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B190" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="I190">
         <v>20</v>
@@ -18166,15 +18175,15 @@
         <v>93.75</v>
       </c>
       <c r="AF190" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG190" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="191" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="I191">
         <v>12</v>
@@ -18226,10 +18235,10 @@
         <v>1068.75</v>
       </c>
       <c r="AF191" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG191" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="192" spans="1:33" x14ac:dyDescent="0.3">
@@ -18286,15 +18295,15 @@
         <v>1087.5</v>
       </c>
       <c r="AF192" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG192" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="193" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B193" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="I193">
         <v>12</v>
@@ -18346,15 +18355,15 @@
         <v>1050</v>
       </c>
       <c r="AF193" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG193" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="194" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B194" t="s">
         <v>134</v>
@@ -18409,10 +18418,10 @@
         <v>300</v>
       </c>
       <c r="AF194" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG194" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="195" spans="1:33" x14ac:dyDescent="0.3">
@@ -18469,15 +18478,15 @@
         <v>281.25</v>
       </c>
       <c r="AF195" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG195" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="196" spans="1:33" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" s="9" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="I196">
         <v>5</v>
@@ -18532,10 +18541,10 @@
         <v>1368.75</v>
       </c>
       <c r="AF196" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG196" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="197" spans="1:33" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -18595,10 +18604,10 @@
         <v>1331.25</v>
       </c>
       <c r="AF197" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG197" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="198" spans="1:33" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -18658,10 +18667,10 @@
         <v>1387.5</v>
       </c>
       <c r="AF198" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG198" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="199" spans="1:33" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -18721,10 +18730,10 @@
         <v>1481.25</v>
       </c>
       <c r="AF199" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG199" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="200" spans="1:33" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -18784,10 +18793,10 @@
         <v>1500</v>
       </c>
       <c r="AF200" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG200" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="201" spans="1:33" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -18847,15 +18856,15 @@
         <v>1312.5</v>
       </c>
       <c r="AF201" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG201" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="202" spans="1:33" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B202" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="I202">
         <v>5</v>
@@ -18910,10 +18919,10 @@
         <v>1293.75</v>
       </c>
       <c r="AF202" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG202" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="203" spans="1:33" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -18976,10 +18985,10 @@
         <v>243.75</v>
       </c>
       <c r="AF203" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG203" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="204" spans="1:33" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -19039,10 +19048,10 @@
         <v>300</v>
       </c>
       <c r="AF204" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG204" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="205" spans="1:33" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -19102,10 +19111,10 @@
         <v>393.75</v>
       </c>
       <c r="AF205" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG205" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="206" spans="1:33" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -19165,10 +19174,10 @@
         <v>412.5</v>
       </c>
       <c r="AF206" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG206" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="207" spans="1:33" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -19228,15 +19237,15 @@
         <v>225</v>
       </c>
       <c r="AF207" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG207" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="208" spans="1:33" ht="17" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B208" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="I208">
         <v>5</v>
@@ -19291,15 +19300,15 @@
         <v>225</v>
       </c>
       <c r="AF208" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG208" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="209" spans="1:33" ht="28" x14ac:dyDescent="0.3">
       <c r="A209" s="9" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="I209">
         <v>5</v>
@@ -19354,10 +19363,10 @@
         <v>1387.5</v>
       </c>
       <c r="AF209" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG209" t="s">
         <v>421</v>
-      </c>
-      <c r="AG209" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="210" spans="1:33" x14ac:dyDescent="0.3">
@@ -19417,10 +19426,10 @@
         <v>1350</v>
       </c>
       <c r="AF210" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG210" t="s">
         <v>421</v>
-      </c>
-      <c r="AG210" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="211" spans="1:33" x14ac:dyDescent="0.3">
@@ -19480,10 +19489,10 @@
         <v>1406.25</v>
       </c>
       <c r="AF211" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG211" t="s">
         <v>421</v>
-      </c>
-      <c r="AG211" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="212" spans="1:33" x14ac:dyDescent="0.3">
@@ -19543,10 +19552,10 @@
         <v>1500</v>
       </c>
       <c r="AF212" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG212" t="s">
         <v>421</v>
-      </c>
-      <c r="AG212" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="213" spans="1:33" x14ac:dyDescent="0.3">
@@ -19606,10 +19615,10 @@
         <v>1518.75</v>
       </c>
       <c r="AF213" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG213" t="s">
         <v>421</v>
-      </c>
-      <c r="AG213" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="214" spans="1:33" x14ac:dyDescent="0.3">
@@ -19669,15 +19678,15 @@
         <v>1331.25</v>
       </c>
       <c r="AF214" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG214" t="s">
         <v>421</v>
-      </c>
-      <c r="AG214" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="215" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B215" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="I215">
         <v>5</v>
@@ -19732,10 +19741,10 @@
         <v>1312.5</v>
       </c>
       <c r="AF215" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG215" t="s">
         <v>421</v>
-      </c>
-      <c r="AG215" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="216" spans="1:33" x14ac:dyDescent="0.3">
@@ -19798,10 +19807,10 @@
         <v>243.75</v>
       </c>
       <c r="AF216" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG216" t="s">
         <v>421</v>
-      </c>
-      <c r="AG216" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="217" spans="1:33" x14ac:dyDescent="0.3">
@@ -19861,10 +19870,10 @@
         <v>300</v>
       </c>
       <c r="AF217" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG217" t="s">
         <v>421</v>
-      </c>
-      <c r="AG217" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="218" spans="1:33" x14ac:dyDescent="0.3">
@@ -19924,10 +19933,10 @@
         <v>393.75</v>
       </c>
       <c r="AF218" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG218" t="s">
         <v>421</v>
-      </c>
-      <c r="AG218" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="219" spans="1:33" x14ac:dyDescent="0.3">
@@ -19987,10 +19996,10 @@
         <v>412.5</v>
       </c>
       <c r="AF219" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG219" t="s">
         <v>421</v>
-      </c>
-      <c r="AG219" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="220" spans="1:33" x14ac:dyDescent="0.3">
@@ -20050,15 +20059,15 @@
         <v>225</v>
       </c>
       <c r="AF220" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG220" t="s">
         <v>421</v>
-      </c>
-      <c r="AG220" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="221" spans="1:33" x14ac:dyDescent="0.3">
       <c r="B221" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="I221">
         <v>5</v>
@@ -20113,21 +20122,21 @@
         <v>225</v>
       </c>
       <c r="AF221" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG221" t="s">
         <v>421</v>
-      </c>
-      <c r="AG221" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="222" spans="1:33" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" s="9" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="G222" s="9" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="H222" s="9" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="I222">
         <v>3</v>
@@ -20182,10 +20191,10 @@
         <v>1612.5</v>
       </c>
       <c r="AF222" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG222" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="223" spans="1:33" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -20245,10 +20254,10 @@
         <v>1443.75</v>
       </c>
       <c r="AF223" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG223" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="224" spans="1:33" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -20308,10 +20317,10 @@
         <v>1518.75</v>
       </c>
       <c r="AF224" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG224" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="225" spans="1:33" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -20371,10 +20380,10 @@
         <v>1593.75</v>
       </c>
       <c r="AF225" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG225" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="226" spans="1:33" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -20434,10 +20443,10 @@
         <v>1612.5</v>
       </c>
       <c r="AF226" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG226" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="227" spans="1:33" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -20497,15 +20506,15 @@
         <v>1443.75</v>
       </c>
       <c r="AF227" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG227" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="228" spans="1:33" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B228" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="I228">
         <v>3</v>
@@ -20560,10 +20569,10 @@
         <v>1443.75</v>
       </c>
       <c r="AF228" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG228" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="229" spans="1:33" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -20626,10 +20635,10 @@
         <v>337.5</v>
       </c>
       <c r="AF229" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG229" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="230" spans="1:33" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -20689,10 +20698,10 @@
         <v>412.5</v>
       </c>
       <c r="AF230" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG230" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="231" spans="1:33" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -20752,10 +20761,10 @@
         <v>487.5</v>
       </c>
       <c r="AF231" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG231" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="232" spans="1:33" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -20815,10 +20824,10 @@
         <v>506.25</v>
       </c>
       <c r="AF232" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG232" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="233" spans="1:33" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -20878,15 +20887,15 @@
         <v>337.5</v>
       </c>
       <c r="AF233" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG233" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="234" spans="1:33" ht="17" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B234" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="I234">
         <v>3</v>
@@ -20941,15 +20950,15 @@
         <v>337.5</v>
       </c>
       <c r="AF234" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG234" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="235" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="I235">
         <v>5</v>
@@ -21004,10 +21013,10 @@
         <v>1106.25</v>
       </c>
       <c r="AF235" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG235" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="236" spans="1:33" x14ac:dyDescent="0.3">
@@ -21067,10 +21076,10 @@
         <v>1050</v>
       </c>
       <c r="AF236" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG236" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="237" spans="1:33" x14ac:dyDescent="0.3">
@@ -21130,10 +21139,10 @@
         <v>1125</v>
       </c>
       <c r="AF237" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG237" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="238" spans="1:33" x14ac:dyDescent="0.3">
@@ -21193,10 +21202,10 @@
         <v>1200</v>
       </c>
       <c r="AF238" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG238" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="239" spans="1:33" x14ac:dyDescent="0.3">
@@ -21256,10 +21265,10 @@
         <v>1218.75</v>
       </c>
       <c r="AF239" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG239" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="240" spans="1:33" x14ac:dyDescent="0.3">
@@ -21319,10 +21328,10 @@
         <v>1031.25</v>
       </c>
       <c r="AF240" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG240" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="241" spans="1:33" x14ac:dyDescent="0.3">
@@ -21385,10 +21394,10 @@
         <v>243.75</v>
       </c>
       <c r="AF241" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG241" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="242" spans="1:33" x14ac:dyDescent="0.3">
@@ -21448,10 +21457,10 @@
         <v>300</v>
       </c>
       <c r="AF242" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG242" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="243" spans="1:33" x14ac:dyDescent="0.3">
@@ -21511,10 +21520,10 @@
         <v>393.75</v>
       </c>
       <c r="AF243" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG243" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="244" spans="1:33" x14ac:dyDescent="0.3">
@@ -21574,10 +21583,10 @@
         <v>412.5</v>
       </c>
       <c r="AF244" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG244" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="245" spans="1:33" x14ac:dyDescent="0.3">
@@ -21637,15 +21646,15 @@
         <v>225</v>
       </c>
       <c r="AF245" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AG245" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="246" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="I246">
         <v>5</v>
@@ -21700,10 +21709,10 @@
         <v>1106.25</v>
       </c>
       <c r="AF246" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG246" t="s">
         <v>421</v>
-      </c>
-      <c r="AG246" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="247" spans="1:33" x14ac:dyDescent="0.3">
@@ -21763,10 +21772,10 @@
         <v>1050</v>
       </c>
       <c r="AF247" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG247" t="s">
         <v>421</v>
-      </c>
-      <c r="AG247" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="248" spans="1:33" x14ac:dyDescent="0.3">
@@ -21826,10 +21835,10 @@
         <v>1125</v>
       </c>
       <c r="AF248" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG248" t="s">
         <v>421</v>
-      </c>
-      <c r="AG248" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="249" spans="1:33" x14ac:dyDescent="0.3">
@@ -21889,10 +21898,10 @@
         <v>1200</v>
       </c>
       <c r="AF249" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG249" t="s">
         <v>421</v>
-      </c>
-      <c r="AG249" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="250" spans="1:33" x14ac:dyDescent="0.3">
@@ -21952,10 +21961,10 @@
         <v>1218.75</v>
       </c>
       <c r="AF250" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG250" t="s">
         <v>421</v>
-      </c>
-      <c r="AG250" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="251" spans="1:33" x14ac:dyDescent="0.3">
@@ -22015,10 +22024,10 @@
         <v>1031.25</v>
       </c>
       <c r="AF251" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG251" t="s">
         <v>421</v>
-      </c>
-      <c r="AG251" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="252" spans="1:33" x14ac:dyDescent="0.3">
@@ -22081,10 +22090,10 @@
         <v>243.75</v>
       </c>
       <c r="AF252" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG252" t="s">
         <v>421</v>
-      </c>
-      <c r="AG252" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="253" spans="1:33" x14ac:dyDescent="0.3">
@@ -22144,10 +22153,10 @@
         <v>300</v>
       </c>
       <c r="AF253" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG253" t="s">
         <v>421</v>
-      </c>
-      <c r="AG253" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="254" spans="1:33" x14ac:dyDescent="0.3">
@@ -22207,10 +22216,10 @@
         <v>393.75</v>
       </c>
       <c r="AF254" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG254" t="s">
         <v>421</v>
-      </c>
-      <c r="AG254" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="255" spans="1:33" x14ac:dyDescent="0.3">
@@ -22270,10 +22279,10 @@
         <v>412.5</v>
       </c>
       <c r="AF255" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG255" t="s">
         <v>421</v>
-      </c>
-      <c r="AG255" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="256" spans="1:33" x14ac:dyDescent="0.3">
@@ -22333,15 +22342,15 @@
         <v>225</v>
       </c>
       <c r="AF256" t="s">
+        <v>420</v>
+      </c>
+      <c r="AG256" t="s">
         <v>421</v>
-      </c>
-      <c r="AG256" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="257" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="I257">
         <v>16</v>
@@ -22462,10 +22471,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8540264-B3C1-4C71-9FC9-001ABF042657}">
-  <dimension ref="A1:AD25"/>
+  <dimension ref="A1:AD26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="U23" sqref="U23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -22600,11 +22609,11 @@
         <v>22.5</v>
       </c>
       <c r="U2">
-        <f t="shared" ref="U2:U17" si="0">MEDIAN(0,255,ROUND(S2/20+SQRT(J2)/40+SQRT(P2)/2+(SQRT(R2)-SQRT(185)),0))</f>
+        <f t="shared" ref="U2:U26" si="0">MEDIAN(0,255,ROUND(S2/20+SQRT(J2)/40+SQRT(P2)/2+(SQRT(R2)-SQRT(185)),0))</f>
         <v>5</v>
       </c>
       <c r="W2">
-        <f t="shared" ref="W2:W11" si="1">MEDIAN(0,255,ROUND(SQRT(J2)/200+SQRT(P2)/2+(SQRT(R2)-SQRT(185)),0))</f>
+        <f t="shared" ref="W2:W26" si="1">MEDIAN(0,255,ROUND(SQRT(J2)/200+SQRT(P2)/2+(SQRT(R2)-SQRT(185)),0))</f>
         <v>4</v>
       </c>
     </row>
@@ -22648,7 +22657,7 @@
         <v>4</v>
       </c>
       <c r="AD3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.3">
@@ -23016,16 +23025,16 @@
         <v>11</v>
       </c>
       <c r="W12">
-        <f t="shared" ref="W12:W17" si="2">MEDIAN(0,255,ROUND(SQRT(J12)/200+SQRT(P12)/2+(SQRT(R12)-SQRT(185)),0))</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>361</v>
+      </c>
+      <c r="B13" t="s">
         <v>362</v>
-      </c>
-      <c r="B13" t="s">
-        <v>363</v>
       </c>
       <c r="F13">
         <v>2008</v>
@@ -23056,16 +23065,16 @@
         <v>11</v>
       </c>
       <c r="W13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>363</v>
+      </c>
+      <c r="B14" t="s">
         <v>364</v>
-      </c>
-      <c r="B14" t="s">
-        <v>365</v>
       </c>
       <c r="F14">
         <v>1980</v>
@@ -23099,16 +23108,16 @@
         <v>20</v>
       </c>
       <c r="W14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>387</v>
+      </c>
+      <c r="B15" t="s">
         <v>388</v>
-      </c>
-      <c r="B15" t="s">
-        <v>389</v>
       </c>
       <c r="F15">
         <v>1986</v>
@@ -23139,19 +23148,19 @@
         <v>43</v>
       </c>
       <c r="W15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="AD15" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>392</v>
+      </c>
+      <c r="B16" t="s">
         <v>393</v>
-      </c>
-      <c r="B16" t="s">
-        <v>394</v>
       </c>
       <c r="F16">
         <v>2010</v>
@@ -23182,19 +23191,19 @@
         <v>6</v>
       </c>
       <c r="W16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="AD16" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>394</v>
+      </c>
+      <c r="B17" t="s">
         <v>395</v>
-      </c>
-      <c r="B17" t="s">
-        <v>396</v>
       </c>
       <c r="F17">
         <v>2010</v>
@@ -23225,21 +23234,29 @@
         <v>6</v>
       </c>
       <c r="W17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>431</v>
+        <v>430</v>
+      </c>
+      <c r="U18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -23275,11 +23292,13 @@
         <v>24</v>
       </c>
       <c r="T19" s="4"/>
-      <c r="U19" s="5">
+      <c r="U19">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="V19" s="6"/>
-      <c r="W19" s="5">
+      <c r="W19">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="X19" s="4"/>
@@ -23289,15 +23308,15 @@
       <c r="AB19" s="4"/>
       <c r="AC19" s="4"/>
       <c r="AD19" s="3" t="s">
-        <v>470</v>
+        <v>391</v>
       </c>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -23335,11 +23354,13 @@
         <v>24</v>
       </c>
       <c r="T20" s="4"/>
-      <c r="U20" s="5">
+      <c r="U20">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="V20" s="6"/>
-      <c r="W20" s="5">
+      <c r="W20">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="X20" s="4"/>
@@ -23349,15 +23370,15 @@
       <c r="AB20" s="4"/>
       <c r="AC20" s="4"/>
       <c r="AD20" s="3" t="s">
-        <v>470</v>
+        <v>391</v>
       </c>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -23393,11 +23414,13 @@
         <v>25.6</v>
       </c>
       <c r="T21" s="4"/>
-      <c r="U21" s="5">
+      <c r="U21">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="V21" s="6"/>
-      <c r="W21" s="5">
+      <c r="W21">
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="X21" s="4"/>
@@ -23407,15 +23430,15 @@
       <c r="AB21" s="4"/>
       <c r="AC21" s="4"/>
       <c r="AD21" s="3" t="s">
-        <v>470</v>
+        <v>391</v>
       </c>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -23451,11 +23474,13 @@
         <v>22.3</v>
       </c>
       <c r="T22" s="4"/>
-      <c r="U22" s="5">
+      <c r="U22">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="V22" s="6"/>
-      <c r="W22" s="5">
+      <c r="W22">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="X22" s="4"/>
@@ -23465,15 +23490,15 @@
       <c r="AB22" s="4"/>
       <c r="AC22" s="4"/>
       <c r="AD22" s="3" t="s">
-        <v>470</v>
+        <v>391</v>
       </c>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -23497,7 +23522,7 @@
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
       <c r="P23" s="5">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="Q23" s="5">
         <v>16</v>
@@ -23509,12 +23534,14 @@
         <v>28</v>
       </c>
       <c r="T23" s="4"/>
-      <c r="U23" s="5">
+      <c r="U23">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="V23" s="6"/>
+      <c r="W23">
+        <f t="shared" si="1"/>
         <v>5</v>
-      </c>
-      <c r="V23" s="6"/>
-      <c r="W23" s="5">
-        <v>3</v>
       </c>
       <c r="X23" s="4"/>
       <c r="Y23" s="4"/>
@@ -23523,15 +23550,15 @@
       <c r="AB23" s="4"/>
       <c r="AC23" s="4"/>
       <c r="AD23" s="3" t="s">
-        <v>470</v>
+        <v>391</v>
       </c>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
@@ -23569,11 +23596,13 @@
         <v>27</v>
       </c>
       <c r="T24" s="4"/>
-      <c r="U24" s="5">
+      <c r="U24">
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="V24" s="6"/>
-      <c r="W24" s="5">
+      <c r="W24">
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="X24" s="4"/>
@@ -23583,15 +23612,15 @@
       <c r="AB24" s="4"/>
       <c r="AC24" s="4"/>
       <c r="AD24" s="3" t="s">
-        <v>470</v>
+        <v>391</v>
       </c>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="F25" s="5">
         <v>1951</v>
@@ -23620,12 +23649,51 @@
       <c r="S25" s="5">
         <v>19</v>
       </c>
-      <c r="U25" s="5">
+      <c r="U25">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="V25" s="6"/>
-      <c r="W25" s="5">
-        <v>3</v>
+      <c r="W25">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="F26" s="5">
+        <v>2015</v>
+      </c>
+      <c r="G26" s="5">
+        <v>30</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="J26" s="5">
+        <v>120</v>
+      </c>
+      <c r="P26" s="5">
+        <v>80</v>
+      </c>
+      <c r="Q26" s="5">
+        <v>12</v>
+      </c>
+      <c r="R26" s="5">
+        <v>185</v>
+      </c>
+      <c r="S26" s="5">
+        <v>26</v>
+      </c>
+      <c r="U26">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="W26">
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -23639,7 +23707,7 @@
   <dimension ref="A1:Z81"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E77" sqref="E77:E79"/>
     </sheetView>
   </sheetViews>
@@ -26823,10 +26891,10 @@
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B60" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E60">
         <v>1997</v>
@@ -26875,15 +26943,15 @@
         <v>339</v>
       </c>
       <c r="Z60" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B61" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E61">
         <v>2007.5</v>
@@ -26932,15 +27000,15 @@
         <v>339</v>
       </c>
       <c r="Z61" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
+        <v>370</v>
+      </c>
+      <c r="B62" t="s">
         <v>371</v>
-      </c>
-      <c r="B62" t="s">
-        <v>372</v>
       </c>
       <c r="E62">
         <v>1959</v>
@@ -26955,7 +27023,7 @@
         <v>120</v>
       </c>
       <c r="I62" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="M62">
         <v>68</v>
@@ -26989,15 +27057,15 @@
         <v>339</v>
       </c>
       <c r="Z62" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="63" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B63" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E63">
         <v>1985</v>
@@ -27046,15 +27114,15 @@
         <v>339</v>
       </c>
       <c r="Z63" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="64" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
+        <v>375</v>
+      </c>
+      <c r="B64" t="s">
         <v>376</v>
-      </c>
-      <c r="B64" t="s">
-        <v>377</v>
       </c>
       <c r="E64">
         <v>1985</v>
@@ -27103,15 +27171,15 @@
         <v>339</v>
       </c>
       <c r="Z64" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="65" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
+        <v>377</v>
+      </c>
+      <c r="B65" t="s">
         <v>378</v>
-      </c>
-      <c r="B65" t="s">
-        <v>379</v>
       </c>
       <c r="E65">
         <v>1985</v>
@@ -27160,15 +27228,15 @@
         <v>339</v>
       </c>
       <c r="Z65" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="66" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
+        <v>379</v>
+      </c>
+      <c r="B66" t="s">
         <v>380</v>
-      </c>
-      <c r="B66" t="s">
-        <v>381</v>
       </c>
       <c r="E66">
         <v>1985</v>
@@ -27217,15 +27285,15 @@
         <v>339</v>
       </c>
       <c r="Z66" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="67" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
+        <v>383</v>
+      </c>
+      <c r="B67" t="s">
         <v>384</v>
-      </c>
-      <c r="B67" t="s">
-        <v>385</v>
       </c>
       <c r="E67">
         <v>1985</v>
@@ -27274,15 +27342,15 @@
         <v>339</v>
       </c>
       <c r="Z67" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="68" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B68" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E68">
         <v>1963</v>
@@ -27331,15 +27399,15 @@
         <v>339</v>
       </c>
       <c r="Z68" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="69" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
+        <v>381</v>
+      </c>
+      <c r="B69" t="s">
         <v>382</v>
-      </c>
-      <c r="B69" t="s">
-        <v>383</v>
       </c>
       <c r="E69">
         <v>1985</v>
@@ -27393,10 +27461,10 @@
     </row>
     <row r="70" spans="1:26" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B70" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E70">
         <v>2001</v>
@@ -27444,10 +27512,10 @@
     </row>
     <row r="71" spans="1:26" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B71" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E71">
         <v>2001</v>
@@ -27495,10 +27563,10 @@
     </row>
     <row r="72" spans="1:26" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
+        <v>422</v>
+      </c>
+      <c r="B72" t="s">
         <v>423</v>
-      </c>
-      <c r="B72" t="s">
-        <v>424</v>
       </c>
       <c r="E72">
         <v>2001</v>
@@ -27546,10 +27614,10 @@
     </row>
     <row r="73" spans="1:26" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B73" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E73">
         <v>2001</v>
@@ -27597,10 +27665,10 @@
     </row>
     <row r="74" spans="1:26" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B74" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E74">
         <v>2001</v>
@@ -27648,10 +27716,10 @@
     </row>
     <row r="75" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
+        <v>428</v>
+      </c>
+      <c r="B75" t="s">
         <v>429</v>
-      </c>
-      <c r="B75" t="s">
-        <v>430</v>
       </c>
       <c r="E75">
         <v>1964</v>
@@ -27699,10 +27767,10 @@
     </row>
     <row r="76" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B76" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E76">
         <v>1981</v>
@@ -27756,7 +27824,7 @@
     </row>
     <row r="77" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B77" t="s">
         <v>76</v>
@@ -27807,7 +27875,7 @@
     </row>
     <row r="78" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B78" t="s">
         <v>83</v>
@@ -27858,7 +27926,7 @@
     </row>
     <row r="79" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B79" t="s">
         <v>84</v>
@@ -27909,10 +27977,10 @@
     </row>
     <row r="80" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B80" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E80">
         <v>1981</v>
@@ -27960,7 +28028,7 @@
     </row>
     <row r="81" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B81" t="s">
         <v>276</v>

</xml_diff>

<commit_message>
add p65 renwel p70
</commit_message>
<xml_diff>
--- a/docs/China Set Trains.xlsx
+++ b/docs/China Set Trains.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CNS\CNST\local\China-Set-Trains\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD40C55-3E03-4252-BFB4-B4C549917869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5709D583-FEC7-4EEE-85C8-4D01EE1F75A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Loco" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1604" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1605" uniqueCount="512">
   <si>
     <t>name</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1975,6 +1975,10 @@
   </si>
   <si>
     <t>P80</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>P65</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2356,7 +2360,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A37" sqref="A37:XFD37"/>
     </sheetView>
@@ -22471,10 +22475,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8540264-B3C1-4C71-9FC9-001ABF042657}">
-  <dimension ref="A1:AD26"/>
+  <dimension ref="A1:AD27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U23" sqref="U23"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Q26" sqref="Q26:Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -23694,6 +23698,26 @@
       <c r="W26">
         <f t="shared" si="1"/>
         <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="F27" s="5">
+        <v>1998</v>
+      </c>
+      <c r="G27" s="5">
+        <v>30</v>
+      </c>
+      <c r="J27" s="5">
+        <v>120</v>
+      </c>
+      <c r="P27" s="5">
+        <v>58</v>
+      </c>
+      <c r="Q27" s="5">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add cha1c (with bugs)
</commit_message>
<xml_diff>
--- a/docs/China Set Trains.xlsx
+++ b/docs/China Set Trains.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CNS\CNST\local\China-Set-Trains\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD27BBE-3415-45FB-B55E-52FB0A194ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BFF7820-1BBF-411E-8D60-8EE9DF93FE7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1832" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="527">
   <si>
     <t>name</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2020,6 +2020,26 @@
   </si>
   <si>
     <t>hxd21000</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>P64</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>power/hpI</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CHA1A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(electry)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(battery)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2399,21 +2419,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE69"/>
+  <dimension ref="A1:AF71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B69" sqref="B69"/>
+      <selection pane="bottomLeft" activeCell="M70" sqref="M70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="8.58203125" style="1"/>
-    <col min="28" max="29" width="8.58203125" style="2"/>
+    <col min="26" max="28" width="8.58203125" style="1"/>
+    <col min="29" max="30" width="8.58203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2451,61 +2471,64 @@
         <v>519</v>
       </c>
       <c r="M1" t="s">
+        <v>523</v>
+      </c>
+      <c r="N1" t="s">
         <v>55</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>53</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>18</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>19</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>28</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>20</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>27</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>56</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>57</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>92</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>93</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -2536,60 +2559,60 @@
       <c r="K2">
         <v>80</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>1545</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>174.85</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>0.13750000000000001</v>
       </c>
-      <c r="P2">
-        <f>N2*O2*9.8</f>
+      <c r="Q2">
+        <f>O2*P2*9.8</f>
         <v>235.61037500000003</v>
       </c>
-      <c r="Q2">
-        <f t="shared" ref="Q2:Q45" si="0">MEDIAN(255, ROUND((N2/10+SQRT(K2)/20+SQRT(M2)+O2+20-J2), 0), 0)</f>
+      <c r="R2">
+        <f t="shared" ref="R2:R45" si="0">MEDIAN(255, ROUND((O2/10+SQRT(K2)/20+SQRT(N2)+P2+20-J2), 0), 0)</f>
         <v>53</v>
       </c>
-      <c r="R2">
-        <f>Q2*50000/16</f>
+      <c r="S2">
+        <f>R2*50000/16</f>
         <v>165625</v>
       </c>
-      <c r="S2">
-        <f t="shared" ref="S2:S45" si="1">MEDIAN(0, 255, ROUND(SQRT(K2)/100+SQRT(M2)+O2+40/J2-2,0))</f>
+      <c r="T2">
+        <f t="shared" ref="T2:T45" si="1">MEDIAN(0, 255, ROUND(SQRT(K2)/100+SQRT(N2)+P2+40/J2-2,0))</f>
         <v>39</v>
       </c>
-      <c r="T2">
-        <f t="shared" ref="T2:T45" si="2">IF(E2="Steam", S2*350/16*12, IF(E2="Diesel", S2*325/16*12,  S2*300/16*12))</f>
+      <c r="U2">
+        <f t="shared" ref="U2:U45" si="2">IF(E2="Steam", T2*350/16*12, IF(E2="Diesel", T2*325/16*12,  T2*300/16*12))</f>
         <v>10237.5</v>
       </c>
-      <c r="U2">
-        <f>V2+W2+X2</f>
+      <c r="V2">
+        <f>W2+X2+Y2</f>
         <v>11</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>6</v>
       </c>
-      <c r="X2">
+      <c r="Y2">
         <v>5</v>
       </c>
-      <c r="Y2" s="1">
+      <c r="Z2" s="1">
         <v>1</v>
       </c>
-      <c r="Z2" s="1">
-        <v>0</v>
-      </c>
       <c r="AA2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="AB2" s="2">
-        <f>AVERAGE(Y2:AA2)</f>
+      <c r="AC2" s="2">
+        <f>AVERAGE(Z2:AB2)</f>
         <v>0.44444444444444442</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -2605,36 +2628,36 @@
       <c r="F3">
         <v>1934</v>
       </c>
-      <c r="P3">
-        <f t="shared" ref="P3:P59" si="3">N3*O3*9.8</f>
-        <v>0</v>
-      </c>
       <c r="Q3">
+        <f t="shared" ref="Q3:Q59" si="3">O3*P3*9.8</f>
+        <v>0</v>
+      </c>
+      <c r="R3">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="R3">
-        <f t="shared" ref="R3:R20" si="4">Q3*50000/16</f>
+      <c r="S3">
+        <f t="shared" ref="S3:S20" si="4">R3*50000/16</f>
         <v>62500</v>
       </c>
-      <c r="S3" t="e">
+      <c r="T3" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="T3" t="e">
+      <c r="U3" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="U3">
-        <f t="shared" ref="U3:U37" si="5">V3+W3+X3</f>
-        <v>0</v>
-      </c>
-      <c r="AB3" s="2" t="e">
-        <f t="shared" ref="AB3:AB37" si="6">AVERAGE(Y3:AA3)</f>
+      <c r="V3">
+        <f t="shared" ref="V3:V37" si="5">W3+X3+Y3</f>
+        <v>0</v>
+      </c>
+      <c r="AC3" s="2" t="e">
+        <f t="shared" ref="AC3:AC37" si="6">AVERAGE(Z3:AB3)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -2650,36 +2673,36 @@
       <c r="F4">
         <v>1933</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <f t="shared" si="4"/>
         <v>62500</v>
       </c>
-      <c r="S4" t="e">
+      <c r="T4" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="T4" t="e">
+      <c r="U4" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AB4" s="2" t="e">
+      <c r="AC4" s="2" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -2695,36 +2718,36 @@
       <c r="F5">
         <v>1956</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <f t="shared" si="4"/>
         <v>62500</v>
       </c>
-      <c r="S5" t="e">
+      <c r="T5" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="T5" t="e">
+      <c r="U5" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="U5">
+      <c r="V5">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AB5" s="2" t="e">
+      <c r="AC5" s="2" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -2740,36 +2763,36 @@
       <c r="F6">
         <v>1957</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <f t="shared" si="4"/>
         <v>62500</v>
       </c>
-      <c r="S6" t="e">
+      <c r="T6" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="T6" t="e">
+      <c r="U6" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="U6">
+      <c r="V6">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AB6" s="2" t="e">
+      <c r="AC6" s="2" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -2800,45 +2823,45 @@
       <c r="K7">
         <v>80</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>1500</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>140</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>0.14849999999999999</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <f t="shared" si="3"/>
         <v>203.74200000000002</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <f t="shared" si="4"/>
         <v>190625</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <f t="shared" si="2"/>
         <v>10500</v>
       </c>
-      <c r="U7">
+      <c r="V7">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AB7" s="2" t="e">
+      <c r="AC7" s="2" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>104</v>
       </c>
@@ -2869,54 +2892,54 @@
       <c r="K8">
         <v>120</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>2610</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>138</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>0.24199999999999999</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <f t="shared" si="3"/>
         <v>327.28080000000006</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <f t="shared" si="4"/>
         <v>168750</v>
       </c>
-      <c r="S8">
+      <c r="T8">
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <f t="shared" si="2"/>
         <v>12431.25</v>
       </c>
-      <c r="U8">
+      <c r="V8">
         <f t="shared" si="5"/>
         <v>10</v>
       </c>
-      <c r="V8">
+      <c r="W8">
         <v>1</v>
       </c>
-      <c r="W8">
+      <c r="X8">
         <v>8</v>
       </c>
-      <c r="X8">
+      <c r="Y8">
         <v>1</v>
       </c>
-      <c r="AB8" s="2" t="e">
+      <c r="AC8" s="2" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>105</v>
       </c>
@@ -2947,49 +2970,46 @@
       <c r="K9">
         <v>100</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>2610</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>138</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>0.30499999999999999</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <f t="shared" si="3"/>
         <v>412.48199999999997</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="R9">
-        <f t="shared" ref="R9" si="7">Q9*50000/16</f>
+      <c r="S9">
+        <f t="shared" ref="S9" si="7">R9*50000/16</f>
         <v>168750</v>
       </c>
-      <c r="S9">
+      <c r="T9">
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <f t="shared" si="2"/>
         <v>12431.25</v>
       </c>
-      <c r="U9">
-        <f t="shared" ref="U9" si="8">V9+W9+X9</f>
+      <c r="V9">
+        <f t="shared" ref="V9" si="8">W9+X9+Y9</f>
         <v>10</v>
       </c>
-      <c r="V9">
+      <c r="W9">
         <v>1</v>
       </c>
-      <c r="W9">
+      <c r="X9">
         <v>8</v>
       </c>
-      <c r="X9">
-        <v>1</v>
-      </c>
-      <c r="Y9" s="1">
+      <c r="Y9">
         <v>1</v>
       </c>
       <c r="Z9" s="1">
@@ -2998,18 +3018,21 @@
       <c r="AA9" s="1">
         <v>1</v>
       </c>
-      <c r="AB9" s="2">
+      <c r="AB9" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC9" s="2">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="AC9" s="2" t="s">
+      <c r="AD9" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="AD9" t="s">
+      <c r="AE9" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>197</v>
       </c>
@@ -3037,44 +3060,44 @@
       <c r="K10">
         <v>145</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>4000</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>138</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>0.224</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <f t="shared" si="3"/>
         <v>302.93760000000003</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <f t="shared" si="0"/>
         <v>84</v>
       </c>
-      <c r="R10">
-        <f t="shared" ref="R10:R12" si="9">Q10*50000/16</f>
+      <c r="S10">
+        <f t="shared" ref="S10:S12" si="9">R10*50000/16</f>
         <v>262500</v>
       </c>
-      <c r="S10">
+      <c r="T10">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <f t="shared" si="2"/>
         <v>15600</v>
       </c>
-      <c r="U10">
-        <f t="shared" ref="U10:U12" si="10">V10+W10+X10</f>
-        <v>0</v>
-      </c>
-      <c r="AD10" t="s">
+      <c r="V10">
+        <f t="shared" ref="V10:V12" si="10">W10+X10+Y10</f>
+        <v>0</v>
+      </c>
+      <c r="AE10" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>198</v>
       </c>
@@ -3102,44 +3125,44 @@
       <c r="K11">
         <v>170</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>4000</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>138</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>0.224</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <f t="shared" si="3"/>
         <v>302.93760000000003</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <f t="shared" si="0"/>
         <v>84</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <f t="shared" si="9"/>
         <v>262500</v>
       </c>
-      <c r="S11">
+      <c r="T11">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <f t="shared" si="2"/>
         <v>15600</v>
       </c>
-      <c r="U11">
+      <c r="V11">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AD11" t="s">
+      <c r="AE11" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>199</v>
       </c>
@@ -3167,44 +3190,44 @@
       <c r="K12">
         <v>100</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>4000</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>138</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>0.35499999999999998</v>
       </c>
-      <c r="P12">
+      <c r="Q12">
         <f t="shared" si="3"/>
         <v>480.10199999999998</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <f t="shared" si="0"/>
         <v>84</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <f t="shared" si="9"/>
         <v>262500</v>
       </c>
-      <c r="S12">
+      <c r="T12">
         <f t="shared" si="1"/>
         <v>65</v>
       </c>
-      <c r="T12">
+      <c r="U12">
         <f t="shared" si="2"/>
         <v>15843.75</v>
       </c>
-      <c r="U12">
+      <c r="V12">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AD12" t="s">
+      <c r="AE12" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>231</v>
       </c>
@@ -3220,36 +3243,36 @@
       <c r="F13">
         <v>1976</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="R13">
+      <c r="S13">
         <f t="shared" si="4"/>
         <v>62500</v>
       </c>
-      <c r="S13" t="e">
+      <c r="T13" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="T13" t="e">
+      <c r="U13" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="U13">
+      <c r="V13">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AB13" s="2" t="e">
+      <c r="AC13" s="2" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -3280,44 +3303,44 @@
       <c r="K14">
         <v>80</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>1414</v>
       </c>
-      <c r="N14">
+      <c r="O14">
         <v>138</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <v>0.32200000000000001</v>
       </c>
-      <c r="P14">
+      <c r="Q14">
         <f t="shared" si="3"/>
         <v>435.47280000000001</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="R14">
-        <f t="shared" ref="R14" si="11">Q14*50000/16</f>
+      <c r="S14">
+        <f t="shared" ref="S14" si="11">R14*50000/16</f>
         <v>175000</v>
       </c>
-      <c r="S14">
+      <c r="T14">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="T14">
+      <c r="U14">
         <f t="shared" si="2"/>
         <v>9506.25</v>
       </c>
-      <c r="U14">
-        <f t="shared" ref="U14" si="12">V14+W14+X14</f>
-        <v>0</v>
-      </c>
-      <c r="AD14" t="s">
+      <c r="V14">
+        <f t="shared" ref="V14" si="12">W14+X14+Y14</f>
+        <v>0</v>
+      </c>
+      <c r="AE14" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -3333,36 +3356,36 @@
       <c r="F15">
         <v>1974</v>
       </c>
-      <c r="P15">
+      <c r="Q15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="R15">
+      <c r="S15">
         <f t="shared" si="4"/>
         <v>62500</v>
       </c>
-      <c r="S15" t="e">
+      <c r="T15" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="T15" t="e">
+      <c r="U15" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="U15">
+      <c r="V15">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AB15" s="2" t="e">
+      <c r="AC15" s="2" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -3393,48 +3416,48 @@
       <c r="K16">
         <v>170</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>4133</v>
       </c>
-      <c r="N16">
+      <c r="O16">
         <v>138</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <v>0.18099999999999999</v>
       </c>
-      <c r="P16">
+      <c r="Q16">
         <f t="shared" si="3"/>
         <v>244.78440000000001</v>
       </c>
-      <c r="Q16">
+      <c r="R16">
         <f t="shared" si="0"/>
         <v>89</v>
       </c>
-      <c r="R16">
+      <c r="S16">
         <f t="shared" si="4"/>
         <v>278125</v>
       </c>
-      <c r="S16">
+      <c r="T16">
         <f t="shared" si="1"/>
         <v>67</v>
       </c>
-      <c r="T16">
+      <c r="U16">
         <f t="shared" si="2"/>
         <v>16331.25</v>
       </c>
-      <c r="U16">
+      <c r="V16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AB16" s="2" t="e">
+      <c r="AC16" s="2" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD16" t="s">
+      <c r="AE16" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -3447,36 +3470,36 @@
       <c r="E17" t="s">
         <v>51</v>
       </c>
-      <c r="P17">
+      <c r="Q17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Q17">
+      <c r="R17">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="R17">
+      <c r="S17">
         <f t="shared" si="4"/>
         <v>62500</v>
       </c>
-      <c r="S17" t="e">
+      <c r="T17" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="T17" t="e">
+      <c r="U17" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="U17">
+      <c r="V17">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AB17" s="2" t="e">
+      <c r="AC17" s="2" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>232</v>
       </c>
@@ -3504,41 +3527,41 @@
       <c r="K18">
         <v>120</v>
       </c>
-      <c r="M18">
+      <c r="N18">
         <v>3480</v>
       </c>
-      <c r="N18">
+      <c r="O18">
         <v>138</v>
       </c>
-      <c r="O18">
+      <c r="P18">
         <v>0.39500000000000002</v>
       </c>
-      <c r="P18">
+      <c r="Q18">
         <f t="shared" si="3"/>
         <v>534.19800000000009</v>
       </c>
-      <c r="Q18">
+      <c r="R18">
         <f t="shared" si="0"/>
         <v>86</v>
       </c>
-      <c r="R18">
-        <f t="shared" ref="R18" si="13">Q18*50000/16</f>
+      <c r="S18">
+        <f t="shared" ref="S18" si="13">R18*50000/16</f>
         <v>268750</v>
       </c>
-      <c r="S18">
+      <c r="T18">
         <f t="shared" si="1"/>
         <v>62</v>
       </c>
-      <c r="T18">
+      <c r="U18">
         <f t="shared" si="2"/>
         <v>15112.5</v>
       </c>
-      <c r="U18">
-        <f t="shared" ref="U18" si="14">V18+W18+X18</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="V18">
+        <f t="shared" ref="V18" si="14">W18+X18+Y18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -3554,36 +3577,36 @@
       <c r="F19">
         <v>2005</v>
       </c>
-      <c r="P19">
+      <c r="Q19">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Q19">
+      <c r="R19">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="R19">
+      <c r="S19">
         <f t="shared" si="4"/>
         <v>62500</v>
       </c>
-      <c r="S19" t="e">
+      <c r="T19" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="T19" t="e">
+      <c r="U19" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="U19">
+      <c r="V19">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AB19" s="2" t="e">
+      <c r="AC19" s="2" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>150</v>
       </c>
@@ -3611,69 +3634,69 @@
       <c r="K20">
         <v>170</v>
       </c>
-      <c r="M20">
+      <c r="N20">
         <v>4133</v>
       </c>
-      <c r="N20">
+      <c r="O20">
         <v>138</v>
       </c>
-      <c r="O20">
+      <c r="P20">
         <v>0.14299999999999999</v>
       </c>
-      <c r="P20">
+      <c r="Q20">
         <f t="shared" si="3"/>
         <v>193.39320000000001</v>
       </c>
-      <c r="Q20">
+      <c r="R20">
         <f t="shared" si="0"/>
         <v>93</v>
       </c>
-      <c r="R20">
+      <c r="S20">
         <f t="shared" si="4"/>
         <v>290625</v>
       </c>
-      <c r="S20">
+      <c r="T20">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-      <c r="T20">
+      <c r="U20">
         <f t="shared" si="2"/>
         <v>16818.75</v>
       </c>
-      <c r="U20">
-        <f t="shared" ref="U20" si="15">V20+W20+X20</f>
+      <c r="V20">
+        <f t="shared" ref="V20" si="15">W20+X20+Y20</f>
         <v>11</v>
       </c>
-      <c r="V20">
+      <c r="W20">
         <v>2</v>
       </c>
-      <c r="W20">
+      <c r="X20">
         <v>7</v>
       </c>
-      <c r="X20">
+      <c r="Y20">
         <v>2</v>
-      </c>
-      <c r="Y20" s="1">
-        <v>1</v>
       </c>
       <c r="Z20" s="1">
         <v>1</v>
       </c>
       <c r="AA20" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB20" s="1">
         <v>0.5</v>
       </c>
-      <c r="AB20" s="2">
+      <c r="AC20" s="2">
         <f t="shared" si="6"/>
         <v>0.83333333333333337</v>
       </c>
-      <c r="AC20" s="2" t="s">
+      <c r="AD20" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="AD20" t="s">
+      <c r="AE20" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>315</v>
       </c>
@@ -3704,58 +3727,58 @@
       <c r="K21">
         <v>120</v>
       </c>
-      <c r="M21">
+      <c r="N21">
         <v>2610</v>
       </c>
-      <c r="N21">
+      <c r="O21">
         <v>138</v>
       </c>
-      <c r="O21">
+      <c r="P21">
         <v>0.24199999999999999</v>
       </c>
-      <c r="P21">
+      <c r="Q21">
         <f t="shared" si="3"/>
         <v>327.28080000000006</v>
       </c>
-      <c r="Q21">
+      <c r="R21">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="R21">
-        <f t="shared" ref="R21:R45" si="16">Q21*50000/16</f>
+      <c r="S21">
+        <f t="shared" ref="S21:S45" si="16">R21*50000/16</f>
         <v>225000</v>
       </c>
-      <c r="S21">
+      <c r="T21">
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
-      <c r="T21">
+      <c r="U21">
         <f t="shared" si="2"/>
         <v>12675</v>
       </c>
-      <c r="U21">
+      <c r="V21">
         <v>10</v>
       </c>
-      <c r="V21">
+      <c r="W21">
         <v>1</v>
       </c>
-      <c r="W21">
+      <c r="X21">
         <v>8</v>
       </c>
-      <c r="X21">
+      <c r="Y21">
         <v>1</v>
       </c>
-      <c r="AB21" s="2" t="e">
+      <c r="AC21" s="2" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="AC21" s="2" t="s">
+      <c r="AD21" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="AD21" t="s">
+      <c r="AE21" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>320</v>
       </c>
@@ -3786,48 +3809,45 @@
       <c r="K22">
         <v>100</v>
       </c>
-      <c r="M22">
+      <c r="N22">
         <v>2610</v>
       </c>
-      <c r="N22">
+      <c r="O22">
         <v>138</v>
       </c>
-      <c r="O22">
+      <c r="P22">
         <v>0.30499999999999999</v>
       </c>
-      <c r="P22">
+      <c r="Q22">
         <f t="shared" si="3"/>
         <v>412.48199999999997</v>
       </c>
-      <c r="Q22">
+      <c r="R22">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="R22">
+      <c r="S22">
         <f t="shared" si="16"/>
         <v>225000</v>
       </c>
-      <c r="S22">
+      <c r="T22">
         <f t="shared" si="1"/>
         <v>52</v>
       </c>
-      <c r="T22">
+      <c r="U22">
         <f t="shared" si="2"/>
         <v>12675</v>
       </c>
-      <c r="U22">
+      <c r="V22">
         <v>10</v>
       </c>
-      <c r="V22">
+      <c r="W22">
         <v>1</v>
       </c>
-      <c r="W22">
+      <c r="X22">
         <v>8</v>
       </c>
-      <c r="X22">
-        <v>1</v>
-      </c>
-      <c r="Y22" s="1">
+      <c r="Y22">
         <v>1</v>
       </c>
       <c r="Z22" s="1">
@@ -3836,17 +3856,20 @@
       <c r="AA22" s="1">
         <v>1</v>
       </c>
-      <c r="AB22" s="2">
+      <c r="AB22" s="1">
         <v>1</v>
       </c>
-      <c r="AC22" s="2" t="s">
+      <c r="AC22" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD22" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="AD22" t="s">
+      <c r="AE22" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>323</v>
       </c>
@@ -3877,56 +3900,56 @@
       <c r="K23">
         <v>100</v>
       </c>
-      <c r="M23">
+      <c r="N23">
         <v>2189</v>
       </c>
-      <c r="N23">
+      <c r="O23">
         <v>138</v>
       </c>
-      <c r="O23">
+      <c r="P23">
         <v>0.32700000000000001</v>
       </c>
-      <c r="P23">
+      <c r="Q23">
         <f t="shared" si="3"/>
         <v>442.23480000000006</v>
       </c>
-      <c r="Q23">
+      <c r="R23">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="R23">
+      <c r="S23">
         <f t="shared" si="16"/>
         <v>190625</v>
       </c>
-      <c r="S23">
+      <c r="T23">
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="T23">
+      <c r="U23">
         <f t="shared" si="2"/>
         <v>11456.25</v>
       </c>
-      <c r="U23">
-        <f t="shared" ref="U23:U27" si="17">V23+W23+X23</f>
+      <c r="V23">
+        <f t="shared" ref="V23:V27" si="17">W23+X23+Y23</f>
         <v>9</v>
       </c>
-      <c r="V23">
+      <c r="W23">
         <v>2</v>
       </c>
-      <c r="W23">
+      <c r="X23">
         <v>5</v>
       </c>
-      <c r="X23">
+      <c r="Y23">
         <v>2</v>
       </c>
-      <c r="AC23" s="2" t="s">
+      <c r="AD23" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="AD23" t="s">
+      <c r="AE23" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>327</v>
       </c>
@@ -3954,47 +3977,47 @@
       <c r="K24">
         <v>100</v>
       </c>
-      <c r="M24">
+      <c r="N24">
         <v>2039</v>
       </c>
-      <c r="N24">
+      <c r="O24">
         <v>138</v>
       </c>
-      <c r="O24">
+      <c r="P24">
         <v>0.32200000000000001</v>
       </c>
-      <c r="P24">
+      <c r="Q24">
         <f t="shared" si="3"/>
         <v>435.47280000000001</v>
       </c>
-      <c r="Q24">
+      <c r="R24">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="R24">
+      <c r="S24">
         <f t="shared" si="16"/>
         <v>200000</v>
       </c>
-      <c r="S24">
+      <c r="T24">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="T24">
+      <c r="U24">
         <f t="shared" si="2"/>
         <v>11212.5</v>
       </c>
-      <c r="U24">
+      <c r="V24">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="AC24" s="2" t="s">
+      <c r="AD24" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="AD24" t="s">
+      <c r="AE24" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>329</v>
       </c>
@@ -4022,47 +4045,47 @@
       <c r="K25">
         <v>100</v>
       </c>
-      <c r="M25">
+      <c r="N25">
         <v>2175</v>
       </c>
-      <c r="N25">
+      <c r="O25">
         <v>140</v>
       </c>
-      <c r="O25">
+      <c r="P25">
         <v>0.32100000000000001</v>
       </c>
-      <c r="P25">
+      <c r="Q25">
         <f t="shared" si="3"/>
         <v>440.41200000000003</v>
       </c>
-      <c r="Q25">
+      <c r="R25">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-      <c r="R25">
+      <c r="S25">
         <f t="shared" si="16"/>
         <v>203125</v>
       </c>
-      <c r="S25">
+      <c r="T25">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="T25">
+      <c r="U25">
         <f t="shared" si="2"/>
         <v>11700</v>
       </c>
-      <c r="U25">
+      <c r="V25">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="AC25" s="2" t="s">
+      <c r="AD25" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="AD25" t="s">
+      <c r="AE25" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>331</v>
       </c>
@@ -4093,47 +4116,47 @@
       <c r="K26">
         <v>80</v>
       </c>
-      <c r="M26">
+      <c r="N26">
         <v>1080</v>
       </c>
-      <c r="N26">
+      <c r="O26">
         <v>92</v>
       </c>
-      <c r="O26">
+      <c r="P26">
         <v>0.32900000000000001</v>
       </c>
-      <c r="P26">
+      <c r="Q26">
         <f t="shared" si="3"/>
         <v>296.62640000000005</v>
       </c>
-      <c r="Q26">
+      <c r="R26">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="R26">
+      <c r="S26">
         <f t="shared" si="16"/>
         <v>121875</v>
       </c>
-      <c r="S26">
+      <c r="T26">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="T26">
+      <c r="U26">
         <f t="shared" si="2"/>
         <v>8043.75</v>
       </c>
-      <c r="U26">
+      <c r="V26">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="AC26" s="2" t="s">
+      <c r="AD26" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="AD26" t="s">
+      <c r="AE26" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>334</v>
       </c>
@@ -4164,47 +4187,47 @@
       <c r="K27">
         <v>80</v>
       </c>
-      <c r="M27">
+      <c r="N27">
         <v>1080</v>
       </c>
-      <c r="N27">
+      <c r="O27">
         <v>92</v>
       </c>
-      <c r="O27">
+      <c r="P27">
         <v>0.32900000000000001</v>
       </c>
-      <c r="P27">
+      <c r="Q27">
         <f t="shared" si="3"/>
         <v>296.62640000000005</v>
       </c>
-      <c r="Q27">
+      <c r="R27">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="R27">
+      <c r="S27">
         <f t="shared" si="16"/>
         <v>121875</v>
       </c>
-      <c r="S27">
+      <c r="T27">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="T27">
+      <c r="U27">
         <f t="shared" si="2"/>
         <v>8043.75</v>
       </c>
-      <c r="U27">
+      <c r="V27">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="AC27" s="2" t="s">
+      <c r="AD27" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="AD27" t="s">
+      <c r="AE27" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>336</v>
       </c>
@@ -4232,60 +4255,60 @@
       <c r="K28">
         <v>100</v>
       </c>
-      <c r="M28">
+      <c r="N28">
         <v>4800</v>
       </c>
-      <c r="N28">
+      <c r="O28">
         <v>150</v>
       </c>
-      <c r="O28">
+      <c r="P28">
         <v>0.38100000000000001</v>
       </c>
-      <c r="P28">
+      <c r="Q28">
         <f t="shared" si="3"/>
         <v>560.07000000000005</v>
       </c>
-      <c r="Q28">
+      <c r="R28">
         <f t="shared" si="0"/>
         <v>91</v>
       </c>
-      <c r="R28">
+      <c r="S28">
         <f t="shared" si="16"/>
         <v>284375</v>
       </c>
-      <c r="S28">
+      <c r="T28">
         <f t="shared" si="1"/>
         <v>71</v>
       </c>
-      <c r="T28">
+      <c r="U28">
         <f t="shared" si="2"/>
         <v>17306.25</v>
       </c>
-      <c r="U28">
-        <f t="shared" ref="U28" si="18">V28+W28+X28</f>
+      <c r="V28">
+        <f t="shared" ref="V28" si="18">W28+X28+Y28</f>
         <v>11</v>
       </c>
-      <c r="V28">
+      <c r="W28">
         <v>2</v>
       </c>
-      <c r="W28">
+      <c r="X28">
         <v>7</v>
       </c>
-      <c r="X28">
+      <c r="Y28">
         <v>2</v>
       </c>
-      <c r="AB28" s="2" t="e">
-        <f t="shared" ref="AB28" si="19">AVERAGE(Y28:AA28)</f>
+      <c r="AC28" s="2" t="e">
+        <f t="shared" ref="AC28" si="19">AVERAGE(Z28:AB28)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AC28" s="2" t="s">
+      <c r="AD28" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="AD28" t="s">
+      <c r="AE28" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -4301,36 +4324,36 @@
       <c r="F29">
         <v>1958</v>
       </c>
-      <c r="P29">
+      <c r="Q29">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="Q29">
+      <c r="R29">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="R29">
+      <c r="S29">
         <f t="shared" si="16"/>
         <v>62500</v>
       </c>
-      <c r="S29" t="e">
+      <c r="T29" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="T29" t="e">
+      <c r="U29" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="U29">
+      <c r="V29">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AB29" s="2" t="e">
+      <c r="AC29" s="2" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -4361,45 +4384,45 @@
       <c r="K30">
         <v>100</v>
       </c>
-      <c r="M30">
+      <c r="N30">
         <v>5914</v>
       </c>
-      <c r="N30">
+      <c r="O30">
         <v>138</v>
       </c>
-      <c r="O30">
+      <c r="P30">
         <v>0.34699999999999998</v>
       </c>
-      <c r="P30">
+      <c r="Q30">
         <f t="shared" si="3"/>
         <v>469.28280000000001</v>
       </c>
-      <c r="Q30">
+      <c r="R30">
         <f t="shared" si="0"/>
         <v>102</v>
       </c>
-      <c r="R30">
+      <c r="S30">
         <f t="shared" si="16"/>
         <v>318750</v>
       </c>
-      <c r="S30">
+      <c r="T30">
         <f t="shared" si="1"/>
         <v>79</v>
       </c>
-      <c r="T30">
+      <c r="U30">
         <f t="shared" si="2"/>
         <v>17775</v>
       </c>
-      <c r="U30">
+      <c r="V30">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AB30" s="2" t="e">
+      <c r="AC30" s="2" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -4430,45 +4453,45 @@
       <c r="K31">
         <v>100</v>
       </c>
-      <c r="M31">
+      <c r="N31">
         <v>8702</v>
       </c>
-      <c r="N31">
+      <c r="O31">
         <v>184</v>
       </c>
-      <c r="O31">
+      <c r="P31">
         <v>0.34799999999999998</v>
       </c>
-      <c r="P31">
+      <c r="Q31">
         <f t="shared" si="3"/>
         <v>627.5136</v>
       </c>
-      <c r="Q31">
+      <c r="R31">
         <f t="shared" si="0"/>
         <v>113</v>
       </c>
-      <c r="R31">
+      <c r="S31">
         <f t="shared" si="16"/>
         <v>353125</v>
       </c>
-      <c r="S31">
+      <c r="T31">
         <f t="shared" si="1"/>
         <v>94</v>
       </c>
-      <c r="T31">
+      <c r="U31">
         <f t="shared" si="2"/>
         <v>21150</v>
       </c>
-      <c r="U31">
+      <c r="V31">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AB31" s="2" t="e">
+      <c r="AC31" s="2" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -4499,48 +4522,48 @@
       <c r="K32">
         <v>170</v>
       </c>
-      <c r="M32">
+      <c r="N32">
         <v>4894</v>
       </c>
-      <c r="N32">
+      <c r="O32">
         <v>88</v>
       </c>
-      <c r="O32">
+      <c r="P32">
         <v>0.24299999999999999</v>
       </c>
-      <c r="P32">
+      <c r="Q32">
         <f t="shared" si="3"/>
         <v>209.56320000000002</v>
       </c>
-      <c r="Q32">
+      <c r="R32">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="R32">
+      <c r="S32">
         <f t="shared" si="16"/>
         <v>281250</v>
       </c>
-      <c r="S32">
+      <c r="T32">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
-      <c r="T32">
+      <c r="U32">
         <f t="shared" si="2"/>
         <v>16200</v>
       </c>
-      <c r="U32">
+      <c r="V32">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AB32" s="2" t="e">
+      <c r="AC32" s="2" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AD32" t="s">
+      <c r="AE32" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -4571,49 +4594,46 @@
       <c r="K33">
         <v>120</v>
       </c>
-      <c r="M33">
+      <c r="N33">
         <v>9655</v>
       </c>
-      <c r="N33">
+      <c r="O33">
         <v>138</v>
       </c>
-      <c r="O33">
+      <c r="P33">
         <v>0.38450000000000001</v>
       </c>
-      <c r="P33">
+      <c r="Q33">
         <f t="shared" si="3"/>
         <v>519.99779999999998</v>
       </c>
-      <c r="Q33">
+      <c r="R33">
         <f t="shared" si="0"/>
         <v>127</v>
       </c>
-      <c r="R33">
+      <c r="S33">
         <f t="shared" si="16"/>
         <v>396875</v>
       </c>
-      <c r="S33">
+      <c r="T33">
         <f t="shared" si="1"/>
         <v>103</v>
       </c>
-      <c r="T33">
+      <c r="U33">
         <f t="shared" si="2"/>
         <v>23175</v>
       </c>
-      <c r="U33">
+      <c r="V33">
         <f t="shared" si="5"/>
         <v>10</v>
       </c>
-      <c r="V33">
+      <c r="W33">
         <v>1</v>
       </c>
-      <c r="W33">
+      <c r="X33">
         <v>8</v>
       </c>
-      <c r="X33">
-        <v>1</v>
-      </c>
-      <c r="Y33" s="1">
+      <c r="Y33">
         <v>1</v>
       </c>
       <c r="Z33" s="1">
@@ -4622,18 +4642,21 @@
       <c r="AA33" s="1">
         <v>1</v>
       </c>
-      <c r="AB33" s="2">
+      <c r="AB33" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC33" s="2">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="AC33" s="2" t="s">
+      <c r="AD33" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="AD33" t="s">
+      <c r="AE33" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>41</v>
       </c>
@@ -4661,51 +4684,51 @@
       <c r="K34">
         <v>170</v>
       </c>
-      <c r="M34">
+      <c r="N34">
         <v>9655</v>
       </c>
-      <c r="N34">
+      <c r="O34">
         <v>126</v>
       </c>
-      <c r="O34">
+      <c r="P34">
         <v>0.34</v>
       </c>
-      <c r="P34">
+      <c r="Q34">
         <f t="shared" si="3"/>
         <v>419.83200000000005</v>
       </c>
-      <c r="Q34">
+      <c r="R34">
         <f t="shared" si="0"/>
         <v>126</v>
       </c>
-      <c r="R34">
+      <c r="S34">
         <f t="shared" si="16"/>
         <v>393750</v>
       </c>
-      <c r="S34">
+      <c r="T34">
         <f t="shared" si="1"/>
         <v>103</v>
       </c>
-      <c r="T34">
+      <c r="U34">
         <f t="shared" si="2"/>
         <v>23175</v>
       </c>
-      <c r="U34">
+      <c r="V34">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AB34" s="2" t="e">
+      <c r="AC34" s="2" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AC34" s="2" t="s">
-        <v>419</v>
-      </c>
       <c r="AD34" s="2" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="AE34" s="2" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="35" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>137</v>
       </c>
@@ -4736,49 +4759,46 @@
       <c r="K35">
         <v>170</v>
       </c>
-      <c r="M35">
+      <c r="N35">
         <v>9655</v>
       </c>
-      <c r="N35">
+      <c r="O35">
         <v>126</v>
       </c>
-      <c r="O35">
+      <c r="P35">
         <v>0.34</v>
       </c>
-      <c r="P35">
+      <c r="Q35">
         <f t="shared" si="3"/>
         <v>419.83200000000005</v>
       </c>
-      <c r="Q35">
+      <c r="R35">
         <f t="shared" si="0"/>
         <v>126</v>
       </c>
-      <c r="R35">
+      <c r="S35">
         <f t="shared" si="16"/>
         <v>393750</v>
       </c>
-      <c r="S35">
+      <c r="T35">
         <f t="shared" si="1"/>
         <v>103</v>
       </c>
-      <c r="T35">
+      <c r="U35">
         <f t="shared" si="2"/>
         <v>23175</v>
       </c>
-      <c r="U35">
+      <c r="V35">
         <f t="shared" si="5"/>
         <v>10</v>
       </c>
-      <c r="V35">
+      <c r="W35">
         <v>1</v>
       </c>
-      <c r="W35">
+      <c r="X35">
         <v>8</v>
       </c>
-      <c r="X35">
-        <v>1</v>
-      </c>
-      <c r="Y35" s="1">
+      <c r="Y35">
         <v>1</v>
       </c>
       <c r="Z35" s="1">
@@ -4787,18 +4807,21 @@
       <c r="AA35" s="1">
         <v>1</v>
       </c>
-      <c r="AB35" s="2">
+      <c r="AB35" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC35" s="2">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="AC35" s="2" t="s">
+      <c r="AD35" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="AD35" t="s">
+      <c r="AE35" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>191</v>
       </c>
@@ -4820,45 +4843,45 @@
       <c r="K36">
         <v>120</v>
       </c>
-      <c r="M36">
+      <c r="N36">
         <v>13052</v>
       </c>
-      <c r="N36">
+      <c r="O36">
         <v>150</v>
       </c>
-      <c r="O36">
+      <c r="P36">
         <v>0.38750000000000001</v>
       </c>
-      <c r="P36">
+      <c r="Q36">
         <f t="shared" si="3"/>
         <v>569.625</v>
       </c>
-      <c r="Q36">
+      <c r="R36">
         <f t="shared" si="0"/>
         <v>144</v>
       </c>
-      <c r="R36">
+      <c r="S36">
         <f t="shared" si="16"/>
         <v>450000</v>
       </c>
-      <c r="S36">
+      <c r="T36">
         <f t="shared" si="1"/>
         <v>119</v>
       </c>
-      <c r="T36">
+      <c r="U36">
         <f t="shared" si="2"/>
         <v>26775</v>
       </c>
-      <c r="U36">
+      <c r="V36">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AB36" s="2" t="e">
+      <c r="AC36" s="2" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>194</v>
       </c>
@@ -4883,45 +4906,45 @@
       <c r="K37">
         <v>120</v>
       </c>
-      <c r="M37">
+      <c r="N37">
         <v>13052</v>
       </c>
-      <c r="N37">
+      <c r="O37">
         <v>184</v>
       </c>
-      <c r="O37">
+      <c r="P37">
         <v>0.42099999999999999</v>
       </c>
-      <c r="P37">
+      <c r="Q37">
         <f t="shared" si="3"/>
         <v>759.1472</v>
       </c>
-      <c r="Q37">
+      <c r="R37">
         <f t="shared" si="0"/>
         <v>146</v>
       </c>
-      <c r="R37">
+      <c r="S37">
         <f t="shared" si="16"/>
         <v>456250</v>
       </c>
-      <c r="S37">
+      <c r="T37">
         <f t="shared" si="1"/>
         <v>118</v>
       </c>
-      <c r="T37">
+      <c r="U37">
         <f t="shared" si="2"/>
         <v>26550</v>
       </c>
-      <c r="U37">
+      <c r="V37">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AB37" s="2" t="e">
+      <c r="AC37" s="2" t="e">
         <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>254</v>
       </c>
@@ -4949,61 +4972,61 @@
       <c r="K38">
         <v>100</v>
       </c>
-      <c r="M38">
+      <c r="N38">
         <v>8702</v>
       </c>
-      <c r="N38">
+      <c r="O38">
         <v>184</v>
       </c>
-      <c r="O38">
+      <c r="P38">
         <v>0.34799999999999998</v>
       </c>
-      <c r="P38">
+      <c r="Q38">
         <f t="shared" si="3"/>
         <v>627.5136</v>
       </c>
-      <c r="Q38">
+      <c r="R38">
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
-      <c r="R38">
+      <c r="S38">
         <f t="shared" si="16"/>
         <v>390625</v>
       </c>
-      <c r="S38">
+      <c r="T38">
         <f t="shared" si="1"/>
         <v>97</v>
       </c>
-      <c r="T38">
+      <c r="U38">
         <f t="shared" si="2"/>
         <v>21825</v>
       </c>
-      <c r="U38">
+      <c r="V38">
         <v>8</v>
       </c>
-      <c r="V38">
+      <c r="W38">
         <v>2</v>
       </c>
-      <c r="W38">
+      <c r="X38">
         <v>4</v>
       </c>
-      <c r="X38">
+      <c r="Y38">
         <v>2</v>
       </c>
-      <c r="Y38"/>
       <c r="Z38"/>
       <c r="AA38"/>
-      <c r="AB38" s="2" t="e">
+      <c r="AB38"/>
+      <c r="AC38" s="2" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="AC38" s="2" t="s">
+      <c r="AD38" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="AD38" t="s">
+      <c r="AE38" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>259</v>
       </c>
@@ -5034,61 +5057,61 @@
       <c r="K39">
         <v>140</v>
       </c>
-      <c r="M39">
+      <c r="N39">
         <v>4351</v>
       </c>
-      <c r="N39">
+      <c r="O39">
         <v>86</v>
       </c>
-      <c r="O39">
+      <c r="P39">
         <v>0.27900000000000003</v>
       </c>
-      <c r="P39">
+      <c r="Q39">
         <f t="shared" si="3"/>
         <v>235.14120000000005</v>
       </c>
-      <c r="Q39">
+      <c r="R39">
         <f t="shared" si="0"/>
         <v>79</v>
       </c>
-      <c r="R39">
+      <c r="S39">
         <f t="shared" si="16"/>
         <v>246875</v>
       </c>
-      <c r="S39">
+      <c r="T39">
         <f t="shared" si="1"/>
         <v>67</v>
       </c>
-      <c r="T39">
+      <c r="U39">
         <f t="shared" si="2"/>
         <v>15075</v>
       </c>
-      <c r="U39">
+      <c r="V39">
         <v>10</v>
       </c>
-      <c r="V39">
+      <c r="W39">
         <v>2</v>
       </c>
-      <c r="W39">
+      <c r="X39">
         <v>6</v>
       </c>
-      <c r="X39">
+      <c r="Y39">
         <v>2</v>
       </c>
-      <c r="Y39"/>
       <c r="Z39"/>
       <c r="AA39"/>
-      <c r="AB39" s="2" t="e">
+      <c r="AB39"/>
+      <c r="AC39" s="2" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="AC39" s="2" t="s">
+      <c r="AD39" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="AD39" t="s">
+      <c r="AE39" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>261</v>
       </c>
@@ -5119,61 +5142,61 @@
       <c r="K40">
         <v>100</v>
       </c>
-      <c r="M40">
+      <c r="N40">
         <v>6526</v>
       </c>
-      <c r="N40">
+      <c r="O40">
         <v>138</v>
       </c>
-      <c r="O40">
+      <c r="P40">
         <v>0.35899999999999999</v>
       </c>
-      <c r="P40">
+      <c r="Q40">
         <f t="shared" si="3"/>
         <v>485.51160000000004</v>
       </c>
-      <c r="Q40">
+      <c r="R40">
         <f t="shared" si="0"/>
         <v>105</v>
       </c>
-      <c r="R40">
+      <c r="S40">
         <f t="shared" si="16"/>
         <v>328125</v>
       </c>
-      <c r="S40">
+      <c r="T40">
         <f t="shared" si="1"/>
         <v>83</v>
       </c>
-      <c r="T40">
+      <c r="U40">
         <f t="shared" si="2"/>
         <v>18675</v>
       </c>
-      <c r="U40">
+      <c r="V40">
         <v>10</v>
       </c>
-      <c r="V40">
+      <c r="W40">
         <v>2</v>
       </c>
-      <c r="W40">
+      <c r="X40">
         <v>6</v>
       </c>
-      <c r="X40">
+      <c r="Y40">
         <v>2</v>
       </c>
-      <c r="Y40"/>
       <c r="Z40"/>
       <c r="AA40"/>
-      <c r="AB40" s="2" t="e">
+      <c r="AB40"/>
+      <c r="AC40" s="2" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="AC40" s="2" t="s">
+      <c r="AD40" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="AD40" t="s">
+      <c r="AE40" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>263</v>
       </c>
@@ -5204,61 +5227,61 @@
       <c r="K41">
         <v>100</v>
       </c>
-      <c r="M41">
+      <c r="N41">
         <v>6526</v>
       </c>
-      <c r="N41">
+      <c r="O41">
         <v>138</v>
       </c>
-      <c r="O41">
+      <c r="P41">
         <v>0.35899999999999999</v>
       </c>
-      <c r="P41">
+      <c r="Q41">
         <f t="shared" si="3"/>
         <v>485.51160000000004</v>
       </c>
-      <c r="Q41">
+      <c r="R41">
         <f t="shared" si="0"/>
         <v>107</v>
       </c>
-      <c r="R41">
+      <c r="S41">
         <f t="shared" si="16"/>
         <v>334375</v>
       </c>
-      <c r="S41">
+      <c r="T41">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
-      <c r="T41">
+      <c r="U41">
         <f t="shared" si="2"/>
         <v>18900</v>
       </c>
-      <c r="U41">
+      <c r="V41">
         <v>10</v>
       </c>
-      <c r="V41">
+      <c r="W41">
         <v>2</v>
       </c>
-      <c r="W41">
+      <c r="X41">
         <v>6</v>
       </c>
-      <c r="X41">
+      <c r="Y41">
         <v>2</v>
       </c>
-      <c r="Y41"/>
       <c r="Z41"/>
       <c r="AA41"/>
-      <c r="AB41" s="2" t="e">
+      <c r="AB41"/>
+      <c r="AC41" s="2" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="AC41" s="2" t="s">
+      <c r="AD41" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="AD41" t="s">
+      <c r="AE41" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>265</v>
       </c>
@@ -5289,61 +5312,61 @@
       <c r="K42">
         <v>100</v>
       </c>
-      <c r="M42">
+      <c r="N42">
         <v>6526</v>
       </c>
-      <c r="N42">
+      <c r="O42">
         <v>138</v>
       </c>
-      <c r="O42">
+      <c r="P42">
         <v>0.35899999999999999</v>
       </c>
-      <c r="P42">
+      <c r="Q42">
         <f t="shared" si="3"/>
         <v>485.51160000000004</v>
       </c>
-      <c r="Q42">
+      <c r="R42">
         <f t="shared" si="0"/>
         <v>99</v>
       </c>
-      <c r="R42">
+      <c r="S42">
         <f t="shared" si="16"/>
         <v>309375</v>
       </c>
-      <c r="S42">
+      <c r="T42">
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
-      <c r="T42">
+      <c r="U42">
         <f t="shared" si="2"/>
         <v>18450</v>
       </c>
-      <c r="U42">
+      <c r="V42">
         <v>10</v>
       </c>
-      <c r="V42">
+      <c r="W42">
         <v>2</v>
       </c>
-      <c r="W42">
+      <c r="X42">
         <v>6</v>
       </c>
-      <c r="X42">
+      <c r="Y42">
         <v>2</v>
       </c>
-      <c r="Y42"/>
       <c r="Z42"/>
       <c r="AA42"/>
-      <c r="AB42" s="2" t="e">
+      <c r="AB42"/>
+      <c r="AC42" s="2" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="AC42" s="2" t="s">
+      <c r="AD42" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="AD42" t="s">
+      <c r="AE42" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>268</v>
       </c>
@@ -5374,61 +5397,61 @@
       <c r="K43">
         <v>100</v>
       </c>
-      <c r="M43">
+      <c r="N43">
         <v>6526</v>
       </c>
-      <c r="N43">
+      <c r="O43">
         <v>150</v>
       </c>
-      <c r="O43">
+      <c r="P43">
         <v>0.33</v>
       </c>
-      <c r="P43">
+      <c r="Q43">
         <f t="shared" si="3"/>
         <v>485.1</v>
       </c>
-      <c r="Q43">
+      <c r="R43">
         <f t="shared" si="0"/>
         <v>101</v>
       </c>
-      <c r="R43">
+      <c r="S43">
         <f t="shared" si="16"/>
         <v>315625</v>
       </c>
-      <c r="S43">
+      <c r="T43">
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
-      <c r="T43">
+      <c r="U43">
         <f t="shared" si="2"/>
         <v>18450</v>
       </c>
-      <c r="U43">
+      <c r="V43">
         <v>10</v>
       </c>
-      <c r="V43">
+      <c r="W43">
         <v>2</v>
       </c>
-      <c r="W43">
+      <c r="X43">
         <v>6</v>
       </c>
-      <c r="X43">
+      <c r="Y43">
         <v>2</v>
       </c>
-      <c r="Y43"/>
       <c r="Z43"/>
       <c r="AA43"/>
-      <c r="AB43" s="2" t="e">
+      <c r="AB43"/>
+      <c r="AC43" s="2" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="AC43" s="2" t="s">
+      <c r="AD43" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="AD43" t="s">
+      <c r="AE43" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>270</v>
       </c>
@@ -5459,64 +5482,64 @@
       <c r="K44">
         <v>120</v>
       </c>
-      <c r="M44">
+      <c r="N44">
         <v>6526</v>
       </c>
-      <c r="N44">
+      <c r="O44">
         <v>132</v>
       </c>
-      <c r="O44">
+      <c r="P44">
         <v>0.24099999999999999</v>
       </c>
-      <c r="P44">
+      <c r="Q44">
         <f t="shared" si="3"/>
         <v>311.75760000000002</v>
       </c>
-      <c r="Q44">
+      <c r="R44">
         <f t="shared" si="0"/>
         <v>105</v>
       </c>
-      <c r="R44">
+      <c r="S44">
         <f t="shared" si="16"/>
         <v>328125</v>
       </c>
-      <c r="S44">
+      <c r="T44">
         <f t="shared" si="1"/>
         <v>83</v>
       </c>
-      <c r="T44">
+      <c r="U44">
         <f t="shared" si="2"/>
         <v>18675</v>
       </c>
-      <c r="U44">
+      <c r="V44">
         <v>10</v>
       </c>
-      <c r="V44">
+      <c r="W44">
         <v>2</v>
       </c>
-      <c r="W44">
+      <c r="X44">
         <v>6</v>
       </c>
-      <c r="X44">
+      <c r="Y44">
         <v>2</v>
       </c>
-      <c r="Y44"/>
       <c r="Z44"/>
       <c r="AA44"/>
-      <c r="AB44" s="2" t="e">
+      <c r="AB44"/>
+      <c r="AC44" s="2" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="AC44" s="2" t="s">
+      <c r="AD44" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="AD44" t="s">
+      <c r="AE44" t="s">
         <v>267</v>
       </c>
-      <c r="AE44" t="s">
+      <c r="AF44" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>273</v>
       </c>
@@ -5544,64 +5567,64 @@
       <c r="K45">
         <v>170</v>
       </c>
-      <c r="M45">
+      <c r="N45">
         <v>6526</v>
       </c>
-      <c r="N45">
+      <c r="O45">
         <v>126</v>
       </c>
-      <c r="O45">
+      <c r="P45">
         <v>0.19800000000000001</v>
       </c>
-      <c r="P45">
+      <c r="Q45">
         <f t="shared" si="3"/>
         <v>244.49040000000002</v>
       </c>
-      <c r="Q45">
+      <c r="R45">
         <f t="shared" si="0"/>
         <v>108</v>
       </c>
-      <c r="R45">
+      <c r="S45">
         <f t="shared" si="16"/>
         <v>337500</v>
       </c>
-      <c r="S45">
+      <c r="T45">
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
-      <c r="T45">
+      <c r="U45">
         <f t="shared" si="2"/>
         <v>19350</v>
       </c>
-      <c r="U45">
+      <c r="V45">
         <v>10</v>
       </c>
-      <c r="V45">
+      <c r="W45">
         <v>2</v>
       </c>
-      <c r="W45">
+      <c r="X45">
         <v>6</v>
       </c>
-      <c r="X45">
+      <c r="Y45">
         <v>2</v>
       </c>
-      <c r="Y45"/>
       <c r="Z45"/>
       <c r="AA45"/>
-      <c r="AB45" s="2" t="e">
+      <c r="AB45"/>
+      <c r="AC45" s="2" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="AC45" s="2" t="s">
+      <c r="AD45" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="AD45" t="s">
+      <c r="AE45" t="s">
         <v>267</v>
       </c>
-      <c r="AE45" t="s">
+      <c r="AF45" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>347</v>
       </c>
@@ -5634,51 +5657,52 @@
         <v>120</v>
       </c>
       <c r="L46" s="5"/>
-      <c r="M46" s="5">
+      <c r="M46" s="5"/>
+      <c r="N46" s="5">
         <v>3300</v>
       </c>
-      <c r="N46" s="5">
+      <c r="O46" s="5">
         <v>138</v>
       </c>
-      <c r="O46" s="5">
+      <c r="P46" s="5">
         <v>0.27876367899999999</v>
       </c>
-      <c r="P46">
+      <c r="Q46">
         <f t="shared" si="3"/>
         <v>376.99999947960004</v>
       </c>
-      <c r="Q46" s="5">
+      <c r="R46" s="5">
         <v>76</v>
       </c>
-      <c r="R46" s="5">
+      <c r="S46" s="5">
         <v>237500</v>
       </c>
-      <c r="S46" s="5">
+      <c r="T46" s="5">
         <v>58</v>
       </c>
-      <c r="T46" s="5">
+      <c r="U46" s="5">
         <v>14137.5</v>
       </c>
-      <c r="U46" s="5">
+      <c r="V46" s="5">
         <v>10</v>
       </c>
-      <c r="V46">
+      <c r="W46">
         <v>2</v>
       </c>
-      <c r="W46">
+      <c r="X46">
         <v>6</v>
       </c>
-      <c r="X46">
+      <c r="Y46">
         <v>2</v>
       </c>
-      <c r="AC46" s="2" t="s">
+      <c r="AD46" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="AD46" t="s">
+      <c r="AE46" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>349</v>
       </c>
@@ -5711,51 +5735,52 @@
         <v>100</v>
       </c>
       <c r="L47" s="5"/>
-      <c r="M47" s="5">
+      <c r="M47" s="5"/>
+      <c r="N47" s="5">
         <v>3600</v>
       </c>
-      <c r="N47" s="5">
+      <c r="O47" s="5">
         <v>138</v>
       </c>
-      <c r="O47" s="5">
+      <c r="P47" s="5">
         <v>0.32534753</v>
       </c>
-      <c r="P47">
+      <c r="Q47">
         <f t="shared" si="3"/>
         <v>439.99999957200004</v>
       </c>
-      <c r="Q47" s="5">
+      <c r="R47" s="5">
         <v>81</v>
       </c>
-      <c r="R47" s="5">
+      <c r="S47" s="5">
         <v>253125</v>
       </c>
-      <c r="S47" s="5">
+      <c r="T47" s="5">
         <v>61</v>
       </c>
-      <c r="T47" s="5">
+      <c r="U47" s="5">
         <v>14868.75</v>
       </c>
-      <c r="U47" s="5">
+      <c r="V47" s="5">
         <v>10</v>
       </c>
-      <c r="V47">
+      <c r="W47">
         <v>2</v>
       </c>
-      <c r="W47">
+      <c r="X47">
         <v>6</v>
       </c>
-      <c r="X47">
+      <c r="Y47">
         <v>2</v>
       </c>
-      <c r="AC47" s="2" t="s">
+      <c r="AD47" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="AD47" t="s">
+      <c r="AE47" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>351</v>
       </c>
@@ -5786,51 +5811,52 @@
         <v>100</v>
       </c>
       <c r="L48" s="5"/>
-      <c r="M48" s="5">
+      <c r="M48" s="5"/>
+      <c r="N48" s="5">
         <v>4214</v>
       </c>
-      <c r="N48" s="5">
+      <c r="O48" s="5">
         <v>143.5</v>
       </c>
-      <c r="O48" s="5">
+      <c r="P48" s="5">
         <v>0.34132119700000002</v>
       </c>
-      <c r="P48">
+      <c r="Q48">
         <f t="shared" si="3"/>
         <v>479.99999934110008</v>
       </c>
-      <c r="Q48" s="5">
+      <c r="R48" s="5">
         <v>86</v>
       </c>
-      <c r="R48" s="5">
+      <c r="S48" s="5">
         <v>268750</v>
       </c>
-      <c r="S48" s="5">
+      <c r="T48" s="5">
         <v>66</v>
       </c>
-      <c r="T48" s="5">
+      <c r="U48" s="5">
         <v>16087.5</v>
       </c>
-      <c r="U48" s="5">
+      <c r="V48" s="5">
         <v>10</v>
       </c>
-      <c r="V48">
+      <c r="W48">
         <v>2</v>
       </c>
-      <c r="W48">
+      <c r="X48">
         <v>6</v>
       </c>
-      <c r="X48">
+      <c r="Y48">
         <v>2</v>
       </c>
-      <c r="AC48" s="2" t="s">
+      <c r="AD48" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="AD48" t="s">
+      <c r="AE48" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="49" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>355</v>
       </c>
@@ -5858,56 +5884,56 @@
       <c r="K49">
         <v>100</v>
       </c>
-      <c r="M49">
+      <c r="N49">
         <v>4000</v>
       </c>
-      <c r="N49">
+      <c r="O49">
         <v>138</v>
       </c>
-      <c r="O49">
+      <c r="P49">
         <v>0.35499999999999998</v>
       </c>
-      <c r="P49">
+      <c r="Q49">
         <f t="shared" si="3"/>
         <v>480.10199999999998</v>
       </c>
-      <c r="Q49">
-        <f>MEDIAN(255, ROUND((N49/10+SQRT(K49)/20+SQRT(M49)+O49+20-J49), 0), 0)</f>
+      <c r="R49">
+        <f>MEDIAN(255, ROUND((O49/10+SQRT(K49)/20+SQRT(N49)+P49+20-J49), 0), 0)</f>
         <v>84</v>
       </c>
-      <c r="R49">
-        <f t="shared" ref="R49:R52" si="20">Q49*50000/16</f>
+      <c r="S49">
+        <f t="shared" ref="S49:S52" si="20">R49*50000/16</f>
         <v>262500</v>
       </c>
-      <c r="S49">
-        <f>MEDIAN(0, 255, ROUND(SQRT(K49)/100+SQRT(M49)+O49+40/J49-2,0))</f>
+      <c r="T49">
+        <f>MEDIAN(0, 255, ROUND(SQRT(K49)/100+SQRT(N49)+P49+40/J49-2,0))</f>
         <v>65</v>
       </c>
-      <c r="T49">
-        <f>IF(E49="Steam", S49*350/16*12, IF(E49="Diesel", S49*325/16*12,  S49*300/16*12))</f>
+      <c r="U49">
+        <f>IF(E49="Steam", T49*350/16*12, IF(E49="Diesel", T49*325/16*12,  T49*300/16*12))</f>
         <v>15843.75</v>
       </c>
-      <c r="U49">
-        <f t="shared" ref="U49" si="21">V49+W49+X49</f>
+      <c r="V49">
+        <f t="shared" ref="V49" si="21">W49+X49+Y49</f>
         <v>10</v>
       </c>
-      <c r="V49">
+      <c r="W49">
         <v>2</v>
       </c>
-      <c r="W49">
+      <c r="X49">
         <v>6</v>
       </c>
-      <c r="X49">
+      <c r="Y49">
         <v>2</v>
-      </c>
-      <c r="AC49" s="2" t="s">
-        <v>258</v>
       </c>
       <c r="AD49" s="2" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="50" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE49" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="50" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>388</v>
       </c>
@@ -5936,55 +5962,56 @@
         <v>100</v>
       </c>
       <c r="L50" s="5"/>
-      <c r="M50" s="5">
+      <c r="M50" s="5"/>
+      <c r="N50" s="5">
         <v>11828</v>
       </c>
-      <c r="N50" s="5">
+      <c r="O50" s="5">
         <v>276</v>
       </c>
-      <c r="O50">
+      <c r="P50">
         <v>0.34699999999999998</v>
       </c>
-      <c r="P50">
+      <c r="Q50">
         <f t="shared" si="3"/>
         <v>938.56560000000002</v>
       </c>
-      <c r="Q50">
-        <f>MEDIAN(255, ROUND((N50/10+SQRT(K50)/20+SQRT(M50)+O50+20-J50), 0), 0)</f>
+      <c r="R50">
+        <f>MEDIAN(255, ROUND((O50/10+SQRT(K50)/20+SQRT(N50)+P50+20-J50), 0), 0)</f>
         <v>147</v>
       </c>
-      <c r="R50">
+      <c r="S50">
         <f t="shared" si="20"/>
         <v>459375</v>
       </c>
-      <c r="S50">
-        <f>MEDIAN(0, 255, ROUND(SQRT(K50)/100+SQRT(M50)+O50+40/J50-2,0))</f>
+      <c r="T50">
+        <f>MEDIAN(0, 255, ROUND(SQRT(K50)/100+SQRT(N50)+P50+40/J50-2,0))</f>
         <v>111</v>
       </c>
-      <c r="T50">
-        <f>IF(E50="Steam", S50*350/16*12, IF(E50="Diesel", S50*325/16*12,  S50*300/16*12))</f>
+      <c r="U50">
+        <f>IF(E50="Steam", T50*350/16*12, IF(E50="Diesel", T50*325/16*12,  T50*300/16*12))</f>
         <v>24975</v>
       </c>
-      <c r="U50" s="5">
+      <c r="V50" s="5">
         <v>10</v>
       </c>
-      <c r="V50">
+      <c r="W50">
         <v>2</v>
       </c>
-      <c r="W50">
+      <c r="X50">
         <v>6</v>
       </c>
-      <c r="X50">
+      <c r="Y50">
         <v>2</v>
       </c>
-      <c r="AC50" s="2" t="s">
+      <c r="AD50" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="AD50" t="s">
+      <c r="AE50" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>417</v>
       </c>
@@ -6010,55 +6037,56 @@
         <v>100</v>
       </c>
       <c r="L51" s="5"/>
-      <c r="M51" s="5">
+      <c r="M51" s="5"/>
+      <c r="N51" s="5">
         <v>1800</v>
       </c>
-      <c r="N51" s="5">
+      <c r="O51" s="5">
         <v>126</v>
       </c>
-      <c r="O51" s="5">
+      <c r="P51" s="5">
         <v>0.245</v>
       </c>
-      <c r="P51">
+      <c r="Q51">
         <f t="shared" si="3"/>
         <v>302.52600000000001</v>
       </c>
-      <c r="Q51">
-        <f>MEDIAN(255, ROUND((N51/10+SQRT(K51)/20+SQRT(M51)+O51+20-J51), 0), 0)</f>
+      <c r="R51">
+        <f>MEDIAN(255, ROUND((O51/10+SQRT(K51)/20+SQRT(N51)+P51+20-J51), 0), 0)</f>
         <v>60</v>
       </c>
-      <c r="R51">
+      <c r="S51">
         <f t="shared" si="20"/>
         <v>187500</v>
       </c>
-      <c r="S51">
-        <f>MEDIAN(0, 255, ROUND(SQRT(K51)/100+SQRT(M51)+O51+40/J51-2,0))</f>
+      <c r="T51">
+        <f>MEDIAN(0, 255, ROUND(SQRT(K51)/100+SQRT(N51)+P51+40/J51-2,0))</f>
         <v>43</v>
       </c>
-      <c r="T51">
-        <f>IF(E51="Steam", S51*350/16*12, IF(E51="Diesel", S51*325/16*12,  S51*300/16*12))</f>
+      <c r="U51">
+        <f>IF(E51="Steam", T51*350/16*12, IF(E51="Diesel", T51*325/16*12,  T51*300/16*12))</f>
         <v>10481.25</v>
       </c>
-      <c r="U51" s="5">
+      <c r="V51" s="5">
         <v>10</v>
       </c>
-      <c r="V51">
+      <c r="W51">
         <v>2</v>
       </c>
-      <c r="W51">
+      <c r="X51">
         <v>4</v>
       </c>
-      <c r="X51">
+      <c r="Y51">
         <v>2</v>
       </c>
-      <c r="AC51" s="2" t="s">
+      <c r="AD51" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="AD51" t="s">
+      <c r="AE51" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="52" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>418</v>
       </c>
@@ -6084,55 +6112,59 @@
         <v>100</v>
       </c>
       <c r="L52" s="5"/>
-      <c r="M52" s="5">
+      <c r="M52">
+        <f t="shared" ref="M52:M67" si="22">ROUND(L52*0.745699872,0)</f>
+        <v>0</v>
+      </c>
+      <c r="N52" s="5">
         <v>6282</v>
       </c>
-      <c r="N52" s="5">
+      <c r="O52" s="5">
         <v>138</v>
       </c>
-      <c r="O52" s="5">
+      <c r="P52" s="5">
         <v>0.377</v>
       </c>
-      <c r="P52">
+      <c r="Q52">
         <f t="shared" si="3"/>
         <v>509.85480000000007</v>
       </c>
-      <c r="Q52">
-        <f>MEDIAN(255, ROUND((N52/10+SQRT(K52)/20+SQRT(M52)+O52+20-J52), 0), 0)</f>
+      <c r="R52">
+        <f>MEDIAN(255, ROUND((O52/10+SQRT(K52)/20+SQRT(N52)+P52+20-J52), 0), 0)</f>
         <v>102</v>
       </c>
-      <c r="R52">
+      <c r="S52">
         <f t="shared" si="20"/>
         <v>318750</v>
       </c>
-      <c r="S52">
-        <f>MEDIAN(0, 255, ROUND(SQRT(K52)/100+SQRT(M52)+O52+40/J52-2,0))</f>
+      <c r="T52">
+        <f>MEDIAN(0, 255, ROUND(SQRT(K52)/100+SQRT(N52)+P52+40/J52-2,0))</f>
         <v>81</v>
       </c>
-      <c r="T52">
-        <f>IF(E52="Steam", S52*350/16*12, IF(E52="Diesel", S52*325/16*12,  S52*300/16*12))</f>
+      <c r="U52">
+        <f>IF(E52="Steam", T52*350/16*12, IF(E52="Diesel", T52*325/16*12,  T52*300/16*12))</f>
         <v>18225</v>
       </c>
-      <c r="U52" s="5">
+      <c r="V52" s="5">
         <v>10</v>
       </c>
-      <c r="V52">
+      <c r="W52">
         <v>2</v>
       </c>
-      <c r="W52">
+      <c r="X52">
         <v>6</v>
       </c>
-      <c r="X52">
+      <c r="Y52">
         <v>2</v>
       </c>
-      <c r="AC52" s="2" t="s">
+      <c r="AD52" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="AD52" t="s">
+      <c r="AE52" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="53" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>431</v>
       </c>
@@ -6161,50 +6193,54 @@
         <v>160</v>
       </c>
       <c r="M53">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="N53">
         <v>9816</v>
       </c>
-      <c r="N53">
+      <c r="O53">
         <v>291</v>
       </c>
-      <c r="O53">
+      <c r="P53">
         <v>0.17199999999999999</v>
       </c>
-      <c r="P53">
+      <c r="Q53">
         <f t="shared" si="3"/>
         <v>490.50959999999998</v>
       </c>
-      <c r="Q53" s="5">
+      <c r="R53" s="5">
         <v>135</v>
       </c>
-      <c r="R53">
+      <c r="S53">
         <v>421875</v>
       </c>
-      <c r="S53">
+      <c r="T53">
         <v>100</v>
       </c>
-      <c r="T53">
+      <c r="U53">
         <v>24375</v>
       </c>
-      <c r="U53" t="s">
+      <c r="V53" t="s">
         <v>433</v>
       </c>
-      <c r="V53">
+      <c r="W53">
         <v>2</v>
       </c>
-      <c r="W53">
+      <c r="X53">
         <v>6</v>
       </c>
-      <c r="X53">
+      <c r="Y53">
         <v>2</v>
       </c>
-      <c r="AC53" s="2" t="s">
+      <c r="AD53" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="AD53" t="s">
+      <c r="AE53" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="54" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>435</v>
       </c>
@@ -6236,38 +6272,42 @@
         <v>100</v>
       </c>
       <c r="M54">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="N54">
         <v>1264</v>
       </c>
-      <c r="N54">
+      <c r="O54">
         <v>120</v>
       </c>
-      <c r="O54">
+      <c r="P54">
         <v>0.32300000000000001</v>
       </c>
-      <c r="P54">
+      <c r="Q54">
         <f t="shared" si="3"/>
         <v>379.84800000000001</v>
       </c>
-      <c r="Q54">
+      <c r="R54">
         <v>48</v>
       </c>
-      <c r="R54">
+      <c r="S54">
         <v>150000</v>
       </c>
-      <c r="S54">
+      <c r="T54">
         <v>36</v>
       </c>
-      <c r="T54">
+      <c r="U54">
         <v>8775</v>
       </c>
-      <c r="AC54" s="2" t="s">
+      <c r="AD54" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="AD54" t="s">
+      <c r="AE54" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="55" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>437</v>
       </c>
@@ -6290,41 +6330,45 @@
         <v>120</v>
       </c>
       <c r="M55">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="N55">
         <v>13052</v>
       </c>
-      <c r="N55">
+      <c r="O55">
         <v>184</v>
       </c>
-      <c r="O55">
+      <c r="P55">
         <v>0.42099999999999999</v>
       </c>
-      <c r="P55">
+      <c r="Q55">
         <f t="shared" si="3"/>
         <v>759.1472</v>
       </c>
-      <c r="Q55">
+      <c r="R55">
         <v>146</v>
       </c>
-      <c r="R55">
+      <c r="S55">
         <v>456250</v>
       </c>
-      <c r="S55">
+      <c r="T55">
         <v>118</v>
       </c>
-      <c r="T55">
+      <c r="U55">
         <v>26550</v>
       </c>
-      <c r="U55">
-        <v>0</v>
-      </c>
-      <c r="AB55" s="2" t="e">
+      <c r="V55">
+        <v>0</v>
+      </c>
+      <c r="AC55" s="2" t="e">
         <v>#DIV/0!</v>
       </c>
-      <c r="AC55" s="2" t="s">
+      <c r="AD55" s="2" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="56" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>439</v>
       </c>
@@ -6353,38 +6397,42 @@
         <v>100</v>
       </c>
       <c r="M56">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="N56">
         <v>13052</v>
       </c>
-      <c r="N56">
+      <c r="O56">
         <v>240</v>
       </c>
-      <c r="O56">
+      <c r="P56">
         <v>0.38690476200000001</v>
       </c>
-      <c r="P56">
+      <c r="Q56">
         <f t="shared" si="3"/>
         <v>910.00000022400002</v>
       </c>
-      <c r="Q56">
+      <c r="R56">
         <v>151</v>
       </c>
-      <c r="R56">
+      <c r="S56">
         <v>471875</v>
       </c>
-      <c r="S56">
+      <c r="T56">
         <v>118</v>
       </c>
-      <c r="T56">
+      <c r="U56">
         <v>26550</v>
       </c>
-      <c r="U56" t="s">
+      <c r="V56" t="s">
         <v>442</v>
       </c>
-      <c r="AC56" s="2" t="s">
+      <c r="AD56" s="2" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="57" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>443</v>
       </c>
@@ -6413,41 +6461,45 @@
         <v>100</v>
       </c>
       <c r="M57">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="N57">
         <v>5438</v>
       </c>
-      <c r="N57">
+      <c r="O57">
         <v>276</v>
       </c>
-      <c r="O57">
+      <c r="P57">
         <v>0.31425613699999999</v>
       </c>
-      <c r="P57">
+      <c r="Q57">
         <f t="shared" si="3"/>
         <v>849.99999935760013</v>
       </c>
-      <c r="Q57">
+      <c r="R57">
         <v>108</v>
       </c>
-      <c r="R57">
+      <c r="S57">
         <v>337500</v>
       </c>
-      <c r="S57">
+      <c r="T57">
         <v>75</v>
       </c>
-      <c r="T57">
+      <c r="U57">
         <v>18281.25</v>
       </c>
-      <c r="U57" t="s">
+      <c r="V57" t="s">
         <v>433</v>
       </c>
-      <c r="AC57" s="2" t="s">
+      <c r="AD57" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="AD57" t="s">
+      <c r="AE57" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="58" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>445</v>
       </c>
@@ -6476,41 +6528,45 @@
         <v>90</v>
       </c>
       <c r="M58">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="N58">
         <v>5302</v>
       </c>
-      <c r="N58">
+      <c r="O58">
         <v>138</v>
       </c>
-      <c r="O58">
+      <c r="P58">
         <v>0.36010056200000001</v>
       </c>
-      <c r="P58">
+      <c r="Q58">
         <f t="shared" si="3"/>
         <v>487.00000004880008</v>
       </c>
-      <c r="Q58">
+      <c r="R58">
         <v>87</v>
       </c>
-      <c r="R58">
+      <c r="S58">
         <v>271875</v>
       </c>
-      <c r="S58">
+      <c r="T58">
         <v>73</v>
       </c>
-      <c r="T58">
+      <c r="U58">
         <v>16425</v>
       </c>
-      <c r="U58">
+      <c r="V58">
         <v>10</v>
       </c>
-      <c r="AC58" s="2" t="s">
+      <c r="AD58" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="AD58" t="s">
+      <c r="AE58" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="59" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>447</v>
       </c>
@@ -6542,43 +6598,44 @@
         <v>100</v>
       </c>
       <c r="M59">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="N59">
         <v>2610</v>
       </c>
-      <c r="N59">
+      <c r="O59">
         <v>138</v>
       </c>
-      <c r="O59">
+      <c r="P59">
         <v>0.30499999999999999</v>
       </c>
-      <c r="P59">
+      <c r="Q59">
         <f t="shared" si="3"/>
         <v>412.48199999999997</v>
       </c>
-      <c r="Q59">
+      <c r="R59">
         <v>72</v>
       </c>
-      <c r="R59">
+      <c r="S59">
         <v>225000</v>
       </c>
-      <c r="S59">
+      <c r="T59">
         <v>52</v>
       </c>
-      <c r="T59">
+      <c r="U59">
         <v>12675</v>
       </c>
-      <c r="U59">
+      <c r="V59">
         <v>10</v>
       </c>
-      <c r="V59">
+      <c r="W59">
         <v>1</v>
       </c>
-      <c r="W59">
+      <c r="X59">
         <v>8</v>
       </c>
-      <c r="X59">
-        <v>1</v>
-      </c>
-      <c r="Y59" s="1">
+      <c r="Y59">
         <v>1</v>
       </c>
       <c r="Z59" s="1">
@@ -6587,17 +6644,20 @@
       <c r="AA59" s="1">
         <v>1</v>
       </c>
-      <c r="AB59" s="2">
+      <c r="AB59" s="1">
         <v>1</v>
       </c>
-      <c r="AC59" s="2" t="s">
+      <c r="AC59" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD59" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="AD59" t="s">
+      <c r="AE59" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="s">
         <v>451</v>
       </c>
@@ -6629,35 +6689,39 @@
         <v>80</v>
       </c>
       <c r="L60" s="8"/>
-      <c r="M60" s="8">
+      <c r="M60">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="N60" s="8">
         <v>1500</v>
       </c>
-      <c r="N60" s="8">
+      <c r="O60" s="8">
         <v>140</v>
       </c>
-      <c r="O60" s="8">
+      <c r="P60" s="8">
         <v>0.14868804699999999</v>
       </c>
-      <c r="P60" s="8">
+      <c r="Q60" s="8">
         <v>204</v>
       </c>
-      <c r="Q60" s="8">
+      <c r="R60" s="8">
         <v>53</v>
       </c>
-      <c r="R60" s="8">
+      <c r="S60" s="8">
         <v>165625</v>
       </c>
-      <c r="S60" s="8">
+      <c r="T60" s="8">
         <v>39</v>
       </c>
-      <c r="T60" s="8">
+      <c r="U60" s="8">
         <v>10237.5</v>
       </c>
-      <c r="AC60" s="2" t="s">
+      <c r="AD60" s="2" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="61" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
         <v>453</v>
       </c>
@@ -6689,51 +6753,55 @@
         <v>170</v>
       </c>
       <c r="L61" s="8"/>
-      <c r="M61" s="8">
+      <c r="M61">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="N61" s="8">
         <v>6526</v>
       </c>
-      <c r="N61" s="8">
+      <c r="O61" s="8">
         <v>126</v>
       </c>
-      <c r="O61" s="8">
+      <c r="P61" s="8">
         <v>0.198412698</v>
       </c>
-      <c r="P61" s="8">
+      <c r="Q61" s="8">
         <v>245</v>
       </c>
-      <c r="Q61" s="8">
+      <c r="R61" s="8">
         <v>106</v>
       </c>
-      <c r="R61" s="8">
+      <c r="S61" s="8">
         <v>331250</v>
       </c>
-      <c r="S61" s="8">
+      <c r="T61" s="8">
         <v>84</v>
       </c>
-      <c r="T61" s="8">
+      <c r="U61" s="8">
         <v>18900</v>
       </c>
-      <c r="U61" s="8">
+      <c r="V61" s="8">
         <v>10</v>
       </c>
-      <c r="V61" s="8">
+      <c r="W61" s="8">
         <v>2</v>
       </c>
-      <c r="W61" s="8">
+      <c r="X61" s="8">
         <v>6</v>
       </c>
-      <c r="X61" s="8">
+      <c r="Y61" s="8">
         <v>2</v>
       </c>
-      <c r="Y61" s="7"/>
-      <c r="AC61" s="2" t="s">
-        <v>258</v>
-      </c>
+      <c r="Z61" s="7"/>
       <c r="AD61" s="2" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="62" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE61" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="62" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A62" s="7" t="s">
         <v>455</v>
       </c>
@@ -6765,51 +6833,55 @@
         <v>170</v>
       </c>
       <c r="L62" s="8"/>
-      <c r="M62" s="8">
+      <c r="M62">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="N62" s="8">
         <v>6526</v>
       </c>
-      <c r="N62" s="8">
+      <c r="O62" s="8">
         <v>126</v>
       </c>
-      <c r="O62" s="8">
+      <c r="P62" s="8">
         <v>0.231616456</v>
       </c>
-      <c r="P62" s="8">
+      <c r="Q62" s="8">
         <v>286</v>
       </c>
-      <c r="Q62" s="8">
+      <c r="R62" s="8">
         <v>106</v>
       </c>
-      <c r="R62" s="8">
+      <c r="S62" s="8">
         <v>331250</v>
       </c>
-      <c r="S62" s="8">
+      <c r="T62" s="8">
         <v>84</v>
       </c>
-      <c r="T62" s="8">
+      <c r="U62" s="8">
         <v>18900</v>
       </c>
-      <c r="U62" s="8">
+      <c r="V62" s="8">
         <v>10</v>
       </c>
-      <c r="V62" s="8">
+      <c r="W62" s="8">
         <v>2</v>
       </c>
-      <c r="W62" s="8">
+      <c r="X62" s="8">
         <v>6</v>
       </c>
-      <c r="X62" s="8">
+      <c r="Y62" s="8">
         <v>2</v>
       </c>
-      <c r="Y62" s="7"/>
-      <c r="AC62" s="2" t="s">
-        <v>258</v>
-      </c>
+      <c r="Z62" s="7"/>
       <c r="AD62" s="2" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="63" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE62" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="63" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="s">
         <v>457</v>
       </c>
@@ -6841,51 +6913,55 @@
         <v>170</v>
       </c>
       <c r="L63" s="8"/>
-      <c r="M63" s="8">
+      <c r="M63">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="N63" s="8">
         <v>6526</v>
       </c>
-      <c r="N63" s="8">
+      <c r="O63" s="8">
         <v>126</v>
       </c>
-      <c r="O63" s="8">
+      <c r="P63" s="8">
         <v>0.231616456</v>
       </c>
-      <c r="P63" s="8">
+      <c r="Q63" s="8">
         <v>286</v>
       </c>
-      <c r="Q63" s="8">
+      <c r="R63" s="8">
         <v>106</v>
       </c>
-      <c r="R63" s="8">
+      <c r="S63" s="8">
         <v>331250</v>
       </c>
-      <c r="S63" s="8">
+      <c r="T63" s="8">
         <v>84</v>
       </c>
-      <c r="T63" s="8">
+      <c r="U63" s="8">
         <v>18900</v>
       </c>
-      <c r="U63" s="8">
+      <c r="V63" s="8">
         <v>10</v>
       </c>
-      <c r="V63" s="8">
+      <c r="W63" s="8">
         <v>2</v>
       </c>
-      <c r="W63" s="8">
+      <c r="X63" s="8">
         <v>6</v>
       </c>
-      <c r="X63" s="8">
+      <c r="Y63" s="8">
         <v>2</v>
       </c>
-      <c r="Y63" s="7"/>
-      <c r="AC63" s="2" t="s">
-        <v>258</v>
-      </c>
+      <c r="Z63" s="7"/>
       <c r="AD63" s="2" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="64" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AE63" s="2" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="64" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A64" s="7" t="s">
         <v>459</v>
       </c>
@@ -6917,51 +6993,55 @@
         <v>118</v>
       </c>
       <c r="L64" s="8"/>
-      <c r="M64" s="8">
+      <c r="M64">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="N64" s="8">
         <v>3467</v>
       </c>
-      <c r="N64" s="8">
+      <c r="O64" s="8">
         <v>138</v>
       </c>
-      <c r="O64" s="8">
+      <c r="P64" s="8">
         <v>0.39485359399999997</v>
       </c>
-      <c r="P64" s="8">
+      <c r="Q64" s="8">
         <v>534</v>
       </c>
-      <c r="Q64" s="8">
+      <c r="R64" s="8">
         <v>80</v>
       </c>
-      <c r="R64" s="8">
+      <c r="S64" s="8">
         <v>250000</v>
       </c>
-      <c r="S64" s="8">
+      <c r="T64" s="8">
         <v>60</v>
       </c>
-      <c r="T64" s="8">
+      <c r="U64" s="8">
         <v>14625</v>
       </c>
-      <c r="U64" s="8">
+      <c r="V64" s="8">
         <v>9</v>
       </c>
-      <c r="V64" s="8">
+      <c r="W64" s="8">
         <v>2</v>
       </c>
-      <c r="W64" s="8">
+      <c r="X64" s="8">
         <v>5</v>
       </c>
-      <c r="X64" s="8">
+      <c r="Y64" s="8">
         <v>2</v>
       </c>
-      <c r="Y64" s="7"/>
-      <c r="AC64" s="2" t="s">
+      <c r="Z64" s="7"/>
+      <c r="AD64" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="AD64" s="2" t="s">
+      <c r="AE64" s="2" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="65" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A65" s="7" t="s">
         <v>461</v>
       </c>
@@ -6993,51 +7073,55 @@
         <v>120</v>
       </c>
       <c r="L65" s="8"/>
-      <c r="M65" s="8">
+      <c r="M65">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="N65" s="8">
         <v>6336</v>
       </c>
-      <c r="N65" s="8">
+      <c r="O65" s="8">
         <v>150</v>
       </c>
-      <c r="O65" s="8">
+      <c r="P65" s="8">
         <v>0.42176870700000002</v>
       </c>
-      <c r="P65" s="8">
+      <c r="Q65" s="8">
         <v>620</v>
       </c>
-      <c r="Q65" s="8">
+      <c r="R65" s="8">
         <v>108</v>
       </c>
-      <c r="R65" s="8">
+      <c r="S65" s="8">
         <v>337500</v>
       </c>
-      <c r="S65" s="8">
+      <c r="T65" s="8">
         <v>83</v>
       </c>
-      <c r="T65" s="8">
+      <c r="U65" s="8">
         <v>20231.25</v>
       </c>
-      <c r="U65" s="8">
+      <c r="V65" s="8">
         <v>11</v>
       </c>
-      <c r="V65" s="8">
+      <c r="W65" s="8">
         <v>2</v>
       </c>
-      <c r="W65" s="8">
+      <c r="X65" s="8">
         <v>7</v>
       </c>
-      <c r="X65" s="8">
+      <c r="Y65" s="8">
         <v>2</v>
       </c>
-      <c r="Y65" s="7"/>
-      <c r="AC65" s="2" t="s">
+      <c r="Z65" s="7"/>
+      <c r="AD65" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="AD65" s="2" t="s">
+      <c r="AE65" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="66" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>479</v>
       </c>
@@ -7066,50 +7150,54 @@
         <v>120</v>
       </c>
       <c r="L66" s="5"/>
-      <c r="M66" s="5">
+      <c r="M66">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="N66" s="5">
         <v>6336</v>
       </c>
-      <c r="N66" s="5">
+      <c r="O66" s="5">
         <v>150</v>
       </c>
-      <c r="O66" s="5">
+      <c r="P66" s="5">
         <v>0.42176870700000002</v>
       </c>
-      <c r="P66" s="5">
+      <c r="Q66" s="5">
         <v>620</v>
       </c>
-      <c r="Q66" s="5">
+      <c r="R66" s="5">
         <v>108</v>
       </c>
-      <c r="R66" s="5">
+      <c r="S66" s="5">
         <v>337500</v>
       </c>
-      <c r="S66" s="5">
+      <c r="T66" s="5">
         <v>83</v>
       </c>
-      <c r="T66" s="5">
+      <c r="U66" s="5">
         <v>20231.25</v>
       </c>
-      <c r="U66" s="5">
+      <c r="V66" s="5">
         <v>11</v>
       </c>
-      <c r="V66" s="8">
+      <c r="W66" s="8">
         <v>2</v>
       </c>
-      <c r="W66" s="8">
+      <c r="X66" s="8">
         <v>7</v>
       </c>
-      <c r="X66" s="8">
+      <c r="Y66" s="8">
         <v>2</v>
       </c>
-      <c r="AC66" s="2" t="s">
+      <c r="AD66" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="AD66" s="2" t="s">
+      <c r="AE66" s="2" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="67" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>481</v>
       </c>
@@ -7136,50 +7224,54 @@
         <v>120</v>
       </c>
       <c r="L67" s="5"/>
-      <c r="M67" s="5">
+      <c r="M67">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="N67" s="5">
         <v>4487</v>
       </c>
-      <c r="N67" s="5">
+      <c r="O67" s="5">
         <v>150</v>
       </c>
-      <c r="O67" s="5">
+      <c r="P67" s="5">
         <v>0.42176870700000002</v>
       </c>
-      <c r="P67" s="5">
+      <c r="Q67" s="5">
         <v>620</v>
       </c>
-      <c r="Q67" s="5">
+      <c r="R67" s="5">
         <v>95</v>
       </c>
-      <c r="R67" s="5">
+      <c r="S67" s="5">
         <v>296875</v>
       </c>
-      <c r="S67" s="5">
+      <c r="T67" s="5">
         <v>71</v>
       </c>
-      <c r="T67" s="5">
+      <c r="U67" s="5">
         <v>17306.25</v>
       </c>
-      <c r="U67" s="5">
+      <c r="V67" s="5">
         <v>11</v>
       </c>
-      <c r="V67" s="8">
+      <c r="W67" s="8">
         <v>2</v>
       </c>
-      <c r="W67" s="8">
+      <c r="X67" s="8">
         <v>7</v>
       </c>
-      <c r="X67" s="8">
+      <c r="Y67" s="8">
         <v>2</v>
       </c>
-      <c r="AC67" s="2" t="s">
+      <c r="AD67" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="AD67" s="2" t="s">
+      <c r="AE67" s="2" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="68" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>517</v>
       </c>
@@ -7208,47 +7300,52 @@
         <v>9600</v>
       </c>
       <c r="M68">
-        <v>6253</v>
+        <f>ROUND(L68/0.745699872,0)</f>
+        <v>12874</v>
       </c>
       <c r="N68">
+        <f>ROUND(L68*1.3596216173,0)</f>
+        <v>13052</v>
+      </c>
+      <c r="O68">
         <v>184</v>
       </c>
-      <c r="O68">
+      <c r="P68">
         <v>0.38800000000000001</v>
       </c>
-      <c r="P68">
-        <f t="shared" ref="P68" si="22">N68*O68*9.8</f>
+      <c r="Q68">
+        <f t="shared" ref="Q68" si="23">O68*P68*9.8</f>
         <v>699.64160000000004</v>
       </c>
-      <c r="Q68">
-        <f t="shared" ref="Q68" si="23">MEDIAN(255, ROUND((N68/10+SQRT(K68)/20+SQRT(M68)+O68+20-J68), 0), 0)</f>
-        <v>110</v>
-      </c>
       <c r="R68">
-        <f t="shared" ref="R68" si="24">Q68*50000/16</f>
-        <v>343750</v>
+        <f t="shared" ref="R68" si="24">MEDIAN(255, ROUND((O68/10+SQRT(K68)/20+SQRT(N68)+P68+20-J68), 0), 0)</f>
+        <v>146</v>
       </c>
       <c r="S68">
-        <f t="shared" ref="S68" si="25">MEDIAN(0, 255, ROUND(SQRT(K68)/100+SQRT(M68)+O68+40/J68-2,0))</f>
-        <v>83</v>
+        <f t="shared" ref="S68" si="25">R68*50000/16</f>
+        <v>456250</v>
       </c>
       <c r="T68">
-        <f t="shared" ref="T68" si="26">IF(E68="Steam", S68*350/16*12, IF(E68="Diesel", S68*325/16*12,  S68*300/16*12))</f>
-        <v>18675</v>
+        <f t="shared" ref="T68" si="26">MEDIAN(0, 255, ROUND(SQRT(K68)/100+SQRT(N68)+P68+40/J68-2,0))</f>
+        <v>118</v>
       </c>
       <c r="U68">
-        <f>V68+W68+X68</f>
-        <v>0</v>
-      </c>
-      <c r="AB68" s="2" t="e">
-        <f t="shared" ref="AB68" si="27">AVERAGE(Y68:AA68)</f>
+        <f t="shared" ref="U68" si="27">IF(E68="Steam", T68*350/16*12, IF(E68="Diesel", T68*325/16*12,  T68*300/16*12))</f>
+        <v>26550</v>
+      </c>
+      <c r="V68">
+        <f>W68+X68+Y68</f>
+        <v>0</v>
+      </c>
+      <c r="AC68" s="2" t="e">
+        <f t="shared" ref="AC68" si="28">AVERAGE(Z68:AB68)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AC68" s="2" t="s">
+      <c r="AD68" s="2" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="69" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>520</v>
       </c>
@@ -7277,44 +7374,151 @@
         <v>9600</v>
       </c>
       <c r="M69">
-        <v>6253</v>
+        <f>ROUND(L69/0.745699872,0)</f>
+        <v>12874</v>
       </c>
       <c r="N69">
+        <f>ROUND(L69*1.3596216173,0)</f>
+        <v>13052</v>
+      </c>
+      <c r="O69">
         <v>184</v>
       </c>
-      <c r="O69">
+      <c r="P69">
         <v>0.38800000000000001</v>
       </c>
-      <c r="P69">
-        <f t="shared" ref="P69" si="28">N69*O69*9.8</f>
+      <c r="Q69">
+        <f t="shared" ref="Q69:Q71" si="29">O69*P69*9.8</f>
         <v>699.64160000000004</v>
       </c>
-      <c r="Q69">
-        <f t="shared" ref="Q69" si="29">MEDIAN(255, ROUND((N69/10+SQRT(K69)/20+SQRT(M69)+O69+20-J69), 0), 0)</f>
-        <v>110</v>
-      </c>
       <c r="R69">
-        <f t="shared" ref="R69" si="30">Q69*50000/16</f>
-        <v>343750</v>
+        <f t="shared" ref="R69:R70" si="30">MEDIAN(255, ROUND((O69/10+SQRT(K69)/20+SQRT(N69)+P69+20-J69), 0), 0)</f>
+        <v>146</v>
       </c>
       <c r="S69">
-        <f t="shared" ref="S69" si="31">MEDIAN(0, 255, ROUND(SQRT(K69)/100+SQRT(M69)+O69+40/J69-2,0))</f>
-        <v>83</v>
+        <f t="shared" ref="S69:S70" si="31">R69*50000/16</f>
+        <v>456250</v>
       </c>
       <c r="T69">
-        <f t="shared" ref="T69" si="32">IF(E69="Steam", S69*350/16*12, IF(E69="Diesel", S69*325/16*12,  S69*300/16*12))</f>
-        <v>18675</v>
+        <f t="shared" ref="T69:T70" si="32">MEDIAN(0, 255, ROUND(SQRT(K69)/100+SQRT(N69)+P69+40/J69-2,0))</f>
+        <v>118</v>
       </c>
       <c r="U69">
-        <f>V69+W69+X69</f>
-        <v>0</v>
-      </c>
-      <c r="AB69" s="2" t="e">
-        <f t="shared" ref="AB69" si="33">AVERAGE(Y69:AA69)</f>
+        <f t="shared" ref="U69:U70" si="33">IF(E69="Steam", T69*350/16*12, IF(E69="Diesel", T69*325/16*12,  T69*300/16*12))</f>
+        <v>26550</v>
+      </c>
+      <c r="V69">
+        <f>W69+X69+Y69</f>
+        <v>0</v>
+      </c>
+      <c r="AC69" s="2" t="e">
+        <f t="shared" ref="AC69" si="34">AVERAGE(Z69:AB69)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AC69" s="2" t="s">
+      <c r="AD69" s="2" t="s">
         <v>419</v>
+      </c>
+    </row>
+    <row r="70" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A70" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="B70" t="s">
+        <v>525</v>
+      </c>
+      <c r="E70" t="s">
+        <v>52</v>
+      </c>
+      <c r="F70" s="5">
+        <v>2020</v>
+      </c>
+      <c r="G70" s="5">
+        <v>30</v>
+      </c>
+      <c r="H70" t="s">
+        <v>89</v>
+      </c>
+      <c r="J70" s="5">
+        <v>8</v>
+      </c>
+      <c r="K70" s="5">
+        <v>100</v>
+      </c>
+      <c r="L70" s="5">
+        <v>2400</v>
+      </c>
+      <c r="M70">
+        <f>ROUND(L70/0.745699872,0)</f>
+        <v>3218</v>
+      </c>
+      <c r="N70">
+        <f>ROUND(L70*1.3596216173,0)</f>
+        <v>3263</v>
+      </c>
+      <c r="O70" s="5">
+        <v>150</v>
+      </c>
+      <c r="P70" s="5">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="Q70">
+        <f t="shared" si="29"/>
+        <v>560.07000000000005</v>
+      </c>
+      <c r="R70">
+        <f t="shared" si="30"/>
+        <v>85</v>
+      </c>
+      <c r="S70">
+        <f t="shared" si="31"/>
+        <v>265625</v>
+      </c>
+      <c r="T70">
+        <f t="shared" si="32"/>
+        <v>61</v>
+      </c>
+      <c r="U70">
+        <f t="shared" si="33"/>
+        <v>13725</v>
+      </c>
+      <c r="V70">
+        <f>W70+X70+Y70</f>
+        <v>10</v>
+      </c>
+      <c r="W70" s="5">
+        <v>2</v>
+      </c>
+      <c r="X70" s="5">
+        <v>6</v>
+      </c>
+      <c r="Y70" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
+        <v>526</v>
+      </c>
+      <c r="L71" s="5">
+        <v>2000</v>
+      </c>
+      <c r="M71">
+        <f>ROUND(L71/0.745699872,0)</f>
+        <v>2682</v>
+      </c>
+      <c r="N71">
+        <f>ROUND(L71*1.3596216173,0)</f>
+        <v>2719</v>
+      </c>
+      <c r="O71" s="5">
+        <v>150</v>
+      </c>
+      <c r="P71" s="5">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="Q71">
+        <f t="shared" si="29"/>
+        <v>560.07000000000005</v>
       </c>
     </row>
   </sheetData>
@@ -7327,9 +7531,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB4625FC-685F-4E56-AE60-F05D51350408}">
   <dimension ref="A1:AG324"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A310" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P300" sqref="P300"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A202" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K222" sqref="K222:K223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -25647,10 +25851,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8540264-B3C1-4C71-9FC9-001ABF042657}">
-  <dimension ref="A1:AD28"/>
+  <dimension ref="A1:AD29"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="R33" sqref="R33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -26917,7 +27121,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>511</v>
       </c>
@@ -26951,6 +27155,43 @@
         <v>4</v>
       </c>
       <c r="AD28" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" ht="17" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>522</v>
+      </c>
+      <c r="F29" s="5">
+        <v>1992</v>
+      </c>
+      <c r="G29" s="5">
+        <v>30</v>
+      </c>
+      <c r="J29" s="5">
+        <v>100</v>
+      </c>
+      <c r="P29" s="5">
+        <v>58</v>
+      </c>
+      <c r="Q29" s="5">
+        <v>12</v>
+      </c>
+      <c r="R29" s="5">
+        <v>185</v>
+      </c>
+      <c r="S29" s="5">
+        <v>21.5</v>
+      </c>
+      <c r="U29">
+        <f t="shared" ref="U29" si="2">MEDIAN(0,255,ROUND(S29/20+SQRT(J29)/40+SQRT(P29)/2+(SQRT(R29)-SQRT(185)),0))</f>
+        <v>5</v>
+      </c>
+      <c r="W29">
+        <f t="shared" ref="W29" si="3">MEDIAN(0,255,ROUND(SQRT(J29)/200+SQRT(P29)/2+(SQRT(R29)-SQRT(185)),0))</f>
+        <v>4</v>
+      </c>
+      <c r="AD29" s="3" t="s">
         <v>390</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add livery of cr400bfz/c
</commit_message>
<xml_diff>
--- a/docs/China Set Trains.xlsx
+++ b/docs/China Set Trains.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CNS\CNST\local\China-Set-Trains\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BFF7820-1BBF-411E-8D60-8EE9DF93FE7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C528903B-EC23-41E6-9AF5-4A9185F9D651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Loco" sheetId="1" r:id="rId1"/>
@@ -2421,7 +2421,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M70" sqref="M70"/>
     </sheetView>
@@ -7531,9 +7531,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB4625FC-685F-4E56-AE60-F05D51350408}">
   <dimension ref="A1:AG324"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A202" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K222" sqref="K222:K223"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A307" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AB314" sqref="AB314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -25486,7 +25486,7 @@
         <v>88</v>
       </c>
       <c r="R319">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="T319">
         <v>240</v>
@@ -25503,11 +25503,11 @@
       </c>
       <c r="X319">
         <f t="shared" si="103"/>
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Y319">
         <f t="shared" si="112"/>
-        <v>275000</v>
+        <v>271875</v>
       </c>
       <c r="Z319">
         <f t="shared" si="102"/>
@@ -25804,7 +25804,7 @@
         <v>88</v>
       </c>
       <c r="R324">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="T324">
         <v>240</v>

</xml_diff>

<commit_message>
update the data xlxs
</commit_message>
<xml_diff>
--- a/docs/China Set Trains.xlsx
+++ b/docs/China Set Trains.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CNS\CNST\local\China-Set-Trains\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C528903B-EC23-41E6-9AF5-4A9185F9D651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD790D70-BFC1-43A1-BDF9-1D0713B3FB8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Loco" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1853" uniqueCount="530">
   <si>
     <t>name</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2040,6 +2040,18 @@
   </si>
   <si>
     <t>(battery)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SS4B</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SS4C</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>8+8</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2419,11 +2431,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF71"/>
+  <dimension ref="A1:AF73"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M70" sqref="M70"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AE72" sqref="AE72:AE73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -7388,23 +7400,23 @@
         <v>0.38800000000000001</v>
       </c>
       <c r="Q69">
-        <f t="shared" ref="Q69:Q71" si="29">O69*P69*9.8</f>
+        <f t="shared" ref="Q69:Q73" si="29">O69*P69*9.8</f>
         <v>699.64160000000004</v>
       </c>
       <c r="R69">
-        <f t="shared" ref="R69:R70" si="30">MEDIAN(255, ROUND((O69/10+SQRT(K69)/20+SQRT(N69)+P69+20-J69), 0), 0)</f>
+        <f t="shared" ref="R69:R73" si="30">MEDIAN(255, ROUND((O69/10+SQRT(K69)/20+SQRT(N69)+P69+20-J69), 0), 0)</f>
         <v>146</v>
       </c>
       <c r="S69">
-        <f t="shared" ref="S69:S70" si="31">R69*50000/16</f>
+        <f t="shared" ref="S69:S73" si="31">R69*50000/16</f>
         <v>456250</v>
       </c>
       <c r="T69">
-        <f t="shared" ref="T69:T70" si="32">MEDIAN(0, 255, ROUND(SQRT(K69)/100+SQRT(N69)+P69+40/J69-2,0))</f>
+        <f t="shared" ref="T69:T73" si="32">MEDIAN(0, 255, ROUND(SQRT(K69)/100+SQRT(N69)+P69+40/J69-2,0))</f>
         <v>118</v>
       </c>
       <c r="U69">
-        <f t="shared" ref="U69:U70" si="33">IF(E69="Steam", T69*350/16*12, IF(E69="Diesel", T69*325/16*12,  T69*300/16*12))</f>
+        <f t="shared" ref="U69:U73" si="33">IF(E69="Steam", T69*350/16*12, IF(E69="Diesel", T69*325/16*12,  T69*300/16*12))</f>
         <v>26550</v>
       </c>
       <c r="V69">
@@ -7494,6 +7506,9 @@
       <c r="Y70" s="5">
         <v>2</v>
       </c>
+      <c r="AD70" s="2" t="s">
+        <v>419</v>
+      </c>
     </row>
     <row r="71" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
@@ -7519,6 +7534,152 @@
       <c r="Q71">
         <f t="shared" si="29"/>
         <v>560.07000000000005</v>
+      </c>
+      <c r="R71">
+        <f t="shared" si="30"/>
+        <v>88</v>
+      </c>
+      <c r="S71">
+        <f t="shared" si="31"/>
+        <v>275000</v>
+      </c>
+    </row>
+    <row r="72" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>527</v>
+      </c>
+      <c r="E72" t="s">
+        <v>52</v>
+      </c>
+      <c r="F72">
+        <v>1995</v>
+      </c>
+      <c r="G72">
+        <v>30</v>
+      </c>
+      <c r="H72" t="s">
+        <v>89</v>
+      </c>
+      <c r="J72">
+        <v>8</v>
+      </c>
+      <c r="K72">
+        <v>100</v>
+      </c>
+      <c r="L72" s="5">
+        <v>6400</v>
+      </c>
+      <c r="M72">
+        <f t="shared" ref="M72:M73" si="35">ROUND(L72/0.745699872,0)</f>
+        <v>8583</v>
+      </c>
+      <c r="N72">
+        <f t="shared" ref="N72:N73" si="36">ROUND(L72*1.3596216173,0)</f>
+        <v>8702</v>
+      </c>
+      <c r="O72" s="5">
+        <v>184</v>
+      </c>
+      <c r="P72" s="5">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="Q72">
+        <f t="shared" si="29"/>
+        <v>627.5136</v>
+      </c>
+      <c r="R72">
+        <f t="shared" si="30"/>
+        <v>125</v>
+      </c>
+      <c r="S72">
+        <f t="shared" si="31"/>
+        <v>390625</v>
+      </c>
+      <c r="T72">
+        <f t="shared" si="32"/>
+        <v>97</v>
+      </c>
+      <c r="U72">
+        <f t="shared" si="33"/>
+        <v>21825</v>
+      </c>
+      <c r="V72" t="s">
+        <v>529</v>
+      </c>
+      <c r="AD72" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="AE72" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="73" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>528</v>
+      </c>
+      <c r="E73" t="s">
+        <v>52</v>
+      </c>
+      <c r="F73">
+        <v>1997</v>
+      </c>
+      <c r="G73">
+        <v>30</v>
+      </c>
+      <c r="H73" t="s">
+        <v>89</v>
+      </c>
+      <c r="J73">
+        <v>24</v>
+      </c>
+      <c r="K73">
+        <v>100</v>
+      </c>
+      <c r="L73" s="5">
+        <v>6400</v>
+      </c>
+      <c r="M73">
+        <f t="shared" si="35"/>
+        <v>8583</v>
+      </c>
+      <c r="N73">
+        <f t="shared" si="36"/>
+        <v>8702</v>
+      </c>
+      <c r="O73" s="5">
+        <v>200</v>
+      </c>
+      <c r="P73" s="5">
+        <v>0.34799999999999998</v>
+      </c>
+      <c r="Q73">
+        <f t="shared" si="29"/>
+        <v>682.08</v>
+      </c>
+      <c r="R73">
+        <f t="shared" si="30"/>
+        <v>110</v>
+      </c>
+      <c r="S73">
+        <f t="shared" si="31"/>
+        <v>343750</v>
+      </c>
+      <c r="T73">
+        <f t="shared" si="32"/>
+        <v>93</v>
+      </c>
+      <c r="U73">
+        <f t="shared" si="33"/>
+        <v>20925</v>
+      </c>
+      <c r="V73" t="s">
+        <v>529</v>
+      </c>
+      <c r="AD73" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="AE73" t="s">
+        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -7531,7 +7692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB4625FC-685F-4E56-AE60-F05D51350408}">
   <dimension ref="A1:AG324"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A307" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AB314" sqref="AB314"/>
     </sheetView>

</xml_diff>

<commit_message>
add livery of g60
</commit_message>
<xml_diff>
--- a/docs/China Set Trains.xlsx
+++ b/docs/China Set Trains.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CNS\CNST\local\China-Set-Trains\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{830E1E70-7DFE-4807-9E94-57B94608BB60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DFA7B32-BD84-487F-9ED0-93E6293977F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1925" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1948" uniqueCount="562">
   <si>
     <t>name</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2156,6 +2156,30 @@
   </si>
   <si>
     <t>C80</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>alex weight</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>alex weight class</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>G70</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2953,7 +2977,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="V6">
-        <f t="shared" ref="V4:V39" si="15">W6+X6+Y6</f>
+        <f t="shared" ref="V6:V39" si="15">W6+X6+Y6</f>
         <v>0</v>
       </c>
       <c r="AC6" s="2" t="e">
@@ -26799,15 +26823,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8540264-B3C1-4C71-9FC9-001ABF042657}">
-  <dimension ref="A1:AD43"/>
+  <dimension ref="A1:AF45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="V47" sqref="V47"/>
+    <sheetView tabSelected="1" topLeftCell="L43" workbookViewId="0">
+      <selection activeCell="AF19" sqref="AF19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -26842,64 +26866,70 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
+        <v>556</v>
+      </c>
+      <c r="M1" t="s">
+        <v>557</v>
+      </c>
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>30</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>28</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>27</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>140</v>
       </c>
@@ -26918,34 +26948,34 @@
       <c r="J2">
         <v>100</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>142</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>143</v>
       </c>
-      <c r="P2">
+      <c r="R2">
         <v>61</v>
       </c>
-      <c r="Q2">
+      <c r="S2">
         <v>16</v>
       </c>
-      <c r="R2">
+      <c r="T2">
         <v>185</v>
       </c>
-      <c r="S2">
+      <c r="U2">
         <v>22.5</v>
       </c>
-      <c r="U2">
-        <f t="shared" ref="U2:U28" si="0">MEDIAN(0,255,ROUND(S2/20+SQRT(J2)/40+SQRT(P2)/2+(SQRT(R2)-SQRT(185)),0))</f>
+      <c r="W2">
+        <f t="shared" ref="W2:W28" si="0">MEDIAN(0,255,ROUND(U2/20+SQRT(J2)/40+SQRT(R2)/2+(SQRT(T2)-SQRT(185)),0))</f>
         <v>5</v>
       </c>
-      <c r="W2">
-        <f t="shared" ref="W2:W28" si="1">MEDIAN(0,255,ROUND(SQRT(J2)/200+SQRT(P2)/2+(SQRT(R2)-SQRT(185)),0))</f>
+      <c r="Y2">
+        <f t="shared" ref="Y2:Y28" si="1">MEDIAN(0,255,ROUND(SQRT(J2)/200+SQRT(R2)/2+(SQRT(T2)-SQRT(185)),0))</f>
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>144</v>
       </c>
@@ -26964,28 +26994,28 @@
       <c r="J3">
         <v>100</v>
       </c>
-      <c r="P3">
+      <c r="R3">
         <v>60</v>
       </c>
-      <c r="Q3">
+      <c r="S3">
         <v>12</v>
       </c>
-      <c r="R3">
+      <c r="T3">
         <v>185</v>
       </c>
-      <c r="S3">
+      <c r="U3">
         <v>24</v>
       </c>
-      <c r="U3">
+      <c r="W3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="W3">
+      <c r="Y3">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>176</v>
       </c>
@@ -27004,31 +27034,31 @@
       <c r="J4">
         <v>100</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>175</v>
       </c>
-      <c r="P4">
+      <c r="R4">
         <v>52</v>
       </c>
-      <c r="Q4">
+      <c r="S4">
         <v>8</v>
       </c>
-      <c r="R4">
+      <c r="T4">
         <v>185</v>
       </c>
-      <c r="S4">
+      <c r="U4">
         <v>20.6</v>
       </c>
-      <c r="U4">
+      <c r="W4">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="W4">
+      <c r="Y4">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>187</v>
       </c>
@@ -27047,28 +27077,28 @@
       <c r="J5">
         <v>100</v>
       </c>
-      <c r="P5">
+      <c r="R5">
         <v>60</v>
       </c>
-      <c r="Q5">
+      <c r="S5">
         <v>12</v>
       </c>
-      <c r="R5">
+      <c r="T5">
         <v>185</v>
       </c>
-      <c r="S5">
+      <c r="U5">
         <v>22.2</v>
       </c>
-      <c r="U5">
+      <c r="W5">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="W5">
+      <c r="Y5">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>191</v>
       </c>
@@ -27090,28 +27120,28 @@
       <c r="J6">
         <v>100</v>
       </c>
-      <c r="P6">
+      <c r="R6">
         <v>60</v>
       </c>
-      <c r="Q6">
+      <c r="S6">
         <v>16</v>
       </c>
-      <c r="R6">
+      <c r="T6">
         <v>185</v>
       </c>
-      <c r="S6">
+      <c r="U6">
         <v>20.6</v>
       </c>
-      <c r="U6">
+      <c r="W6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="W6">
+      <c r="Y6">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>200</v>
       </c>
@@ -27130,28 +27160,28 @@
       <c r="J7">
         <v>100</v>
       </c>
-      <c r="P7">
+      <c r="R7">
         <v>60</v>
       </c>
-      <c r="Q7">
+      <c r="S7">
         <v>20</v>
       </c>
-      <c r="R7">
+      <c r="T7">
         <v>185</v>
       </c>
-      <c r="S7">
+      <c r="U7">
         <v>22.1</v>
       </c>
-      <c r="U7">
+      <c r="W7">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="W7">
+      <c r="Y7">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>232</v>
       </c>
@@ -27173,28 +27203,28 @@
       <c r="J8">
         <v>90</v>
       </c>
-      <c r="P8">
+      <c r="R8">
         <v>60</v>
       </c>
-      <c r="Q8">
+      <c r="S8">
         <v>20</v>
       </c>
-      <c r="R8">
+      <c r="T8">
         <v>185</v>
       </c>
-      <c r="S8">
+      <c r="U8">
         <v>18</v>
       </c>
-      <c r="U8">
+      <c r="W8">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="W8">
+      <c r="Y8">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>234</v>
       </c>
@@ -27213,28 +27243,28 @@
       <c r="J9">
         <v>120</v>
       </c>
-      <c r="P9">
+      <c r="R9">
         <v>70</v>
       </c>
-      <c r="Q9">
+      <c r="S9">
         <v>16</v>
       </c>
-      <c r="R9">
+      <c r="T9">
         <v>185</v>
       </c>
-      <c r="S9">
+      <c r="U9">
         <v>23.8</v>
       </c>
-      <c r="U9">
+      <c r="W9">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="W9">
+      <c r="Y9">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>235</v>
       </c>
@@ -27253,28 +27283,28 @@
       <c r="J10">
         <v>120</v>
       </c>
-      <c r="P10">
+      <c r="R10">
         <v>70</v>
       </c>
-      <c r="Q10">
+      <c r="S10">
         <v>12</v>
       </c>
-      <c r="R10">
+      <c r="T10">
         <v>185</v>
       </c>
-      <c r="S10">
+      <c r="U10">
         <v>24.5</v>
       </c>
-      <c r="U10">
+      <c r="W10">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="W10">
+      <c r="Y10">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>236</v>
       </c>
@@ -27293,28 +27323,28 @@
       <c r="J11">
         <v>120</v>
       </c>
-      <c r="P11">
+      <c r="R11">
         <v>70</v>
       </c>
-      <c r="Q11">
+      <c r="S11">
         <v>8</v>
       </c>
-      <c r="R11">
+      <c r="T11">
         <v>185</v>
       </c>
-      <c r="S11">
+      <c r="U11">
         <v>23.4</v>
       </c>
-      <c r="U11">
+      <c r="W11">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="W11">
+      <c r="Y11">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>288</v>
       </c>
@@ -27333,28 +27363,28 @@
       <c r="J12">
         <v>120</v>
       </c>
-      <c r="P12">
+      <c r="R12">
         <v>20</v>
       </c>
-      <c r="Q12">
+      <c r="S12">
         <v>6</v>
       </c>
-      <c r="R12">
+      <c r="T12">
         <v>400</v>
       </c>
-      <c r="S12">
+      <c r="U12">
         <v>37</v>
       </c>
-      <c r="U12">
+      <c r="W12">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="W12">
+      <c r="Y12">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>358</v>
       </c>
@@ -27373,28 +27403,28 @@
       <c r="J13">
         <v>120</v>
       </c>
-      <c r="P13">
+      <c r="R13">
         <v>22</v>
       </c>
-      <c r="Q13">
+      <c r="S13">
         <v>6</v>
       </c>
-      <c r="R13">
+      <c r="T13">
         <v>400</v>
       </c>
-      <c r="S13">
+      <c r="U13">
         <v>37</v>
       </c>
-      <c r="U13">
+      <c r="W13">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="W13">
+      <c r="Y13">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>360</v>
       </c>
@@ -27416,28 +27446,28 @@
       <c r="J14">
         <v>100</v>
       </c>
-      <c r="P14">
+      <c r="R14">
         <v>45</v>
       </c>
-      <c r="Q14">
+      <c r="S14">
         <v>12</v>
       </c>
-      <c r="R14">
+      <c r="T14">
         <v>800</v>
       </c>
-      <c r="S14">
+      <c r="U14">
         <v>34</v>
       </c>
-      <c r="U14">
+      <c r="W14">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="W14">
+      <c r="Y14">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>384</v>
       </c>
@@ -27456,31 +27486,31 @@
       <c r="J15">
         <v>120</v>
       </c>
-      <c r="P15">
+      <c r="R15">
         <v>184</v>
       </c>
-      <c r="Q15">
+      <c r="S15">
         <v>48</v>
       </c>
-      <c r="R15">
+      <c r="T15">
         <v>1600</v>
       </c>
-      <c r="S15">
+      <c r="U15">
         <v>184</v>
       </c>
-      <c r="U15">
+      <c r="W15">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="W15">
+      <c r="Y15">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="AD15" t="s">
+      <c r="AF15" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>389</v>
       </c>
@@ -27499,31 +27529,31 @@
       <c r="J16">
         <v>120</v>
       </c>
-      <c r="P16">
+      <c r="R16">
         <v>70</v>
       </c>
-      <c r="Q16">
+      <c r="S16">
         <v>24</v>
       </c>
-      <c r="R16">
+      <c r="T16">
         <v>185</v>
       </c>
-      <c r="S16">
+      <c r="U16">
         <v>23</v>
       </c>
-      <c r="U16">
+      <c r="W16">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="W16">
+      <c r="Y16">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="AD16" t="s">
+      <c r="AF16" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>391</v>
       </c>
@@ -27542,41 +27572,41 @@
       <c r="J17">
         <v>120</v>
       </c>
-      <c r="P17">
+      <c r="R17">
         <v>70</v>
       </c>
-      <c r="Q17">
+      <c r="S17">
         <v>20</v>
       </c>
-      <c r="R17">
+      <c r="T17">
         <v>185</v>
       </c>
-      <c r="S17">
+      <c r="U17">
         <v>23.8</v>
       </c>
-      <c r="U17">
+      <c r="W17">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="W17">
+      <c r="Y17">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>427</v>
       </c>
-      <c r="U18">
+      <c r="W18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="W18">
+      <c r="Y18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>465</v>
       </c>
@@ -27604,39 +27634,41 @@
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
-      <c r="P19" s="5">
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="5">
         <v>60</v>
       </c>
-      <c r="Q19" s="5">
+      <c r="S19" s="5">
         <v>12</v>
       </c>
-      <c r="R19" s="5">
+      <c r="T19" s="5">
         <v>185</v>
       </c>
-      <c r="S19" s="5">
+      <c r="U19" s="5">
         <v>24</v>
       </c>
-      <c r="T19" s="4"/>
-      <c r="U19">
+      <c r="V19" s="4"/>
+      <c r="W19">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="V19" s="6"/>
-      <c r="W19">
+      <c r="X19" s="6"/>
+      <c r="Y19">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="X19" s="4"/>
-      <c r="Y19" s="4"/>
       <c r="Z19" s="4"/>
       <c r="AA19" s="4"/>
       <c r="AB19" s="4"/>
       <c r="AC19" s="4"/>
-      <c r="AD19" s="3" t="s">
+      <c r="AD19" s="4"/>
+      <c r="AE19" s="4"/>
+      <c r="AF19" s="3" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>466</v>
       </c>
@@ -27666,39 +27698,41 @@
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
-      <c r="P20" s="5">
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="5">
         <v>60</v>
       </c>
-      <c r="Q20" s="5">
+      <c r="S20" s="5">
         <v>16</v>
       </c>
-      <c r="R20" s="5">
+      <c r="T20" s="5">
         <v>185</v>
       </c>
-      <c r="S20" s="5">
+      <c r="U20" s="5">
         <v>24</v>
       </c>
-      <c r="T20" s="4"/>
-      <c r="U20">
+      <c r="V20" s="4"/>
+      <c r="W20">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="V20" s="6"/>
-      <c r="W20">
+      <c r="X20" s="6"/>
+      <c r="Y20">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="X20" s="4"/>
-      <c r="Y20" s="4"/>
       <c r="Z20" s="4"/>
       <c r="AA20" s="4"/>
       <c r="AB20" s="4"/>
       <c r="AC20" s="4"/>
-      <c r="AD20" s="3" t="s">
+      <c r="AD20" s="4"/>
+      <c r="AE20" s="4"/>
+      <c r="AF20" s="3" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>467</v>
       </c>
@@ -27726,39 +27760,41 @@
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
-      <c r="P21" s="5">
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="5">
         <v>80</v>
       </c>
-      <c r="Q21" s="5">
+      <c r="S21" s="5">
         <v>12</v>
       </c>
-      <c r="R21" s="5">
+      <c r="T21" s="5">
         <v>185</v>
       </c>
-      <c r="S21" s="5">
+      <c r="U21" s="5">
         <v>25.6</v>
       </c>
-      <c r="T21" s="4"/>
-      <c r="U21">
+      <c r="V21" s="4"/>
+      <c r="W21">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="V21" s="6"/>
-      <c r="W21">
+      <c r="X21" s="6"/>
+      <c r="Y21">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="X21" s="4"/>
-      <c r="Y21" s="4"/>
       <c r="Z21" s="4"/>
       <c r="AA21" s="4"/>
       <c r="AB21" s="4"/>
       <c r="AC21" s="4"/>
-      <c r="AD21" s="3" t="s">
+      <c r="AD21" s="4"/>
+      <c r="AE21" s="4"/>
+      <c r="AF21" s="3" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>468</v>
       </c>
@@ -27786,39 +27822,41 @@
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
-      <c r="P22" s="5">
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="5">
         <v>52</v>
       </c>
-      <c r="Q22" s="5">
+      <c r="S22" s="5">
         <v>12</v>
       </c>
-      <c r="R22" s="5">
+      <c r="T22" s="5">
         <v>185</v>
       </c>
-      <c r="S22" s="5">
+      <c r="U22" s="5">
         <v>22.3</v>
       </c>
-      <c r="T22" s="4"/>
-      <c r="U22">
+      <c r="V22" s="4"/>
+      <c r="W22">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="V22" s="6"/>
-      <c r="W22">
+      <c r="X22" s="6"/>
+      <c r="Y22">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="X22" s="4"/>
-      <c r="Y22" s="4"/>
       <c r="Z22" s="4"/>
       <c r="AA22" s="4"/>
       <c r="AB22" s="4"/>
       <c r="AC22" s="4"/>
-      <c r="AD22" s="3" t="s">
+      <c r="AD22" s="4"/>
+      <c r="AE22" s="4"/>
+      <c r="AF22" s="3" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>469</v>
       </c>
@@ -27848,39 +27886,41 @@
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
-      <c r="P23" s="5">
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="5">
         <v>90</v>
       </c>
-      <c r="Q23" s="5">
+      <c r="S23" s="5">
         <v>12</v>
       </c>
-      <c r="R23" s="5">
+      <c r="T23" s="5">
         <v>185</v>
       </c>
-      <c r="S23" s="5">
+      <c r="U23" s="5">
         <v>28</v>
       </c>
-      <c r="T23" s="4"/>
-      <c r="U23">
+      <c r="V23" s="4"/>
+      <c r="W23">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="V23" s="6"/>
-      <c r="W23">
+      <c r="X23" s="6"/>
+      <c r="Y23">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="X23" s="4"/>
-      <c r="Y23" s="4"/>
       <c r="Z23" s="4"/>
       <c r="AA23" s="4"/>
       <c r="AB23" s="4"/>
       <c r="AC23" s="4"/>
-      <c r="AD23" s="3" t="s">
+      <c r="AD23" s="4"/>
+      <c r="AE23" s="4"/>
+      <c r="AF23" s="3" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>480</v>
       </c>
@@ -27910,39 +27950,41 @@
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
-      <c r="P24" s="5">
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
+      <c r="R24" s="5">
         <v>20</v>
       </c>
-      <c r="Q24" s="5">
+      <c r="S24" s="5">
         <v>12</v>
       </c>
-      <c r="R24" s="5">
+      <c r="T24" s="5">
         <v>800</v>
       </c>
-      <c r="S24" s="5">
+      <c r="U24" s="5">
         <v>27</v>
       </c>
-      <c r="T24" s="4"/>
-      <c r="U24">
+      <c r="V24" s="4"/>
+      <c r="W24">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="V24" s="6"/>
-      <c r="W24">
+      <c r="X24" s="6"/>
+      <c r="Y24">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="X24" s="4"/>
-      <c r="Y24" s="4"/>
       <c r="Z24" s="4"/>
       <c r="AA24" s="4"/>
       <c r="AB24" s="4"/>
       <c r="AC24" s="4"/>
-      <c r="AD24" s="3" t="s">
+      <c r="AD24" s="4"/>
+      <c r="AE24" s="4"/>
+      <c r="AF24" s="3" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>482</v>
       </c>
@@ -27964,32 +28006,32 @@
       <c r="J25" s="5">
         <v>75</v>
       </c>
-      <c r="P25" s="5">
+      <c r="R25" s="5">
         <v>50</v>
       </c>
-      <c r="Q25" s="5">
+      <c r="S25" s="5">
         <v>20</v>
       </c>
-      <c r="R25" s="5">
+      <c r="T25" s="5">
         <v>185</v>
       </c>
-      <c r="S25" s="5">
+      <c r="U25" s="5">
         <v>19</v>
       </c>
-      <c r="U25">
+      <c r="W25">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="V25" s="6"/>
-      <c r="W25">
+      <c r="X25" s="6"/>
+      <c r="Y25">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="AD25" s="3" t="s">
+      <c r="AF25" s="3" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>507</v>
       </c>
@@ -28005,31 +28047,31 @@
       <c r="J26" s="5">
         <v>120</v>
       </c>
-      <c r="P26" s="5">
+      <c r="R26" s="5">
         <v>80</v>
       </c>
-      <c r="Q26" s="5">
+      <c r="S26" s="5">
         <v>12</v>
       </c>
-      <c r="R26" s="5">
+      <c r="T26" s="5">
         <v>185</v>
       </c>
-      <c r="S26" s="5">
+      <c r="U26" s="5">
         <v>26</v>
       </c>
-      <c r="U26">
+      <c r="W26">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="W26">
+      <c r="Y26">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="AD26" s="3" t="s">
+      <c r="AF26" s="3" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>508</v>
       </c>
@@ -28045,31 +28087,31 @@
       <c r="J27" s="5">
         <v>120</v>
       </c>
-      <c r="P27" s="5">
+      <c r="R27" s="5">
         <v>58</v>
       </c>
-      <c r="Q27" s="5">
+      <c r="S27" s="5">
         <v>12</v>
       </c>
-      <c r="R27" s="5">
+      <c r="T27" s="5">
         <v>185</v>
       </c>
-      <c r="S27" s="5">
+      <c r="U27" s="5">
         <v>25.2</v>
       </c>
-      <c r="U27">
+      <c r="W27">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="W27">
+      <c r="Y27">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="AD27" s="3" t="s">
+      <c r="AF27" s="3" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="28" spans="1:30" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:32" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>509</v>
       </c>
@@ -28082,31 +28124,31 @@
       <c r="J28" s="5">
         <v>80</v>
       </c>
-      <c r="P28" s="5">
+      <c r="R28" s="5">
         <v>50</v>
       </c>
-      <c r="Q28" s="5">
+      <c r="S28" s="5">
         <v>12</v>
       </c>
-      <c r="R28" s="5">
+      <c r="T28" s="5">
         <v>185</v>
       </c>
-      <c r="S28" s="5">
+      <c r="U28" s="5">
         <v>21.5</v>
       </c>
-      <c r="U28">
+      <c r="W28">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="W28">
+      <c r="Y28">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="AD28" s="3" t="s">
+      <c r="AF28" s="3" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="29" spans="1:30" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:32" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>520</v>
       </c>
@@ -28119,31 +28161,31 @@
       <c r="J29" s="5">
         <v>100</v>
       </c>
-      <c r="P29" s="5">
+      <c r="R29" s="5">
         <v>58</v>
       </c>
-      <c r="Q29" s="5">
+      <c r="S29" s="5">
         <v>12</v>
       </c>
-      <c r="R29" s="5">
+      <c r="T29" s="5">
         <v>185</v>
       </c>
-      <c r="S29" s="5">
+      <c r="U29" s="5">
         <v>21.5</v>
       </c>
-      <c r="U29">
-        <f t="shared" ref="U29:U31" si="2">MEDIAN(0,255,ROUND(S29/20+SQRT(J29)/40+SQRT(P29)/2+(SQRT(R29)-SQRT(185)),0))</f>
+      <c r="W29">
+        <f t="shared" ref="W29:W31" si="2">MEDIAN(0,255,ROUND(U29/20+SQRT(J29)/40+SQRT(R29)/2+(SQRT(T29)-SQRT(185)),0))</f>
         <v>5</v>
       </c>
-      <c r="W29">
-        <f t="shared" ref="W29:W31" si="3">MEDIAN(0,255,ROUND(SQRT(J29)/200+SQRT(P29)/2+(SQRT(R29)-SQRT(185)),0))</f>
+      <c r="Y29">
+        <f t="shared" ref="Y29:Y31" si="3">MEDIAN(0,255,ROUND(SQRT(J29)/200+SQRT(R29)/2+(SQRT(T29)-SQRT(185)),0))</f>
         <v>4</v>
       </c>
-      <c r="AD29" s="3" t="s">
+      <c r="AF29" s="3" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>534</v>
       </c>
@@ -28162,31 +28204,34 @@
       <c r="J30" s="5">
         <v>100</v>
       </c>
-      <c r="P30" s="5">
+      <c r="R30" s="5">
         <v>18</v>
       </c>
-      <c r="Q30" s="5">
+      <c r="S30" s="5">
         <v>6</v>
       </c>
-      <c r="R30" s="5">
+      <c r="T30" s="5">
         <v>400</v>
       </c>
-      <c r="S30" s="5">
+      <c r="U30" s="5">
         <v>27</v>
       </c>
-      <c r="U30">
+      <c r="W30">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="W30">
+      <c r="Y30">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="Y30">
+      <c r="AA30">
         <v>10</v>
       </c>
-    </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AF30" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="31" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>536</v>
       </c>
@@ -28205,31 +28250,34 @@
       <c r="J31" s="5">
         <v>85</v>
       </c>
-      <c r="P31" s="5">
+      <c r="R31" s="5">
         <v>50</v>
       </c>
-      <c r="Q31" s="5">
+      <c r="S31" s="5">
         <v>12</v>
       </c>
-      <c r="R31" s="5">
+      <c r="T31" s="5">
         <v>185</v>
       </c>
-      <c r="S31" s="5">
+      <c r="U31" s="5">
         <v>26.5</v>
       </c>
-      <c r="U31">
+      <c r="W31">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="W31">
+      <c r="Y31">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="Y31">
+      <c r="AA31">
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="AF31" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="32" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>537</v>
       </c>
@@ -28248,31 +28296,34 @@
       <c r="J32" s="5">
         <v>85</v>
       </c>
-      <c r="P32" s="5">
+      <c r="R32" s="5">
         <v>50</v>
       </c>
-      <c r="Q32" s="5">
+      <c r="S32" s="5">
         <v>12</v>
       </c>
-      <c r="R32" s="5">
+      <c r="T32" s="5">
         <v>400</v>
       </c>
-      <c r="S32" s="5">
+      <c r="U32" s="5">
         <v>26.5</v>
       </c>
-      <c r="U32">
-        <f t="shared" ref="U32:U43" si="4">MEDIAN(0,255,ROUND(S32/20+SQRT(J32)/40+SQRT(P32)/2+(SQRT(R32)-SQRT(185)),0))</f>
+      <c r="W32">
+        <f t="shared" ref="W32:W44" si="4">MEDIAN(0,255,ROUND(U32/20+SQRT(J32)/40+SQRT(R32)/2+(SQRT(T32)-SQRT(185)),0))</f>
         <v>11</v>
       </c>
-      <c r="W32">
-        <f t="shared" ref="W32:W43" si="5">MEDIAN(0,255,ROUND(SQRT(J32)/200+SQRT(P32)/2+(SQRT(R32)-SQRT(185)),0))</f>
+      <c r="Y32">
+        <f t="shared" ref="Y32:Y44" si="5">MEDIAN(0,255,ROUND(SQRT(J32)/200+SQRT(R32)/2+(SQRT(T32)-SQRT(185)),0))</f>
         <v>10</v>
       </c>
-      <c r="Y32">
+      <c r="AA32">
         <v>8</v>
       </c>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="AF32" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="33" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>543</v>
       </c>
@@ -28291,31 +28342,34 @@
       <c r="J33" s="5">
         <v>120</v>
       </c>
-      <c r="P33" s="5">
+      <c r="R33" s="5">
         <v>50</v>
       </c>
-      <c r="Q33" s="5">
+      <c r="S33" s="5">
         <v>12</v>
       </c>
-      <c r="R33" s="5">
+      <c r="T33" s="5">
         <v>400</v>
       </c>
-      <c r="S33" s="5">
+      <c r="U33" s="5">
         <v>26.5</v>
       </c>
-      <c r="U33">
+      <c r="W33">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="W33">
+      <c r="Y33">
         <f t="shared" si="5"/>
         <v>10</v>
       </c>
-      <c r="Y33">
+      <c r="AA33">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="AF33" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="34" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>538</v>
       </c>
@@ -28331,31 +28385,34 @@
       <c r="J34" s="5">
         <v>120</v>
       </c>
-      <c r="P34" s="5">
+      <c r="R34" s="5">
         <v>60</v>
       </c>
-      <c r="Q34" s="5">
+      <c r="S34" s="5">
         <v>16</v>
       </c>
-      <c r="R34" s="5">
+      <c r="T34" s="5">
         <v>185</v>
       </c>
-      <c r="S34" s="5">
+      <c r="U34" s="5">
         <v>24</v>
       </c>
-      <c r="U34">
+      <c r="W34">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="W34">
+      <c r="Y34">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="Y34">
+      <c r="AA34">
         <v>8</v>
       </c>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="AF34" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="35" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>535</v>
       </c>
@@ -28371,31 +28428,34 @@
       <c r="J35" s="5">
         <v>120</v>
       </c>
-      <c r="P35" s="5">
+      <c r="R35" s="5">
         <v>55</v>
       </c>
-      <c r="Q35" s="5">
+      <c r="S35" s="5">
         <v>16</v>
       </c>
-      <c r="R35" s="5">
+      <c r="T35" s="5">
         <v>400</v>
       </c>
-      <c r="S35" s="5">
+      <c r="U35" s="5">
         <v>24</v>
       </c>
-      <c r="U35">
+      <c r="W35">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="W35">
+      <c r="Y35">
         <f t="shared" si="5"/>
         <v>10</v>
       </c>
-      <c r="Y35">
+      <c r="AA35">
         <v>8</v>
       </c>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="AF35" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="36" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>539</v>
       </c>
@@ -28411,31 +28471,34 @@
       <c r="J36" s="5">
         <v>120</v>
       </c>
-      <c r="P36" s="5">
+      <c r="R36" s="5">
         <v>64</v>
       </c>
-      <c r="Q36" s="5">
+      <c r="S36" s="5">
         <v>16</v>
       </c>
-      <c r="R36" s="5">
+      <c r="T36" s="5">
         <v>800</v>
       </c>
-      <c r="S36" s="5">
+      <c r="U36" s="5">
         <v>29.5</v>
       </c>
-      <c r="U36">
+      <c r="W36">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
-      <c r="W36">
+      <c r="Y36">
         <f t="shared" si="5"/>
         <v>19</v>
       </c>
-      <c r="Y36">
+      <c r="AA36">
         <v>10</v>
       </c>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="AF36" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="37" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>540</v>
       </c>
@@ -28454,31 +28517,34 @@
       <c r="J37" s="5">
         <v>120</v>
       </c>
-      <c r="P37" s="5">
+      <c r="R37" s="5">
         <v>60</v>
       </c>
-      <c r="Q37" s="5">
+      <c r="S37" s="5">
         <v>48</v>
       </c>
-      <c r="R37" s="5">
+      <c r="T37" s="5">
         <v>185</v>
       </c>
-      <c r="S37" s="5">
+      <c r="U37" s="5">
         <v>23.8</v>
       </c>
-      <c r="U37">
+      <c r="W37">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="W37">
+      <c r="Y37">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="Y37">
+      <c r="AA37">
         <v>8</v>
       </c>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="AF37" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="38" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>541</v>
       </c>
@@ -28497,31 +28563,34 @@
       <c r="J38" s="5">
         <v>100</v>
       </c>
-      <c r="P38" s="5">
+      <c r="R38" s="5">
         <v>58</v>
       </c>
-      <c r="Q38" s="5">
+      <c r="S38" s="5">
         <v>12</v>
       </c>
-      <c r="R38" s="5">
+      <c r="T38" s="5">
         <v>185</v>
       </c>
-      <c r="S38" s="5">
+      <c r="U38" s="5">
         <v>25.3</v>
       </c>
-      <c r="U38">
+      <c r="W38">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="W38">
+      <c r="Y38">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="Y38">
+      <c r="AA38">
         <v>8</v>
       </c>
-    </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="AF38" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="39" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>542</v>
       </c>
@@ -28540,31 +28609,34 @@
       <c r="J39" s="5">
         <v>100</v>
       </c>
-      <c r="P39" s="5">
+      <c r="R39" s="5">
         <v>60</v>
       </c>
-      <c r="Q39" s="5">
+      <c r="S39" s="5">
         <v>12</v>
       </c>
-      <c r="R39" s="5">
+      <c r="T39" s="5">
         <v>185</v>
       </c>
-      <c r="S39" s="5">
+      <c r="U39" s="5">
         <v>23.4</v>
       </c>
-      <c r="U39">
+      <c r="W39">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="W39">
+      <c r="Y39">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="Y39">
+      <c r="AA39">
         <v>8</v>
       </c>
-    </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="AF39" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="40" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>544</v>
       </c>
@@ -28580,31 +28652,34 @@
       <c r="J40" s="5">
         <v>120</v>
       </c>
-      <c r="P40" s="5">
+      <c r="R40" s="5">
         <v>78</v>
       </c>
-      <c r="Q40" s="5">
+      <c r="S40" s="5">
         <v>24</v>
       </c>
-      <c r="R40" s="5">
+      <c r="T40" s="5">
         <v>185</v>
       </c>
-      <c r="S40" s="5">
+      <c r="U40" s="5">
         <v>21.8</v>
       </c>
-      <c r="U40">
+      <c r="W40">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="W40">
+      <c r="Y40">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="Y40">
+      <c r="AA40">
         <v>11</v>
       </c>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="AF40" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="41" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>554</v>
       </c>
@@ -28623,25 +28698,37 @@
       <c r="J41" s="5">
         <v>75</v>
       </c>
-      <c r="P41" s="5">
+      <c r="L41">
+        <v>11</v>
+      </c>
+      <c r="M41" t="s">
+        <v>559</v>
+      </c>
+      <c r="R41" s="5">
         <v>30</v>
       </c>
-      <c r="Q41" s="5">
+      <c r="S41" s="5">
         <v>16</v>
       </c>
-      <c r="R41" s="5">
+      <c r="T41" s="5">
         <v>185</v>
       </c>
-      <c r="U41">
+      <c r="U41" s="5">
+        <v>15</v>
+      </c>
+      <c r="W41">
         <f t="shared" si="4"/>
-        <v>3</v>
-      </c>
-      <c r="W41">
+        <v>4</v>
+      </c>
+      <c r="Y41">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="AF41" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="42" spans="1:32" x14ac:dyDescent="0.3">
       <c r="F42" s="5">
         <v>1956</v>
       </c>
@@ -28657,16 +28744,37 @@
       <c r="J42" s="5">
         <v>75</v>
       </c>
-      <c r="U42">
+      <c r="L42">
+        <v>13</v>
+      </c>
+      <c r="M42" t="s">
+        <v>559</v>
+      </c>
+      <c r="R42" s="5">
+        <v>30</v>
+      </c>
+      <c r="S42" s="5">
+        <v>16</v>
+      </c>
+      <c r="T42" s="5">
+        <v>185</v>
+      </c>
+      <c r="U42" s="5">
+        <v>13.5</v>
+      </c>
+      <c r="W42">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="W42">
+        <v>4</v>
+      </c>
+      <c r="Y42">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="AF42" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="43" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>555</v>
       </c>
@@ -28682,25 +28790,88 @@
       <c r="J43" s="5">
         <v>100</v>
       </c>
-      <c r="P43" s="5">
-        <v>240</v>
-      </c>
-      <c r="Q43" s="5">
+      <c r="L43">
+        <v>25</v>
+      </c>
+      <c r="M43" t="s">
+        <v>558</v>
+      </c>
+      <c r="R43" s="5">
+        <v>80</v>
+      </c>
+      <c r="S43" s="5">
         <v>24</v>
       </c>
-      <c r="R43" s="5">
+      <c r="T43" s="5">
         <v>185</v>
       </c>
-      <c r="S43" s="5">
+      <c r="U43" s="5">
+        <v>20</v>
+      </c>
+      <c r="W43">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="Y43">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="AF43" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="44" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>560</v>
+      </c>
+      <c r="F44" s="5">
+        <v>1992</v>
+      </c>
+      <c r="G44" s="5">
+        <v>30</v>
+      </c>
+      <c r="H44">
         <v>60</v>
       </c>
-      <c r="U43">
+      <c r="I44">
+        <v>30</v>
+      </c>
+      <c r="J44" s="5">
+        <v>100</v>
+      </c>
+      <c r="L44">
+        <v>18</v>
+      </c>
+      <c r="M44" t="s">
+        <v>561</v>
+      </c>
+      <c r="R44" s="5">
+        <v>62</v>
+      </c>
+      <c r="S44" s="5">
+        <v>8</v>
+      </c>
+      <c r="T44" s="5">
+        <v>185</v>
+      </c>
+      <c r="U44" s="5">
+        <v>20</v>
+      </c>
+      <c r="W44">
         <f t="shared" si="4"/>
-        <v>11</v>
-      </c>
-      <c r="W43">
+        <v>5</v>
+      </c>
+      <c r="Y44">
         <f t="shared" si="5"/>
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="AF44" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="45" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="AF45" s="3" t="s">
+        <v>388</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change the capcity of rzxl25z
</commit_message>
<xml_diff>
--- a/docs/China Set Trains.xlsx
+++ b/docs/China Set Trains.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CNS\CNST\local\China-Set-Trains\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F1A18D-3C64-43A2-9D69-D64971793426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A71394B9-7263-42AB-AF28-E08120DED3BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1959" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1962" uniqueCount="566">
   <si>
     <t>name</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2131,10 +2131,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>8+6</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>RZT25G</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -2192,6 +2188,14 @@
   </si>
   <si>
     <t>UZ25T</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>16+12</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>56+24</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2261,7 +2265,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
@@ -2283,12 +2287,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2763,7 +2761,7 @@
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="E3" t="s">
         <v>26</v>
@@ -2913,10 +2911,10 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D5" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E5" t="s">
         <v>26</v>
@@ -26878,10 +26876,10 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
+        <v>555</v>
+      </c>
+      <c r="M1" t="s">
         <v>556</v>
-      </c>
-      <c r="M1" t="s">
-        <v>557</v>
       </c>
       <c r="N1" t="s">
         <v>11</v>
@@ -28693,7 +28691,7 @@
     </row>
     <row r="41" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="F41" s="5">
         <v>1949</v>
@@ -28714,7 +28712,7 @@
         <v>11</v>
       </c>
       <c r="M41" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="R41" s="5">
         <v>30</v>
@@ -28760,7 +28758,7 @@
         <v>13</v>
       </c>
       <c r="M42" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="R42" s="5">
         <v>30</v>
@@ -28788,7 +28786,7 @@
     </row>
     <row r="43" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F43" s="5">
         <v>2003</v>
@@ -28806,7 +28804,7 @@
         <v>25</v>
       </c>
       <c r="M43" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="R43" s="5">
         <v>80</v>
@@ -28834,7 +28832,7 @@
     </row>
     <row r="44" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F44" s="5">
         <v>1992</v>
@@ -28855,7 +28853,7 @@
         <v>18</v>
       </c>
       <c r="M44" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="R44" s="5">
         <v>62</v>
@@ -28897,8 +28895,8 @@
   <dimension ref="A1:AB86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S90" sqref="S90"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V90" sqref="V90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -28941,10 +28939,10 @@
         <v>14</v>
       </c>
       <c r="M1" t="s">
+        <v>555</v>
+      </c>
+      <c r="N1" t="s">
         <v>556</v>
-      </c>
-      <c r="N1" t="s">
-        <v>557</v>
       </c>
       <c r="O1" t="s">
         <v>15</v>
@@ -31389,7 +31387,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:28" ht="14" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>290</v>
       </c>
@@ -31427,25 +31425,25 @@
         <v>46.4</v>
       </c>
       <c r="S48">
-        <f t="shared" ref="S48:S62" si="29">MEDIAN(0,255,ROUND(R48/20+SQRT(H48)/40+SQRT(O48)/2+(SQRT(Q48)-SQRT(185)), 0))</f>
+        <f t="shared" ref="S48:S61" si="29">MEDIAN(0,255,ROUND(R48/20+SQRT(H48)/40+SQRT(O48)/2+(SQRT(Q48)-SQRT(185)), 0))</f>
         <v>9</v>
       </c>
       <c r="T48">
-        <f t="shared" ref="T48:T62" si="30">S48*50000/16</f>
+        <f t="shared" ref="T48:T61" si="30">S48*50000/16</f>
         <v>28125</v>
       </c>
       <c r="U48">
-        <f t="shared" ref="U48:U62" si="31">MEDIAN(0,255,ROUND(SQRT(H48)/200+SQRT(O48)/2+(SQRT(Q48)-SQRT(185)),0))</f>
+        <f t="shared" ref="U48:U61" si="31">MEDIAN(0,255,ROUND(SQRT(H48)/200+SQRT(O48)/2+(SQRT(Q48)-SQRT(185)),0))</f>
         <v>7</v>
       </c>
       <c r="V48">
-        <f t="shared" ref="V48:V62" si="32">U48*300/16*12</f>
+        <f t="shared" ref="V48:V61" si="32">U48*300/16*12</f>
         <v>1575</v>
       </c>
       <c r="AA48" t="s">
         <v>344</v>
       </c>
-      <c r="AB48" s="10" t="s">
+      <c r="AB48" s="9" t="s">
         <v>312</v>
       </c>
     </row>
@@ -31505,7 +31503,7 @@
       <c r="AA49" t="s">
         <v>344</v>
       </c>
-      <c r="AB49" s="11"/>
+      <c r="AB49" s="9"/>
     </row>
     <row r="50" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
@@ -31563,7 +31561,7 @@
       <c r="AA50" t="s">
         <v>344</v>
       </c>
-      <c r="AB50" s="11"/>
+      <c r="AB50" s="9"/>
     </row>
     <row r="51" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
@@ -31621,7 +31619,7 @@
       <c r="AA51" t="s">
         <v>344</v>
       </c>
-      <c r="AB51" s="11"/>
+      <c r="AB51" s="9"/>
     </row>
     <row r="52" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
@@ -31679,17 +31677,17 @@
       <c r="AA52" t="s">
         <v>344</v>
       </c>
-      <c r="AB52" s="11"/>
+      <c r="AB52" s="9"/>
     </row>
     <row r="53" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="B53" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="D53" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="E53">
         <v>1993</v>
@@ -31704,50 +31702,50 @@
         <v>140</v>
       </c>
       <c r="I53" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="O53">
-        <v>71</v>
+        <v>124</v>
       </c>
       <c r="P53">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Q53">
-        <v>200</v>
+        <v>240</v>
       </c>
       <c r="R53">
-        <v>42</v>
+        <v>52.7</v>
       </c>
       <c r="S53">
         <f t="shared" si="29"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="T53">
         <f t="shared" si="30"/>
-        <v>21875</v>
+        <v>31250</v>
       </c>
       <c r="U53">
         <f t="shared" si="31"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="V53">
         <f t="shared" si="32"/>
-        <v>1125</v>
+        <v>1800</v>
       </c>
       <c r="AA53" t="s">
         <v>344</v>
       </c>
-      <c r="AB53" s="11"/>
+      <c r="AB53" s="9"/>
     </row>
     <row r="54" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B54" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="D54" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="E54">
         <v>1993</v>
@@ -31765,47 +31763,47 @@
         <v>292</v>
       </c>
       <c r="O54">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="P54">
         <v>16</v>
       </c>
       <c r="Q54">
-        <v>240</v>
+        <v>320</v>
       </c>
       <c r="R54">
-        <v>52.7</v>
+        <v>53</v>
       </c>
       <c r="S54">
         <f t="shared" si="29"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="T54">
         <f t="shared" si="30"/>
-        <v>31250</v>
+        <v>37500</v>
       </c>
       <c r="U54">
         <f t="shared" si="31"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="V54">
         <f t="shared" si="32"/>
-        <v>1800</v>
+        <v>2250</v>
       </c>
       <c r="AA54" t="s">
         <v>344</v>
       </c>
-      <c r="AB54" s="11"/>
+      <c r="AB54" s="9"/>
     </row>
     <row r="55" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B55" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="D55" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="E55">
         <v>1993</v>
@@ -31823,47 +31821,47 @@
         <v>292</v>
       </c>
       <c r="O55">
-        <v>108</v>
+        <v>60</v>
       </c>
       <c r="P55">
         <v>16</v>
       </c>
       <c r="Q55">
-        <v>320</v>
+        <v>240</v>
       </c>
       <c r="R55">
-        <v>53</v>
+        <v>50.1</v>
       </c>
       <c r="S55">
         <f t="shared" si="29"/>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="T55">
         <f t="shared" si="30"/>
-        <v>37500</v>
+        <v>28125</v>
       </c>
       <c r="U55">
         <f t="shared" si="31"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="V55">
         <f t="shared" si="32"/>
-        <v>2250</v>
+        <v>1350</v>
       </c>
       <c r="AA55" t="s">
         <v>344</v>
       </c>
-      <c r="AB55" s="11"/>
+      <c r="AB55" s="9"/>
     </row>
     <row r="56" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B56" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="D56" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="E56">
         <v>1993</v>
@@ -31878,105 +31876,104 @@
         <v>140</v>
       </c>
       <c r="I56" t="s">
-        <v>292</v>
+        <v>303</v>
       </c>
       <c r="O56">
-        <v>60</v>
+        <v>92</v>
       </c>
       <c r="P56">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="Q56">
-        <v>240</v>
+        <v>200</v>
       </c>
       <c r="R56">
-        <v>50.1</v>
+        <v>49.2</v>
       </c>
       <c r="S56">
         <f t="shared" si="29"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T56">
         <f t="shared" si="30"/>
-        <v>28125</v>
+        <v>25000</v>
       </c>
       <c r="U56">
         <f t="shared" si="31"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V56">
         <f t="shared" si="32"/>
-        <v>1350</v>
+        <v>1125</v>
       </c>
       <c r="AA56" t="s">
         <v>344</v>
       </c>
-      <c r="AB56" s="11"/>
+      <c r="AB56" s="9"/>
     </row>
     <row r="57" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>310</v>
+        <v>339</v>
       </c>
       <c r="B57" t="s">
-        <v>311</v>
-      </c>
-      <c r="D57" t="s">
-        <v>310</v>
+        <v>341</v>
       </c>
       <c r="E57">
-        <v>1993</v>
+        <v>2014</v>
       </c>
       <c r="F57">
         <v>30</v>
       </c>
-      <c r="G57">
-        <v>20</v>
+      <c r="G57" t="s">
+        <v>87</v>
       </c>
       <c r="H57">
         <v>140</v>
       </c>
       <c r="I57" t="s">
-        <v>303</v>
+        <v>86</v>
       </c>
       <c r="O57">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="P57">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Q57">
-        <v>200</v>
+        <v>360</v>
       </c>
       <c r="R57">
-        <v>49.2</v>
+        <v>53.6</v>
       </c>
       <c r="S57">
         <f t="shared" si="29"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="T57">
         <f t="shared" si="30"/>
-        <v>25000</v>
+        <v>40625</v>
       </c>
       <c r="U57">
         <f t="shared" si="31"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="V57">
         <f t="shared" si="32"/>
-        <v>1125</v>
+        <v>2250</v>
       </c>
       <c r="AA57" t="s">
         <v>344</v>
       </c>
-      <c r="AB57" s="11"/>
+      <c r="AB57" t="s">
+        <v>343</v>
+      </c>
     </row>
     <row r="58" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B58" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="E58">
         <v>2014</v>
@@ -31994,32 +31991,32 @@
         <v>86</v>
       </c>
       <c r="O58">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="P58">
         <v>16</v>
       </c>
       <c r="Q58">
-        <v>360</v>
+        <v>480</v>
       </c>
       <c r="R58">
-        <v>53.6</v>
+        <v>56</v>
       </c>
       <c r="S58">
         <f t="shared" si="29"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="T58">
         <f t="shared" si="30"/>
-        <v>40625</v>
+        <v>46875</v>
       </c>
       <c r="U58">
         <f t="shared" si="31"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="V58">
         <f t="shared" si="32"/>
-        <v>2250</v>
+        <v>2700</v>
       </c>
       <c r="AA58" t="s">
         <v>344</v>
@@ -32030,13 +32027,13 @@
     </row>
     <row r="59" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>340</v>
+        <v>362</v>
       </c>
       <c r="B59" t="s">
-        <v>342</v>
+        <v>364</v>
       </c>
       <c r="E59">
-        <v>2014</v>
+        <v>1997</v>
       </c>
       <c r="F59">
         <v>30</v>
@@ -32045,55 +32042,55 @@
         <v>87</v>
       </c>
       <c r="H59">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="I59" t="s">
         <v>86</v>
       </c>
       <c r="O59">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="P59">
         <v>16</v>
       </c>
       <c r="Q59">
-        <v>480</v>
+        <v>640</v>
       </c>
       <c r="R59">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="S59">
         <f t="shared" si="29"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="T59">
         <f t="shared" si="30"/>
-        <v>46875</v>
+        <v>53125</v>
       </c>
       <c r="U59">
         <f t="shared" si="31"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="V59">
         <f t="shared" si="32"/>
-        <v>2700</v>
+        <v>3150</v>
       </c>
       <c r="AA59" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="AB59" t="s">
-        <v>343</v>
+        <v>366</v>
       </c>
     </row>
     <row r="60" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B60" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="E60">
-        <v>1997</v>
+        <v>2007.5</v>
       </c>
       <c r="F60">
         <v>30</v>
@@ -32117,7 +32114,7 @@
         <v>640</v>
       </c>
       <c r="R60">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="S60">
         <f t="shared" si="29"/>
@@ -32144,53 +32141,53 @@
     </row>
     <row r="61" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="B61" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="E61">
-        <v>2007.5</v>
+        <v>1959</v>
       </c>
       <c r="F61">
         <v>30</v>
       </c>
-      <c r="G61" t="s">
-        <v>87</v>
+      <c r="G61">
+        <v>35</v>
       </c>
       <c r="H61">
-        <v>160</v>
+        <v>120</v>
       </c>
       <c r="I61" t="s">
-        <v>86</v>
+        <v>369</v>
       </c>
       <c r="O61">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="P61">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="Q61">
-        <v>640</v>
+        <v>200</v>
       </c>
       <c r="R61">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="S61">
         <f t="shared" si="29"/>
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="T61">
         <f t="shared" si="30"/>
-        <v>53125</v>
+        <v>21875</v>
       </c>
       <c r="U61">
         <f t="shared" si="31"/>
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="V61">
         <f t="shared" si="32"/>
-        <v>3150</v>
+        <v>1125</v>
       </c>
       <c r="AA61" t="s">
         <v>337</v>
@@ -32201,13 +32198,13 @@
     </row>
     <row r="62" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="B62" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="E62">
-        <v>1959</v>
+        <v>1985</v>
       </c>
       <c r="F62">
         <v>30</v>
@@ -32216,38 +32213,38 @@
         <v>35</v>
       </c>
       <c r="H62">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="I62" t="s">
-        <v>369</v>
+        <v>86</v>
       </c>
       <c r="O62">
-        <v>68</v>
+        <v>118</v>
       </c>
       <c r="P62">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Q62">
         <v>200</v>
       </c>
       <c r="R62">
-        <v>43</v>
+        <v>42.5</v>
       </c>
       <c r="S62">
-        <f t="shared" si="29"/>
-        <v>7</v>
+        <f t="shared" ref="S62:S71" si="33">MEDIAN(0,255,ROUND(R62/20+SQRT(H62)/40+SQRT(O62)/2+(SQRT(Q62)-SQRT(185)), 0))</f>
+        <v>8</v>
       </c>
       <c r="T62">
-        <f t="shared" si="30"/>
-        <v>21875</v>
+        <f t="shared" ref="T62:T71" si="34">S62*50000/16</f>
+        <v>25000</v>
       </c>
       <c r="U62">
-        <f t="shared" si="31"/>
-        <v>5</v>
+        <f t="shared" ref="U62:U71" si="35">MEDIAN(0,255,ROUND(SQRT(H62)/200+SQRT(O62)/2+(SQRT(Q62)-SQRT(185)),0))</f>
+        <v>6</v>
       </c>
       <c r="V62">
-        <f t="shared" si="32"/>
-        <v>1125</v>
+        <f t="shared" ref="V62:V71" si="36">U62*300/16*12</f>
+        <v>1350</v>
       </c>
       <c r="AA62" t="s">
         <v>337</v>
@@ -32258,10 +32255,10 @@
     </row>
     <row r="63" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B63" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="E63">
         <v>1985</v>
@@ -32279,31 +32276,31 @@
         <v>86</v>
       </c>
       <c r="O63">
-        <v>118</v>
+        <v>64</v>
       </c>
       <c r="P63">
         <v>16</v>
       </c>
       <c r="Q63">
-        <v>200</v>
+        <v>240</v>
       </c>
       <c r="R63">
-        <v>42.5</v>
+        <v>46</v>
       </c>
       <c r="S63">
-        <f t="shared" ref="S63:S72" si="33">MEDIAN(0,255,ROUND(R63/20+SQRT(H63)/40+SQRT(O63)/2+(SQRT(Q63)-SQRT(185)), 0))</f>
+        <f t="shared" si="33"/>
         <v>8</v>
       </c>
       <c r="T63">
-        <f t="shared" ref="T63:T72" si="34">S63*50000/16</f>
+        <f t="shared" si="34"/>
         <v>25000</v>
       </c>
       <c r="U63">
-        <f t="shared" ref="U63:U72" si="35">MEDIAN(0,255,ROUND(SQRT(H63)/200+SQRT(O63)/2+(SQRT(Q63)-SQRT(185)),0))</f>
+        <f t="shared" si="35"/>
         <v>6</v>
       </c>
       <c r="V63">
-        <f t="shared" ref="V63:V72" si="36">U63*300/16*12</f>
+        <f t="shared" si="36"/>
         <v>1350</v>
       </c>
       <c r="AA63" t="s">
@@ -32315,10 +32312,10 @@
     </row>
     <row r="64" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="B64" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="E64">
         <v>1985</v>
@@ -32336,32 +32333,32 @@
         <v>86</v>
       </c>
       <c r="O64">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="P64">
         <v>16</v>
       </c>
       <c r="Q64">
-        <v>240</v>
+        <v>360</v>
       </c>
       <c r="R64">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="S64">
         <f t="shared" si="33"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="T64">
         <f t="shared" si="34"/>
-        <v>25000</v>
+        <v>37500</v>
       </c>
       <c r="U64">
         <f t="shared" si="35"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="V64">
         <f t="shared" si="36"/>
-        <v>1350</v>
+        <v>2025</v>
       </c>
       <c r="AA64" t="s">
         <v>337</v>
@@ -32372,10 +32369,10 @@
     </row>
     <row r="65" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="B65" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="E65">
         <v>1985</v>
@@ -32393,32 +32390,32 @@
         <v>86</v>
       </c>
       <c r="O65">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="P65">
         <v>16</v>
       </c>
       <c r="Q65">
-        <v>360</v>
+        <v>480</v>
       </c>
       <c r="R65">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="S65">
         <f t="shared" si="33"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="T65">
         <f t="shared" si="34"/>
-        <v>37500</v>
+        <v>43750</v>
       </c>
       <c r="U65">
         <f t="shared" si="35"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="V65">
         <f t="shared" si="36"/>
-        <v>2025</v>
+        <v>2475</v>
       </c>
       <c r="AA65" t="s">
         <v>337</v>
@@ -32429,10 +32426,10 @@
     </row>
     <row r="66" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="B66" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="E66">
         <v>1985</v>
@@ -32450,32 +32447,32 @@
         <v>86</v>
       </c>
       <c r="O66">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="P66">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="Q66">
-        <v>480</v>
+        <v>200</v>
       </c>
       <c r="R66">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="S66">
         <f t="shared" si="33"/>
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="T66">
         <f t="shared" si="34"/>
-        <v>43750</v>
+        <v>21875</v>
       </c>
       <c r="U66">
         <f t="shared" si="35"/>
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="V66">
         <f t="shared" si="36"/>
-        <v>2475</v>
+        <v>900</v>
       </c>
       <c r="AA66" t="s">
         <v>337</v>
@@ -32486,13 +32483,13 @@
     </row>
     <row r="67" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="B67" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="E67">
-        <v>1985</v>
+        <v>1963</v>
       </c>
       <c r="F67">
         <v>30</v>
@@ -32501,7 +32498,7 @@
         <v>35</v>
       </c>
       <c r="H67">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="I67" t="s">
         <v>86</v>
@@ -32513,26 +32510,26 @@
         <v>8</v>
       </c>
       <c r="Q67">
-        <v>200</v>
+        <v>144</v>
       </c>
       <c r="R67">
         <v>45</v>
       </c>
       <c r="S67">
         <f t="shared" si="33"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="T67">
         <f t="shared" si="34"/>
-        <v>21875</v>
+        <v>12500</v>
       </c>
       <c r="U67">
         <f t="shared" si="35"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="V67">
         <f t="shared" si="36"/>
-        <v>900</v>
+        <v>450</v>
       </c>
       <c r="AA67" t="s">
         <v>337</v>
@@ -32543,13 +32540,13 @@
     </row>
     <row r="68" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="B68" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="E68">
-        <v>1963</v>
+        <v>1985</v>
       </c>
       <c r="F68">
         <v>30</v>
@@ -32564,100 +32561,94 @@
         <v>86</v>
       </c>
       <c r="O68">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="P68">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="Q68">
-        <v>144</v>
+        <v>185</v>
       </c>
       <c r="R68">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="S68">
         <f t="shared" si="33"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T68">
         <f t="shared" si="34"/>
-        <v>12500</v>
+        <v>9375</v>
       </c>
       <c r="U68">
         <f t="shared" si="35"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="V68">
         <f t="shared" si="36"/>
-        <v>450</v>
+        <v>0</v>
       </c>
       <c r="AA68" t="s">
         <v>337</v>
       </c>
       <c r="AB68" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="69" spans="1:28" x14ac:dyDescent="0.3">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="69" spans="1:28" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>378</v>
+        <v>423</v>
       </c>
       <c r="B69" t="s">
-        <v>379</v>
+        <v>420</v>
       </c>
       <c r="E69">
-        <v>1985</v>
+        <v>2001</v>
       </c>
       <c r="F69">
         <v>30</v>
       </c>
       <c r="G69">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="H69">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="I69" t="s">
         <v>86</v>
       </c>
       <c r="O69">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="P69">
         <v>16</v>
       </c>
       <c r="Q69">
-        <v>185</v>
+        <v>160</v>
       </c>
       <c r="R69">
-        <v>60</v>
+        <v>49.2</v>
       </c>
       <c r="S69">
-        <f t="shared" si="33"/>
-        <v>3</v>
+        <f t="shared" ref="S69" si="37">MEDIAN(0,255,ROUND(R69/20+SQRT(H69)/40+SQRT(O69)/2+(SQRT(Q69)-SQRT(185)), 0))</f>
+        <v>7</v>
       </c>
       <c r="T69">
-        <f t="shared" si="34"/>
-        <v>9375</v>
+        <f t="shared" ref="T69" si="38">S69*50000/16</f>
+        <v>21875</v>
       </c>
       <c r="U69">
-        <f t="shared" si="35"/>
-        <v>0</v>
+        <f t="shared" ref="U69" si="39">MEDIAN(0,255,ROUND(SQRT(H69)/200+SQRT(O69)/2+(SQRT(Q69)-SQRT(185)),0))</f>
+        <v>4</v>
       </c>
       <c r="V69">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AA69" t="s">
-        <v>337</v>
-      </c>
-      <c r="AB69" t="s">
-        <v>337</v>
+        <f t="shared" ref="V69" si="40">U69*300/16*12</f>
+        <v>900</v>
       </c>
     </row>
     <row r="70" spans="1:28" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B70" t="s">
         <v>420</v>
@@ -32678,37 +32669,37 @@
         <v>86</v>
       </c>
       <c r="O70">
-        <v>98</v>
+        <v>36</v>
       </c>
       <c r="P70">
         <v>16</v>
       </c>
       <c r="Q70">
-        <v>160</v>
+        <v>288</v>
       </c>
       <c r="R70">
         <v>49.2</v>
       </c>
       <c r="S70">
-        <f t="shared" ref="S70" si="37">MEDIAN(0,255,ROUND(R70/20+SQRT(H70)/40+SQRT(O70)/2+(SQRT(Q70)-SQRT(185)), 0))</f>
-        <v>7</v>
+        <f t="shared" ref="S70" si="41">MEDIAN(0,255,ROUND(R70/20+SQRT(H70)/40+SQRT(O70)/2+(SQRT(Q70)-SQRT(185)), 0))</f>
+        <v>9</v>
       </c>
       <c r="T70">
-        <f t="shared" ref="T70" si="38">S70*50000/16</f>
-        <v>21875</v>
+        <f t="shared" ref="T70" si="42">S70*50000/16</f>
+        <v>28125</v>
       </c>
       <c r="U70">
-        <f t="shared" ref="U70" si="39">MEDIAN(0,255,ROUND(SQRT(H70)/200+SQRT(O70)/2+(SQRT(Q70)-SQRT(185)),0))</f>
-        <v>4</v>
+        <f t="shared" ref="U70" si="43">MEDIAN(0,255,ROUND(SQRT(H70)/200+SQRT(O70)/2+(SQRT(Q70)-SQRT(185)),0))</f>
+        <v>6</v>
       </c>
       <c r="V70">
-        <f t="shared" ref="V70" si="40">U70*300/16*12</f>
-        <v>900</v>
+        <f t="shared" ref="V70" si="44">U70*300/16*12</f>
+        <v>1350</v>
       </c>
     </row>
     <row r="71" spans="1:28" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="B71" t="s">
         <v>420</v>
@@ -32735,31 +32726,31 @@
         <v>16</v>
       </c>
       <c r="Q71">
-        <v>288</v>
+        <v>384</v>
       </c>
       <c r="R71">
         <v>49.2</v>
       </c>
       <c r="S71">
-        <f t="shared" ref="S71" si="41">MEDIAN(0,255,ROUND(R71/20+SQRT(H71)/40+SQRT(O71)/2+(SQRT(Q71)-SQRT(185)), 0))</f>
+        <f t="shared" si="33"/>
+        <v>12</v>
+      </c>
+      <c r="T71">
+        <f t="shared" si="34"/>
+        <v>37500</v>
+      </c>
+      <c r="U71">
+        <f t="shared" si="35"/>
         <v>9</v>
       </c>
-      <c r="T71">
-        <f t="shared" ref="T71" si="42">S71*50000/16</f>
-        <v>28125</v>
-      </c>
-      <c r="U71">
-        <f t="shared" ref="U71" si="43">MEDIAN(0,255,ROUND(SQRT(H71)/200+SQRT(O71)/2+(SQRT(Q71)-SQRT(185)),0))</f>
-        <v>6</v>
-      </c>
       <c r="V71">
-        <f t="shared" ref="V71" si="44">U71*300/16*12</f>
-        <v>1350</v>
+        <f t="shared" si="36"/>
+        <v>2025</v>
       </c>
     </row>
     <row r="72" spans="1:28" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="B72" t="s">
         <v>420</v>
@@ -32786,31 +32777,31 @@
         <v>16</v>
       </c>
       <c r="Q72">
-        <v>384</v>
+        <v>160</v>
       </c>
       <c r="R72">
         <v>49.2</v>
       </c>
       <c r="S72">
-        <f t="shared" si="33"/>
-        <v>12</v>
+        <f t="shared" ref="S72:S79" si="45">MEDIAN(0,255,ROUND(R72/20+SQRT(H72)/40+SQRT(O72)/2+(SQRT(Q72)-SQRT(185)), 0))</f>
+        <v>5</v>
       </c>
       <c r="T72">
-        <f t="shared" si="34"/>
-        <v>37500</v>
+        <f t="shared" ref="T72:T85" si="46">S72*50000/16</f>
+        <v>15625</v>
       </c>
       <c r="U72">
-        <f t="shared" si="35"/>
-        <v>9</v>
+        <f t="shared" ref="U72:U79" si="47">MEDIAN(0,255,ROUND(SQRT(H72)/200+SQRT(O72)/2+(SQRT(Q72)-SQRT(185)),0))</f>
+        <v>2</v>
       </c>
       <c r="V72">
-        <f t="shared" si="36"/>
-        <v>2025</v>
+        <f t="shared" ref="V72:V85" si="48">U72*300/16*12</f>
+        <v>450</v>
       </c>
     </row>
     <row r="73" spans="1:28" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B73" t="s">
         <v>420</v>
@@ -32837,136 +32828,142 @@
         <v>16</v>
       </c>
       <c r="Q73">
-        <v>160</v>
+        <v>192</v>
       </c>
       <c r="R73">
         <v>49.2</v>
       </c>
       <c r="S73">
-        <f t="shared" ref="S73:S80" si="45">MEDIAN(0,255,ROUND(R73/20+SQRT(H73)/40+SQRT(O73)/2+(SQRT(Q73)-SQRT(185)), 0))</f>
-        <v>5</v>
+        <f t="shared" si="45"/>
+        <v>6</v>
       </c>
       <c r="T73">
-        <f t="shared" ref="T73:T86" si="46">S73*50000/16</f>
-        <v>15625</v>
+        <f t="shared" si="46"/>
+        <v>18750</v>
       </c>
       <c r="U73">
-        <f t="shared" ref="U73:U80" si="47">MEDIAN(0,255,ROUND(SQRT(H73)/200+SQRT(O73)/2+(SQRT(Q73)-SQRT(185)),0))</f>
-        <v>2</v>
+        <f t="shared" si="47"/>
+        <v>3</v>
       </c>
       <c r="V73">
-        <f t="shared" ref="V73:V86" si="48">U73*300/16*12</f>
-        <v>450</v>
-      </c>
-    </row>
-    <row r="74" spans="1:28" ht="12.65" customHeight="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="48"/>
+        <v>675</v>
+      </c>
+    </row>
+    <row r="74" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="B74" t="s">
-        <v>420</v>
+        <v>426</v>
       </c>
       <c r="E74">
-        <v>2001</v>
+        <v>1964</v>
       </c>
       <c r="F74">
         <v>30</v>
       </c>
       <c r="G74">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H74">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="I74" t="s">
         <v>86</v>
       </c>
       <c r="O74">
-        <v>36</v>
+        <v>300</v>
       </c>
       <c r="P74">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="Q74">
-        <v>192</v>
+        <v>108</v>
       </c>
       <c r="R74">
-        <v>49.2</v>
+        <v>41</v>
       </c>
       <c r="S74">
         <f t="shared" si="45"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="T74">
         <f t="shared" si="46"/>
-        <v>18750</v>
+        <v>25000</v>
       </c>
       <c r="U74">
         <f t="shared" si="47"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="V74">
         <f t="shared" si="48"/>
-        <v>675</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="75" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>425</v>
+        <v>470</v>
       </c>
       <c r="B75" t="s">
-        <v>426</v>
+        <v>471</v>
       </c>
       <c r="E75">
-        <v>1964</v>
+        <v>1981</v>
       </c>
       <c r="F75">
         <v>30</v>
       </c>
-      <c r="G75">
-        <v>20</v>
+      <c r="G75" t="s">
+        <v>87</v>
       </c>
       <c r="H75">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="I75" t="s">
         <v>86</v>
       </c>
       <c r="O75">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="P75">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="Q75">
-        <v>108</v>
+        <v>185</v>
       </c>
       <c r="R75">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="S75">
         <f t="shared" si="45"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="T75">
         <f t="shared" si="46"/>
-        <v>25000</v>
+        <v>9375</v>
       </c>
       <c r="U75">
         <f t="shared" si="47"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="V75">
         <f t="shared" si="48"/>
-        <v>1350</v>
+        <v>0</v>
+      </c>
+      <c r="AA75" t="s">
+        <v>337</v>
+      </c>
+      <c r="AB75" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="76" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="B76" t="s">
-        <v>471</v>
+        <v>74</v>
       </c>
       <c r="E76">
         <v>1981</v>
@@ -32984,46 +32981,40 @@
         <v>86</v>
       </c>
       <c r="O76">
-        <v>0</v>
+        <v>118</v>
       </c>
       <c r="P76">
         <v>16</v>
       </c>
       <c r="Q76">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="R76">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="S76">
-        <f t="shared" si="45"/>
-        <v>3</v>
+        <f>MEDIAN(0,255,ROUND(R76/20+SQRT(H76)/40+SQRT(O76)/2+(SQRT(Q76)-SQRT(185)), 0))</f>
+        <v>8</v>
       </c>
       <c r="T76">
-        <f t="shared" si="46"/>
-        <v>9375</v>
+        <f>S76*50000/16</f>
+        <v>25000</v>
       </c>
       <c r="U76">
-        <f t="shared" si="47"/>
-        <v>0</v>
+        <f>MEDIAN(0,255,ROUND(SQRT(H76)/200+SQRT(O76)/2+(SQRT(Q76)-SQRT(185)),0))</f>
+        <v>6</v>
       </c>
       <c r="V76">
-        <f t="shared" si="48"/>
-        <v>0</v>
-      </c>
-      <c r="AA76" t="s">
-        <v>337</v>
-      </c>
-      <c r="AB76" t="s">
-        <v>337</v>
+        <f>U76*300/16*12</f>
+        <v>1350</v>
       </c>
     </row>
     <row r="77" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="B77" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="E77">
         <v>1981</v>
@@ -33041,40 +33032,40 @@
         <v>86</v>
       </c>
       <c r="O77">
-        <v>118</v>
+        <v>66</v>
       </c>
       <c r="P77">
         <v>16</v>
       </c>
       <c r="Q77">
-        <v>200</v>
+        <v>360</v>
       </c>
       <c r="R77">
-        <v>42</v>
+        <v>44.7</v>
       </c>
       <c r="S77">
-        <f>MEDIAN(0,255,ROUND(R77/20+SQRT(H77)/40+SQRT(O77)/2+(SQRT(Q77)-SQRT(185)), 0))</f>
-        <v>8</v>
+        <f t="shared" ref="S77:S78" si="49">MEDIAN(0,255,ROUND(R77/20+SQRT(H77)/40+SQRT(O77)/2+(SQRT(Q77)-SQRT(185)), 0))</f>
+        <v>12</v>
       </c>
       <c r="T77">
-        <f>S77*50000/16</f>
-        <v>25000</v>
+        <f t="shared" ref="T77:T78" si="50">S77*50000/16</f>
+        <v>37500</v>
       </c>
       <c r="U77">
-        <f>MEDIAN(0,255,ROUND(SQRT(H77)/200+SQRT(O77)/2+(SQRT(Q77)-SQRT(185)),0))</f>
-        <v>6</v>
+        <f t="shared" ref="U77:U78" si="51">MEDIAN(0,255,ROUND(SQRT(H77)/200+SQRT(O77)/2+(SQRT(Q77)-SQRT(185)),0))</f>
+        <v>9</v>
       </c>
       <c r="V77">
-        <f>U77*300/16*12</f>
-        <v>1350</v>
+        <f t="shared" ref="V77:V78" si="52">U77*300/16*12</f>
+        <v>2025</v>
       </c>
     </row>
     <row r="78" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B78" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E78">
         <v>1981</v>
@@ -33092,40 +33083,37 @@
         <v>86</v>
       </c>
       <c r="O78">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="P78">
         <v>16</v>
       </c>
       <c r="Q78">
-        <v>360</v>
+        <v>480</v>
       </c>
       <c r="R78">
-        <v>44.7</v>
+        <v>47.3</v>
       </c>
       <c r="S78">
-        <f t="shared" ref="S78:S79" si="49">MEDIAN(0,255,ROUND(R78/20+SQRT(H78)/40+SQRT(O78)/2+(SQRT(Q78)-SQRT(185)), 0))</f>
-        <v>12</v>
+        <f t="shared" si="49"/>
+        <v>14</v>
       </c>
       <c r="T78">
-        <f t="shared" ref="T78:T79" si="50">S78*50000/16</f>
-        <v>37500</v>
+        <f t="shared" si="50"/>
+        <v>43750</v>
       </c>
       <c r="U78">
-        <f t="shared" ref="U78:U79" si="51">MEDIAN(0,255,ROUND(SQRT(H78)/200+SQRT(O78)/2+(SQRT(Q78)-SQRT(185)),0))</f>
-        <v>9</v>
+        <f t="shared" si="51"/>
+        <v>11</v>
       </c>
       <c r="V78">
-        <f t="shared" ref="V78:V79" si="52">U78*300/16*12</f>
-        <v>2025</v>
+        <f t="shared" si="52"/>
+        <v>2475</v>
       </c>
     </row>
     <row r="79" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>474</v>
-      </c>
-      <c r="B79" t="s">
-        <v>82</v>
+        <v>475</v>
       </c>
       <c r="E79">
         <v>1981</v>
@@ -33143,37 +33131,37 @@
         <v>86</v>
       </c>
       <c r="O79">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="P79">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="Q79">
-        <v>480</v>
+        <v>200</v>
       </c>
       <c r="R79">
-        <v>47.3</v>
+        <v>47.5</v>
       </c>
       <c r="S79">
-        <f t="shared" si="49"/>
-        <v>14</v>
+        <f t="shared" si="45"/>
+        <v>7</v>
       </c>
       <c r="T79">
-        <f t="shared" si="50"/>
-        <v>43750</v>
+        <f t="shared" si="46"/>
+        <v>21875</v>
       </c>
       <c r="U79">
-        <f t="shared" si="51"/>
-        <v>11</v>
+        <f t="shared" si="47"/>
+        <v>4</v>
       </c>
       <c r="V79">
-        <f t="shared" si="52"/>
-        <v>2475</v>
+        <f t="shared" si="48"/>
+        <v>900</v>
       </c>
     </row>
     <row r="80" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="E80">
         <v>1981</v>
@@ -33188,22 +33176,22 @@
         <v>120</v>
       </c>
       <c r="I80" t="s">
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="O80">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="P80">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="Q80">
         <v>200</v>
       </c>
       <c r="R80">
-        <v>47.5</v>
+        <v>42</v>
       </c>
       <c r="S80">
-        <f t="shared" si="45"/>
+        <f>MEDIAN(0,255,ROUND(R80/20+SQRT(H80)/40+SQRT(O80)/2+(SQRT(Q80)-SQRT(185)), 0))</f>
         <v>7</v>
       </c>
       <c r="T80">
@@ -33211,108 +33199,108 @@
         <v>21875</v>
       </c>
       <c r="U80">
-        <f t="shared" si="47"/>
-        <v>4</v>
+        <f>MEDIAN(0,255,ROUND(SQRT(H80)/200+SQRT(O80)/2+(SQRT(Q80)-SQRT(185)),0))</f>
+        <v>5</v>
       </c>
       <c r="V80">
         <f t="shared" si="48"/>
-        <v>900</v>
-      </c>
-    </row>
-    <row r="81" spans="1:22" x14ac:dyDescent="0.3">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="81" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>476</v>
+        <v>545</v>
       </c>
       <c r="E81">
-        <v>1981</v>
+        <v>2012</v>
       </c>
       <c r="F81">
         <v>30</v>
       </c>
-      <c r="G81" t="s">
-        <v>87</v>
-      </c>
       <c r="H81">
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="I81" t="s">
-        <v>109</v>
-      </c>
-      <c r="O81">
-        <v>68</v>
-      </c>
-      <c r="P81">
-        <v>12</v>
-      </c>
-      <c r="Q81">
-        <v>200</v>
+        <v>546</v>
+      </c>
+      <c r="O81" t="s">
+        <v>547</v>
+      </c>
+      <c r="P81" t="s">
+        <v>564</v>
+      </c>
+      <c r="Q81" t="s">
+        <v>548</v>
       </c>
       <c r="R81">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="S81">
-        <f>MEDIAN(0,255,ROUND(R81/20+SQRT(H81)/40+SQRT(O81)/2+(SQRT(Q81)-SQRT(185)), 0))</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="T81">
         <f t="shared" si="46"/>
-        <v>21875</v>
+        <v>25000</v>
       </c>
       <c r="U81">
-        <f>MEDIAN(0,255,ROUND(SQRT(H81)/200+SQRT(O81)/2+(SQRT(Q81)-SQRT(185)),0))</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="V81">
         <f t="shared" si="48"/>
-        <v>1125</v>
-      </c>
-    </row>
-    <row r="82" spans="1:22" x14ac:dyDescent="0.3">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="82" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
       <c r="E82">
-        <v>2012</v>
+        <v>1998</v>
       </c>
       <c r="F82">
         <v>30</v>
       </c>
+      <c r="G82" t="s">
+        <v>87</v>
+      </c>
       <c r="H82">
-        <v>160</v>
+        <v>120</v>
       </c>
       <c r="I82" t="s">
-        <v>546</v>
-      </c>
-      <c r="O82" t="s">
-        <v>547</v>
-      </c>
-      <c r="P82" t="s">
-        <v>549</v>
-      </c>
-      <c r="Q82" t="s">
-        <v>548</v>
+        <v>86</v>
+      </c>
+      <c r="O82">
+        <v>42</v>
+      </c>
+      <c r="P82">
+        <v>16</v>
+      </c>
+      <c r="Q82">
+        <v>400</v>
       </c>
       <c r="R82">
         <v>46</v>
       </c>
       <c r="S82">
-        <v>8</v>
+        <f t="shared" ref="S82:S85" si="53">MEDIAN(0,255,ROUND(R82/20+SQRT(H82)/40+SQRT(O82)/2+(SQRT(Q82)-SQRT(185)), 0))</f>
+        <v>12</v>
       </c>
       <c r="T82">
         <f t="shared" si="46"/>
-        <v>25000</v>
+        <v>37500</v>
       </c>
       <c r="U82">
-        <v>6</v>
+        <f t="shared" ref="U82:U84" si="54">MEDIAN(0,255,ROUND(SQRT(H82)/200+SQRT(O82)/2+(SQRT(Q82)-SQRT(185)),0))</f>
+        <v>10</v>
       </c>
       <c r="V82">
         <f t="shared" si="48"/>
-        <v>1350</v>
-      </c>
-    </row>
-    <row r="83" spans="1:22" x14ac:dyDescent="0.3">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="83" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>550</v>
+        <v>561</v>
       </c>
       <c r="E83">
         <v>1998</v>
@@ -33330,35 +33318,35 @@
         <v>86</v>
       </c>
       <c r="O83">
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="P83">
         <v>16</v>
       </c>
       <c r="Q83">
-        <v>400</v>
+        <v>240</v>
       </c>
       <c r="R83">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="S83">
-        <f t="shared" ref="S83:S86" si="53">MEDIAN(0,255,ROUND(R83/20+SQRT(H83)/40+SQRT(O83)/2+(SQRT(Q83)-SQRT(185)), 0))</f>
-        <v>12</v>
+        <f t="shared" si="53"/>
+        <v>9</v>
       </c>
       <c r="T83">
         <f t="shared" si="46"/>
-        <v>37500</v>
+        <v>28125</v>
       </c>
       <c r="U83">
-        <f t="shared" ref="U83:U86" si="54">MEDIAN(0,255,ROUND(SQRT(H83)/200+SQRT(O83)/2+(SQRT(Q83)-SQRT(185)),0))</f>
-        <v>10</v>
+        <f t="shared" si="54"/>
+        <v>7</v>
       </c>
       <c r="V83">
         <f t="shared" si="48"/>
-        <v>2250</v>
-      </c>
-    </row>
-    <row r="84" spans="1:22" x14ac:dyDescent="0.3">
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="84" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>562</v>
       </c>
@@ -33372,46 +33360,34 @@
         <v>87</v>
       </c>
       <c r="H84">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I84" t="s">
         <v>86</v>
       </c>
-      <c r="O84">
-        <v>88</v>
-      </c>
-      <c r="P84">
-        <v>16</v>
-      </c>
-      <c r="Q84">
-        <v>240</v>
-      </c>
-      <c r="R84">
-        <v>45</v>
-      </c>
       <c r="S84">
         <f t="shared" si="53"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="T84">
         <f t="shared" si="46"/>
-        <v>28125</v>
+        <v>0</v>
       </c>
       <c r="U84">
         <f t="shared" si="54"/>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="V84">
         <f t="shared" si="48"/>
-        <v>1575</v>
-      </c>
-    </row>
-    <row r="85" spans="1:22" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>563</v>
       </c>
       <c r="E85">
-        <v>1998</v>
+        <v>1992</v>
       </c>
       <c r="F85">
         <v>30</v>
@@ -33420,80 +33396,97 @@
         <v>87</v>
       </c>
       <c r="H85">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I85" t="s">
-        <v>86</v>
+        <v>109</v>
+      </c>
+      <c r="O85">
+        <v>72</v>
+      </c>
+      <c r="P85">
+        <v>16</v>
+      </c>
+      <c r="Q85">
+        <v>200</v>
+      </c>
+      <c r="R85">
+        <v>49</v>
       </c>
       <c r="S85">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T85">
         <f t="shared" si="46"/>
-        <v>0</v>
+        <v>25000</v>
       </c>
       <c r="U85">
-        <f t="shared" si="54"/>
-        <v>0</v>
+        <f>MEDIAN(0,255,ROUND(SQRT(H85)/200+SQRT(O85)/2+(SQRT(Q85)-SQRT(185)),0))</f>
+        <v>5</v>
       </c>
       <c r="V85">
         <f t="shared" si="48"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:22" x14ac:dyDescent="0.3">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="86" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>564</v>
+        <v>301</v>
+      </c>
+      <c r="B86" t="s">
+        <v>302</v>
+      </c>
+      <c r="D86" t="s">
+        <v>301</v>
       </c>
       <c r="E86">
-        <v>1992</v>
+        <v>1993</v>
       </c>
       <c r="F86">
         <v>30</v>
       </c>
-      <c r="G86" t="s">
-        <v>87</v>
+      <c r="G86">
+        <v>20</v>
       </c>
       <c r="H86">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="I86" t="s">
-        <v>109</v>
-      </c>
-      <c r="O86">
-        <v>72</v>
-      </c>
-      <c r="P86">
-        <v>16</v>
-      </c>
-      <c r="Q86">
-        <v>200</v>
+        <v>303</v>
+      </c>
+      <c r="O86" t="s">
+        <v>565</v>
+      </c>
+      <c r="P86" t="s">
+        <v>564</v>
+      </c>
+      <c r="Q86" t="s">
+        <v>548</v>
       </c>
       <c r="R86">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="S86">
-        <f t="shared" si="53"/>
         <v>8</v>
       </c>
       <c r="T86">
-        <f t="shared" si="46"/>
+        <f>S86*50000/16</f>
         <v>25000</v>
       </c>
       <c r="U86">
-        <f>MEDIAN(0,255,ROUND(SQRT(H86)/200+SQRT(O86)/2+(SQRT(Q86)-SQRT(185)),0))</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="V86">
-        <f t="shared" si="48"/>
-        <v>1125</v>
-      </c>
+        <f>U86*300/16*12</f>
+        <v>1350</v>
+      </c>
+      <c r="AA86" t="s">
+        <v>344</v>
+      </c>
+      <c r="AB86" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="AB48:AB57"/>
-  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add syz25 and srz25
</commit_message>
<xml_diff>
--- a/docs/China Set Trains.xlsx
+++ b/docs/China Set Trains.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CNS\CNST\local\China-Set-Trains\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6AA8F8-F353-422A-8397-0EC9CBC55550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9865968-CC1F-4074-B7E7-449F8D74C6AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Loco" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2105" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2109" uniqueCount="597">
   <si>
     <t>name</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2313,6 +2313,14 @@
   </si>
   <si>
     <t>ky</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SYZ25</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SRZ25</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -8935,8 +8943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB4625FC-685F-4E56-AE60-F05D51350408}">
   <dimension ref="A1:AG356"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A331" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A198" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="V355" sqref="V355:AA356"/>
     </sheetView>
   </sheetViews>
@@ -32612,11 +32620,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{392CFCAE-41E9-4295-93E2-AE0B308CC62A}">
-  <dimension ref="A1:AB94"/>
+  <dimension ref="A1:AB96"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S94" sqref="S94"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I94" sqref="I94:I96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -37296,7 +37304,7 @@
         <v>301</v>
       </c>
       <c r="N88" t="str">
-        <f t="shared" ref="N88:N94" si="58">IF(M88&gt;=26.5,"E",IF(M88&gt;23.5,"D",IF(M88&gt;19.5,"C",IF(M88&gt;14.5,"B","A"))))</f>
+        <f t="shared" ref="N88:N96" si="58">IF(M88&gt;=26.5,"E",IF(M88&gt;23.5,"D",IF(M88&gt;19.5,"C",IF(M88&gt;14.5,"B","A"))))</f>
         <v>A</v>
       </c>
       <c r="O88" t="s">
@@ -37315,14 +37323,14 @@
         <v>17</v>
       </c>
       <c r="T88">
-        <f t="shared" ref="T88:T94" si="59">S88*50000/16</f>
+        <f t="shared" ref="T88:T96" si="59">S88*50000/16</f>
         <v>53125</v>
       </c>
       <c r="U88">
         <v>11</v>
       </c>
       <c r="V88">
-        <f t="shared" ref="V88:V94" si="60">U88*300/16*12</f>
+        <f t="shared" ref="V88:V96" si="60">U88*300/16*12</f>
         <v>2475</v>
       </c>
       <c r="AA88" t="s">
@@ -37366,7 +37374,7 @@
         <v>46.8</v>
       </c>
       <c r="S89">
-        <f t="shared" ref="S89:S94" si="61">MEDIAN(0,255,ROUND(R89/20+SQRT(H89)/40+SQRT(O89)/2+(SQRT(Q89)-SQRT(185)), 0))</f>
+        <f t="shared" ref="S89:S96" si="61">MEDIAN(0,255,ROUND(R89/20+SQRT(H89)/40+SQRT(O89)/2+(SQRT(Q89)-SQRT(185)), 0))</f>
         <v>7</v>
       </c>
       <c r="T89">
@@ -37374,7 +37382,7 @@
         <v>21875</v>
       </c>
       <c r="U89">
-        <f t="shared" ref="U89:U94" si="62">MEDIAN(0,255,ROUND(SQRT(H89)/200+SQRT(O89)/2+(SQRT(Q89)-SQRT(185)),0))</f>
+        <f t="shared" ref="U89:U96" si="62">MEDIAN(0,255,ROUND(SQRT(H89)/200+SQRT(O89)/2+(SQRT(Q89)-SQRT(185)),0))</f>
         <v>5</v>
       </c>
       <c r="V89">
@@ -37652,6 +37660,116 @@
       <c r="V94">
         <f t="shared" si="60"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>595</v>
+      </c>
+      <c r="E95">
+        <v>1987</v>
+      </c>
+      <c r="F95">
+        <v>30</v>
+      </c>
+      <c r="G95">
+        <v>20</v>
+      </c>
+      <c r="H95">
+        <v>120</v>
+      </c>
+      <c r="I95" t="s">
+        <v>290</v>
+      </c>
+      <c r="M95">
+        <v>17</v>
+      </c>
+      <c r="N95" t="str">
+        <f t="shared" si="58"/>
+        <v>B</v>
+      </c>
+      <c r="O95">
+        <v>176</v>
+      </c>
+      <c r="P95">
+        <v>24</v>
+      </c>
+      <c r="Q95">
+        <v>200</v>
+      </c>
+      <c r="R95">
+        <v>50</v>
+      </c>
+      <c r="S95">
+        <f t="shared" si="61"/>
+        <v>10</v>
+      </c>
+      <c r="T95">
+        <f t="shared" si="59"/>
+        <v>31250</v>
+      </c>
+      <c r="U95">
+        <f t="shared" si="62"/>
+        <v>7</v>
+      </c>
+      <c r="V95">
+        <f t="shared" si="60"/>
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="96" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>596</v>
+      </c>
+      <c r="E96">
+        <v>1987</v>
+      </c>
+      <c r="F96">
+        <v>30</v>
+      </c>
+      <c r="G96">
+        <v>20</v>
+      </c>
+      <c r="H96">
+        <v>120</v>
+      </c>
+      <c r="I96" t="s">
+        <v>290</v>
+      </c>
+      <c r="M96">
+        <v>17</v>
+      </c>
+      <c r="N96" t="str">
+        <f t="shared" si="58"/>
+        <v>B</v>
+      </c>
+      <c r="O96">
+        <v>108</v>
+      </c>
+      <c r="P96">
+        <v>24</v>
+      </c>
+      <c r="Q96">
+        <v>240</v>
+      </c>
+      <c r="R96">
+        <v>52</v>
+      </c>
+      <c r="S96">
+        <f t="shared" si="61"/>
+        <v>10</v>
+      </c>
+      <c r="T96">
+        <f t="shared" si="59"/>
+        <v>31250</v>
+      </c>
+      <c r="U96">
+        <f t="shared" si="62"/>
+        <v>7</v>
+      </c>
+      <c r="V96">
+        <f t="shared" si="60"/>
+        <v>1575</v>
       </c>
     </row>
   </sheetData>

</xml_diff>